<commit_message>
Program scale-up reader initialised
Still needs some work
</commit_message>
<xml_diff>
--- a/autumn/xls/programs_fiji.xlsx
+++ b/autumn/xls/programs_fiji.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="255" windowWidth="20370" windowHeight="7590" tabRatio="807"/>
+    <workbookView xWindow="120" yWindow="255" windowWidth="20370" windowHeight="7590" tabRatio="807" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="miscellaneous_constants" sheetId="1" r:id="rId1"/>
+    <sheet name="programs" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
   <si>
     <t>program_proportion_detect</t>
   </si>
@@ -83,6 +84,24 @@
   </si>
   <si>
     <t>tb_n_contact</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>program_prop_vaccination</t>
+  </si>
+  <si>
+    <t>program_prop_detect</t>
+  </si>
+  <si>
+    <t>program_prop_algorithm_sensitivity</t>
+  </si>
+  <si>
+    <t>program_prop_firstline_dst</t>
+  </si>
+  <si>
+    <t>program_prop_secondline_dst</t>
   </si>
 </sst>
 </file>
@@ -91,7 +110,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="0.00000"/>
+    <numFmt numFmtId="165" formatCode="0.00000"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -893,13 +912,13 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="1" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="165" fontId="1" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1872,7 +1891,7 @@
   </sheetPr>
   <dimension ref="A1:B23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -2066,4 +2085,234 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AX7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K19" sqref="K19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="34.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="12" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="50" width="6.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1">
+        <v>1920</v>
+      </c>
+      <c r="C1">
+        <v>1930</v>
+      </c>
+      <c r="D1">
+        <v>1940</v>
+      </c>
+      <c r="E1">
+        <v>1950</v>
+      </c>
+      <c r="F1">
+        <v>1955</v>
+      </c>
+      <c r="G1">
+        <v>1960</v>
+      </c>
+      <c r="H1">
+        <v>1965</v>
+      </c>
+      <c r="I1">
+        <v>1970</v>
+      </c>
+      <c r="J1">
+        <v>1975</v>
+      </c>
+      <c r="K1">
+        <v>1976</v>
+      </c>
+      <c r="L1">
+        <v>1977</v>
+      </c>
+      <c r="M1">
+        <v>1978</v>
+      </c>
+      <c r="N1">
+        <v>1979</v>
+      </c>
+      <c r="O1">
+        <v>1980</v>
+      </c>
+      <c r="P1">
+        <v>1981</v>
+      </c>
+      <c r="Q1">
+        <v>1982</v>
+      </c>
+      <c r="R1">
+        <v>1983</v>
+      </c>
+      <c r="S1">
+        <v>1984</v>
+      </c>
+      <c r="T1">
+        <v>1985</v>
+      </c>
+      <c r="U1">
+        <v>1986</v>
+      </c>
+      <c r="V1">
+        <v>1987</v>
+      </c>
+      <c r="W1">
+        <v>1988</v>
+      </c>
+      <c r="X1">
+        <v>1989</v>
+      </c>
+      <c r="Y1">
+        <v>1990</v>
+      </c>
+      <c r="Z1">
+        <v>1991</v>
+      </c>
+      <c r="AA1">
+        <v>1992</v>
+      </c>
+      <c r="AB1">
+        <v>1993</v>
+      </c>
+      <c r="AC1">
+        <v>1994</v>
+      </c>
+      <c r="AD1">
+        <v>1995</v>
+      </c>
+      <c r="AE1">
+        <v>1996</v>
+      </c>
+      <c r="AF1">
+        <v>1997</v>
+      </c>
+      <c r="AG1">
+        <v>1998</v>
+      </c>
+      <c r="AH1">
+        <v>1999</v>
+      </c>
+      <c r="AI1">
+        <v>2000</v>
+      </c>
+      <c r="AJ1">
+        <v>2001</v>
+      </c>
+      <c r="AK1">
+        <v>2002</v>
+      </c>
+      <c r="AL1">
+        <v>2003</v>
+      </c>
+      <c r="AM1">
+        <v>2004</v>
+      </c>
+      <c r="AN1">
+        <v>2005</v>
+      </c>
+      <c r="AO1">
+        <v>2006</v>
+      </c>
+      <c r="AP1">
+        <v>2007</v>
+      </c>
+      <c r="AQ1">
+        <v>2008</v>
+      </c>
+      <c r="AR1">
+        <v>2009</v>
+      </c>
+      <c r="AS1">
+        <v>2010</v>
+      </c>
+      <c r="AT1">
+        <v>2011</v>
+      </c>
+      <c r="AU1">
+        <v>2012</v>
+      </c>
+      <c r="AV1">
+        <v>2013</v>
+      </c>
+      <c r="AW1">
+        <v>2014</v>
+      </c>
+      <c r="AX1">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="2" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="H3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4">
+        <v>5</v>
+      </c>
+      <c r="G4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5">
+        <v>3</v>
+      </c>
+      <c r="H5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Code to combine inputs and loaded data
So far only for vaccination
</commit_message>
<xml_diff>
--- a/autumn/xls/programs_fiji.xlsx
+++ b/autumn/xls/programs_fiji.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="32">
   <si>
     <t>program_proportion_detect</t>
   </si>
@@ -86,9 +86,6 @@
     <t>tb_n_contact</t>
   </si>
   <si>
-    <t>year</t>
-  </si>
-  <si>
     <t>program_prop_vaccination</t>
   </si>
   <si>
@@ -102,6 +99,18 @@
   </si>
   <si>
     <t>program_prop_secondline_dst</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>load_data</t>
+  </si>
+  <si>
+    <t>program</t>
   </si>
 </sst>
 </file>
@@ -2089,226 +2098,248 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AX7"/>
+  <dimension ref="A1:AY7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="34.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="12" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="50" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="13" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="51" width="6.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1">
+        <v>1920</v>
+      </c>
+      <c r="D1">
+        <v>1930</v>
+      </c>
+      <c r="E1">
+        <v>1940</v>
+      </c>
+      <c r="F1">
+        <v>1950</v>
+      </c>
+      <c r="G1">
+        <v>1955</v>
+      </c>
+      <c r="H1">
+        <v>1960</v>
+      </c>
+      <c r="I1">
+        <v>1965</v>
+      </c>
+      <c r="J1">
+        <v>1970</v>
+      </c>
+      <c r="K1">
+        <v>1975</v>
+      </c>
+      <c r="L1">
+        <v>1976</v>
+      </c>
+      <c r="M1">
+        <v>1977</v>
+      </c>
+      <c r="N1">
+        <v>1978</v>
+      </c>
+      <c r="O1">
+        <v>1979</v>
+      </c>
+      <c r="P1">
+        <v>1980</v>
+      </c>
+      <c r="Q1">
+        <v>1981</v>
+      </c>
+      <c r="R1">
+        <v>1982</v>
+      </c>
+      <c r="S1">
+        <v>1983</v>
+      </c>
+      <c r="T1">
+        <v>1984</v>
+      </c>
+      <c r="U1">
+        <v>1985</v>
+      </c>
+      <c r="V1">
+        <v>1986</v>
+      </c>
+      <c r="W1">
+        <v>1987</v>
+      </c>
+      <c r="X1">
+        <v>1988</v>
+      </c>
+      <c r="Y1">
+        <v>1989</v>
+      </c>
+      <c r="Z1">
+        <v>1990</v>
+      </c>
+      <c r="AA1">
+        <v>1991</v>
+      </c>
+      <c r="AB1">
+        <v>1992</v>
+      </c>
+      <c r="AC1">
+        <v>1993</v>
+      </c>
+      <c r="AD1">
+        <v>1994</v>
+      </c>
+      <c r="AE1">
+        <v>1995</v>
+      </c>
+      <c r="AF1">
+        <v>1996</v>
+      </c>
+      <c r="AG1">
+        <v>1997</v>
+      </c>
+      <c r="AH1">
+        <v>1998</v>
+      </c>
+      <c r="AI1">
+        <v>1999</v>
+      </c>
+      <c r="AJ1">
+        <v>2000</v>
+      </c>
+      <c r="AK1">
+        <v>2001</v>
+      </c>
+      <c r="AL1">
+        <v>2002</v>
+      </c>
+      <c r="AM1">
+        <v>2003</v>
+      </c>
+      <c r="AN1">
+        <v>2004</v>
+      </c>
+      <c r="AO1">
+        <v>2005</v>
+      </c>
+      <c r="AP1">
+        <v>2006</v>
+      </c>
+      <c r="AQ1">
+        <v>2007</v>
+      </c>
+      <c r="AR1">
+        <v>2008</v>
+      </c>
+      <c r="AS1">
+        <v>2009</v>
+      </c>
+      <c r="AT1">
+        <v>2010</v>
+      </c>
+      <c r="AU1">
+        <v>2011</v>
+      </c>
+      <c r="AV1">
+        <v>2012</v>
+      </c>
+      <c r="AW1">
+        <v>2013</v>
+      </c>
+      <c r="AX1">
+        <v>2014</v>
+      </c>
+      <c r="AY1">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="2" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>23</v>
       </c>
-      <c r="B1">
-        <v>1920</v>
-      </c>
-      <c r="C1">
-        <v>1930</v>
-      </c>
-      <c r="D1">
-        <v>1940</v>
-      </c>
-      <c r="E1">
-        <v>1950</v>
-      </c>
-      <c r="F1">
-        <v>1955</v>
-      </c>
-      <c r="G1">
-        <v>1960</v>
-      </c>
-      <c r="H1">
-        <v>1965</v>
-      </c>
-      <c r="I1">
-        <v>1970</v>
-      </c>
-      <c r="J1">
-        <v>1975</v>
-      </c>
-      <c r="K1">
-        <v>1976</v>
-      </c>
-      <c r="L1">
-        <v>1977</v>
-      </c>
-      <c r="M1">
-        <v>1978</v>
-      </c>
-      <c r="N1">
-        <v>1979</v>
-      </c>
-      <c r="O1">
-        <v>1980</v>
-      </c>
-      <c r="P1">
-        <v>1981</v>
-      </c>
-      <c r="Q1">
-        <v>1982</v>
-      </c>
-      <c r="R1">
-        <v>1983</v>
-      </c>
-      <c r="S1">
-        <v>1984</v>
-      </c>
-      <c r="T1">
-        <v>1985</v>
-      </c>
-      <c r="U1">
-        <v>1986</v>
-      </c>
-      <c r="V1">
-        <v>1987</v>
-      </c>
-      <c r="W1">
-        <v>1988</v>
-      </c>
-      <c r="X1">
-        <v>1989</v>
-      </c>
-      <c r="Y1">
-        <v>1990</v>
-      </c>
-      <c r="Z1">
-        <v>1991</v>
-      </c>
-      <c r="AA1">
-        <v>1992</v>
-      </c>
-      <c r="AB1">
-        <v>1993</v>
-      </c>
-      <c r="AC1">
-        <v>1994</v>
-      </c>
-      <c r="AD1">
-        <v>1995</v>
-      </c>
-      <c r="AE1">
-        <v>1996</v>
-      </c>
-      <c r="AF1">
-        <v>1997</v>
-      </c>
-      <c r="AG1">
-        <v>1998</v>
-      </c>
-      <c r="AH1">
-        <v>1999</v>
-      </c>
-      <c r="AI1">
-        <v>2000</v>
-      </c>
-      <c r="AJ1">
-        <v>2001</v>
-      </c>
-      <c r="AK1">
-        <v>2002</v>
-      </c>
-      <c r="AL1">
-        <v>2003</v>
-      </c>
-      <c r="AM1">
-        <v>2004</v>
-      </c>
-      <c r="AN1">
-        <v>2005</v>
-      </c>
-      <c r="AO1">
-        <v>2006</v>
-      </c>
-      <c r="AP1">
-        <v>2007</v>
-      </c>
-      <c r="AQ1">
-        <v>2008</v>
-      </c>
-      <c r="AR1">
-        <v>2009</v>
-      </c>
-      <c r="AS1">
-        <v>2010</v>
-      </c>
-      <c r="AT1">
-        <v>2011</v>
-      </c>
-      <c r="AU1">
-        <v>2012</v>
-      </c>
-      <c r="AV1">
-        <v>2013</v>
-      </c>
-      <c r="AW1">
-        <v>2014</v>
-      </c>
-      <c r="AX1">
-        <v>2015</v>
-      </c>
-    </row>
-    <row r="2" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>24</v>
       </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="G2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="I3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>25</v>
       </c>
-      <c r="C3">
-        <v>2</v>
-      </c>
-      <c r="H3">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="4" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D4">
+      <c r="B4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4">
         <v>5</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>18</v>
       </c>
-      <c r="E5">
+      <c r="B5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5">
         <v>3</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="7" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>28</v>
-      </c>
-      <c r="F7">
+      <c r="B7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G7">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Working towards external program setting
Nearly have half the programs set through the spreadsheet now.
</commit_message>
<xml_diff>
--- a/autumn/xls/programs_fiji.xlsx
+++ b/autumn/xls/programs_fiji.xlsx
@@ -9,13 +9,14 @@
   <sheets>
     <sheet name="miscellaneous_constants" sheetId="1" r:id="rId1"/>
     <sheet name="programs" sheetId="2" r:id="rId2"/>
+    <sheet name="dropdown_lists" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="39">
   <si>
     <t>program_proportion_detect</t>
   </si>
@@ -111,6 +112,27 @@
   </si>
   <si>
     <t>program</t>
+  </si>
+  <si>
+    <t>program_cost_vaccination</t>
+  </si>
+  <si>
+    <t>program_cost_detect</t>
+  </si>
+  <si>
+    <t>program_cost_algorithm_sensitivity</t>
+  </si>
+  <si>
+    <t>program_cost_lowquality</t>
+  </si>
+  <si>
+    <t>program_cost_firstline_dst</t>
+  </si>
+  <si>
+    <t>program_cost_secondline_dst</t>
+  </si>
+  <si>
+    <t>na</t>
   </si>
 </sst>
 </file>
@@ -121,7 +143,7 @@
     <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -175,8 +197,36 @@
       <name val="Courier New"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="3" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="5" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="6" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -200,8 +250,14 @@
         <bgColor auto="1"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -248,6 +304,50 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="664">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -915,7 +1015,7 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -931,6 +1031,13 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="664">
     <cellStyle name="Comma 2" xfId="5"/>
@@ -2098,249 +2205,435 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AY7"/>
+  <dimension ref="A1:AZ13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="13" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="51" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" style="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.42578125" style="7" customWidth="1"/>
+    <col min="5" max="8" width="7.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.42578125" style="7" customWidth="1"/>
+    <col min="10" max="47" width="7.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="6.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="49" max="52" width="7.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="53" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:51" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:52" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="C1">
+      <c r="C1" s="13">
+        <v>1850</v>
+      </c>
+      <c r="D1" s="13">
         <v>1920</v>
       </c>
-      <c r="D1">
+      <c r="E1" s="13">
         <v>1930</v>
       </c>
-      <c r="E1">
+      <c r="F1" s="13">
         <v>1940</v>
       </c>
-      <c r="F1">
+      <c r="G1" s="13">
         <v>1950</v>
       </c>
-      <c r="G1">
+      <c r="H1" s="13">
         <v>1955</v>
       </c>
-      <c r="H1">
+      <c r="I1" s="13">
         <v>1960</v>
       </c>
-      <c r="I1">
+      <c r="J1" s="13">
         <v>1965</v>
       </c>
-      <c r="J1">
+      <c r="K1" s="13">
         <v>1970</v>
       </c>
-      <c r="K1">
+      <c r="L1" s="13">
         <v>1975</v>
       </c>
-      <c r="L1">
+      <c r="M1" s="13">
         <v>1976</v>
       </c>
-      <c r="M1">
+      <c r="N1" s="13">
         <v>1977</v>
       </c>
-      <c r="N1">
+      <c r="O1" s="13">
         <v>1978</v>
       </c>
-      <c r="O1">
+      <c r="P1" s="13">
         <v>1979</v>
       </c>
-      <c r="P1">
+      <c r="Q1" s="13">
         <v>1980</v>
       </c>
-      <c r="Q1">
+      <c r="R1" s="13">
         <v>1981</v>
       </c>
-      <c r="R1">
+      <c r="S1" s="13">
         <v>1982</v>
       </c>
-      <c r="S1">
+      <c r="T1" s="13">
         <v>1983</v>
       </c>
-      <c r="T1">
+      <c r="U1" s="13">
         <v>1984</v>
       </c>
-      <c r="U1">
+      <c r="V1" s="13">
         <v>1985</v>
       </c>
-      <c r="V1">
+      <c r="W1" s="13">
         <v>1986</v>
       </c>
-      <c r="W1">
+      <c r="X1" s="13">
         <v>1987</v>
       </c>
-      <c r="X1">
+      <c r="Y1" s="13">
         <v>1988</v>
       </c>
-      <c r="Y1">
+      <c r="Z1" s="13">
         <v>1989</v>
       </c>
-      <c r="Z1">
+      <c r="AA1" s="13">
         <v>1990</v>
       </c>
-      <c r="AA1">
+      <c r="AB1" s="13">
         <v>1991</v>
       </c>
-      <c r="AB1">
+      <c r="AC1" s="13">
         <v>1992</v>
       </c>
-      <c r="AC1">
+      <c r="AD1" s="13">
         <v>1993</v>
       </c>
-      <c r="AD1">
+      <c r="AE1" s="13">
         <v>1994</v>
       </c>
-      <c r="AE1">
+      <c r="AF1" s="13">
         <v>1995</v>
       </c>
-      <c r="AF1">
+      <c r="AG1" s="13">
         <v>1996</v>
       </c>
-      <c r="AG1">
+      <c r="AH1" s="13">
         <v>1997</v>
       </c>
-      <c r="AH1">
+      <c r="AI1" s="13">
         <v>1998</v>
       </c>
-      <c r="AI1">
+      <c r="AJ1" s="13">
         <v>1999</v>
       </c>
-      <c r="AJ1">
+      <c r="AK1" s="13">
         <v>2000</v>
       </c>
-      <c r="AK1">
+      <c r="AL1" s="13">
         <v>2001</v>
       </c>
-      <c r="AL1">
+      <c r="AM1" s="13">
         <v>2002</v>
       </c>
-      <c r="AM1">
+      <c r="AN1" s="13">
         <v>2003</v>
       </c>
-      <c r="AN1">
+      <c r="AO1" s="13">
         <v>2004</v>
       </c>
-      <c r="AO1">
+      <c r="AP1" s="13">
         <v>2005</v>
       </c>
-      <c r="AP1">
+      <c r="AQ1" s="13">
         <v>2006</v>
       </c>
-      <c r="AQ1">
+      <c r="AR1" s="13">
         <v>2007</v>
       </c>
-      <c r="AR1">
+      <c r="AS1" s="13">
         <v>2008</v>
       </c>
-      <c r="AS1">
+      <c r="AT1" s="13">
         <v>2009</v>
       </c>
-      <c r="AT1">
+      <c r="AU1" s="13">
         <v>2010</v>
       </c>
-      <c r="AU1">
+      <c r="AV1" s="13">
         <v>2011</v>
       </c>
-      <c r="AV1">
+      <c r="AW1" s="13">
         <v>2012</v>
       </c>
-      <c r="AW1">
+      <c r="AX1" s="13">
         <v>2013</v>
       </c>
-      <c r="AX1">
+      <c r="AY1" s="13">
         <v>2014</v>
       </c>
-      <c r="AY1">
+      <c r="AZ1" s="13">
         <v>2015</v>
       </c>
     </row>
-    <row r="2" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="7">
+        <v>0</v>
+      </c>
+      <c r="G2" s="7">
+        <v>0</v>
+      </c>
+      <c r="I2" s="7">
+        <v>10</v>
+      </c>
+      <c r="Q2" s="8"/>
+      <c r="R2" s="8"/>
+      <c r="S2" s="8"/>
+      <c r="T2" s="8"/>
+      <c r="U2" s="8"/>
+      <c r="V2" s="8"/>
+      <c r="W2" s="8"/>
+      <c r="X2" s="8"/>
+      <c r="Y2" s="8"/>
+      <c r="Z2" s="8"/>
+      <c r="AA2" s="8"/>
+      <c r="AB2" s="8"/>
+      <c r="AC2" s="8"/>
+      <c r="AD2" s="8"/>
+      <c r="AE2" s="8"/>
+      <c r="AF2" s="8"/>
+      <c r="AG2" s="8"/>
+      <c r="AH2" s="8"/>
+      <c r="AI2" s="8"/>
+      <c r="AJ2" s="8"/>
+      <c r="AK2" s="8"/>
+      <c r="AL2" s="8"/>
+      <c r="AM2" s="8"/>
+      <c r="AN2" s="8"/>
+      <c r="AO2" s="8"/>
+      <c r="AP2" s="8"/>
+      <c r="AQ2" s="8"/>
+      <c r="AR2" s="8"/>
+      <c r="AS2" s="8"/>
+      <c r="AT2" s="8"/>
+      <c r="AU2" s="8"/>
+      <c r="AV2" s="8"/>
+      <c r="AW2" s="8"/>
+      <c r="AX2" s="8"/>
+      <c r="AY2" s="8"/>
+    </row>
+    <row r="3" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="G3" s="7">
+        <v>0</v>
+      </c>
+      <c r="I3" s="7">
+        <v>10000000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="7">
+        <v>0</v>
+      </c>
+      <c r="E4" s="7">
+        <v>0</v>
+      </c>
+      <c r="J4" s="7">
+        <v>10</v>
+      </c>
+      <c r="S4" s="7">
+        <v>50</v>
+      </c>
+      <c r="AA4" s="8"/>
+      <c r="AB4" s="8"/>
+      <c r="AC4" s="8"/>
+      <c r="AD4" s="8"/>
+      <c r="AE4" s="8"/>
+      <c r="AF4" s="8"/>
+      <c r="AG4" s="8"/>
+      <c r="AH4" s="8"/>
+      <c r="AI4" s="8"/>
+      <c r="AJ4" s="8"/>
+      <c r="AK4" s="8"/>
+      <c r="AL4" s="8"/>
+      <c r="AM4" s="8"/>
+      <c r="AN4" s="8"/>
+      <c r="AO4" s="8"/>
+      <c r="AP4" s="8"/>
+      <c r="AQ4" s="8"/>
+      <c r="AR4" s="8"/>
+      <c r="AS4" s="8"/>
+      <c r="AT4" s="8"/>
+      <c r="AU4" s="8"/>
+      <c r="AV4" s="8"/>
+      <c r="AW4" s="8"/>
+      <c r="AX4" s="8"/>
+      <c r="AY4" s="8"/>
+    </row>
+    <row r="5" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="7">
+        <v>70</v>
+      </c>
+      <c r="F6" s="7">
+        <v>70</v>
+      </c>
+      <c r="I6" s="7">
+        <v>80</v>
+      </c>
+      <c r="Y6" s="7">
+        <v>82</v>
+      </c>
+      <c r="AL6" s="7">
+        <v>84</v>
+      </c>
+      <c r="AY6" s="7">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="7" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="G8" s="7">
+        <v>3</v>
+      </c>
+      <c r="J8" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A11" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A12" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="H12" s="7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A13" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>dropdown_lists!$A$2:$A$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>B2:B13</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:A4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2" t="s">
         <v>28</v>
       </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:51" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B3" t="s">
         <v>29</v>
       </c>
-      <c r="D3">
-        <v>2</v>
-      </c>
-      <c r="I3">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="4" spans="1:51" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B4" t="s">
-        <v>29</v>
-      </c>
-      <c r="E4">
-        <v>5</v>
-      </c>
-      <c r="H4">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:51" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" t="s">
-        <v>29</v>
-      </c>
-      <c r="F5">
-        <v>3</v>
-      </c>
-      <c r="I5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:51" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B6" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="7" spans="1:51" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>27</v>
-      </c>
-      <c r="B7" t="s">
-        <v>29</v>
-      </c>
-      <c r="G7">
-        <v>7</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Work on loading program data
Getting there, hope to have the model running again soon.
</commit_message>
<xml_diff>
--- a/autumn/xls/programs_fiji.xlsx
+++ b/autumn/xls/programs_fiji.xlsx
@@ -206,13 +206,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="5" tint="-0.499984740745262"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="6" tint="-0.499984740745262"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -225,8 +218,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="5" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -252,7 +253,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.249977111117893"/>
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1015,7 +1058,7 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1032,12 +1075,31 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="664">
     <cellStyle name="Comma 2" xfId="5"/>
@@ -2208,389 +2270,466 @@
   <dimension ref="A1:AZ13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="U5" sqref="U5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11" style="10" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="43.140625" style="32" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" style="8" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.42578125" style="7" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.42578125" style="7" customWidth="1"/>
-    <col min="5" max="8" width="7.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7" style="7" customWidth="1"/>
+    <col min="7" max="8" width="7.42578125" style="7" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="7.42578125" style="7" customWidth="1"/>
-    <col min="10" max="47" width="7.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="7.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.7109375" style="7" customWidth="1"/>
+    <col min="13" max="21" width="7.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="7.42578125" style="7" customWidth="1"/>
+    <col min="23" max="24" width="7.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="7.140625" style="7" customWidth="1"/>
+    <col min="26" max="47" width="7.42578125" style="7" bestFit="1" customWidth="1"/>
     <col min="48" max="48" width="6.28515625" style="7" bestFit="1" customWidth="1"/>
     <col min="49" max="52" width="7.42578125" style="7" bestFit="1" customWidth="1"/>
     <col min="53" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:52" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:52" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="13">
+      <c r="C1" s="11">
         <v>1850</v>
       </c>
-      <c r="D1" s="13">
+      <c r="D1" s="11">
         <v>1920</v>
       </c>
-      <c r="E1" s="13">
+      <c r="E1" s="11">
         <v>1930</v>
       </c>
-      <c r="F1" s="13">
+      <c r="F1" s="11">
         <v>1940</v>
       </c>
-      <c r="G1" s="13">
+      <c r="G1" s="11">
         <v>1950</v>
       </c>
-      <c r="H1" s="13">
+      <c r="H1" s="11">
         <v>1955</v>
       </c>
-      <c r="I1" s="13">
+      <c r="I1" s="11">
         <v>1960</v>
       </c>
-      <c r="J1" s="13">
+      <c r="J1" s="11">
         <v>1965</v>
       </c>
-      <c r="K1" s="13">
+      <c r="K1" s="11">
         <v>1970</v>
       </c>
-      <c r="L1" s="13">
+      <c r="L1" s="11">
         <v>1975</v>
       </c>
-      <c r="M1" s="13">
+      <c r="M1" s="11">
         <v>1976</v>
       </c>
-      <c r="N1" s="13">
+      <c r="N1" s="11">
         <v>1977</v>
       </c>
-      <c r="O1" s="13">
+      <c r="O1" s="11">
         <v>1978</v>
       </c>
-      <c r="P1" s="13">
+      <c r="P1" s="11">
         <v>1979</v>
       </c>
-      <c r="Q1" s="13">
+      <c r="Q1" s="11">
         <v>1980</v>
       </c>
-      <c r="R1" s="13">
+      <c r="R1" s="11">
         <v>1981</v>
       </c>
-      <c r="S1" s="13">
+      <c r="S1" s="11">
         <v>1982</v>
       </c>
-      <c r="T1" s="13">
+      <c r="T1" s="11">
         <v>1983</v>
       </c>
-      <c r="U1" s="13">
+      <c r="U1" s="11">
         <v>1984</v>
       </c>
-      <c r="V1" s="13">
+      <c r="V1" s="11">
         <v>1985</v>
       </c>
-      <c r="W1" s="13">
+      <c r="W1" s="11">
         <v>1986</v>
       </c>
-      <c r="X1" s="13">
+      <c r="X1" s="11">
         <v>1987</v>
       </c>
-      <c r="Y1" s="13">
+      <c r="Y1" s="11">
         <v>1988</v>
       </c>
-      <c r="Z1" s="13">
+      <c r="Z1" s="11">
         <v>1989</v>
       </c>
-      <c r="AA1" s="13">
+      <c r="AA1" s="11">
         <v>1990</v>
       </c>
-      <c r="AB1" s="13">
+      <c r="AB1" s="11">
         <v>1991</v>
       </c>
-      <c r="AC1" s="13">
+      <c r="AC1" s="11">
         <v>1992</v>
       </c>
-      <c r="AD1" s="13">
+      <c r="AD1" s="11">
         <v>1993</v>
       </c>
-      <c r="AE1" s="13">
+      <c r="AE1" s="11">
         <v>1994</v>
       </c>
-      <c r="AF1" s="13">
+      <c r="AF1" s="11">
         <v>1995</v>
       </c>
-      <c r="AG1" s="13">
+      <c r="AG1" s="11">
         <v>1996</v>
       </c>
-      <c r="AH1" s="13">
+      <c r="AH1" s="11">
         <v>1997</v>
       </c>
-      <c r="AI1" s="13">
+      <c r="AI1" s="11">
         <v>1998</v>
       </c>
-      <c r="AJ1" s="13">
+      <c r="AJ1" s="11">
         <v>1999</v>
       </c>
-      <c r="AK1" s="13">
+      <c r="AK1" s="11">
         <v>2000</v>
       </c>
-      <c r="AL1" s="13">
+      <c r="AL1" s="11">
         <v>2001</v>
       </c>
-      <c r="AM1" s="13">
+      <c r="AM1" s="11">
         <v>2002</v>
       </c>
-      <c r="AN1" s="13">
+      <c r="AN1" s="11">
         <v>2003</v>
       </c>
-      <c r="AO1" s="13">
+      <c r="AO1" s="11">
         <v>2004</v>
       </c>
-      <c r="AP1" s="13">
+      <c r="AP1" s="11">
         <v>2005</v>
       </c>
-      <c r="AQ1" s="13">
+      <c r="AQ1" s="11">
         <v>2006</v>
       </c>
-      <c r="AR1" s="13">
+      <c r="AR1" s="11">
         <v>2007</v>
       </c>
-      <c r="AS1" s="13">
+      <c r="AS1" s="11">
         <v>2008</v>
       </c>
-      <c r="AT1" s="13">
+      <c r="AT1" s="11">
         <v>2009</v>
       </c>
-      <c r="AU1" s="13">
+      <c r="AU1" s="11">
         <v>2010</v>
       </c>
-      <c r="AV1" s="13">
+      <c r="AV1" s="11">
         <v>2011</v>
       </c>
-      <c r="AW1" s="13">
+      <c r="AW1" s="11">
         <v>2012</v>
       </c>
-      <c r="AX1" s="13">
+      <c r="AX1" s="11">
         <v>2013</v>
       </c>
-      <c r="AY1" s="13">
+      <c r="AY1" s="11">
         <v>2014</v>
       </c>
-      <c r="AZ1" s="13">
+      <c r="AZ1" s="11">
         <v>2015</v>
       </c>
     </row>
-    <row r="2" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
+    <row r="2" spans="1:52" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="7">
+      <c r="C2" s="13">
         <v>0</v>
       </c>
-      <c r="G2" s="7">
+      <c r="G2" s="13">
         <v>0</v>
       </c>
-      <c r="I2" s="7">
+      <c r="I2" s="13">
+        <v>25</v>
+      </c>
+      <c r="L2" s="13">
+        <v>40</v>
+      </c>
+      <c r="Q2" s="14"/>
+      <c r="R2" s="14"/>
+      <c r="S2" s="14"/>
+      <c r="T2" s="14"/>
+      <c r="U2" s="14"/>
+      <c r="V2" s="14"/>
+      <c r="W2" s="14"/>
+      <c r="X2" s="14"/>
+      <c r="Y2" s="14"/>
+      <c r="Z2" s="14"/>
+      <c r="AA2" s="14"/>
+      <c r="AB2" s="14"/>
+      <c r="AC2" s="14"/>
+      <c r="AD2" s="14"/>
+      <c r="AE2" s="14"/>
+      <c r="AF2" s="14"/>
+      <c r="AG2" s="14"/>
+      <c r="AH2" s="14"/>
+      <c r="AI2" s="14"/>
+      <c r="AJ2" s="14"/>
+      <c r="AK2" s="14"/>
+      <c r="AL2" s="14"/>
+      <c r="AM2" s="14"/>
+      <c r="AN2" s="14"/>
+      <c r="AO2" s="14"/>
+      <c r="AP2" s="14"/>
+      <c r="AQ2" s="14"/>
+      <c r="AR2" s="14"/>
+      <c r="AS2" s="14"/>
+      <c r="AT2" s="14"/>
+      <c r="AU2" s="14"/>
+      <c r="AV2" s="14"/>
+      <c r="AW2" s="14"/>
+      <c r="AX2" s="14"/>
+      <c r="AY2" s="14"/>
+    </row>
+    <row r="3" spans="1:52" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="13">
+        <v>0</v>
+      </c>
+      <c r="G3" s="13">
+        <v>0</v>
+      </c>
+      <c r="I3" s="13">
+        <v>10000000</v>
+      </c>
+      <c r="L3" s="13">
+        <v>15040500</v>
+      </c>
+      <c r="V3" s="13">
+        <v>39034561</v>
+      </c>
+    </row>
+    <row r="4" spans="1:52" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="16">
+        <v>0</v>
+      </c>
+      <c r="E4" s="16">
+        <v>0</v>
+      </c>
+      <c r="J4" s="16">
         <v>10</v>
       </c>
-      <c r="Q2" s="8"/>
-      <c r="R2" s="8"/>
-      <c r="S2" s="8"/>
-      <c r="T2" s="8"/>
-      <c r="U2" s="8"/>
-      <c r="V2" s="8"/>
-      <c r="W2" s="8"/>
-      <c r="X2" s="8"/>
-      <c r="Y2" s="8"/>
-      <c r="Z2" s="8"/>
-      <c r="AA2" s="8"/>
-      <c r="AB2" s="8"/>
-      <c r="AC2" s="8"/>
-      <c r="AD2" s="8"/>
-      <c r="AE2" s="8"/>
-      <c r="AF2" s="8"/>
-      <c r="AG2" s="8"/>
-      <c r="AH2" s="8"/>
-      <c r="AI2" s="8"/>
-      <c r="AJ2" s="8"/>
-      <c r="AK2" s="8"/>
-      <c r="AL2" s="8"/>
-      <c r="AM2" s="8"/>
-      <c r="AN2" s="8"/>
-      <c r="AO2" s="8"/>
-      <c r="AP2" s="8"/>
-      <c r="AQ2" s="8"/>
-      <c r="AR2" s="8"/>
-      <c r="AS2" s="8"/>
-      <c r="AT2" s="8"/>
-      <c r="AU2" s="8"/>
-      <c r="AV2" s="8"/>
-      <c r="AW2" s="8"/>
-      <c r="AX2" s="8"/>
-      <c r="AY2" s="8"/>
-    </row>
-    <row r="3" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="B3" s="10" t="s">
+      <c r="S4" s="16">
+        <v>50</v>
+      </c>
+      <c r="AA4" s="17"/>
+      <c r="AB4" s="17"/>
+      <c r="AC4" s="17"/>
+      <c r="AD4" s="17"/>
+      <c r="AE4" s="17"/>
+      <c r="AF4" s="17"/>
+      <c r="AG4" s="17"/>
+      <c r="AH4" s="17"/>
+      <c r="AI4" s="17"/>
+      <c r="AJ4" s="17"/>
+      <c r="AK4" s="17"/>
+      <c r="AL4" s="17"/>
+      <c r="AM4" s="17"/>
+      <c r="AN4" s="17"/>
+      <c r="AO4" s="17"/>
+      <c r="AP4" s="17"/>
+      <c r="AQ4" s="17"/>
+      <c r="AR4" s="17"/>
+      <c r="AS4" s="17"/>
+      <c r="AT4" s="17"/>
+      <c r="AU4" s="17"/>
+      <c r="AV4" s="17"/>
+      <c r="AW4" s="17"/>
+      <c r="AX4" s="17"/>
+      <c r="AY4" s="17"/>
+    </row>
+    <row r="5" spans="1:52" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="G3" s="7">
+      <c r="C5" s="16">
         <v>0</v>
       </c>
-      <c r="I3" s="7">
-        <v>10000000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="C4" s="7">
+      <c r="E5" s="16">
         <v>0</v>
       </c>
-      <c r="E4" s="7">
+    </row>
+    <row r="6" spans="1:52" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="28" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="19">
+        <v>70</v>
+      </c>
+      <c r="F6" s="19">
+        <v>70</v>
+      </c>
+      <c r="I6" s="19">
+        <v>80</v>
+      </c>
+      <c r="Y6" s="19">
+        <v>82</v>
+      </c>
+      <c r="AL6" s="19">
+        <v>84</v>
+      </c>
+      <c r="AY6" s="19">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="7" spans="1:52" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="19">
         <v>0</v>
       </c>
-      <c r="J4" s="7">
-        <v>10</v>
-      </c>
-      <c r="S4" s="7">
+      <c r="F7" s="19">
+        <v>1005000</v>
+      </c>
+      <c r="I7" s="19">
+        <v>2040504</v>
+      </c>
+      <c r="Y7" s="19">
+        <v>4049504</v>
+      </c>
+    </row>
+    <row r="8" spans="1:52" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="21">
+        <v>0</v>
+      </c>
+      <c r="G8" s="21">
+        <v>30</v>
+      </c>
+      <c r="J8" s="21">
+        <v>40</v>
+      </c>
+      <c r="AA8" s="21">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:52" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" s="21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:52" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="23">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="23">
+        <v>30</v>
+      </c>
+      <c r="AA10" s="23">
+        <v>40</v>
+      </c>
+      <c r="AK10" s="23">
         <v>50</v>
       </c>
-      <c r="AA4" s="8"/>
-      <c r="AB4" s="8"/>
-      <c r="AC4" s="8"/>
-      <c r="AD4" s="8"/>
-      <c r="AE4" s="8"/>
-      <c r="AF4" s="8"/>
-      <c r="AG4" s="8"/>
-      <c r="AH4" s="8"/>
-      <c r="AI4" s="8"/>
-      <c r="AJ4" s="8"/>
-      <c r="AK4" s="8"/>
-      <c r="AL4" s="8"/>
-      <c r="AM4" s="8"/>
-      <c r="AN4" s="8"/>
-      <c r="AO4" s="8"/>
-      <c r="AP4" s="8"/>
-      <c r="AQ4" s="8"/>
-      <c r="AR4" s="8"/>
-      <c r="AS4" s="8"/>
-      <c r="AT4" s="8"/>
-      <c r="AU4" s="8"/>
-      <c r="AV4" s="8"/>
-      <c r="AW4" s="8"/>
-      <c r="AX4" s="8"/>
-      <c r="AY4" s="8"/>
-    </row>
-    <row r="5" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B5" s="10" t="s">
+    </row>
+    <row r="11" spans="1:52" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" s="22" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="6" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="B6" s="10" t="s">
+      <c r="C11" s="23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:52" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C12" s="25">
+        <v>0</v>
+      </c>
+      <c r="H12" s="25">
+        <v>7</v>
+      </c>
+      <c r="V12" s="25">
+        <v>0</v>
+      </c>
+      <c r="AF12" s="25">
+        <v>50</v>
+      </c>
+      <c r="AK12" s="25">
         <v>70</v>
       </c>
-      <c r="F6" s="7">
-        <v>70</v>
-      </c>
-      <c r="I6" s="7">
-        <v>80</v>
-      </c>
-      <c r="Y6" s="7">
-        <v>82</v>
-      </c>
-      <c r="AL6" s="7">
-        <v>84</v>
-      </c>
-      <c r="AY6" s="7">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="7" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="B7" s="10" t="s">
+    </row>
+    <row r="13" spans="1:52" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="31" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" s="24" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="8" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="G8" s="7">
-        <v>3</v>
-      </c>
-      <c r="J8" s="7">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="B9" s="10" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="10" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="11" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="12" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A12" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="B12" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="H12" s="7">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A13" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="B13" s="10" t="s">
-        <v>38</v>
+      <c r="C13" s="25">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2598,7 +2737,7 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>dropdown_lists!$A$2:$A$4</xm:f>

</xml_diff>

<commit_message>
Add a zero to the start of all programs
Add a zero to the start of all programs at the time that the model
begins from (e.g. data['programs'][program_in_question][1850] is 0.).
</commit_message>
<xml_diff>
--- a/autumn/xls/programs_fiji.xlsx
+++ b/autumn/xls/programs_fiji.xlsx
@@ -2267,35 +2267,34 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AZ13"/>
+  <dimension ref="A1:AY13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="U5" sqref="U5"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="43.140625" style="32" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.42578125" style="7" customWidth="1"/>
-    <col min="5" max="5" width="7.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7" style="7" customWidth="1"/>
-    <col min="7" max="8" width="7.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.42578125" style="7" customWidth="1"/>
-    <col min="10" max="11" width="7.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.7109375" style="7" customWidth="1"/>
-    <col min="13" max="21" width="7.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="7.42578125" style="7" customWidth="1"/>
-    <col min="23" max="24" width="7.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="7.140625" style="7" customWidth="1"/>
-    <col min="26" max="47" width="7.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="6.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="49" max="52" width="7.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="53" max="16384" width="9.140625" style="7"/>
+    <col min="3" max="3" width="7.42578125" style="7" customWidth="1"/>
+    <col min="4" max="4" width="7.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7" style="7" customWidth="1"/>
+    <col min="6" max="7" width="7.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.42578125" style="7" customWidth="1"/>
+    <col min="9" max="10" width="7.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.7109375" style="7" customWidth="1"/>
+    <col min="12" max="20" width="7.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="7.42578125" style="7" customWidth="1"/>
+    <col min="22" max="23" width="7.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="7.140625" style="7" customWidth="1"/>
+    <col min="25" max="46" width="7.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="6.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="48" max="51" width="7.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="52" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:52" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>31</v>
       </c>
@@ -2303,175 +2302,170 @@
         <v>30</v>
       </c>
       <c r="C1" s="11">
-        <v>1850</v>
+        <v>1920</v>
       </c>
       <c r="D1" s="11">
-        <v>1920</v>
+        <v>1930</v>
       </c>
       <c r="E1" s="11">
-        <v>1930</v>
+        <v>1940</v>
       </c>
       <c r="F1" s="11">
-        <v>1940</v>
+        <v>1950</v>
       </c>
       <c r="G1" s="11">
-        <v>1950</v>
+        <v>1955</v>
       </c>
       <c r="H1" s="11">
-        <v>1955</v>
+        <v>1960</v>
       </c>
       <c r="I1" s="11">
-        <v>1960</v>
+        <v>1965</v>
       </c>
       <c r="J1" s="11">
-        <v>1965</v>
+        <v>1970</v>
       </c>
       <c r="K1" s="11">
-        <v>1970</v>
+        <v>1975</v>
       </c>
       <c r="L1" s="11">
-        <v>1975</v>
+        <v>1976</v>
       </c>
       <c r="M1" s="11">
-        <v>1976</v>
+        <v>1977</v>
       </c>
       <c r="N1" s="11">
-        <v>1977</v>
+        <v>1978</v>
       </c>
       <c r="O1" s="11">
-        <v>1978</v>
+        <v>1979</v>
       </c>
       <c r="P1" s="11">
-        <v>1979</v>
+        <v>1980</v>
       </c>
       <c r="Q1" s="11">
-        <v>1980</v>
+        <v>1981</v>
       </c>
       <c r="R1" s="11">
-        <v>1981</v>
+        <v>1982</v>
       </c>
       <c r="S1" s="11">
-        <v>1982</v>
+        <v>1983</v>
       </c>
       <c r="T1" s="11">
-        <v>1983</v>
+        <v>1984</v>
       </c>
       <c r="U1" s="11">
-        <v>1984</v>
+        <v>1985</v>
       </c>
       <c r="V1" s="11">
-        <v>1985</v>
+        <v>1986</v>
       </c>
       <c r="W1" s="11">
-        <v>1986</v>
+        <v>1987</v>
       </c>
       <c r="X1" s="11">
-        <v>1987</v>
+        <v>1988</v>
       </c>
       <c r="Y1" s="11">
-        <v>1988</v>
+        <v>1989</v>
       </c>
       <c r="Z1" s="11">
-        <v>1989</v>
+        <v>1990</v>
       </c>
       <c r="AA1" s="11">
-        <v>1990</v>
+        <v>1991</v>
       </c>
       <c r="AB1" s="11">
-        <v>1991</v>
+        <v>1992</v>
       </c>
       <c r="AC1" s="11">
-        <v>1992</v>
+        <v>1993</v>
       </c>
       <c r="AD1" s="11">
-        <v>1993</v>
+        <v>1994</v>
       </c>
       <c r="AE1" s="11">
-        <v>1994</v>
+        <v>1995</v>
       </c>
       <c r="AF1" s="11">
-        <v>1995</v>
+        <v>1996</v>
       </c>
       <c r="AG1" s="11">
-        <v>1996</v>
+        <v>1997</v>
       </c>
       <c r="AH1" s="11">
-        <v>1997</v>
+        <v>1998</v>
       </c>
       <c r="AI1" s="11">
-        <v>1998</v>
+        <v>1999</v>
       </c>
       <c r="AJ1" s="11">
-        <v>1999</v>
+        <v>2000</v>
       </c>
       <c r="AK1" s="11">
-        <v>2000</v>
+        <v>2001</v>
       </c>
       <c r="AL1" s="11">
-        <v>2001</v>
+        <v>2002</v>
       </c>
       <c r="AM1" s="11">
-        <v>2002</v>
+        <v>2003</v>
       </c>
       <c r="AN1" s="11">
-        <v>2003</v>
+        <v>2004</v>
       </c>
       <c r="AO1" s="11">
-        <v>2004</v>
+        <v>2005</v>
       </c>
       <c r="AP1" s="11">
-        <v>2005</v>
+        <v>2006</v>
       </c>
       <c r="AQ1" s="11">
-        <v>2006</v>
+        <v>2007</v>
       </c>
       <c r="AR1" s="11">
-        <v>2007</v>
+        <v>2008</v>
       </c>
       <c r="AS1" s="11">
-        <v>2008</v>
+        <v>2009</v>
       </c>
       <c r="AT1" s="11">
-        <v>2009</v>
+        <v>2010</v>
       </c>
       <c r="AU1" s="11">
-        <v>2010</v>
+        <v>2011</v>
       </c>
       <c r="AV1" s="11">
-        <v>2011</v>
+        <v>2012</v>
       </c>
       <c r="AW1" s="11">
-        <v>2012</v>
+        <v>2013</v>
       </c>
       <c r="AX1" s="11">
-        <v>2013</v>
+        <v>2014</v>
       </c>
       <c r="AY1" s="11">
-        <v>2014</v>
-      </c>
-      <c r="AZ1" s="11">
         <v>2015</v>
       </c>
     </row>
-    <row r="2" spans="1:52" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:51" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="26" t="s">
         <v>23</v>
       </c>
       <c r="B2" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="13">
+      <c r="F2" s="13">
         <v>0</v>
       </c>
-      <c r="G2" s="13">
-        <v>0</v>
-      </c>
-      <c r="I2" s="13">
+      <c r="H2" s="13">
         <v>25</v>
       </c>
-      <c r="L2" s="13">
+      <c r="K2" s="13">
         <v>40</v>
       </c>
+      <c r="P2" s="14"/>
       <c r="Q2" s="14"/>
       <c r="R2" s="14"/>
       <c r="S2" s="14"/>
@@ -2506,50 +2500,44 @@
       <c r="AV2" s="14"/>
       <c r="AW2" s="14"/>
       <c r="AX2" s="14"/>
-      <c r="AY2" s="14"/>
-    </row>
-    <row r="3" spans="1:52" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:51" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="26" t="s">
         <v>32</v>
       </c>
       <c r="B3" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="C3" s="13">
+      <c r="F3" s="13">
         <v>0</v>
       </c>
-      <c r="G3" s="13">
-        <v>0</v>
-      </c>
-      <c r="I3" s="13">
+      <c r="H3" s="13">
         <v>10000000</v>
       </c>
-      <c r="L3" s="13">
+      <c r="K3" s="13">
         <v>15040500</v>
       </c>
-      <c r="V3" s="13">
+      <c r="U3" s="13">
         <v>39034561</v>
       </c>
     </row>
-    <row r="4" spans="1:52" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:51" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="27" t="s">
         <v>24</v>
       </c>
       <c r="B4" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="C4" s="16">
+      <c r="D4" s="16">
         <v>0</v>
       </c>
-      <c r="E4" s="16">
-        <v>0</v>
-      </c>
-      <c r="J4" s="16">
+      <c r="I4" s="16">
         <v>10</v>
       </c>
-      <c r="S4" s="16">
+      <c r="R4" s="16">
         <v>50</v>
       </c>
+      <c r="Z4" s="17"/>
       <c r="AA4" s="17"/>
       <c r="AB4" s="17"/>
       <c r="AC4" s="17"/>
@@ -2574,162 +2562,134 @@
       <c r="AV4" s="17"/>
       <c r="AW4" s="17"/>
       <c r="AX4" s="17"/>
-      <c r="AY4" s="17"/>
-    </row>
-    <row r="5" spans="1:52" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:51" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="27" t="s">
         <v>33</v>
       </c>
       <c r="B5" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="C5" s="16">
+      <c r="D5" s="16">
         <v>0</v>
       </c>
-      <c r="E5" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:52" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:51" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="28" t="s">
         <v>25</v>
       </c>
       <c r="B6" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="19">
+      <c r="E6" s="19">
         <v>70</v>
       </c>
-      <c r="F6" s="19">
-        <v>70</v>
-      </c>
-      <c r="I6" s="19">
+      <c r="H6" s="19">
         <v>80</v>
       </c>
-      <c r="Y6" s="19">
+      <c r="X6" s="19">
         <v>82</v>
       </c>
-      <c r="AL6" s="19">
+      <c r="AK6" s="19">
         <v>84</v>
       </c>
-      <c r="AY6" s="19">
+      <c r="AX6" s="19">
         <v>85</v>
       </c>
     </row>
-    <row r="7" spans="1:52" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:51" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="28" t="s">
         <v>34</v>
       </c>
       <c r="B7" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="C7" s="19">
-        <v>0</v>
-      </c>
-      <c r="F7" s="19">
+      <c r="E7" s="19">
         <v>1005000</v>
       </c>
-      <c r="I7" s="19">
+      <c r="H7" s="19">
         <v>2040504</v>
       </c>
-      <c r="Y7" s="19">
+      <c r="X7" s="19">
         <v>4049504</v>
       </c>
     </row>
-    <row r="8" spans="1:52" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:51" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="29" t="s">
         <v>18</v>
       </c>
       <c r="B8" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="21">
-        <v>0</v>
-      </c>
-      <c r="G8" s="21">
+      <c r="F8" s="21">
         <v>30</v>
       </c>
-      <c r="J8" s="21">
+      <c r="I8" s="21">
         <v>40</v>
       </c>
-      <c r="AA8" s="21">
+      <c r="Z8" s="21">
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:52" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:51" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="29" t="s">
         <v>35</v>
       </c>
       <c r="B9" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="C9" s="21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:52" s="23" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:51" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="30" t="s">
         <v>26</v>
       </c>
       <c r="B10" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="23">
-        <v>0</v>
-      </c>
-      <c r="Q10" s="23">
+      <c r="P10" s="23">
         <v>30</v>
       </c>
-      <c r="AA10" s="23">
+      <c r="Z10" s="23">
         <v>40</v>
       </c>
-      <c r="AK10" s="23">
+      <c r="AJ10" s="23">
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:52" s="23" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:51" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="30" t="s">
         <v>36</v>
       </c>
       <c r="B11" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="C11" s="23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:52" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:51" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="31" t="s">
         <v>27</v>
       </c>
       <c r="B12" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="25">
+      <c r="G12" s="25">
+        <v>7</v>
+      </c>
+      <c r="U12" s="25">
         <v>0</v>
       </c>
-      <c r="H12" s="25">
-        <v>7</v>
-      </c>
-      <c r="V12" s="25">
-        <v>0</v>
-      </c>
-      <c r="AF12" s="25">
+      <c r="AE12" s="25">
         <v>50</v>
       </c>
-      <c r="AK12" s="25">
+      <c r="AJ12" s="25">
         <v>70</v>
       </c>
     </row>
-    <row r="13" spans="1:52" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:51" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="31" t="s">
         <v>37</v>
       </c>
       <c r="B13" s="24" t="s">
         <v>38</v>
-      </c>
-      <c r="C13" s="25">
-        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Code to remove nans from programs
</commit_message>
<xml_diff>
--- a/autumn/xls/programs_fiji.xlsx
+++ b/autumn/xls/programs_fiji.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="41">
   <si>
     <t>program_proportion_detect</t>
   </si>
@@ -133,6 +133,12 @@
   </si>
   <si>
     <t>na</t>
+  </si>
+  <si>
+    <t>program_prop_treatment_success</t>
+  </si>
+  <si>
+    <t>program_cost_treatment_success</t>
   </si>
 </sst>
 </file>
@@ -227,7 +233,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -296,6 +302,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="-0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1058,7 +1070,7 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1100,6 +1112,7 @@
     <xf numFmtId="0" fontId="11" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="664">
     <cellStyle name="Comma 2" xfId="5"/>
@@ -2267,10 +2280,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AY13"/>
+  <dimension ref="A1:AY15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection activeCell="AM15" sqref="AM15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2284,11 +2297,18 @@
     <col min="8" max="8" width="7.42578125" style="7" customWidth="1"/>
     <col min="9" max="10" width="7.42578125" style="7" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="7.7109375" style="7" customWidth="1"/>
-    <col min="12" max="20" width="7.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="12" max="15" width="7.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.28515625" style="7" customWidth="1"/>
+    <col min="17" max="20" width="7.42578125" style="7" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="7.42578125" style="7" customWidth="1"/>
-    <col min="22" max="23" width="7.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="8.85546875" style="7" customWidth="1"/>
+    <col min="23" max="23" width="7.42578125" style="7" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="7.140625" style="7" customWidth="1"/>
-    <col min="25" max="46" width="7.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="25" max="36" width="7.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="8" style="7" customWidth="1"/>
+    <col min="38" max="44" width="7.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="8" style="7" customWidth="1"/>
+    <col min="46" max="46" width="7.42578125" style="7" bestFit="1" customWidth="1"/>
     <col min="47" max="47" width="6.28515625" style="7" bestFit="1" customWidth="1"/>
     <col min="48" max="51" width="7.42578125" style="7" bestFit="1" customWidth="1"/>
     <col min="52" max="16384" width="9.140625" style="7"/>
@@ -2692,6 +2712,66 @@
         <v>38</v>
       </c>
     </row>
+    <row r="14" spans="1:51" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="G14" s="21">
+        <v>0</v>
+      </c>
+      <c r="P14" s="21">
+        <v>30</v>
+      </c>
+      <c r="V14" s="21">
+        <v>50</v>
+      </c>
+      <c r="AD14" s="33"/>
+      <c r="AE14" s="33"/>
+      <c r="AF14" s="33"/>
+      <c r="AG14" s="33"/>
+      <c r="AH14" s="33"/>
+      <c r="AI14" s="33"/>
+      <c r="AJ14" s="33"/>
+      <c r="AK14" s="33"/>
+      <c r="AL14" s="33"/>
+      <c r="AM14" s="33"/>
+      <c r="AN14" s="33"/>
+      <c r="AO14" s="33"/>
+      <c r="AP14" s="33"/>
+      <c r="AQ14" s="33"/>
+      <c r="AR14" s="33"/>
+      <c r="AS14" s="33"/>
+      <c r="AT14" s="33"/>
+      <c r="AU14" s="33"/>
+      <c r="AV14" s="33"/>
+      <c r="AW14" s="33"/>
+    </row>
+    <row r="15" spans="1:51" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="B15" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="G15" s="21">
+        <v>0</v>
+      </c>
+      <c r="P15" s="21">
+        <v>1926492</v>
+      </c>
+      <c r="V15" s="21">
+        <v>4573928</v>
+      </c>
+      <c r="AK15" s="21">
+        <v>9382947</v>
+      </c>
+      <c r="AS15" s="21">
+        <v>52431253</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Create treatment outcomes for all strains
Temporary code with all strains' treatment outcomes set to the same
values.
</commit_message>
<xml_diff>
--- a/autumn/xls/programs_fiji.xlsx
+++ b/autumn/xls/programs_fiji.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="43">
   <si>
     <t>program_proportion_detect</t>
   </si>
@@ -139,6 +139,12 @@
   </si>
   <si>
     <t>program_cost_treatment_success</t>
+  </si>
+  <si>
+    <t>program_prop_treatment_death</t>
+  </si>
+  <si>
+    <t>program_cost_treatment_death</t>
   </si>
 </sst>
 </file>
@@ -2280,10 +2286,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AY15"/>
+  <dimension ref="A1:AY17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AM15" sqref="AM15"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2772,6 +2778,42 @@
         <v>52431253</v>
       </c>
     </row>
+    <row r="16" spans="1:51" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="B16" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD16" s="33"/>
+      <c r="AE16" s="33"/>
+      <c r="AF16" s="33"/>
+      <c r="AG16" s="33"/>
+      <c r="AH16" s="33"/>
+      <c r="AI16" s="33"/>
+      <c r="AJ16" s="33"/>
+      <c r="AK16" s="33"/>
+      <c r="AL16" s="33"/>
+      <c r="AM16" s="33"/>
+      <c r="AN16" s="33"/>
+      <c r="AO16" s="33"/>
+      <c r="AP16" s="33"/>
+      <c r="AQ16" s="33"/>
+      <c r="AR16" s="33"/>
+      <c r="AS16" s="33"/>
+      <c r="AT16" s="33"/>
+      <c r="AU16" s="33"/>
+      <c r="AV16" s="33"/>
+      <c r="AW16" s="33"/>
+    </row>
+    <row r="17" spans="1:2" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="29" t="s">
+        <v>42</v>
+      </c>
+      <c r="B17" s="20" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Read and process MDR/XDR treatment outcomes
Currently the imported data over-rides that entered in the spreadsheet -
probably not ideal.
</commit_message>
<xml_diff>
--- a/autumn/xls/programs_fiji.xlsx
+++ b/autumn/xls/programs_fiji.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="51">
   <si>
     <t>program_proportion_detect</t>
   </si>
@@ -145,6 +145,30 @@
   </si>
   <si>
     <t>program_cost_treatment_death</t>
+  </si>
+  <si>
+    <t>program_prop_treatment_success_mdr</t>
+  </si>
+  <si>
+    <t>program_cost_treatment_success_mdr</t>
+  </si>
+  <si>
+    <t>program_prop_treatment_death_mdr</t>
+  </si>
+  <si>
+    <t>program_cost_treatment_death_mdr</t>
+  </si>
+  <si>
+    <t>program_prop_treatment_success_xdr</t>
+  </si>
+  <si>
+    <t>program_cost_treatment_success_xdr</t>
+  </si>
+  <si>
+    <t>program_prop_treatment_death_xdr</t>
+  </si>
+  <si>
+    <t>program_cost_treatment_death_xdr</t>
   </si>
 </sst>
 </file>
@@ -155,7 +179,7 @@
     <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -238,8 +262,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="14">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -314,6 +345,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="-0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1076,7 +1119,7 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1099,10 +1142,8 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1118,7 +1159,13 @@
     <xf numFmtId="0" fontId="11" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="664">
     <cellStyle name="Comma 2" xfId="5"/>
@@ -2286,15 +2333,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AY17"/>
+  <dimension ref="A1:AY25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AJ15" sqref="AJ15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="43.140625" style="32" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="47.42578125" style="30" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" style="8" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.42578125" style="7" customWidth="1"/>
     <col min="4" max="4" width="7.42578125" style="7" bestFit="1" customWidth="1"/>
@@ -2476,7 +2523,7 @@
       </c>
     </row>
     <row r="2" spans="1:51" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="24" t="s">
         <v>23</v>
       </c>
       <c r="B2" s="12" t="s">
@@ -2491,44 +2538,44 @@
       <c r="K2" s="13">
         <v>40</v>
       </c>
-      <c r="P2" s="14"/>
-      <c r="Q2" s="14"/>
-      <c r="R2" s="14"/>
-      <c r="S2" s="14"/>
-      <c r="T2" s="14"/>
-      <c r="U2" s="14"/>
-      <c r="V2" s="14"/>
-      <c r="W2" s="14"/>
-      <c r="X2" s="14"/>
-      <c r="Y2" s="14"/>
-      <c r="Z2" s="14"/>
-      <c r="AA2" s="14"/>
-      <c r="AB2" s="14"/>
-      <c r="AC2" s="14"/>
-      <c r="AD2" s="14"/>
-      <c r="AE2" s="14"/>
-      <c r="AF2" s="14"/>
-      <c r="AG2" s="14"/>
-      <c r="AH2" s="14"/>
-      <c r="AI2" s="14"/>
-      <c r="AJ2" s="14"/>
-      <c r="AK2" s="14"/>
-      <c r="AL2" s="14"/>
-      <c r="AM2" s="14"/>
-      <c r="AN2" s="14"/>
-      <c r="AO2" s="14"/>
-      <c r="AP2" s="14"/>
-      <c r="AQ2" s="14"/>
-      <c r="AR2" s="14"/>
-      <c r="AS2" s="14"/>
-      <c r="AT2" s="14"/>
-      <c r="AU2" s="14"/>
-      <c r="AV2" s="14"/>
-      <c r="AW2" s="14"/>
-      <c r="AX2" s="14"/>
+      <c r="P2" s="34"/>
+      <c r="Q2" s="34"/>
+      <c r="R2" s="34"/>
+      <c r="S2" s="34"/>
+      <c r="T2" s="34"/>
+      <c r="U2" s="34"/>
+      <c r="V2" s="34"/>
+      <c r="W2" s="34"/>
+      <c r="X2" s="34"/>
+      <c r="Y2" s="34"/>
+      <c r="Z2" s="34"/>
+      <c r="AA2" s="34"/>
+      <c r="AB2" s="34"/>
+      <c r="AC2" s="34"/>
+      <c r="AD2" s="34"/>
+      <c r="AE2" s="34"/>
+      <c r="AF2" s="34"/>
+      <c r="AG2" s="34"/>
+      <c r="AH2" s="34"/>
+      <c r="AI2" s="34"/>
+      <c r="AJ2" s="34"/>
+      <c r="AK2" s="34"/>
+      <c r="AL2" s="34"/>
+      <c r="AM2" s="34"/>
+      <c r="AN2" s="34"/>
+      <c r="AO2" s="34"/>
+      <c r="AP2" s="34"/>
+      <c r="AQ2" s="34"/>
+      <c r="AR2" s="34"/>
+      <c r="AS2" s="34"/>
+      <c r="AT2" s="34"/>
+      <c r="AU2" s="34"/>
+      <c r="AV2" s="34"/>
+      <c r="AW2" s="34"/>
+      <c r="AX2" s="34"/>
     </row>
     <row r="3" spans="1:51" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="24" t="s">
         <v>32</v>
       </c>
       <c r="B3" s="12" t="s">
@@ -2547,271 +2594,499 @@
         <v>39034561</v>
       </c>
     </row>
-    <row r="4" spans="1:51" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="27" t="s">
+    <row r="4" spans="1:51" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="D4" s="16">
+      <c r="D4" s="15">
         <v>0</v>
       </c>
-      <c r="I4" s="16">
+      <c r="I4" s="15">
         <v>10</v>
       </c>
-      <c r="R4" s="16">
+      <c r="R4" s="15">
         <v>50</v>
       </c>
-      <c r="Z4" s="17"/>
-      <c r="AA4" s="17"/>
-      <c r="AB4" s="17"/>
-      <c r="AC4" s="17"/>
-      <c r="AD4" s="17"/>
-      <c r="AE4" s="17"/>
-      <c r="AF4" s="17"/>
-      <c r="AG4" s="17"/>
-      <c r="AH4" s="17"/>
-      <c r="AI4" s="17"/>
-      <c r="AJ4" s="17"/>
-      <c r="AK4" s="17"/>
-      <c r="AL4" s="17"/>
-      <c r="AM4" s="17"/>
-      <c r="AN4" s="17"/>
-      <c r="AO4" s="17"/>
-      <c r="AP4" s="17"/>
-      <c r="AQ4" s="17"/>
-      <c r="AR4" s="17"/>
-      <c r="AS4" s="17"/>
-      <c r="AT4" s="17"/>
-      <c r="AU4" s="17"/>
-      <c r="AV4" s="17"/>
-      <c r="AW4" s="17"/>
-      <c r="AX4" s="17"/>
-    </row>
-    <row r="5" spans="1:51" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="27" t="s">
+      <c r="Z4" s="35"/>
+      <c r="AA4" s="35"/>
+      <c r="AB4" s="35"/>
+      <c r="AC4" s="35"/>
+      <c r="AD4" s="35"/>
+      <c r="AE4" s="35"/>
+      <c r="AF4" s="35"/>
+      <c r="AG4" s="35"/>
+      <c r="AH4" s="35"/>
+      <c r="AI4" s="35"/>
+      <c r="AJ4" s="35"/>
+      <c r="AK4" s="35"/>
+      <c r="AL4" s="35"/>
+      <c r="AM4" s="35"/>
+      <c r="AN4" s="35"/>
+      <c r="AO4" s="35"/>
+      <c r="AP4" s="35"/>
+      <c r="AQ4" s="35"/>
+      <c r="AR4" s="35"/>
+      <c r="AS4" s="35"/>
+      <c r="AT4" s="35"/>
+      <c r="AU4" s="35"/>
+      <c r="AV4" s="35"/>
+      <c r="AW4" s="35"/>
+      <c r="AX4" s="35"/>
+    </row>
+    <row r="5" spans="1:51" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="D5" s="16">
+      <c r="D5" s="15">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:51" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="28" t="s">
+    <row r="6" spans="1:51" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="18" t="s">
+      <c r="B6" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="E6" s="19">
+      <c r="E6" s="17">
         <v>70</v>
       </c>
-      <c r="H6" s="19">
+      <c r="H6" s="17">
         <v>80</v>
       </c>
-      <c r="X6" s="19">
+      <c r="X6" s="17">
         <v>82</v>
       </c>
-      <c r="AK6" s="19">
+      <c r="AK6" s="17">
         <v>84</v>
       </c>
-      <c r="AX6" s="19">
+      <c r="AX6" s="17">
         <v>85</v>
       </c>
     </row>
-    <row r="7" spans="1:51" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="28" t="s">
+    <row r="7" spans="1:51" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="B7" s="18" t="s">
+      <c r="B7" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="E7" s="19">
+      <c r="E7" s="17">
         <v>1005000</v>
       </c>
-      <c r="H7" s="19">
+      <c r="H7" s="17">
         <v>2040504</v>
       </c>
-      <c r="X7" s="19">
+      <c r="X7" s="17">
         <v>4049504</v>
       </c>
     </row>
-    <row r="8" spans="1:51" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="29" t="s">
+    <row r="8" spans="1:51" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="20" t="s">
+      <c r="B8" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="F8" s="21">
+      <c r="F8" s="19">
         <v>30</v>
       </c>
-      <c r="I8" s="21">
+      <c r="I8" s="19">
         <v>40</v>
       </c>
-      <c r="Z8" s="21">
+      <c r="Z8" s="19">
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:51" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="29" t="s">
+    <row r="9" spans="1:51" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="B9" s="20" t="s">
+      <c r="B9" s="18" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:51" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="30" t="s">
+    <row r="10" spans="1:51" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="22" t="s">
+      <c r="B10" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="P10" s="23">
+      <c r="P10" s="21">
         <v>30</v>
       </c>
-      <c r="Z10" s="23">
+      <c r="Z10" s="21">
         <v>40</v>
       </c>
-      <c r="AJ10" s="23">
+      <c r="AJ10" s="21">
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:51" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="30" t="s">
+    <row r="11" spans="1:51" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="B11" s="22" t="s">
+      <c r="B11" s="20" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:51" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="31" t="s">
+    <row r="12" spans="1:51" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="24" t="s">
+      <c r="B12" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="G12" s="25">
+      <c r="G12" s="23">
         <v>7</v>
       </c>
-      <c r="U12" s="25">
+      <c r="U12" s="23">
         <v>0</v>
       </c>
-      <c r="AE12" s="25">
+      <c r="AE12" s="23">
         <v>50</v>
       </c>
-      <c r="AJ12" s="25">
+      <c r="AJ12" s="23">
         <v>70</v>
       </c>
     </row>
-    <row r="13" spans="1:51" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="31" t="s">
+    <row r="13" spans="1:51" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="B13" s="24" t="s">
+      <c r="B13" s="22" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:51" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="29" t="s">
+    <row r="14" spans="1:51" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="B14" s="20" t="s">
+      <c r="B14" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="G14" s="21">
+      <c r="G14" s="19">
         <v>0</v>
       </c>
-      <c r="P14" s="21">
+      <c r="P14" s="19">
         <v>30</v>
       </c>
-      <c r="V14" s="21">
+      <c r="V14" s="19">
         <v>50</v>
       </c>
-      <c r="AD14" s="33"/>
-      <c r="AE14" s="33"/>
-      <c r="AF14" s="33"/>
-      <c r="AG14" s="33"/>
-      <c r="AH14" s="33"/>
-      <c r="AI14" s="33"/>
-      <c r="AJ14" s="33"/>
-      <c r="AK14" s="33"/>
-      <c r="AL14" s="33"/>
-      <c r="AM14" s="33"/>
-      <c r="AN14" s="33"/>
-      <c r="AO14" s="33"/>
-      <c r="AP14" s="33"/>
-      <c r="AQ14" s="33"/>
-      <c r="AR14" s="33"/>
-      <c r="AS14" s="33"/>
-      <c r="AT14" s="33"/>
-      <c r="AU14" s="33"/>
-      <c r="AV14" s="33"/>
-      <c r="AW14" s="33"/>
-    </row>
-    <row r="15" spans="1:51" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="29" t="s">
+      <c r="AD14" s="36"/>
+      <c r="AE14" s="36"/>
+      <c r="AF14" s="36"/>
+      <c r="AG14" s="36"/>
+      <c r="AH14" s="36"/>
+      <c r="AI14" s="36"/>
+      <c r="AJ14" s="36"/>
+      <c r="AK14" s="36"/>
+      <c r="AL14" s="36"/>
+      <c r="AM14" s="36"/>
+      <c r="AN14" s="36"/>
+      <c r="AO14" s="36"/>
+      <c r="AP14" s="36"/>
+      <c r="AQ14" s="36"/>
+      <c r="AR14" s="36"/>
+      <c r="AS14" s="36"/>
+      <c r="AT14" s="36"/>
+      <c r="AU14" s="36"/>
+      <c r="AV14" s="36"/>
+      <c r="AW14" s="36"/>
+    </row>
+    <row r="15" spans="1:51" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="B15" s="20" t="s">
+      <c r="B15" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="G15" s="21">
+      <c r="G15" s="19">
         <v>0</v>
       </c>
-      <c r="P15" s="21">
+      <c r="P15" s="19">
         <v>1926492</v>
       </c>
-      <c r="V15" s="21">
+      <c r="V15" s="19">
         <v>4573928</v>
       </c>
-      <c r="AK15" s="21">
+      <c r="AK15" s="19">
         <v>9382947</v>
       </c>
-      <c r="AS15" s="21">
+      <c r="AS15" s="19">
         <v>52431253</v>
       </c>
     </row>
-    <row r="16" spans="1:51" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="29" t="s">
+    <row r="16" spans="1:51" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="B16" s="20" t="s">
+      <c r="B16" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="AD16" s="33"/>
-      <c r="AE16" s="33"/>
-      <c r="AF16" s="33"/>
-      <c r="AG16" s="33"/>
-      <c r="AH16" s="33"/>
-      <c r="AI16" s="33"/>
-      <c r="AJ16" s="33"/>
-      <c r="AK16" s="33"/>
-      <c r="AL16" s="33"/>
-      <c r="AM16" s="33"/>
-      <c r="AN16" s="33"/>
-      <c r="AO16" s="33"/>
-      <c r="AP16" s="33"/>
-      <c r="AQ16" s="33"/>
-      <c r="AR16" s="33"/>
-      <c r="AS16" s="33"/>
-      <c r="AT16" s="33"/>
-      <c r="AU16" s="33"/>
-      <c r="AV16" s="33"/>
-      <c r="AW16" s="33"/>
-    </row>
-    <row r="17" spans="1:2" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="29" t="s">
+      <c r="G16" s="19">
+        <v>0</v>
+      </c>
+      <c r="P16" s="19">
+        <v>15</v>
+      </c>
+      <c r="V16" s="19">
+        <v>12</v>
+      </c>
+      <c r="AD16" s="36"/>
+      <c r="AE16" s="36"/>
+      <c r="AF16" s="36"/>
+      <c r="AG16" s="36"/>
+      <c r="AH16" s="36"/>
+      <c r="AI16" s="36"/>
+      <c r="AJ16" s="36"/>
+      <c r="AK16" s="36"/>
+      <c r="AL16" s="36"/>
+      <c r="AM16" s="36"/>
+      <c r="AN16" s="36"/>
+      <c r="AO16" s="36"/>
+      <c r="AP16" s="36"/>
+      <c r="AQ16" s="36"/>
+      <c r="AR16" s="36"/>
+      <c r="AS16" s="36"/>
+      <c r="AT16" s="36"/>
+      <c r="AU16" s="36"/>
+      <c r="AV16" s="36"/>
+      <c r="AW16" s="36"/>
+    </row>
+    <row r="17" spans="1:49" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="B17" s="20" t="s">
+      <c r="B17" s="18" t="s">
         <v>38</v>
+      </c>
+      <c r="G17" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:49" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="31" t="s">
+        <v>43</v>
+      </c>
+      <c r="B18" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="G18" s="33">
+        <v>0</v>
+      </c>
+      <c r="P18" s="33">
+        <v>15</v>
+      </c>
+      <c r="V18" s="33">
+        <v>30</v>
+      </c>
+      <c r="AD18" s="37"/>
+      <c r="AE18" s="37"/>
+      <c r="AF18" s="37"/>
+      <c r="AG18" s="37"/>
+      <c r="AH18" s="37"/>
+      <c r="AI18" s="37"/>
+      <c r="AJ18" s="37"/>
+      <c r="AK18" s="37"/>
+      <c r="AL18" s="37"/>
+      <c r="AM18" s="37"/>
+      <c r="AN18" s="37"/>
+      <c r="AO18" s="37"/>
+      <c r="AP18" s="37"/>
+      <c r="AQ18" s="37"/>
+      <c r="AR18" s="37"/>
+      <c r="AS18" s="37"/>
+      <c r="AT18" s="37"/>
+      <c r="AU18" s="37"/>
+      <c r="AV18" s="37"/>
+      <c r="AW18" s="37"/>
+    </row>
+    <row r="19" spans="1:49" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="31" t="s">
+        <v>44</v>
+      </c>
+      <c r="B19" s="32" t="s">
+        <v>38</v>
+      </c>
+      <c r="G19" s="33">
+        <v>0</v>
+      </c>
+      <c r="P19" s="33">
+        <v>492549</v>
+      </c>
+      <c r="V19" s="33">
+        <v>256491</v>
+      </c>
+      <c r="AK19" s="33">
+        <v>9382947</v>
+      </c>
+      <c r="AS19" s="33">
+        <v>52431253</v>
+      </c>
+    </row>
+    <row r="20" spans="1:49" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="31" t="s">
+        <v>45</v>
+      </c>
+      <c r="B20" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="G20" s="33">
+        <v>0</v>
+      </c>
+      <c r="P20" s="33">
+        <v>55</v>
+      </c>
+      <c r="V20" s="33">
+        <v>50</v>
+      </c>
+      <c r="AD20" s="37"/>
+      <c r="AE20" s="37"/>
+      <c r="AF20" s="37"/>
+      <c r="AG20" s="37"/>
+      <c r="AH20" s="37"/>
+      <c r="AI20" s="37"/>
+      <c r="AJ20" s="37"/>
+      <c r="AK20" s="37"/>
+      <c r="AL20" s="37"/>
+      <c r="AM20" s="37"/>
+      <c r="AN20" s="37"/>
+      <c r="AO20" s="37"/>
+      <c r="AP20" s="37"/>
+      <c r="AQ20" s="37"/>
+      <c r="AR20" s="37"/>
+      <c r="AS20" s="37"/>
+      <c r="AT20" s="37"/>
+      <c r="AU20" s="37"/>
+      <c r="AV20" s="37"/>
+      <c r="AW20" s="37"/>
+    </row>
+    <row r="21" spans="1:49" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="31" t="s">
+        <v>46</v>
+      </c>
+      <c r="B21" s="32" t="s">
+        <v>38</v>
+      </c>
+      <c r="G21" s="33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:49" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="B22" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="G22" s="15">
+        <v>0</v>
+      </c>
+      <c r="P22" s="15">
+        <v>5</v>
+      </c>
+      <c r="V22" s="15">
+        <v>15</v>
+      </c>
+      <c r="AD22" s="35"/>
+      <c r="AE22" s="35"/>
+      <c r="AF22" s="35"/>
+      <c r="AG22" s="35"/>
+      <c r="AH22" s="35"/>
+      <c r="AI22" s="35"/>
+      <c r="AJ22" s="35"/>
+      <c r="AK22" s="35"/>
+      <c r="AL22" s="35"/>
+      <c r="AM22" s="35"/>
+      <c r="AN22" s="35"/>
+      <c r="AO22" s="35"/>
+      <c r="AP22" s="35"/>
+      <c r="AQ22" s="35"/>
+      <c r="AR22" s="35"/>
+      <c r="AS22" s="35"/>
+      <c r="AT22" s="35"/>
+      <c r="AU22" s="35"/>
+      <c r="AV22" s="35"/>
+      <c r="AW22" s="35"/>
+    </row>
+    <row r="23" spans="1:49" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="B23" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="G23" s="15">
+        <v>0</v>
+      </c>
+      <c r="P23" s="15">
+        <v>0</v>
+      </c>
+      <c r="V23" s="15">
+        <v>0</v>
+      </c>
+      <c r="AK23" s="15">
+        <v>0</v>
+      </c>
+      <c r="AS23" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:49" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="25" t="s">
+        <v>49</v>
+      </c>
+      <c r="B24" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="G24" s="15">
+        <v>0</v>
+      </c>
+      <c r="P24" s="15">
+        <v>65</v>
+      </c>
+      <c r="V24" s="15">
+        <v>62</v>
+      </c>
+      <c r="AD24" s="35"/>
+      <c r="AE24" s="35"/>
+      <c r="AF24" s="35"/>
+      <c r="AG24" s="35"/>
+      <c r="AH24" s="35"/>
+      <c r="AI24" s="35"/>
+      <c r="AJ24" s="35"/>
+      <c r="AK24" s="35"/>
+      <c r="AL24" s="35"/>
+      <c r="AM24" s="35"/>
+      <c r="AN24" s="35"/>
+      <c r="AO24" s="35"/>
+      <c r="AP24" s="35"/>
+      <c r="AQ24" s="35"/>
+      <c r="AR24" s="35"/>
+      <c r="AS24" s="35"/>
+      <c r="AT24" s="35"/>
+      <c r="AU24" s="35"/>
+      <c r="AV24" s="35"/>
+      <c r="AW24" s="35"/>
+    </row>
+    <row r="25" spans="1:49" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="B25" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="G25" s="15">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Model attributes reader added
</commit_message>
<xml_diff>
--- a/autumn/xls/programs_fiji.xlsx
+++ b/autumn/xls/programs_fiji.xlsx
@@ -4,37 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="255" windowWidth="20370" windowHeight="7590" tabRatio="807" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="255" windowWidth="20370" windowHeight="7590" tabRatio="807"/>
   </bookViews>
   <sheets>
-    <sheet name="miscellaneous_constants" sheetId="1" r:id="rId1"/>
-    <sheet name="programs" sheetId="2" r:id="rId2"/>
-    <sheet name="dropdown_lists" sheetId="3" r:id="rId3"/>
+    <sheet name="model_attributes" sheetId="4" r:id="rId1"/>
+    <sheet name="miscellaneous_constants" sheetId="1" r:id="rId2"/>
+    <sheet name="programs" sheetId="2" r:id="rId3"/>
+    <sheet name="dropdown_lists" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="51">
-  <si>
-    <t>program_proportion_detect</t>
-  </si>
-  <si>
-    <t>program_algorithm_sensitivity</t>
-  </si>
-  <si>
-    <t>program_proportion_success_ds</t>
-  </si>
-  <si>
-    <t>program_proportion_success_mdr</t>
-  </si>
-  <si>
-    <t>program_proportion_success_xdr</t>
-  </si>
-  <si>
-    <t>program_proportion_success_inappropriate</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="54">
   <si>
     <t>program_rate_restart_presenting</t>
   </si>
@@ -54,18 +37,9 @@
     <t>dots_start_date</t>
   </si>
   <si>
-    <t>dots_start_proportion</t>
-  </si>
-  <si>
     <t>finish_scaleup_date</t>
   </si>
   <si>
-    <t>program_prop_assign_mdr</t>
-  </si>
-  <si>
-    <t>program_prop_assign_xdr</t>
-  </si>
-  <si>
     <t>program_prop_nonsuccessoutcomes_death</t>
   </si>
   <si>
@@ -169,6 +143,42 @@
   </si>
   <si>
     <t>program_cost_treatment_death_xdr</t>
+  </si>
+  <si>
+    <t>attribute</t>
+  </si>
+  <si>
+    <t>n_comorbidities</t>
+  </si>
+  <si>
+    <t>start_time</t>
+  </si>
+  <si>
+    <t>recent_time</t>
+  </si>
+  <si>
+    <t>n_organs</t>
+  </si>
+  <si>
+    <t>n_strains</t>
+  </si>
+  <si>
+    <t>value_at_iteration</t>
+  </si>
+  <si>
+    <t>first_value</t>
+  </si>
+  <si>
+    <t>is_lowquality</t>
+  </si>
+  <si>
+    <t>is_amplification</t>
+  </si>
+  <si>
+    <t>is_misassignment</t>
+  </si>
+  <si>
+    <t>value_at_second_iteration</t>
   </si>
 </sst>
 </file>
@@ -2131,12 +2141,120 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
-    <tabColor rgb="FFFF0000"/>
+    <tabColor theme="3" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:B23"/>
+  <dimension ref="A1:D9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5">
+        <v>1850</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6">
+        <v>1990</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B7" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>52</v>
+      </c>
+      <c r="B9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="9" tint="-0.249977111117893"/>
+  </sheetPr>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2147,15 +2265,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="B1" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="B2" s="5">
         <v>14</v>
@@ -2163,26 +2281,26 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="B3" s="3">
-        <v>0.8</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B4" s="3">
-        <v>0.9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="B5" s="3">
-        <v>26</v>
+        <v>1950</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -2190,7 +2308,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="3">
-        <v>0.9</v>
+        <v>2050</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -2198,132 +2316,52 @@
         <v>3</v>
       </c>
       <c r="B7" s="3">
-        <v>0.6</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B8" s="3">
-        <v>0.4</v>
+        <v>1990</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B9" s="3">
-        <v>0.25</v>
+        <v>2010</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B10" s="3">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B11" s="3">
-        <v>1950</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B12" s="3">
-        <v>2050</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B13" s="3">
-        <v>1940</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B14" s="3">
-        <v>1990</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B15" s="3">
-        <v>2010</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B16" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B17" s="3">
-        <v>0.85</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B18" s="3">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B19" s="3">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B20" s="3">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B21" s="3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B22" s="3">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2331,12 +2369,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="5" tint="0.39997558519241921"/>
+  </sheetPr>
   <dimension ref="A1:AY25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AX14" sqref="AX14"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D59" sqref="D59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2369,10 +2410,10 @@
   <sheetData>
     <row r="1" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="C1" s="11">
         <v>1920</v>
@@ -2524,10 +2565,10 @@
     </row>
     <row r="2" spans="1:51" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="24" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="F2" s="13">
         <v>0</v>
@@ -2576,10 +2617,10 @@
     </row>
     <row r="3" spans="1:51" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="24" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="F3" s="13">
         <v>0</v>
@@ -2596,10 +2637,10 @@
     </row>
     <row r="4" spans="1:51" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="25" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="D4" s="15">
         <v>0</v>
@@ -2638,10 +2679,10 @@
     </row>
     <row r="5" spans="1:51" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="25" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="D5" s="15">
         <v>0</v>
@@ -2649,10 +2690,10 @@
     </row>
     <row r="6" spans="1:51" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="26" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="E6" s="17">
         <v>70</v>
@@ -2672,10 +2713,10 @@
     </row>
     <row r="7" spans="1:51" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="26" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="E7" s="17">
         <v>1005000</v>
@@ -2689,10 +2730,10 @@
     </row>
     <row r="8" spans="1:51" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="27" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="F8" s="19">
         <v>30</v>
@@ -2706,18 +2747,18 @@
     </row>
     <row r="9" spans="1:51" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="27" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:51" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="28" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="B10" s="20" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="P10" s="21">
         <v>30</v>
@@ -2731,18 +2772,18 @@
     </row>
     <row r="11" spans="1:51" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="28" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="B11" s="20" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:51" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="29" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="B12" s="22" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="G12" s="23">
         <v>7</v>
@@ -2759,18 +2800,18 @@
     </row>
     <row r="13" spans="1:51" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="29" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="B13" s="22" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:51" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="27" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="B14" s="18" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="G14" s="19">
         <v>0</v>
@@ -2804,10 +2845,10 @@
     </row>
     <row r="15" spans="1:51" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="27" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="B15" s="18" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="G15" s="19">
         <v>0</v>
@@ -2827,10 +2868,10 @@
     </row>
     <row r="16" spans="1:51" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="27" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="B16" s="18" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="G16" s="19">
         <v>0</v>
@@ -2864,10 +2905,10 @@
     </row>
     <row r="17" spans="1:50" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="27" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="B17" s="18" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="G17" s="19">
         <v>0</v>
@@ -2875,10 +2916,10 @@
     </row>
     <row r="18" spans="1:50" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="31" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="B18" s="32" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="G18" s="33">
         <v>0</v>
@@ -2915,10 +2956,10 @@
     </row>
     <row r="19" spans="1:50" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="31" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="B19" s="32" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="G19" s="33">
         <v>0</v>
@@ -2938,10 +2979,10 @@
     </row>
     <row r="20" spans="1:50" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="31" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="B20" s="32" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="G20" s="33">
         <v>0</v>
@@ -2978,10 +3019,10 @@
     </row>
     <row r="21" spans="1:50" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="31" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="B21" s="32" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="G21" s="33">
         <v>0</v>
@@ -2989,10 +3030,10 @@
     </row>
     <row r="22" spans="1:50" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="25" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="B22" s="14" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="G22" s="15">
         <v>0</v>
@@ -3029,10 +3070,10 @@
     </row>
     <row r="23" spans="1:50" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="25" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="B23" s="14" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="G23" s="15">
         <v>0</v>
@@ -3052,10 +3093,10 @@
     </row>
     <row r="24" spans="1:50" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="25" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="B24" s="14" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="G24" s="15">
         <v>0</v>
@@ -3092,10 +3133,10 @@
     </row>
     <row r="25" spans="1:50" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="25" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="B25" s="14" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="G25" s="15">
         <v>0</v>
@@ -3119,29 +3160,32 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="0" tint="-4.9989318521683403E-2"/>
+  </sheetPr>
   <dimension ref="A2:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ensuring model is fully running
Checks and tidies to make sure that the model runs in all its forms -
any number of strains, comorbidities, organ statuses and added
functionality.
</commit_message>
<xml_diff>
--- a/autumn/xls/programs_fiji.xlsx
+++ b/autumn/xls/programs_fiji.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="255" windowWidth="20370" windowHeight="7590" tabRatio="807" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="255" windowWidth="20370" windowHeight="7590" tabRatio="807"/>
   </bookViews>
   <sheets>
     <sheet name="model_attributes" sheetId="4" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="60">
   <si>
     <t>program_rate_restart_presenting</t>
   </si>
@@ -173,17 +173,40 @@
   </si>
   <si>
     <t>consecutive age breakpoints</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>evidence for value</t>
+  </si>
+  <si>
+    <t>Effective contact rate for TB</t>
+  </si>
+  <si>
+    <t>Inverse of time period that detected patients have to wait before starting treatment</t>
+  </si>
+  <si>
+    <t>Rate at which patients who were told they didn't have TB turn up again to the health system</t>
+  </si>
+  <si>
+    <t>Calendar year that MDR-TB first emerged</t>
+  </si>
+  <si>
+    <t>Calendar year that XDR-TB first emerged</t>
+  </si>
+  <si>
+    <t>Rate at which patients change from the low quality to the high quality health system</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -223,19 +246,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color rgb="FF008000"/>
-      <name val="Courier New"/>
-      <family val="3"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <name val="Courier New"/>
-      <family val="3"/>
     </font>
     <font>
       <sz val="11"/>
@@ -281,8 +291,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="5" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="16">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -292,12 +309,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="40"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
@@ -514,7 +525,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
@@ -1175,78 +1186,78 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="664">
     <cellStyle name="Comma 2" xfId="5"/>
@@ -2216,126 +2227,126 @@
   </sheetPr>
   <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.42578125" style="39" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.42578125" style="55" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="40" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="38" t="s">
+    <row r="1" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="32" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="40" t="s">
+      <c r="B1" s="33" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="40" t="s">
+      <c r="C1" s="33" t="s">
         <v>43</v>
       </c>
-      <c r="D1" s="38" t="s">
+      <c r="D1" s="32" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="41" t="s">
+      <c r="A2" s="49" t="s">
         <v>41</v>
       </c>
-      <c r="B2" s="45">
+      <c r="B2" s="36">
         <v>0</v>
       </c>
-      <c r="C2" s="45"/>
-      <c r="D2" s="42"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="34"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="41" t="s">
+      <c r="A3" s="49" t="s">
         <v>42</v>
       </c>
-      <c r="B3" s="45">
+      <c r="B3" s="36">
         <v>0</v>
       </c>
-      <c r="C3" s="45"/>
-      <c r="D3" s="42"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="34"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="46" t="s">
+      <c r="A4" s="50" t="s">
         <v>38</v>
       </c>
-      <c r="B4" s="47">
+      <c r="B4" s="37">
         <v>0</v>
       </c>
-      <c r="C4" s="47"/>
-      <c r="D4" s="48"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="38"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="43" t="s">
+      <c r="A5" s="51" t="s">
         <v>39</v>
       </c>
-      <c r="B5" s="44">
+      <c r="B5" s="35">
         <v>1850</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="43" t="s">
+      <c r="A6" s="51" t="s">
         <v>40</v>
       </c>
-      <c r="B6" s="44">
+      <c r="B6" s="35">
         <v>1990</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="49" t="s">
+      <c r="A7" s="52" t="s">
         <v>45</v>
       </c>
-      <c r="B7" s="50" t="b">
+      <c r="B7" s="39" t="b">
         <v>0</v>
       </c>
-      <c r="C7" s="51"/>
+      <c r="C7" s="40"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="52" t="s">
+      <c r="A8" s="53" t="s">
         <v>46</v>
       </c>
-      <c r="B8" s="53" t="b">
+      <c r="B8" s="41" t="b">
         <v>0</v>
       </c>
-      <c r="C8" s="54"/>
+      <c r="C8" s="42"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="55" t="s">
+      <c r="A9" s="54" t="s">
         <v>47</v>
       </c>
-      <c r="B9" s="56" t="b">
+      <c r="B9" s="43" t="b">
         <v>0</v>
       </c>
-      <c r="C9" s="57"/>
-    </row>
-    <row r="10" spans="1:10" s="62" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="39" t="s">
+      <c r="C9" s="44"/>
+    </row>
+    <row r="10" spans="1:10" s="48" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="55" t="s">
         <v>50</v>
       </c>
-      <c r="B10" s="62" t="s">
+      <c r="B10" s="48" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="58" t="s">
+      <c r="A11" s="56" t="s">
         <v>49</v>
       </c>
-      <c r="B11" s="59"/>
-      <c r="C11" s="59"/>
-      <c r="D11" s="59"/>
-      <c r="E11" s="60"/>
-      <c r="F11" s="61"/>
-      <c r="G11" s="61"/>
-      <c r="H11" s="61"/>
-      <c r="I11" s="61"/>
-      <c r="J11" s="61"/>
+      <c r="B11" s="45"/>
+      <c r="C11" s="45"/>
+      <c r="D11" s="45"/>
+      <c r="E11" s="46"/>
+      <c r="F11" s="47"/>
+      <c r="G11" s="47"/>
+      <c r="H11" s="47"/>
+      <c r="I11" s="47"/>
+      <c r="J11" s="47"/>
     </row>
   </sheetData>
   <dataValidations xWindow="363" yWindow="440" count="6">
@@ -2410,77 +2421,104 @@
   <sheetPr>
     <tabColor theme="9" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="48.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="48.28515625" style="61" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" style="64" customWidth="1"/>
+    <col min="3" max="3" width="84.28515625" style="59" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" style="59" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="59"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" s="65" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="65" t="s">
         <v>6</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="66" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="C1" s="65" t="s">
+        <v>52</v>
+      </c>
+      <c r="D1" s="65" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" s="58" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="57" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2" s="62">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="C2" s="58" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="62">
         <v>26</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="C3" s="59" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="57" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="62">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="C4" s="59" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="57" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="62">
         <v>1950</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="C5" s="59" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="62">
         <v>2050</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="C6" s="59" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="62">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
+      <c r="C7" s="59" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="60"/>
+      <c r="B8" s="63"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2495,778 +2533,788 @@
   </sheetPr>
   <dimension ref="A1:AY25"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AP16" sqref="AP16"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="47.42578125" style="30" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.42578125" style="7" customWidth="1"/>
-    <col min="4" max="4" width="7.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7" style="7" customWidth="1"/>
-    <col min="6" max="7" width="7.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.42578125" style="7" customWidth="1"/>
-    <col min="9" max="10" width="7.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.7109375" style="7" customWidth="1"/>
-    <col min="12" max="15" width="7.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="7.28515625" style="7" customWidth="1"/>
-    <col min="17" max="20" width="7.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="7.42578125" style="7" customWidth="1"/>
-    <col min="22" max="22" width="8.85546875" style="7" customWidth="1"/>
-    <col min="23" max="23" width="7.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="7.140625" style="7" customWidth="1"/>
-    <col min="25" max="36" width="7.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="8" style="7" customWidth="1"/>
-    <col min="38" max="44" width="7.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="8" style="7" customWidth="1"/>
-    <col min="46" max="46" width="7.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="6.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="48" max="51" width="7.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="52" max="16384" width="9.140625" style="7"/>
+    <col min="1" max="1" width="47.42578125" style="24" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7" style="1" customWidth="1"/>
+    <col min="6" max="7" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.42578125" style="1" customWidth="1"/>
+    <col min="9" max="10" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.7109375" style="1" customWidth="1"/>
+    <col min="12" max="15" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.28515625" style="1" customWidth="1"/>
+    <col min="17" max="20" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="7.42578125" style="1" customWidth="1"/>
+    <col min="22" max="22" width="8.85546875" style="1" customWidth="1"/>
+    <col min="23" max="23" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="7.140625" style="1" customWidth="1"/>
+    <col min="25" max="36" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="8" style="1" customWidth="1"/>
+    <col min="38" max="44" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="8" style="1" customWidth="1"/>
+    <col min="46" max="46" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="6.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="48" max="51" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="52" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:51" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="11">
+      <c r="C1" s="5">
         <v>1920</v>
       </c>
-      <c r="D1" s="11">
+      <c r="D1" s="5">
         <v>1930</v>
       </c>
-      <c r="E1" s="11">
+      <c r="E1" s="5">
         <v>1940</v>
       </c>
-      <c r="F1" s="11">
+      <c r="F1" s="5">
         <v>1950</v>
       </c>
-      <c r="G1" s="11">
+      <c r="G1" s="5">
         <v>1955</v>
       </c>
-      <c r="H1" s="11">
+      <c r="H1" s="5">
         <v>1960</v>
       </c>
-      <c r="I1" s="11">
+      <c r="I1" s="5">
         <v>1965</v>
       </c>
-      <c r="J1" s="11">
+      <c r="J1" s="5">
         <v>1970</v>
       </c>
-      <c r="K1" s="11">
+      <c r="K1" s="5">
         <v>1975</v>
       </c>
-      <c r="L1" s="11">
+      <c r="L1" s="5">
         <v>1976</v>
       </c>
-      <c r="M1" s="11">
+      <c r="M1" s="5">
         <v>1977</v>
       </c>
-      <c r="N1" s="11">
+      <c r="N1" s="5">
         <v>1978</v>
       </c>
-      <c r="O1" s="11">
+      <c r="O1" s="5">
         <v>1979</v>
       </c>
-      <c r="P1" s="11">
+      <c r="P1" s="5">
         <v>1980</v>
       </c>
-      <c r="Q1" s="11">
+      <c r="Q1" s="5">
         <v>1981</v>
       </c>
-      <c r="R1" s="11">
+      <c r="R1" s="5">
         <v>1982</v>
       </c>
-      <c r="S1" s="11">
+      <c r="S1" s="5">
         <v>1983</v>
       </c>
-      <c r="T1" s="11">
+      <c r="T1" s="5">
         <v>1984</v>
       </c>
-      <c r="U1" s="11">
+      <c r="U1" s="5">
         <v>1985</v>
       </c>
-      <c r="V1" s="11">
+      <c r="V1" s="5">
         <v>1986</v>
       </c>
-      <c r="W1" s="11">
+      <c r="W1" s="5">
         <v>1987</v>
       </c>
-      <c r="X1" s="11">
+      <c r="X1" s="5">
         <v>1988</v>
       </c>
-      <c r="Y1" s="11">
+      <c r="Y1" s="5">
         <v>1989</v>
       </c>
-      <c r="Z1" s="11">
+      <c r="Z1" s="5">
         <v>1990</v>
       </c>
-      <c r="AA1" s="11">
+      <c r="AA1" s="5">
         <v>1991</v>
       </c>
-      <c r="AB1" s="11">
+      <c r="AB1" s="5">
         <v>1992</v>
       </c>
-      <c r="AC1" s="11">
+      <c r="AC1" s="5">
         <v>1993</v>
       </c>
-      <c r="AD1" s="11">
+      <c r="AD1" s="5">
         <v>1994</v>
       </c>
-      <c r="AE1" s="11">
+      <c r="AE1" s="5">
         <v>1995</v>
       </c>
-      <c r="AF1" s="11">
+      <c r="AF1" s="5">
         <v>1996</v>
       </c>
-      <c r="AG1" s="11">
+      <c r="AG1" s="5">
         <v>1997</v>
       </c>
-      <c r="AH1" s="11">
+      <c r="AH1" s="5">
         <v>1998</v>
       </c>
-      <c r="AI1" s="11">
+      <c r="AI1" s="5">
         <v>1999</v>
       </c>
-      <c r="AJ1" s="11">
+      <c r="AJ1" s="5">
         <v>2000</v>
       </c>
-      <c r="AK1" s="11">
+      <c r="AK1" s="5">
         <v>2001</v>
       </c>
-      <c r="AL1" s="11">
+      <c r="AL1" s="5">
         <v>2002</v>
       </c>
-      <c r="AM1" s="11">
+      <c r="AM1" s="5">
         <v>2003</v>
       </c>
-      <c r="AN1" s="11">
+      <c r="AN1" s="5">
         <v>2004</v>
       </c>
-      <c r="AO1" s="11">
+      <c r="AO1" s="5">
         <v>2005</v>
       </c>
-      <c r="AP1" s="11">
+      <c r="AP1" s="5">
         <v>2006</v>
       </c>
-      <c r="AQ1" s="11">
+      <c r="AQ1" s="5">
         <v>2007</v>
       </c>
-      <c r="AR1" s="11">
+      <c r="AR1" s="5">
         <v>2008</v>
       </c>
-      <c r="AS1" s="11">
+      <c r="AS1" s="5">
         <v>2009</v>
       </c>
-      <c r="AT1" s="11">
+      <c r="AT1" s="5">
         <v>2010</v>
       </c>
-      <c r="AU1" s="11">
+      <c r="AU1" s="5">
         <v>2011</v>
       </c>
-      <c r="AV1" s="11">
+      <c r="AV1" s="5">
         <v>2012</v>
       </c>
-      <c r="AW1" s="11">
+      <c r="AW1" s="5">
         <v>2013</v>
       </c>
-      <c r="AX1" s="11">
+      <c r="AX1" s="5">
         <v>2014</v>
       </c>
-      <c r="AY1" s="11">
+      <c r="AY1" s="5">
         <v>2015</v>
       </c>
     </row>
-    <row r="2" spans="1:51" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="24" t="s">
+    <row r="2" spans="1:51" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="13">
+      <c r="F2" s="7">
         <v>0</v>
       </c>
-      <c r="H2" s="13">
+      <c r="H2" s="7">
         <v>25</v>
       </c>
-      <c r="K2" s="13">
+      <c r="K2" s="7">
         <v>40</v>
       </c>
-      <c r="P2" s="34"/>
-      <c r="Q2" s="34"/>
-      <c r="R2" s="34"/>
-      <c r="S2" s="34"/>
-      <c r="T2" s="34"/>
-      <c r="U2" s="34"/>
-      <c r="V2" s="34"/>
-      <c r="W2" s="34"/>
-      <c r="X2" s="34"/>
-      <c r="Y2" s="34"/>
-      <c r="Z2" s="34"/>
-      <c r="AA2" s="34"/>
-      <c r="AB2" s="34"/>
-      <c r="AC2" s="34"/>
-      <c r="AD2" s="34"/>
-      <c r="AE2" s="34"/>
-      <c r="AF2" s="34"/>
-      <c r="AG2" s="34"/>
-      <c r="AH2" s="34"/>
-      <c r="AI2" s="34"/>
-      <c r="AJ2" s="34"/>
-      <c r="AK2" s="34"/>
-      <c r="AL2" s="34"/>
-      <c r="AM2" s="34"/>
-      <c r="AN2" s="34"/>
-      <c r="AO2" s="34"/>
-      <c r="AP2" s="34"/>
-      <c r="AQ2" s="34"/>
-      <c r="AR2" s="34"/>
-      <c r="AS2" s="34"/>
-      <c r="AT2" s="34"/>
-      <c r="AU2" s="34"/>
-      <c r="AV2" s="34"/>
-      <c r="AW2" s="34"/>
-      <c r="AX2" s="34"/>
-    </row>
-    <row r="3" spans="1:51" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="24" t="s">
+      <c r="P2" s="28"/>
+      <c r="Q2" s="28"/>
+      <c r="R2" s="28"/>
+      <c r="S2" s="28"/>
+      <c r="T2" s="28"/>
+      <c r="U2" s="28"/>
+      <c r="V2" s="28"/>
+      <c r="W2" s="28"/>
+      <c r="X2" s="28"/>
+      <c r="Y2" s="28"/>
+      <c r="Z2" s="28"/>
+      <c r="AA2" s="28"/>
+      <c r="AB2" s="28"/>
+      <c r="AC2" s="28"/>
+      <c r="AD2" s="28"/>
+      <c r="AE2" s="28"/>
+      <c r="AF2" s="28"/>
+      <c r="AG2" s="28"/>
+      <c r="AH2" s="28"/>
+      <c r="AI2" s="28"/>
+      <c r="AJ2" s="28"/>
+      <c r="AK2" s="28"/>
+      <c r="AL2" s="28"/>
+      <c r="AM2" s="28"/>
+      <c r="AN2" s="28"/>
+      <c r="AO2" s="28"/>
+      <c r="AP2" s="28"/>
+      <c r="AQ2" s="28"/>
+      <c r="AR2" s="28"/>
+      <c r="AS2" s="28"/>
+      <c r="AT2" s="28"/>
+      <c r="AU2" s="28"/>
+      <c r="AV2" s="28"/>
+      <c r="AW2" s="28"/>
+      <c r="AX2" s="28"/>
+    </row>
+    <row r="3" spans="1:51" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="F3" s="13">
+      <c r="F3" s="7">
         <v>0</v>
       </c>
-      <c r="H3" s="13">
+      <c r="H3" s="7">
         <v>10000000</v>
       </c>
-      <c r="K3" s="13">
+      <c r="K3" s="7">
         <v>15040500</v>
       </c>
-      <c r="U3" s="13">
+      <c r="U3" s="7">
         <v>39034561</v>
       </c>
     </row>
-    <row r="4" spans="1:51" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="25" t="s">
+    <row r="4" spans="1:51" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="15">
+      <c r="D4" s="9">
         <v>0</v>
       </c>
-      <c r="I4" s="15">
+      <c r="I4" s="9">
         <v>10</v>
       </c>
-      <c r="R4" s="15">
+      <c r="R4" s="9">
         <v>50</v>
       </c>
-      <c r="Z4" s="35"/>
-      <c r="AA4" s="35"/>
-      <c r="AB4" s="35"/>
-      <c r="AC4" s="35"/>
-      <c r="AD4" s="35"/>
-      <c r="AE4" s="35"/>
-      <c r="AF4" s="35"/>
-      <c r="AG4" s="35"/>
-      <c r="AH4" s="35"/>
-      <c r="AI4" s="35"/>
-      <c r="AJ4" s="35"/>
-      <c r="AK4" s="35"/>
-      <c r="AL4" s="35"/>
-      <c r="AM4" s="35"/>
-      <c r="AN4" s="35"/>
-      <c r="AO4" s="35"/>
-      <c r="AP4" s="35"/>
-      <c r="AQ4" s="35"/>
-      <c r="AR4" s="35"/>
-      <c r="AS4" s="35"/>
-      <c r="AT4" s="35"/>
-      <c r="AU4" s="35"/>
-      <c r="AV4" s="35"/>
-      <c r="AW4" s="35"/>
-      <c r="AX4" s="35"/>
-    </row>
-    <row r="5" spans="1:51" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="25" t="s">
+      <c r="Z4" s="29"/>
+      <c r="AA4" s="29"/>
+      <c r="AB4" s="29"/>
+      <c r="AC4" s="29"/>
+      <c r="AD4" s="29"/>
+      <c r="AE4" s="29"/>
+      <c r="AF4" s="29"/>
+      <c r="AG4" s="29"/>
+      <c r="AH4" s="29"/>
+      <c r="AI4" s="29"/>
+      <c r="AJ4" s="29"/>
+      <c r="AK4" s="29"/>
+      <c r="AL4" s="29"/>
+      <c r="AM4" s="29"/>
+      <c r="AN4" s="29"/>
+      <c r="AO4" s="29"/>
+      <c r="AP4" s="29"/>
+      <c r="AQ4" s="29"/>
+      <c r="AR4" s="29"/>
+      <c r="AS4" s="29"/>
+      <c r="AT4" s="29"/>
+      <c r="AU4" s="29"/>
+      <c r="AV4" s="29"/>
+      <c r="AW4" s="29"/>
+      <c r="AX4" s="29"/>
+    </row>
+    <row r="5" spans="1:51" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="15">
+      <c r="D5" s="9">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:51" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="26" t="s">
+    <row r="6" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="17">
+      <c r="E6" s="11">
         <v>70</v>
       </c>
-      <c r="H6" s="17">
+      <c r="H6" s="11">
         <v>80</v>
       </c>
-      <c r="X6" s="17">
+      <c r="X6" s="11">
         <v>82</v>
       </c>
-      <c r="AK6" s="17">
+      <c r="AK6" s="11">
         <v>84</v>
       </c>
-      <c r="AX6" s="17">
+      <c r="AX6" s="11">
         <v>85</v>
       </c>
     </row>
-    <row r="7" spans="1:51" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="26" t="s">
+    <row r="7" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="16" t="s">
+      <c r="B7" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="E7" s="17">
+      <c r="E7" s="11">
         <v>1005000</v>
       </c>
-      <c r="H7" s="17">
+      <c r="H7" s="11">
         <v>2040504</v>
       </c>
-      <c r="X7" s="17">
+      <c r="X7" s="11">
         <v>4049504</v>
       </c>
     </row>
-    <row r="8" spans="1:51" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="27" t="s">
+    <row r="8" spans="1:51" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="18" t="s">
+      <c r="B8" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="F8" s="19">
+      <c r="F8" s="13">
         <v>30</v>
       </c>
-      <c r="I8" s="19">
+      <c r="I8" s="13">
         <v>40</v>
       </c>
-      <c r="Z8" s="19">
+      <c r="Z8" s="13">
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:51" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="27" t="s">
+    <row r="9" spans="1:51" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="18" t="s">
+      <c r="B9" s="12" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:51" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="28" t="s">
+    <row r="10" spans="1:51" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="20" t="s">
+      <c r="B10" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="P10" s="21">
+      <c r="P10" s="15">
         <v>30</v>
       </c>
-      <c r="Z10" s="21">
+      <c r="Z10" s="15">
         <v>40</v>
       </c>
-      <c r="AJ10" s="21">
+      <c r="AJ10" s="15">
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:51" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="28" t="s">
+    <row r="11" spans="1:51" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="20" t="s">
+      <c r="B11" s="14" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:51" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="29" t="s">
+    <row r="12" spans="1:51" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="22" t="s">
+      <c r="B12" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="G12" s="23">
+      <c r="G12" s="17">
         <v>7</v>
       </c>
-      <c r="U12" s="23">
+      <c r="U12" s="17">
         <v>0</v>
       </c>
-      <c r="AE12" s="23">
+      <c r="AE12" s="17">
         <v>50</v>
       </c>
-      <c r="AJ12" s="23">
+      <c r="AJ12" s="17">
         <v>70</v>
       </c>
     </row>
-    <row r="13" spans="1:51" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="29" t="s">
+    <row r="13" spans="1:51" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="22" t="s">
+      <c r="B13" s="16" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:51" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="27" t="s">
+    <row r="14" spans="1:51" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="B14" s="18" t="s">
+      <c r="B14" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="G14" s="19">
+      <c r="G14" s="13">
         <v>0</v>
       </c>
-      <c r="P14" s="19">
+      <c r="P14" s="13">
         <v>30</v>
       </c>
-      <c r="V14" s="19">
+      <c r="V14" s="13">
         <v>50</v>
       </c>
-      <c r="AD14" s="36"/>
-      <c r="AE14" s="36"/>
-      <c r="AF14" s="36"/>
-      <c r="AG14" s="36"/>
-      <c r="AH14" s="36"/>
-      <c r="AI14" s="36"/>
-      <c r="AJ14" s="36"/>
-      <c r="AK14" s="36"/>
-      <c r="AL14" s="36"/>
-      <c r="AM14" s="36"/>
-      <c r="AN14" s="36"/>
-      <c r="AO14" s="36"/>
-      <c r="AP14" s="36"/>
-      <c r="AQ14" s="36"/>
-      <c r="AR14" s="36"/>
-      <c r="AS14" s="36"/>
-      <c r="AT14" s="36"/>
-      <c r="AU14" s="36"/>
-      <c r="AV14" s="36"/>
-      <c r="AW14" s="36"/>
-    </row>
-    <row r="15" spans="1:51" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="27" t="s">
+      <c r="AD14" s="30"/>
+      <c r="AE14" s="30"/>
+      <c r="AF14" s="30"/>
+      <c r="AG14" s="30"/>
+      <c r="AH14" s="30"/>
+      <c r="AI14" s="30"/>
+      <c r="AJ14" s="30"/>
+      <c r="AK14" s="30"/>
+      <c r="AL14" s="30"/>
+      <c r="AM14" s="30"/>
+      <c r="AN14" s="30"/>
+      <c r="AO14" s="30"/>
+      <c r="AP14" s="30"/>
+      <c r="AQ14" s="30"/>
+      <c r="AR14" s="30"/>
+      <c r="AS14" s="30"/>
+      <c r="AT14" s="30"/>
+      <c r="AU14" s="30"/>
+      <c r="AV14" s="30"/>
+      <c r="AW14" s="30"/>
+    </row>
+    <row r="15" spans="1:51" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="B15" s="18" t="s">
+      <c r="B15" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="G15" s="19">
+      <c r="G15" s="13">
         <v>0</v>
       </c>
-      <c r="P15" s="19">
+      <c r="P15" s="13">
         <v>1926492</v>
       </c>
-      <c r="V15" s="19">
+      <c r="V15" s="13">
         <v>4573928</v>
       </c>
-      <c r="AK15" s="19">
+      <c r="AK15" s="13">
         <v>9382947</v>
       </c>
-      <c r="AS15" s="19">
+      <c r="AS15" s="13">
         <v>52431253</v>
       </c>
     </row>
-    <row r="16" spans="1:51" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="27" t="s">
+    <row r="16" spans="1:51" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="B16" s="18" t="s">
+      <c r="B16" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="G16" s="19">
+      <c r="G16" s="13">
         <v>0</v>
       </c>
-      <c r="P16" s="19">
+      <c r="P16" s="13">
         <v>15</v>
       </c>
-      <c r="V16" s="19">
+      <c r="V16" s="13">
         <v>12</v>
       </c>
-      <c r="AD16" s="36"/>
-      <c r="AE16" s="36"/>
-      <c r="AF16" s="36"/>
-      <c r="AG16" s="36"/>
-      <c r="AH16" s="36"/>
-      <c r="AI16" s="36"/>
-      <c r="AJ16" s="36"/>
-      <c r="AK16" s="36"/>
-      <c r="AL16" s="36"/>
-      <c r="AM16" s="36"/>
-      <c r="AN16" s="36"/>
-      <c r="AO16" s="36"/>
-      <c r="AP16" s="36"/>
-      <c r="AQ16" s="36"/>
-      <c r="AR16" s="36"/>
-      <c r="AS16" s="36"/>
-      <c r="AT16" s="36"/>
-      <c r="AU16" s="36"/>
-      <c r="AV16" s="36"/>
-      <c r="AW16" s="36"/>
-    </row>
-    <row r="17" spans="1:50" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="27" t="s">
+      <c r="AD16" s="30"/>
+      <c r="AE16" s="30"/>
+      <c r="AF16" s="30"/>
+      <c r="AG16" s="30"/>
+      <c r="AH16" s="30"/>
+      <c r="AI16" s="30"/>
+      <c r="AJ16" s="30"/>
+      <c r="AK16" s="30"/>
+      <c r="AL16" s="30"/>
+      <c r="AM16" s="30"/>
+      <c r="AN16" s="30"/>
+      <c r="AO16" s="30"/>
+      <c r="AP16" s="30"/>
+      <c r="AQ16" s="30"/>
+      <c r="AR16" s="30"/>
+      <c r="AS16" s="30"/>
+      <c r="AT16" s="30"/>
+      <c r="AU16" s="30"/>
+      <c r="AV16" s="30"/>
+      <c r="AW16" s="30"/>
+    </row>
+    <row r="17" spans="1:50" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="B17" s="18" t="s">
+      <c r="B17" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="G17" s="19">
+      <c r="G17" s="13">
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:50" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="31" t="s">
+    <row r="18" spans="1:50" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="B18" s="32" t="s">
+      <c r="B18" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="G18" s="33">
+      <c r="G18" s="27">
         <v>0</v>
       </c>
-      <c r="P18" s="33">
+      <c r="P18" s="27">
         <v>15</v>
       </c>
-      <c r="V18" s="33">
+      <c r="V18" s="27">
         <v>30</v>
       </c>
-      <c r="AD18" s="37"/>
-      <c r="AE18" s="37"/>
-      <c r="AF18" s="37"/>
-      <c r="AG18" s="37"/>
-      <c r="AH18" s="37"/>
-      <c r="AI18" s="37"/>
-      <c r="AJ18" s="37"/>
-      <c r="AK18" s="37"/>
-      <c r="AL18" s="37"/>
-      <c r="AM18" s="37"/>
-      <c r="AN18" s="37"/>
-      <c r="AO18" s="37"/>
-      <c r="AP18" s="37"/>
-      <c r="AQ18" s="37"/>
-      <c r="AR18" s="37"/>
-      <c r="AS18" s="37"/>
-      <c r="AT18" s="37"/>
-      <c r="AU18" s="37"/>
-      <c r="AV18" s="37"/>
-      <c r="AW18" s="37"/>
-      <c r="AX18" s="33">
+      <c r="AD18" s="31"/>
+      <c r="AE18" s="31"/>
+      <c r="AF18" s="31"/>
+      <c r="AG18" s="31"/>
+      <c r="AH18" s="31"/>
+      <c r="AI18" s="31"/>
+      <c r="AJ18" s="31"/>
+      <c r="AK18" s="31"/>
+      <c r="AL18" s="31"/>
+      <c r="AM18" s="31"/>
+      <c r="AN18" s="31"/>
+      <c r="AO18" s="31"/>
+      <c r="AP18" s="31"/>
+      <c r="AQ18" s="31"/>
+      <c r="AR18" s="31"/>
+      <c r="AS18" s="31"/>
+      <c r="AT18" s="31"/>
+      <c r="AU18" s="31"/>
+      <c r="AV18" s="31"/>
+      <c r="AW18" s="31"/>
+      <c r="AX18" s="27">
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="1:50" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="31" t="s">
+    <row r="19" spans="1:50" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="B19" s="32" t="s">
+      <c r="B19" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="G19" s="33">
+      <c r="G19" s="27">
         <v>0</v>
       </c>
-      <c r="P19" s="33">
+      <c r="P19" s="27">
         <v>492549</v>
       </c>
-      <c r="V19" s="33">
+      <c r="V19" s="27">
         <v>256491</v>
       </c>
-      <c r="AK19" s="33">
+      <c r="AK19" s="27">
         <v>9382947</v>
       </c>
-      <c r="AS19" s="33">
+      <c r="AS19" s="27">
         <v>52431253</v>
       </c>
     </row>
-    <row r="20" spans="1:50" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="31" t="s">
+    <row r="20" spans="1:50" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="B20" s="32" t="s">
+      <c r="B20" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="G20" s="33">
+      <c r="G20" s="27">
         <v>0</v>
       </c>
-      <c r="P20" s="33">
+      <c r="P20" s="27">
         <v>55</v>
       </c>
-      <c r="V20" s="33">
+      <c r="V20" s="27">
         <v>50</v>
       </c>
-      <c r="AD20" s="37"/>
-      <c r="AE20" s="37"/>
-      <c r="AF20" s="37"/>
-      <c r="AG20" s="37"/>
-      <c r="AH20" s="37"/>
-      <c r="AI20" s="37"/>
-      <c r="AJ20" s="37"/>
-      <c r="AK20" s="37"/>
-      <c r="AL20" s="37"/>
-      <c r="AM20" s="37"/>
-      <c r="AN20" s="37"/>
-      <c r="AO20" s="37"/>
-      <c r="AP20" s="37"/>
-      <c r="AQ20" s="37"/>
-      <c r="AR20" s="37"/>
-      <c r="AS20" s="37"/>
-      <c r="AT20" s="37"/>
-      <c r="AU20" s="37"/>
-      <c r="AV20" s="37"/>
-      <c r="AW20" s="37"/>
-      <c r="AX20" s="33">
+      <c r="AD20" s="31"/>
+      <c r="AE20" s="31"/>
+      <c r="AF20" s="31"/>
+      <c r="AG20" s="31"/>
+      <c r="AH20" s="31"/>
+      <c r="AI20" s="31"/>
+      <c r="AJ20" s="31"/>
+      <c r="AK20" s="31"/>
+      <c r="AL20" s="31"/>
+      <c r="AM20" s="31"/>
+      <c r="AN20" s="31"/>
+      <c r="AO20" s="31"/>
+      <c r="AP20" s="31"/>
+      <c r="AQ20" s="31"/>
+      <c r="AR20" s="31"/>
+      <c r="AS20" s="31"/>
+      <c r="AT20" s="31"/>
+      <c r="AU20" s="31"/>
+      <c r="AV20" s="31"/>
+      <c r="AW20" s="31"/>
+      <c r="AX20" s="27">
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:50" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="31" t="s">
+    <row r="21" spans="1:50" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="B21" s="32" t="s">
+      <c r="B21" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="G21" s="33">
+      <c r="G21" s="27">
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:50" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="25" t="s">
+    <row r="22" spans="1:50" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="B22" s="14" t="s">
+      <c r="B22" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="G22" s="15">
+      <c r="G22" s="9">
         <v>0</v>
       </c>
-      <c r="P22" s="15">
+      <c r="P22" s="9">
         <v>5</v>
       </c>
-      <c r="V22" s="15">
+      <c r="V22" s="9">
         <v>15</v>
       </c>
-      <c r="AD22" s="35"/>
-      <c r="AE22" s="35"/>
-      <c r="AF22" s="35"/>
-      <c r="AG22" s="35"/>
-      <c r="AH22" s="35"/>
-      <c r="AI22" s="35"/>
-      <c r="AJ22" s="35"/>
-      <c r="AK22" s="35"/>
-      <c r="AL22" s="35"/>
-      <c r="AM22" s="35"/>
-      <c r="AN22" s="35"/>
-      <c r="AO22" s="35"/>
-      <c r="AP22" s="35"/>
-      <c r="AQ22" s="35"/>
-      <c r="AR22" s="35"/>
-      <c r="AS22" s="35"/>
-      <c r="AT22" s="35"/>
-      <c r="AU22" s="35"/>
-      <c r="AV22" s="35"/>
-      <c r="AW22" s="35"/>
-      <c r="AX22" s="15">
+      <c r="AD22" s="29"/>
+      <c r="AE22" s="29"/>
+      <c r="AF22" s="29"/>
+      <c r="AG22" s="29"/>
+      <c r="AH22" s="29"/>
+      <c r="AI22" s="29"/>
+      <c r="AJ22" s="29"/>
+      <c r="AK22" s="29"/>
+      <c r="AL22" s="29"/>
+      <c r="AM22" s="29"/>
+      <c r="AN22" s="29"/>
+      <c r="AO22" s="29"/>
+      <c r="AP22" s="29"/>
+      <c r="AQ22" s="29"/>
+      <c r="AR22" s="29"/>
+      <c r="AS22" s="29"/>
+      <c r="AT22" s="29"/>
+      <c r="AU22" s="29"/>
+      <c r="AV22" s="29"/>
+      <c r="AW22" s="29"/>
+      <c r="AX22" s="9">
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="1:50" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="25" t="s">
+    <row r="23" spans="1:50" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="B23" s="14" t="s">
+      <c r="B23" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="G23" s="15">
+      <c r="G23" s="9">
         <v>0</v>
       </c>
-      <c r="P23" s="15">
+      <c r="P23" s="9">
         <v>0</v>
       </c>
-      <c r="V23" s="15">
+      <c r="V23" s="9">
         <v>0</v>
       </c>
-      <c r="AK23" s="15">
+      <c r="AK23" s="9">
         <v>0</v>
       </c>
-      <c r="AS23" s="15">
+      <c r="AS23" s="9">
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:50" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="25" t="s">
+    <row r="24" spans="1:50" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="B24" s="14" t="s">
+      <c r="B24" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="G24" s="15">
+      <c r="G24" s="9">
         <v>0</v>
       </c>
-      <c r="P24" s="15">
+      <c r="P24" s="9">
         <v>65</v>
       </c>
-      <c r="V24" s="15">
+      <c r="V24" s="9">
         <v>62</v>
       </c>
-      <c r="AD24" s="35"/>
-      <c r="AE24" s="35"/>
-      <c r="AF24" s="35"/>
-      <c r="AG24" s="35"/>
-      <c r="AH24" s="35"/>
-      <c r="AI24" s="35"/>
-      <c r="AJ24" s="35"/>
-      <c r="AK24" s="35"/>
-      <c r="AL24" s="35"/>
-      <c r="AM24" s="35"/>
-      <c r="AN24" s="35"/>
-      <c r="AO24" s="35"/>
-      <c r="AP24" s="35"/>
-      <c r="AQ24" s="35"/>
-      <c r="AR24" s="35"/>
-      <c r="AS24" s="35"/>
-      <c r="AT24" s="35"/>
-      <c r="AU24" s="35"/>
-      <c r="AV24" s="35"/>
-      <c r="AW24" s="35"/>
-      <c r="AX24" s="15">
+      <c r="AD24" s="29"/>
+      <c r="AE24" s="29"/>
+      <c r="AF24" s="29"/>
+      <c r="AG24" s="29"/>
+      <c r="AH24" s="29"/>
+      <c r="AI24" s="29"/>
+      <c r="AJ24" s="29"/>
+      <c r="AK24" s="29"/>
+      <c r="AL24" s="29"/>
+      <c r="AM24" s="29"/>
+      <c r="AN24" s="29"/>
+      <c r="AO24" s="29"/>
+      <c r="AP24" s="29"/>
+      <c r="AQ24" s="29"/>
+      <c r="AR24" s="29"/>
+      <c r="AS24" s="29"/>
+      <c r="AT24" s="29"/>
+      <c r="AU24" s="29"/>
+      <c r="AV24" s="29"/>
+      <c r="AW24" s="29"/>
+      <c r="AX24" s="9">
         <v>35</v>
       </c>
     </row>
-    <row r="25" spans="1:50" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="25" t="s">
+    <row r="25" spans="1:50" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="B25" s="14" t="s">
+      <c r="B25" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="G25" s="15">
+      <c r="G25" s="9">
         <v>0</v>
       </c>
     </row>
   </sheetData>
+  <dataValidations count="2">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:BB2 C4:BB4 C6:BB6 C8:BB8 C18:BB18 C10 C10 C20:BB20 C10 C22:BB22 C24:BB24 C10 C10:BB10 C12:BB12 C14:BB14 C16:BB16">
+      <formula1>0</formula1>
+      <formula2>100</formula2>
+    </dataValidation>
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:BB3 C5:BB5 C7:BB7 C9:BB9 C11:BB11 C13:BB13 C15:BB15 C17:BB17 C19:BB19 C21:BB21 C23:BB23 C25:BB25">
+      <formula1>0</formula1>
+      <formula2>100000000000000000000</formula2>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>dropdown_lists!$A$2:$A$4</xm:f>
@@ -3287,7 +3335,7 @@
   <dimension ref="A2:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3314,6 +3362,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetProtection password="D0CB" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Move smoothness of fits to spreadsheets
</commit_message>
<xml_diff>
--- a/autumn/xls/programs_fiji.xlsx
+++ b/autumn/xls/programs_fiji.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="61">
   <si>
     <t>program_rate_restart_presenting</t>
   </si>
@@ -197,6 +197,9 @@
   </si>
   <si>
     <t>Rate at which patients change from the low quality to the high quality health system</t>
+  </si>
+  <si>
+    <t>fitting_smoothness</t>
   </si>
 </sst>
 </file>
@@ -384,7 +387,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -519,6 +522,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="664">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1186,7 +1204,7 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1258,6 +1276,9 @@
     <xf numFmtId="2" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="8" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="664">
     <cellStyle name="Comma 2" xfId="5"/>
@@ -2225,10 +2246,10 @@
   <sheetPr>
     <tabColor theme="3" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2300,56 +2321,64 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="52" t="s">
+      <c r="A7" s="67" t="s">
+        <v>60</v>
+      </c>
+      <c r="B7" s="68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="52" t="s">
         <v>45</v>
       </c>
-      <c r="B7" s="39" t="b">
+      <c r="B8" s="39" t="b">
         <v>0</v>
       </c>
-      <c r="C7" s="40"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="53" t="s">
+      <c r="C8" s="40"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="53" t="s">
         <v>46</v>
       </c>
-      <c r="B8" s="41" t="b">
+      <c r="B9" s="41" t="b">
         <v>0</v>
       </c>
-      <c r="C8" s="42"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="54" t="s">
+      <c r="C9" s="42"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="54" t="s">
         <v>47</v>
       </c>
-      <c r="B9" s="43" t="b">
+      <c r="B10" s="43" t="b">
         <v>0</v>
       </c>
-      <c r="C9" s="44"/>
-    </row>
-    <row r="10" spans="1:10" s="48" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="55" t="s">
+      <c r="C10" s="44"/>
+    </row>
+    <row r="11" spans="1:10" s="48" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="69" t="s">
         <v>50</v>
       </c>
-      <c r="B10" s="48" t="s">
+      <c r="B11" s="48" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="56" t="s">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="56" t="s">
         <v>49</v>
       </c>
-      <c r="B11" s="45"/>
-      <c r="C11" s="45"/>
-      <c r="D11" s="45"/>
-      <c r="E11" s="46"/>
-      <c r="F11" s="47"/>
-      <c r="G11" s="47"/>
-      <c r="H11" s="47"/>
-      <c r="I11" s="47"/>
-      <c r="J11" s="47"/>
+      <c r="B12" s="45"/>
+      <c r="C12" s="45"/>
+      <c r="D12" s="45"/>
+      <c r="E12" s="46"/>
+      <c r="F12" s="47"/>
+      <c r="G12" s="47"/>
+      <c r="H12" s="47"/>
+      <c r="I12" s="47"/>
+      <c r="J12" s="47"/>
     </row>
   </sheetData>
-  <dataValidations xWindow="363" yWindow="440" count="6">
+  <dataValidations xWindow="363" yWindow="440" count="7">
     <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Time to do recent graphs from" prompt="Calendar year that output graphs for recent time start from." sqref="B6">
       <formula1>-10000</formula1>
       <formula2>3000</formula2>
@@ -2364,9 +2393,13 @@
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Strains" prompt="Number of strains (0: single strain model, 2: DS-TB and MDR-TB, 3: DS-TB, MDR-TB and XDR-TB)." sqref="B3:D3"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Comorbidities" prompt="Number of comorbidities (currently up to three, but will be revised as model develops)." sqref="B4:D4"/>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Age breakpoints" prompt="Enter consecutively increasing age breakpoints to create age strata." sqref="B11:E11">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Age breakpoints" prompt="Enter consecutively increasing age breakpoints to create age strata." sqref="B12:E12">
       <formula1>0</formula1>
       <formula2>200</formula2>
+    </dataValidation>
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Function smoothness" prompt="From zero up, with zero being exact fit and higher values being greater smoothness." sqref="B7">
+      <formula1>0</formula1>
+      <formula2>1000</formula2>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2378,15 +2411,9 @@
           <x14:formula1>
             <xm:f>dropdown_lists!$B$2:$B$3</xm:f>
           </x14:formula1>
-          <xm:sqref>B7</xm:sqref>
+          <xm:sqref>B8</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Low quality care access" prompt="Whether to incorporate low quality care access into the model.">
-          <x14:formula1>
-            <xm:f>dropdown_lists!$B$2:$B$4</xm:f>
-          </x14:formula1>
-          <xm:sqref>C7</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Amplification" prompt="Whether amplification to progressively more resistant strains permitted.">
           <x14:formula1>
             <xm:f>dropdown_lists!$B$2:$B$4</xm:f>
           </x14:formula1>
@@ -2394,11 +2421,11 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Amplification" prompt="Whether amplification to progressively more resistant strains permitted.">
           <x14:formula1>
-            <xm:f>dropdown_lists!$B$2:$B$3</xm:f>
+            <xm:f>dropdown_lists!$B$2:$B$4</xm:f>
           </x14:formula1>
-          <xm:sqref>B8</xm:sqref>
+          <xm:sqref>C9</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Misassignment" prompt="Whether patients can be incorrectly detected with the wrong strain.">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Amplification" prompt="Whether amplification to progressively more resistant strains permitted.">
           <x14:formula1>
             <xm:f>dropdown_lists!$B$2:$B$3</xm:f>
           </x14:formula1>
@@ -2406,9 +2433,15 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Misassignment" prompt="Whether patients can be incorrectly detected with the wrong strain.">
           <x14:formula1>
+            <xm:f>dropdown_lists!$B$2:$B$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>B10</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Misassignment" prompt="Whether patients can be incorrectly detected with the wrong strain.">
+          <x14:formula1>
             <xm:f>dropdown_lists!$B$2:$B$4</xm:f>
           </x14:formula1>
-          <xm:sqref>C9</xm:sqref>
+          <xm:sqref>C10</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Smoother dummy scale-up function for Fiji
</commit_message>
<xml_diff>
--- a/autumn/xls/programs_fiji.xlsx
+++ b/autumn/xls/programs_fiji.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="255" windowWidth="20370" windowHeight="7590" tabRatio="807"/>
+    <workbookView xWindow="120" yWindow="255" windowWidth="20370" windowHeight="7590" tabRatio="807" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="model_attributes" sheetId="4" r:id="rId1"/>
@@ -2248,8 +2248,8 @@
   </sheetPr>
   <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2325,7 +2325,7 @@
         <v>60</v>
       </c>
       <c r="B7" s="68">
-        <v>0</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -2566,8 +2566,8 @@
   </sheetPr>
   <dimension ref="A1:AY25"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="N15" sqref="N15"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="R5" sqref="R5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2839,7 +2839,7 @@
         <v>10</v>
       </c>
       <c r="R4" s="9">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="Z4" s="29"/>
       <c r="AA4" s="29"/>

</xml_diff>

<commit_message>
Allow different integration forms from sheet
Looks like the scipy integration isn't running, though. It doesn't seem
to like nan-s very much.
</commit_message>
<xml_diff>
--- a/autumn/xls/programs_fiji.xlsx
+++ b/autumn/xls/programs_fiji.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="255" windowWidth="20370" windowHeight="7590" tabRatio="807" activeTab="2"/>
+    <workbookView xWindow="120" yWindow="255" windowWidth="20370" windowHeight="7590" tabRatio="807"/>
   </bookViews>
   <sheets>
     <sheet name="model_attributes" sheetId="4" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="65">
   <si>
     <t>program_rate_restart_presenting</t>
   </si>
@@ -148,12 +148,6 @@
     <t>n_strains</t>
   </si>
   <si>
-    <t>value_at_iteration</t>
-  </si>
-  <si>
-    <t>first_value</t>
-  </si>
-  <si>
     <t>is_lowquality</t>
   </si>
   <si>
@@ -163,9 +157,6 @@
     <t>is_misassignment</t>
   </si>
   <si>
-    <t>value_at_second_iteration</t>
-  </si>
-  <si>
     <t>age_breakpoints</t>
   </si>
   <si>
@@ -200,6 +191,27 @@
   </si>
   <si>
     <t>fitting_smoothness</t>
+  </si>
+  <si>
+    <t>integration</t>
+  </si>
+  <si>
+    <t>explicit</t>
+  </si>
+  <si>
+    <t>scipy</t>
+  </si>
+  <si>
+    <t>single value needed</t>
+  </si>
+  <si>
+    <t>first value</t>
+  </si>
+  <si>
+    <t>value at iteration</t>
+  </si>
+  <si>
+    <t>value at second iteration</t>
   </si>
 </sst>
 </file>
@@ -1204,7 +1216,7 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1278,7 +1290,14 @@
     <xf numFmtId="2" fontId="8" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="664">
     <cellStyle name="Comma 2" xfId="5"/>
@@ -2246,10 +2265,10 @@
   <sheetPr>
     <tabColor theme="3" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2265,13 +2284,13 @@
         <v>37</v>
       </c>
       <c r="B1" s="33" t="s">
-        <v>44</v>
+        <v>62</v>
       </c>
       <c r="C1" s="33" t="s">
-        <v>43</v>
+        <v>63</v>
       </c>
       <c r="D1" s="32" t="s">
-        <v>48</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -2305,85 +2324,102 @@
       <c r="D4" s="38"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="51" t="s">
+      <c r="A5" s="52" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" s="39" t="b">
+        <v>0</v>
+      </c>
+      <c r="C5" s="40"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="53" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" s="41" t="b">
+        <v>0</v>
+      </c>
+      <c r="C6" s="42"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="54" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" s="43" t="b">
+        <v>0</v>
+      </c>
+      <c r="C7" s="44"/>
+    </row>
+    <row r="8" spans="1:10" s="72" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="75" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" s="76" t="s">
+        <v>61</v>
+      </c>
+      <c r="C8" s="47"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="73" t="s">
         <v>39</v>
       </c>
-      <c r="B5" s="35">
+      <c r="B9" s="74">
         <v>1850</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="51" t="s">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="51" t="s">
         <v>40</v>
       </c>
-      <c r="B6" s="35">
+      <c r="B10" s="35">
         <v>1990</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="67" t="s">
-        <v>60</v>
-      </c>
-      <c r="B7" s="68">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="67" t="s">
+        <v>57</v>
+      </c>
+      <c r="B11" s="68">
         <v>0.25</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="52" t="s">
-        <v>45</v>
-      </c>
-      <c r="B8" s="39" t="b">
-        <v>0</v>
-      </c>
-      <c r="C8" s="40"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="53" t="s">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="69" t="s">
+        <v>58</v>
+      </c>
+      <c r="B12" s="70" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" s="48" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="71" t="s">
+        <v>47</v>
+      </c>
+      <c r="B13" s="48" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="56" t="s">
         <v>46</v>
       </c>
-      <c r="B9" s="41" t="b">
-        <v>0</v>
-      </c>
-      <c r="C9" s="42"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="54" t="s">
-        <v>47</v>
-      </c>
-      <c r="B10" s="43" t="b">
-        <v>0</v>
-      </c>
-      <c r="C10" s="44"/>
-    </row>
-    <row r="11" spans="1:10" s="48" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="69" t="s">
-        <v>50</v>
-      </c>
-      <c r="B11" s="48" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="56" t="s">
-        <v>49</v>
-      </c>
-      <c r="B12" s="45"/>
-      <c r="C12" s="45"/>
-      <c r="D12" s="45"/>
-      <c r="E12" s="46"/>
-      <c r="F12" s="47"/>
-      <c r="G12" s="47"/>
-      <c r="H12" s="47"/>
-      <c r="I12" s="47"/>
-      <c r="J12" s="47"/>
+      <c r="B14" s="45"/>
+      <c r="C14" s="45"/>
+      <c r="D14" s="45"/>
+      <c r="E14" s="46"/>
+      <c r="F14" s="47"/>
+      <c r="G14" s="47"/>
+      <c r="H14" s="47"/>
+      <c r="I14" s="47"/>
+      <c r="J14" s="47"/>
     </row>
   </sheetData>
-  <dataValidations xWindow="363" yWindow="440" count="7">
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Time to do recent graphs from" prompt="Calendar year that output graphs for recent time start from." sqref="B6">
+  <dataValidations xWindow="363" yWindow="440" count="8">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Time to do recent graphs from" prompt="Calendar year that output graphs for recent time start from." sqref="B10">
       <formula1>-10000</formula1>
       <formula2>3000</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Time to start model" prompt="Enter the calendar year that the model runs from." sqref="B5">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Time to start model" prompt="Enter the calendar year that the model runs from." sqref="B9">
       <formula1>-10000</formula1>
       <formula2>3000</formula2>
     </dataValidation>
@@ -2393,55 +2429,59 @@
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Strains" prompt="Number of strains (0: single strain model, 2: DS-TB and MDR-TB, 3: DS-TB, MDR-TB and XDR-TB)." sqref="B3:D3"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Comorbidities" prompt="Number of comorbidities (currently up to three, but will be revised as model develops)." sqref="B4:D4"/>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Age breakpoints" prompt="Enter consecutively increasing age breakpoints to create age strata." sqref="B12:E12">
-      <formula1>0</formula1>
-      <formula2>200</formula2>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Function smoothness" prompt="From zero up, with zero being exact fit and higher values being greater smoothness." sqref="B7">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Function smoothness" prompt="From zero up, with zero being exact fit and higher values being greater smoothness." sqref="B11">
       <formula1>0</formula1>
       <formula2>1000</formula2>
     </dataValidation>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Age breakpoints" prompt="Enter consecutively increasing age breakpoints to create age strata. (Can enter any number, don't enter zero and no upper limit is needed.)" sqref="B14:E14"/>
+    <dataValidation allowBlank="1" showErrorMessage="1" sqref="B8"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xWindow="363" yWindow="440" count="6">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xWindow="363" yWindow="440" count="7">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Low quality care access" prompt="Whether to incorporate low quality care access into the model.">
           <x14:formula1>
             <xm:f>dropdown_lists!$B$2:$B$3</xm:f>
           </x14:formula1>
-          <xm:sqref>B8</xm:sqref>
+          <xm:sqref>B5</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Low quality care access" prompt="Whether to incorporate low quality care access into the model.">
           <x14:formula1>
             <xm:f>dropdown_lists!$B$2:$B$4</xm:f>
           </x14:formula1>
-          <xm:sqref>C8</xm:sqref>
+          <xm:sqref>C5</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Amplification" prompt="Whether amplification to progressively more resistant strains permitted.">
           <x14:formula1>
             <xm:f>dropdown_lists!$B$2:$B$4</xm:f>
           </x14:formula1>
-          <xm:sqref>C9</xm:sqref>
+          <xm:sqref>C6</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Amplification" prompt="Whether amplification to progressively more resistant strains permitted.">
           <x14:formula1>
             <xm:f>dropdown_lists!$B$2:$B$3</xm:f>
           </x14:formula1>
-          <xm:sqref>B9</xm:sqref>
+          <xm:sqref>B6</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Misassignment" prompt="Whether patients can be incorrectly detected with the wrong strain.">
           <x14:formula1>
             <xm:f>dropdown_lists!$B$2:$B$3</xm:f>
           </x14:formula1>
-          <xm:sqref>B10</xm:sqref>
+          <xm:sqref>B7</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Misassignment" prompt="Whether patients can be incorrectly detected with the wrong strain.">
           <x14:formula1>
             <xm:f>dropdown_lists!$B$2:$B$4</xm:f>
           </x14:formula1>
-          <xm:sqref>C10</xm:sqref>
+          <xm:sqref>C7:C8</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Integration" prompt="Which integration package. Explicitly coded or Scipy's integration package.">
+          <x14:formula1>
+            <xm:f>dropdown_lists!$C$2:$C$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>B12</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2477,10 +2517,10 @@
         <v>7</v>
       </c>
       <c r="C1" s="65" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D1" s="65" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:4" s="58" customFormat="1" x14ac:dyDescent="0.25">
@@ -2491,7 +2531,7 @@
         <v>14</v>
       </c>
       <c r="C2" s="58" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -2502,7 +2542,7 @@
         <v>26</v>
       </c>
       <c r="C3" s="59" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -2513,7 +2553,7 @@
         <v>4</v>
       </c>
       <c r="C4" s="59" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -2524,7 +2564,7 @@
         <v>1950</v>
       </c>
       <c r="C5" s="59" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -2535,7 +2575,7 @@
         <v>2050</v>
       </c>
       <c r="C6" s="59" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -2546,7 +2586,7 @@
         <v>2</v>
       </c>
       <c r="C7" s="59" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -2566,7 +2606,7 @@
   </sheetPr>
   <dimension ref="A1:AY25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="R5" sqref="R5"/>
     </sheetView>
   </sheetViews>
@@ -3365,31 +3405,37 @@
   <sheetPr>
     <tabColor theme="0" tint="-4.9989318521683403E-2"/>
   </sheetPr>
-  <dimension ref="A2:B4"/>
+  <dimension ref="A2:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>14</v>
       </c>
       <c r="B2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>15</v>
       </c>
       <c r="B3" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>24</v>
       </c>

</xml_diff>

<commit_message>
Code to prevent the previous bug
Make sure the same round of functions that are needed to calculate
scale-ups are called at both the integration and the diagnostics rounds.
</commit_message>
<xml_diff>
--- a/autumn/xls/programs_fiji.xlsx
+++ b/autumn/xls/programs_fiji.xlsx
@@ -2268,7 +2268,7 @@
   <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2434,7 +2434,7 @@
       <formula2>1000</formula2>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Age breakpoints" prompt="Enter consecutively increasing age breakpoints to create age strata. (Can enter any number, don't enter zero and no upper limit is needed.)" sqref="B14:E14"/>
-    <dataValidation allowBlank="1" showErrorMessage="1" sqref="B8"/>
+    <dataValidation allowBlank="1" showErrorMessage="1" sqref="B8 C8"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2475,7 +2475,7 @@
           <x14:formula1>
             <xm:f>dropdown_lists!$B$2:$B$4</xm:f>
           </x14:formula1>
-          <xm:sqref>C7:C8</xm:sqref>
+          <xm:sqref>C7</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Integration" prompt="Which integration package. Explicitly coded or Scipy's integration package.">
           <x14:formula1>

</xml_diff>

<commit_message>
Forgot to include this with last commit
</commit_message>
<xml_diff>
--- a/autumn/xls/programs_fiji.xlsx
+++ b/autumn/xls/programs_fiji.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="66">
   <si>
     <t>program_rate_restart_presenting</t>
   </si>
@@ -190,9 +190,6 @@
     <t>Rate at which patients change from the low quality to the high quality health system</t>
   </si>
   <si>
-    <t>fitting_smoothness</t>
-  </si>
-  <si>
     <t>integration</t>
   </si>
   <si>
@@ -212,6 +209,12 @@
   </si>
   <si>
     <t>value at second iteration</t>
+  </si>
+  <si>
+    <t>organ_smoothness</t>
+  </si>
+  <si>
+    <t>program_smoothness</t>
   </si>
 </sst>
 </file>
@@ -399,7 +402,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -538,15 +541,35 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -1216,7 +1239,7 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1288,16 +1311,18 @@
     <xf numFmtId="2" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="8" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="664">
     <cellStyle name="Comma 2" xfId="5"/>
@@ -2265,10 +2290,10 @@
   <sheetPr>
     <tabColor theme="3" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2284,13 +2309,13 @@
         <v>37</v>
       </c>
       <c r="B1" s="33" t="s">
+        <v>61</v>
+      </c>
+      <c r="C1" s="33" t="s">
         <v>62</v>
       </c>
-      <c r="C1" s="33" t="s">
+      <c r="D1" s="32" t="s">
         <v>63</v>
-      </c>
-      <c r="D1" s="32" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -2350,20 +2375,20 @@
       </c>
       <c r="C7" s="44"/>
     </row>
-    <row r="8" spans="1:10" s="72" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="75" t="s">
+    <row r="8" spans="1:10" s="69" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="72" t="s">
         <v>37</v>
       </c>
-      <c r="B8" s="76" t="s">
-        <v>61</v>
+      <c r="B8" s="73" t="s">
+        <v>60</v>
       </c>
       <c r="C8" s="47"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="73" t="s">
+      <c r="A9" s="70" t="s">
         <v>39</v>
       </c>
-      <c r="B9" s="74">
+      <c r="B9" s="71">
         <v>1850</v>
       </c>
     </row>
@@ -2376,42 +2401,50 @@
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="67" t="s">
+      <c r="A11" s="75" t="s">
+        <v>65</v>
+      </c>
+      <c r="B11" s="77">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="76" t="s">
+        <v>64</v>
+      </c>
+      <c r="B12" s="78">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="67" t="s">
         <v>57</v>
       </c>
-      <c r="B11" s="68">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="69" t="s">
+      <c r="B13" s="74" t="s">
         <v>58</v>
       </c>
-      <c r="B12" s="70" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" s="48" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="71" t="s">
+    </row>
+    <row r="14" spans="1:10" s="48" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="68" t="s">
         <v>47</v>
       </c>
-      <c r="B13" s="48" t="s">
+      <c r="B14" s="48" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="56" t="s">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="56" t="s">
         <v>46</v>
       </c>
-      <c r="B14" s="45"/>
-      <c r="C14" s="45"/>
-      <c r="D14" s="45"/>
-      <c r="E14" s="46"/>
-      <c r="F14" s="47"/>
-      <c r="G14" s="47"/>
-      <c r="H14" s="47"/>
-      <c r="I14" s="47"/>
-      <c r="J14" s="47"/>
+      <c r="B15" s="45"/>
+      <c r="C15" s="45"/>
+      <c r="D15" s="45"/>
+      <c r="E15" s="46"/>
+      <c r="F15" s="47"/>
+      <c r="G15" s="47"/>
+      <c r="H15" s="47"/>
+      <c r="I15" s="47"/>
+      <c r="J15" s="47"/>
     </row>
   </sheetData>
   <dataValidations xWindow="363" yWindow="440" count="8">
@@ -2429,12 +2462,12 @@
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Strains" prompt="Number of strains (0: single strain model, 2: DS-TB and MDR-TB, 3: DS-TB, MDR-TB and XDR-TB)." sqref="B3:D3"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Comorbidities" prompt="Number of comorbidities (currently up to three, but will be revised as model develops)." sqref="B4:D4"/>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Function smoothness" prompt="From zero up, with zero being exact fit and higher values being greater smoothness." sqref="B11">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Function smoothness" prompt="From zero up, with zero being exact fit and higher values being greater smoothness." sqref="B11:B12">
       <formula1>0</formula1>
       <formula2>1000</formula2>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Age breakpoints" prompt="Enter consecutively increasing age breakpoints to create age strata. (Can enter any number, don't enter zero and no upper limit is needed.)" sqref="B14:E14"/>
-    <dataValidation allowBlank="1" showErrorMessage="1" sqref="B8 C8"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Age breakpoints" prompt="Enter consecutively increasing age breakpoints to create age strata. (Can enter any number, don't enter zero and no upper limit is needed.)" sqref="B15:E15"/>
+    <dataValidation allowBlank="1" showErrorMessage="1" sqref="B8:C8"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2481,7 +2514,7 @@
           <x14:formula1>
             <xm:f>dropdown_lists!$C$2:$C$3</xm:f>
           </x14:formula1>
-          <xm:sqref>B12</xm:sqref>
+          <xm:sqref>B13</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -3421,7 +3454,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -3432,7 +3465,7 @@
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Set initial conditions from sheets
</commit_message>
<xml_diff>
--- a/autumn/xls/programs_fiji.xlsx
+++ b/autumn/xls/programs_fiji.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="70">
   <si>
     <t>program_rate_restart_presenting</t>
   </si>
@@ -215,6 +215,18 @@
   </si>
   <si>
     <t>program_smoothness</t>
+  </si>
+  <si>
+    <t>population</t>
+  </si>
+  <si>
+    <t>susceptible_fully</t>
+  </si>
+  <si>
+    <t>active</t>
+  </si>
+  <si>
+    <t>start_compartments</t>
   </si>
 </sst>
 </file>
@@ -1239,7 +1251,7 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1323,6 +1335,11 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="8" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="664">
     <cellStyle name="Comma 2" xfId="5"/>
@@ -2290,10 +2307,10 @@
   <sheetPr>
     <tabColor theme="3" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:J15"/>
+  <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2304,7 +2321,7 @@
     <col min="4" max="4" width="25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="32" t="s">
         <v>37</v>
       </c>
@@ -2318,17 +2335,17 @@
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="49" t="s">
         <v>41</v>
       </c>
       <c r="B2" s="36">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C2" s="36"/>
       <c r="D2" s="34"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="49" t="s">
         <v>42</v>
       </c>
@@ -2338,7 +2355,7 @@
       <c r="C3" s="36"/>
       <c r="D3" s="34"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="50" t="s">
         <v>38</v>
       </c>
@@ -2348,7 +2365,7 @@
       <c r="C4" s="37"/>
       <c r="D4" s="38"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="52" t="s">
         <v>43</v>
       </c>
@@ -2357,7 +2374,7 @@
       </c>
       <c r="C5" s="40"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="53" t="s">
         <v>44</v>
       </c>
@@ -2366,7 +2383,7 @@
       </c>
       <c r="C6" s="42"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="54" t="s">
         <v>45</v>
       </c>
@@ -2375,84 +2392,111 @@
       </c>
       <c r="C7" s="44"/>
     </row>
-    <row r="8" spans="1:10" s="69" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" s="82" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="72" t="s">
+        <v>69</v>
+      </c>
+      <c r="B8" s="73" t="s">
+        <v>66</v>
+      </c>
+      <c r="C8" s="73"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="79" t="s">
+        <v>67</v>
+      </c>
+      <c r="B9" s="83">
+        <v>20000000</v>
+      </c>
+      <c r="C9" s="47"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="80" t="s">
+        <v>68</v>
+      </c>
+      <c r="B10" s="81">
+        <v>3</v>
+      </c>
+      <c r="C10" s="47"/>
+    </row>
+    <row r="11" spans="1:4" s="69" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="72" t="s">
         <v>37</v>
       </c>
-      <c r="B8" s="73" t="s">
+      <c r="B11" s="73" t="s">
         <v>60</v>
       </c>
-      <c r="C8" s="47"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="70" t="s">
+      <c r="C11" s="47"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="70" t="s">
         <v>39</v>
       </c>
-      <c r="B9" s="71">
+      <c r="B12" s="71">
         <v>1850</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="51" t="s">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="51" t="s">
         <v>40</v>
       </c>
-      <c r="B10" s="35">
+      <c r="B13" s="35">
         <v>1990</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="75" t="s">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="75" t="s">
         <v>65</v>
       </c>
-      <c r="B11" s="77">
+      <c r="B14" s="77">
         <v>0.25</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="76" t="s">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="76" t="s">
         <v>64</v>
       </c>
-      <c r="B12" s="78">
+      <c r="B15" s="78">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="67" t="s">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="67" t="s">
         <v>57</v>
       </c>
-      <c r="B13" s="74" t="s">
+      <c r="B16" s="74" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="14" spans="1:10" s="48" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="68" t="s">
+    <row r="17" spans="1:10" s="48" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="68" t="s">
         <v>47</v>
       </c>
-      <c r="B14" s="48" t="s">
+      <c r="B17" s="48" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="56" t="s">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="56" t="s">
         <v>46</v>
       </c>
-      <c r="B15" s="45"/>
-      <c r="C15" s="45"/>
-      <c r="D15" s="45"/>
-      <c r="E15" s="46"/>
-      <c r="F15" s="47"/>
-      <c r="G15" s="47"/>
-      <c r="H15" s="47"/>
-      <c r="I15" s="47"/>
-      <c r="J15" s="47"/>
+      <c r="B18" s="45"/>
+      <c r="C18" s="45"/>
+      <c r="D18" s="45"/>
+      <c r="E18" s="46"/>
+      <c r="F18" s="47"/>
+      <c r="G18" s="47"/>
+      <c r="H18" s="47"/>
+      <c r="I18" s="47"/>
+      <c r="J18" s="47"/>
     </row>
   </sheetData>
   <dataValidations xWindow="363" yWindow="440" count="8">
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Time to do recent graphs from" prompt="Calendar year that output graphs for recent time start from." sqref="B10">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Time to do recent graphs from" prompt="Calendar year that output graphs for recent time start from." sqref="B13">
       <formula1>-10000</formula1>
       <formula2>3000</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Time to start model" prompt="Enter the calendar year that the model runs from." sqref="B9">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Time to start model" prompt="Enter the calendar year that the model runs from." sqref="B12">
       <formula1>-10000</formula1>
       <formula2>3000</formula2>
     </dataValidation>
@@ -2462,12 +2506,12 @@
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Strains" prompt="Number of strains (0: single strain model, 2: DS-TB and MDR-TB, 3: DS-TB, MDR-TB and XDR-TB)." sqref="B3:D3"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Comorbidities" prompt="Number of comorbidities (currently up to three, but will be revised as model develops)." sqref="B4:D4"/>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Function smoothness" prompt="From zero up, with zero being exact fit and higher values being greater smoothness." sqref="B11:B12">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Function smoothness" prompt="From zero up, with zero being exact fit and higher values being greater smoothness." sqref="B14:B15">
       <formula1>0</formula1>
       <formula2>1000</formula2>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Age breakpoints" prompt="Enter consecutively increasing age breakpoints to create age strata. (Can enter any number, don't enter zero and no upper limit is needed.)" sqref="B15:E15"/>
-    <dataValidation allowBlank="1" showErrorMessage="1" sqref="B8:C8"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Age breakpoints" prompt="Enter consecutively increasing age breakpoints to create age strata. (Can enter any number, don't enter zero and no upper limit is needed.)" sqref="B18:E18"/>
+    <dataValidation allowBlank="1" showErrorMessage="1" sqref="B11:C11 C8:C10 B8:B10"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2514,7 +2558,7 @@
           <x14:formula1>
             <xm:f>dropdown_lists!$C$2:$C$3</xm:f>
           </x14:formula1>
-          <xm:sqref>B13</xm:sqref>
+          <xm:sqref>B16</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Select method of fitting from spreadsheet
</commit_message>
<xml_diff>
--- a/autumn/xls/programs_fiji.xlsx
+++ b/autumn/xls/programs_fiji.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="71">
   <si>
     <t>program_rate_restart_presenting</t>
   </si>
@@ -227,6 +227,9 @@
   </si>
   <si>
     <t>start_compartments</t>
+  </si>
+  <si>
+    <t>fitting_method</t>
   </si>
 </sst>
 </file>
@@ -414,7 +417,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -584,6 +587,15 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="664">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1251,7 +1263,7 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1340,6 +1352,8 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="11" fontId="0" fillId="8" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="664">
     <cellStyle name="Comma 2" xfId="5"/>
@@ -2307,10 +2321,10 @@
   <sheetPr>
     <tabColor theme="3" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:J18"/>
+  <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2446,49 +2460,57 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="75" t="s">
+        <v>70</v>
+      </c>
+      <c r="B14" s="77">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="84" t="s">
         <v>65</v>
       </c>
-      <c r="B14" s="77">
+      <c r="B15" s="85">
         <v>0.25</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="76" t="s">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="76" t="s">
         <v>64</v>
       </c>
-      <c r="B15" s="78">
+      <c r="B16" s="78">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="67" t="s">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="67" t="s">
         <v>57</v>
       </c>
-      <c r="B16" s="74" t="s">
+      <c r="B17" s="74" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="17" spans="1:10" s="48" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="68" t="s">
+    <row r="18" spans="1:10" s="48" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="68" t="s">
         <v>47</v>
       </c>
-      <c r="B17" s="48" t="s">
+      <c r="B18" s="48" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="56" t="s">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="56" t="s">
         <v>46</v>
       </c>
-      <c r="B18" s="45"/>
-      <c r="C18" s="45"/>
-      <c r="D18" s="45"/>
-      <c r="E18" s="46"/>
-      <c r="F18" s="47"/>
-      <c r="G18" s="47"/>
-      <c r="H18" s="47"/>
-      <c r="I18" s="47"/>
-      <c r="J18" s="47"/>
+      <c r="B19" s="45"/>
+      <c r="C19" s="45"/>
+      <c r="D19" s="45"/>
+      <c r="E19" s="46"/>
+      <c r="F19" s="47"/>
+      <c r="G19" s="47"/>
+      <c r="H19" s="47"/>
+      <c r="I19" s="47"/>
+      <c r="J19" s="47"/>
     </row>
   </sheetData>
   <dataValidations xWindow="363" yWindow="440" count="8">
@@ -2506,12 +2528,12 @@
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Strains" prompt="Number of strains (0: single strain model, 2: DS-TB and MDR-TB, 3: DS-TB, MDR-TB and XDR-TB)." sqref="B3:D3"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Comorbidities" prompt="Number of comorbidities (currently up to three, but will be revised as model develops)." sqref="B4:D4"/>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Function smoothness" prompt="From zero up, with zero being exact fit and higher values being greater smoothness." sqref="B14:B15">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Function smoothness" prompt="From zero up, with zero being exact fit and higher values being greater smoothness." sqref="B14:B16">
       <formula1>0</formula1>
       <formula2>1000</formula2>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Age breakpoints" prompt="Enter consecutively increasing age breakpoints to create age strata. (Can enter any number, don't enter zero and no upper limit is needed.)" sqref="B18:E18"/>
-    <dataValidation allowBlank="1" showErrorMessage="1" sqref="B11:C11 C8:C10 B8:B10"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Age breakpoints" prompt="Enter consecutively increasing age breakpoints to create age strata. (Can enter any number, don't enter zero and no upper limit is needed.)" sqref="B19:E19"/>
+    <dataValidation allowBlank="1" showErrorMessage="1" sqref="B8:C11"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2558,7 +2580,7 @@
           <x14:formula1>
             <xm:f>dropdown_lists!$C$2:$C$3</xm:f>
           </x14:formula1>
-          <xm:sqref>B16</xm:sqref>
+          <xm:sqref>B17</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Plotting model outputs against GTB data
Plot incidence, prevalence, mortality and notifications against the GTB
data, with subplotting windows.
</commit_message>
<xml_diff>
--- a/autumn/xls/programs_fiji.xlsx
+++ b/autumn/xls/programs_fiji.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="255" windowWidth="20370" windowHeight="7590" tabRatio="807"/>
+    <workbookView xWindow="120" yWindow="255" windowWidth="20370" windowHeight="7590" tabRatio="807" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="model_attributes" sheetId="4" r:id="rId1"/>
@@ -2323,7 +2323,7 @@
   </sheetPr>
   <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
@@ -2595,8 +2595,8 @@
   </sheetPr>
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2627,7 +2627,7 @@
         <v>8</v>
       </c>
       <c r="B2" s="62">
-        <v>14</v>
+        <v>2.4</v>
       </c>
       <c r="C2" s="58" t="s">
         <v>51</v>

</xml_diff>

<commit_message>
Some default smoothness parameters
... entered into spreadsheet.
</commit_message>
<xml_diff>
--- a/autumn/xls/programs_fiji.xlsx
+++ b/autumn/xls/programs_fiji.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="255" windowWidth="20370" windowHeight="7590" tabRatio="807" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="255" windowWidth="20370" windowHeight="7590" tabRatio="807"/>
   </bookViews>
   <sheets>
     <sheet name="model_attributes" sheetId="4" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="72">
   <si>
     <t>program_rate_restart_presenting</t>
   </si>
@@ -230,6 +230,9 @@
   </si>
   <si>
     <t>fitting_method</t>
+  </si>
+  <si>
+    <t>detection_smoothness</t>
   </si>
 </sst>
 </file>
@@ -2321,15 +2324,15 @@
   <sheetPr>
     <tabColor theme="3" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:J19"/>
+  <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.42578125" style="55" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.7109375" style="55" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25" bestFit="1" customWidth="1"/>
@@ -2471,46 +2474,54 @@
         <v>65</v>
       </c>
       <c r="B15" s="85">
-        <v>0.25</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="76" t="s">
+      <c r="A16" s="84" t="s">
+        <v>71</v>
+      </c>
+      <c r="B16" s="85">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="76" t="s">
         <v>64</v>
       </c>
-      <c r="B16" s="78">
+      <c r="B17" s="78">
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="67" t="s">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="67" t="s">
         <v>57</v>
       </c>
-      <c r="B17" s="74" t="s">
+      <c r="B18" s="74" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="18" spans="1:10" s="48" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="68" t="s">
+    <row r="19" spans="1:10" s="48" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="68" t="s">
         <v>47</v>
       </c>
-      <c r="B18" s="48" t="s">
+      <c r="B19" s="48" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="56" t="s">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="56" t="s">
         <v>46</v>
       </c>
-      <c r="B19" s="45"/>
-      <c r="C19" s="45"/>
-      <c r="D19" s="45"/>
-      <c r="E19" s="46"/>
-      <c r="F19" s="47"/>
-      <c r="G19" s="47"/>
-      <c r="H19" s="47"/>
-      <c r="I19" s="47"/>
-      <c r="J19" s="47"/>
+      <c r="B20" s="45"/>
+      <c r="C20" s="45"/>
+      <c r="D20" s="45"/>
+      <c r="E20" s="46"/>
+      <c r="F20" s="47"/>
+      <c r="G20" s="47"/>
+      <c r="H20" s="47"/>
+      <c r="I20" s="47"/>
+      <c r="J20" s="47"/>
     </row>
   </sheetData>
   <dataValidations xWindow="363" yWindow="440" count="8">
@@ -2528,11 +2539,11 @@
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Strains" prompt="Number of strains (0: single strain model, 2: DS-TB and MDR-TB, 3: DS-TB, MDR-TB and XDR-TB)." sqref="B3:D3"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Comorbidities" prompt="Number of comorbidities (currently up to three, but will be revised as model develops)." sqref="B4:D4"/>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Function smoothness" prompt="From zero up, with zero being exact fit and higher values being greater smoothness." sqref="B14:B16">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Function smoothness" prompt="From zero up, with zero being exact fit and higher values being greater smoothness." sqref="B14:B17">
       <formula1>0</formula1>
       <formula2>1000</formula2>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Age breakpoints" prompt="Enter consecutively increasing age breakpoints to create age strata. (Can enter any number, don't enter zero and no upper limit is needed.)" sqref="B19:E19"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Age breakpoints" prompt="Enter consecutively increasing age breakpoints to create age strata. (Can enter any number, don't enter zero and no upper limit is needed.)" sqref="B20:E20"/>
     <dataValidation allowBlank="1" showErrorMessage="1" sqref="B8:C11"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2580,7 +2591,7 @@
           <x14:formula1>
             <xm:f>dropdown_lists!$C$2:$C$3</xm:f>
           </x14:formula1>
-          <xm:sqref>B17</xm:sqref>
+          <xm:sqref>B18</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2595,8 +2606,8 @@
   </sheetPr>
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Add death under-reporting parameter
Add a multiplier to the mortality calculations that corrects for the
under-reporting of death. At present this is just a single, manually
calculated scalar.
</commit_message>
<xml_diff>
--- a/autumn/xls/programs_fiji.xlsx
+++ b/autumn/xls/programs_fiji.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="255" windowWidth="20370" windowHeight="7590" tabRatio="807"/>
+    <workbookView xWindow="120" yWindow="315" windowWidth="20370" windowHeight="7530" tabRatio="807" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="model_attributes" sheetId="4" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="74">
   <si>
     <t>program_rate_restart_presenting</t>
   </si>
@@ -233,6 +233,12 @@
   </si>
   <si>
     <t>detection_smoothness</t>
+  </si>
+  <si>
+    <t>program_proportion_death_reporting</t>
+  </si>
+  <si>
+    <t>Proportion of all TB-related deaths that are correctly reported as such</t>
   </si>
 </sst>
 </file>
@@ -2326,8 +2332,8 @@
   </sheetPr>
   <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2357,7 +2363,7 @@
         <v>41</v>
       </c>
       <c r="B2" s="36">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C2" s="36"/>
       <c r="D2" s="34"/>
@@ -2423,7 +2429,7 @@
         <v>67</v>
       </c>
       <c r="B9" s="83">
-        <v>20000000</v>
+        <v>457200</v>
       </c>
       <c r="C9" s="47"/>
     </row>
@@ -2450,7 +2456,7 @@
         <v>39</v>
       </c>
       <c r="B12" s="71">
-        <v>1850</v>
+        <v>1900</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -2474,7 +2480,7 @@
         <v>65</v>
       </c>
       <c r="B15" s="85">
-        <v>0.4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -2606,8 +2612,8 @@
   </sheetPr>
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2638,7 +2644,7 @@
         <v>8</v>
       </c>
       <c r="B2" s="62">
-        <v>2.4</v>
+        <v>6.6</v>
       </c>
       <c r="C2" s="58" t="s">
         <v>51</v>
@@ -2700,8 +2706,15 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="60"/>
-      <c r="B8" s="63"/>
+      <c r="A8" s="60" t="s">
+        <v>72</v>
+      </c>
+      <c r="B8" s="63">
+        <v>0.35</v>
+      </c>
+      <c r="C8" s="59" t="s">
+        <v>73</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Tidy spreadsheet and update jobs list
</commit_message>
<xml_diff>
--- a/autumn/xls/programs_fiji.xlsx
+++ b/autumn/xls/programs_fiji.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="315" windowWidth="20370" windowHeight="7530" tabRatio="807" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="315" windowWidth="20370" windowHeight="7530" tabRatio="807" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="model_attributes" sheetId="4" r:id="rId1"/>
@@ -2333,7 +2333,7 @@
   <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2504,7 +2504,7 @@
         <v>57</v>
       </c>
       <c r="B18" s="74" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="19" spans="1:10" s="48" customFormat="1" x14ac:dyDescent="0.25">
@@ -2612,8 +2612,8 @@
   </sheetPr>
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2729,8 +2729,8 @@
   </sheetPr>
   <dimension ref="A1:AY25"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="R5" sqref="R5"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3515,7 +3515,7 @@
           <x14:formula1>
             <xm:f>dropdown_lists!$A$2:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>B2:B13</xm:sqref>
+          <xm:sqref>B24 B22 B20 B18 B16 B14 B2 B4 B6 B8 B10 B12 B3 B5 B7 B9 B11 B13 B15 B17 B19 B21 B23 B25</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Add time to start treatment to spreadsheet
Imported into the model module, but not yet implemented.
</commit_message>
<xml_diff>
--- a/autumn/xls/programs_fiji.xlsx
+++ b/autumn/xls/programs_fiji.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="76">
   <si>
     <t>program_rate_restart_presenting</t>
   </si>
@@ -239,6 +239,12 @@
   </si>
   <si>
     <t>Proportion of all TB-related deaths that are correctly reported as such</t>
+  </si>
+  <si>
+    <t>program_timeperiod_await_treatment</t>
+  </si>
+  <si>
+    <t>program_cost_await_treatment</t>
   </si>
 </sst>
 </file>
@@ -341,7 +347,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="15">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -422,6 +428,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1272,7 +1284,7 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="86">
+  <cellXfs count="90">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1363,6 +1375,10 @@
     <xf numFmtId="11" fontId="0" fillId="8" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="664">
     <cellStyle name="Comma 2" xfId="5"/>
@@ -2727,10 +2743,10 @@
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:AY25"/>
+  <dimension ref="A1:AY27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2757,7 +2773,9 @@
     <col min="45" max="45" width="8" style="1" customWidth="1"/>
     <col min="46" max="46" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="47" max="47" width="6.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="48" max="51" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="48" max="49" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="7.85546875" style="1" customWidth="1"/>
+    <col min="51" max="51" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="52" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
@@ -3495,13 +3513,77 @@
         <v>0</v>
       </c>
     </row>
+    <row r="26" spans="1:50" s="88" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="86" t="s">
+        <v>74</v>
+      </c>
+      <c r="B26" s="87" t="s">
+        <v>14</v>
+      </c>
+      <c r="G26" s="88">
+        <f>14/365</f>
+        <v>3.8356164383561646E-2</v>
+      </c>
+      <c r="P26" s="88">
+        <f>14/365</f>
+        <v>3.8356164383561646E-2</v>
+      </c>
+      <c r="V26" s="88">
+        <f>14/365</f>
+        <v>3.8356164383561646E-2</v>
+      </c>
+      <c r="AD26" s="89"/>
+      <c r="AE26" s="89"/>
+      <c r="AF26" s="89"/>
+      <c r="AG26" s="89"/>
+      <c r="AH26" s="89"/>
+      <c r="AI26" s="89"/>
+      <c r="AJ26" s="89"/>
+      <c r="AK26" s="89"/>
+      <c r="AL26" s="89"/>
+      <c r="AM26" s="89"/>
+      <c r="AN26" s="89"/>
+      <c r="AO26" s="89"/>
+      <c r="AP26" s="89"/>
+      <c r="AQ26" s="89"/>
+      <c r="AR26" s="89"/>
+      <c r="AS26" s="89"/>
+      <c r="AT26" s="89"/>
+      <c r="AU26" s="89"/>
+      <c r="AV26" s="89"/>
+      <c r="AW26" s="89"/>
+      <c r="AX26" s="88">
+        <f>14/365</f>
+        <v>3.8356164383561646E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:50" s="88" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="86" t="s">
+        <v>75</v>
+      </c>
+      <c r="B27" s="87" t="s">
+        <v>24</v>
+      </c>
+      <c r="G27" s="88">
+        <v>0</v>
+      </c>
+      <c r="P27" s="88">
+        <v>532947</v>
+      </c>
+      <c r="V27" s="88">
+        <v>9283747</v>
+      </c>
+      <c r="AX27" s="88">
+        <v>739284639</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:BB2 C4:BB4 C6:BB6 C8:BB8 C18:BB18 C10 C10 C20:BB20 C10 C22:BB22 C24:BB24 C10 C10:BB10 C12:BB12 C14:BB14 C16:BB16">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:BB2 C4:BB4 C6:BB6 C8:BB8 C18:BB18 C20:BB20 C22:BB22 C24:BB24 C10:BB10 C12:BB12 C14:BB14 C16:BB16 C26:BB26">
       <formula1>0</formula1>
       <formula2>100</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:BB3 C5:BB5 C7:BB7 C9:BB9 C11:BB11 C13:BB13 C15:BB15 C17:BB17 C19:BB19 C21:BB21 C23:BB23 C25:BB25">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:BB3 C5:BB5 C7:BB7 C9:BB9 C11:BB11 C13:BB13 C15:BB15 C17:BB17 C19:BB19 C21:BB21 C23:BB23 C25:BB25 C27:BB27">
       <formula1>0</formula1>
       <formula2>100000000000000000000</formula2>
     </dataValidation>
@@ -3515,7 +3597,7 @@
           <x14:formula1>
             <xm:f>dropdown_lists!$A$2:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>B24 B22 B20 B18 B16 B14 B2 B4 B6 B8 B10 B12 B3 B5 B7 B9 B11 B13 B15 B17 B19 B21 B23 B25</xm:sqref>
+          <xm:sqref>B2:B27</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Tidy up await treatment addition to sheet
</commit_message>
<xml_diff>
--- a/autumn/xls/programs_fiji.xlsx
+++ b/autumn/xls/programs_fiji.xlsx
@@ -2349,7 +2349,7 @@
   <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2520,7 +2520,7 @@
         <v>57</v>
       </c>
       <c r="B18" s="74" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="19" spans="1:10" s="48" customFormat="1" x14ac:dyDescent="0.25">
@@ -2629,7 +2629,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2745,8 +2745,8 @@
   </sheetPr>
   <dimension ref="A1:AY27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AX5" sqref="AX5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2763,8 +2763,7 @@
     <col min="12" max="15" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="7.28515625" style="1" customWidth="1"/>
     <col min="17" max="20" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="7.42578125" style="1" customWidth="1"/>
-    <col min="22" max="22" width="8.85546875" style="1" customWidth="1"/>
+    <col min="21" max="22" width="7.42578125" style="1" customWidth="1"/>
     <col min="23" max="23" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="7.140625" style="1" customWidth="1"/>
     <col min="25" max="36" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
@@ -3046,7 +3045,9 @@
       <c r="AU4" s="29"/>
       <c r="AV4" s="29"/>
       <c r="AW4" s="29"/>
-      <c r="AX4" s="29"/>
+      <c r="AX4" s="29">
+        <v>40</v>
+      </c>
     </row>
     <row r="5" spans="1:51" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
@@ -3520,17 +3521,9 @@
       <c r="B26" s="87" t="s">
         <v>14</v>
       </c>
-      <c r="G26" s="88">
-        <f>14/365</f>
-        <v>3.8356164383561646E-2</v>
-      </c>
-      <c r="P26" s="88">
-        <f>14/365</f>
-        <v>3.8356164383561646E-2</v>
-      </c>
-      <c r="V26" s="88">
-        <f>14/365</f>
-        <v>3.8356164383561646E-2</v>
+      <c r="C26" s="88">
+        <f>1/26</f>
+        <v>3.8461538461538464E-2</v>
       </c>
       <c r="AD26" s="89"/>
       <c r="AE26" s="89"/>
@@ -3553,8 +3546,8 @@
       <c r="AV26" s="89"/>
       <c r="AW26" s="89"/>
       <c r="AX26" s="88">
-        <f>14/365</f>
-        <v>3.8356164383561646E-2</v>
+        <f>1/26</f>
+        <v>3.8461538461538464E-2</v>
       </c>
     </row>
     <row r="27" spans="1:50" s="88" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Change that should get variable wait times
Unfortunately, when the set_fixed_transfer_rates_flows functions are
changed to set_var_transfer_rate_flow, the integration won't work for
scipy, but only for explicit. Can't understand why, Romain trying to
debug.
</commit_message>
<xml_diff>
--- a/autumn/xls/programs_fiji.xlsx
+++ b/autumn/xls/programs_fiji.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="315" windowWidth="20370" windowHeight="7530" tabRatio="807" activeTab="2"/>
+    <workbookView xWindow="120" yWindow="315" windowWidth="20370" windowHeight="7530" tabRatio="807"/>
   </bookViews>
   <sheets>
     <sheet name="model_attributes" sheetId="4" r:id="rId1"/>
@@ -2348,8 +2348,8 @@
   </sheetPr>
   <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2745,8 +2745,8 @@
   </sheetPr>
   <dimension ref="A1:AY27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AX5" sqref="AX5"/>
+    <sheetView topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AX27" sqref="AX27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3045,9 +3045,7 @@
       <c r="AU4" s="29"/>
       <c r="AV4" s="29"/>
       <c r="AW4" s="29"/>
-      <c r="AX4" s="29">
-        <v>40</v>
-      </c>
+      <c r="AX4" s="29"/>
     </row>
     <row r="5" spans="1:51" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
@@ -3546,8 +3544,7 @@
       <c r="AV26" s="89"/>
       <c r="AW26" s="89"/>
       <c r="AX26" s="88">
-        <f>1/26</f>
-        <v>3.8461538461538464E-2</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="27" spans="1:50" s="88" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Underpinnings to running scenarios
Spreadsheet reading code to underpin running scenarios.
</commit_message>
<xml_diff>
--- a/autumn/xls/programs_fiji.xlsx
+++ b/autumn/xls/programs_fiji.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="79">
   <si>
     <t>program_rate_restart_presenting</t>
   </si>
@@ -245,6 +245,15 @@
   </si>
   <si>
     <t>program_cost_await_treatment</t>
+  </si>
+  <si>
+    <t>scenario_1</t>
+  </si>
+  <si>
+    <t>scenario_end_time</t>
+  </si>
+  <si>
+    <t>current_time</t>
   </si>
 </sst>
 </file>
@@ -1284,7 +1293,7 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1379,6 +1388,7 @@
     <xf numFmtId="0" fontId="7" fillId="15" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="664">
     <cellStyle name="Comma 2" xfId="5"/>
@@ -2346,10 +2356,10 @@
   <sheetPr>
     <tabColor theme="3" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:J20"/>
+  <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2484,70 +2494,86 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="75" t="s">
+      <c r="A14" s="51" t="s">
+        <v>78</v>
+      </c>
+      <c r="B14" s="35">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="51" t="s">
+        <v>77</v>
+      </c>
+      <c r="B15" s="90">
+        <v>2035</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="75" t="s">
         <v>70</v>
       </c>
-      <c r="B14" s="77">
+      <c r="B16" s="77">
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="84" t="s">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="84" t="s">
         <v>65</v>
       </c>
-      <c r="B15" s="85">
+      <c r="B17" s="85">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="84" t="s">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="84" t="s">
         <v>71</v>
       </c>
-      <c r="B16" s="85">
+      <c r="B18" s="85">
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="76" t="s">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="76" t="s">
         <v>64</v>
       </c>
-      <c r="B17" s="78">
+      <c r="B19" s="78">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="67" t="s">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="67" t="s">
         <v>57</v>
       </c>
-      <c r="B18" s="74" t="s">
+      <c r="B20" s="74" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="19" spans="1:10" s="48" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="68" t="s">
+    <row r="21" spans="1:10" s="48" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="68" t="s">
         <v>47</v>
       </c>
-      <c r="B19" s="48" t="s">
+      <c r="B21" s="48" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="56" t="s">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="56" t="s">
         <v>46</v>
       </c>
-      <c r="B20" s="45"/>
-      <c r="C20" s="45"/>
-      <c r="D20" s="45"/>
-      <c r="E20" s="46"/>
-      <c r="F20" s="47"/>
-      <c r="G20" s="47"/>
-      <c r="H20" s="47"/>
-      <c r="I20" s="47"/>
-      <c r="J20" s="47"/>
+      <c r="B22" s="45"/>
+      <c r="C22" s="45"/>
+      <c r="D22" s="45"/>
+      <c r="E22" s="46"/>
+      <c r="F22" s="47"/>
+      <c r="G22" s="47"/>
+      <c r="H22" s="47"/>
+      <c r="I22" s="47"/>
+      <c r="J22" s="47"/>
     </row>
   </sheetData>
   <dataValidations xWindow="363" yWindow="440" count="8">
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Time to do recent graphs from" prompt="Calendar year that output graphs for recent time start from." sqref="B13">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Time to do recent graphs from" prompt="Calendar year that output graphs for recent time start from." sqref="B13:B14">
       <formula1>-10000</formula1>
       <formula2>3000</formula2>
     </dataValidation>
@@ -2561,11 +2587,11 @@
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Strains" prompt="Number of strains (0: single strain model, 2: DS-TB and MDR-TB, 3: DS-TB, MDR-TB and XDR-TB)." sqref="B3:D3"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Comorbidities" prompt="Number of comorbidities (currently up to three, but will be revised as model develops)." sqref="B4:D4"/>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Function smoothness" prompt="From zero up, with zero being exact fit and higher values being greater smoothness." sqref="B14:B17">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Function smoothness" prompt="From zero up, with zero being exact fit and higher values being greater smoothness." sqref="B16:B19">
       <formula1>0</formula1>
       <formula2>1000</formula2>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Age breakpoints" prompt="Enter consecutively increasing age breakpoints to create age strata. (Can enter any number, don't enter zero and no upper limit is needed.)" sqref="B20:E20"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Age breakpoints" prompt="Enter consecutively increasing age breakpoints to create age strata. (Can enter any number, don't enter zero and no upper limit is needed.)" sqref="B22:E22"/>
     <dataValidation allowBlank="1" showErrorMessage="1" sqref="B8:C11"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2613,7 +2639,7 @@
           <x14:formula1>
             <xm:f>dropdown_lists!$C$2:$C$3</xm:f>
           </x14:formula1>
-          <xm:sqref>B18</xm:sqref>
+          <xm:sqref>B20</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2743,10 +2769,10 @@
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:AY27"/>
+  <dimension ref="A1:AZ27"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AX27" sqref="AX27"/>
+    <sheetView topLeftCell="J1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AX13" sqref="AX13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2778,7 +2804,7 @@
     <col min="52" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:51" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:52" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>17</v>
       </c>
@@ -2932,8 +2958,11 @@
       <c r="AY1" s="5">
         <v>2015</v>
       </c>
-    </row>
-    <row r="2" spans="1:51" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AZ1" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" spans="1:52" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>9</v>
       </c>
@@ -2984,8 +3013,11 @@
       <c r="AV2" s="28"/>
       <c r="AW2" s="28"/>
       <c r="AX2" s="28"/>
-    </row>
-    <row r="3" spans="1:51" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AZ2" s="7">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="3" spans="1:52" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
         <v>18</v>
       </c>
@@ -3005,7 +3037,7 @@
         <v>39034561</v>
       </c>
     </row>
-    <row r="4" spans="1:51" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:52" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="19" t="s">
         <v>10</v>
       </c>
@@ -3047,7 +3079,7 @@
       <c r="AW4" s="29"/>
       <c r="AX4" s="29"/>
     </row>
-    <row r="5" spans="1:51" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:52" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
         <v>19</v>
       </c>
@@ -3058,7 +3090,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:52" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
         <v>11</v>
       </c>
@@ -3080,8 +3112,11 @@
       <c r="AX6" s="11">
         <v>85</v>
       </c>
-    </row>
-    <row r="7" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AZ6" s="11">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="7" spans="1:52" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
         <v>20</v>
       </c>
@@ -3098,7 +3133,7 @@
         <v>4049504</v>
       </c>
     </row>
-    <row r="8" spans="1:51" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:52" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="21" t="s">
         <v>4</v>
       </c>
@@ -3115,7 +3150,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:51" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:52" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="21" t="s">
         <v>21</v>
       </c>
@@ -3123,7 +3158,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:51" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:52" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="22" t="s">
         <v>12</v>
       </c>
@@ -3140,7 +3175,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:51" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:52" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="22" t="s">
         <v>22</v>
       </c>
@@ -3148,7 +3183,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:51" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:52" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="23" t="s">
         <v>13</v>
       </c>
@@ -3168,7 +3203,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="13" spans="1:51" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:52" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="23" t="s">
         <v>23</v>
       </c>
@@ -3176,7 +3211,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:51" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:52" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="21" t="s">
         <v>25</v>
       </c>
@@ -3213,7 +3248,7 @@
       <c r="AV14" s="30"/>
       <c r="AW14" s="30"/>
     </row>
-    <row r="15" spans="1:51" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:52" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="21" t="s">
         <v>26</v>
       </c>
@@ -3236,7 +3271,7 @@
         <v>52431253</v>
       </c>
     </row>
-    <row r="16" spans="1:51" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:52" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="21" t="s">
         <v>27</v>
       </c>

</xml_diff>

<commit_message>
Scenario reading from spreadsheets
Wow, after more extensive problems with bugs, I think the spreadsheet
reader now handles scenarios.
</commit_message>
<xml_diff>
--- a/autumn/xls/programs_fiji.xlsx
+++ b/autumn/xls/programs_fiji.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="315" windowWidth="20370" windowHeight="7530" tabRatio="807"/>
+    <workbookView xWindow="120" yWindow="315" windowWidth="20370" windowHeight="7530" tabRatio="807" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="model_attributes" sheetId="4" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="80">
   <si>
     <t>program_rate_restart_presenting</t>
   </si>
@@ -254,6 +254,9 @@
   </si>
   <si>
     <t>current_time</t>
+  </si>
+  <si>
+    <t>scenarios_to_run</t>
   </si>
 </sst>
 </file>
@@ -356,7 +359,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="16">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -446,8 +449,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="16">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -626,6 +635,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="664">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1293,7 +1317,7 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1389,6 +1413,9 @@
     <xf numFmtId="0" fontId="6" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="664">
     <cellStyle name="Comma 2" xfId="5"/>
@@ -2356,10 +2383,10 @@
   <sheetPr>
     <tabColor theme="3" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:J22"/>
+  <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2441,143 +2468,153 @@
       </c>
       <c r="C7" s="44"/>
     </row>
-    <row r="8" spans="1:4" s="82" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="72" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="91" t="s">
+        <v>79</v>
+      </c>
+      <c r="B8" s="92">
+        <v>1</v>
+      </c>
+      <c r="C8" s="92"/>
+      <c r="D8" s="93"/>
+    </row>
+    <row r="9" spans="1:4" s="82" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="72" t="s">
         <v>69</v>
       </c>
-      <c r="B8" s="73" t="s">
+      <c r="B9" s="73" t="s">
         <v>66</v>
       </c>
-      <c r="C8" s="73"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="79" t="s">
+      <c r="C9" s="73"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="79" t="s">
         <v>67</v>
       </c>
-      <c r="B9" s="83">
+      <c r="B10" s="83">
         <v>457200</v>
       </c>
-      <c r="C9" s="47"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="80" t="s">
+      <c r="C10" s="47"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="80" t="s">
         <v>68</v>
       </c>
-      <c r="B10" s="81">
+      <c r="B11" s="81">
         <v>3</v>
       </c>
-      <c r="C10" s="47"/>
-    </row>
-    <row r="11" spans="1:4" s="69" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="72" t="s">
+      <c r="C11" s="47"/>
+    </row>
+    <row r="12" spans="1:4" s="69" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="72" t="s">
         <v>37</v>
       </c>
-      <c r="B11" s="73" t="s">
+      <c r="B12" s="73" t="s">
         <v>60</v>
       </c>
-      <c r="C11" s="47"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="70" t="s">
+      <c r="C12" s="47"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="70" t="s">
         <v>39</v>
       </c>
-      <c r="B12" s="71">
+      <c r="B13" s="71">
         <v>1900</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="51" t="s">
-        <v>40</v>
-      </c>
-      <c r="B13" s="35">
-        <v>1990</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="51" t="s">
-        <v>78</v>
+        <v>40</v>
       </c>
       <c r="B14" s="35">
-        <v>2015</v>
+        <v>1990</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="51" t="s">
+        <v>78</v>
+      </c>
+      <c r="B15" s="35">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="51" t="s">
         <v>77</v>
       </c>
-      <c r="B15" s="90">
+      <c r="B16" s="90">
         <v>2035</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="75" t="s">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="75" t="s">
         <v>70</v>
       </c>
-      <c r="B16" s="77">
+      <c r="B17" s="77">
         <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="84" t="s">
-        <v>65</v>
-      </c>
-      <c r="B17" s="85">
-        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="84" t="s">
+        <v>65</v>
+      </c>
+      <c r="B18" s="85">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="84" t="s">
         <v>71</v>
       </c>
-      <c r="B18" s="85">
+      <c r="B19" s="85">
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="76" t="s">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="76" t="s">
         <v>64</v>
       </c>
-      <c r="B19" s="78">
+      <c r="B20" s="78">
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="67" t="s">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="67" t="s">
         <v>57</v>
       </c>
-      <c r="B20" s="74" t="s">
+      <c r="B21" s="74" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="21" spans="1:10" s="48" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="68" t="s">
+    <row r="22" spans="1:10" s="48" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="68" t="s">
         <v>47</v>
       </c>
-      <c r="B21" s="48" t="s">
+      <c r="B22" s="48" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="56" t="s">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="56" t="s">
         <v>46</v>
       </c>
-      <c r="B22" s="45"/>
-      <c r="C22" s="45"/>
-      <c r="D22" s="45"/>
-      <c r="E22" s="46"/>
-      <c r="F22" s="47"/>
-      <c r="G22" s="47"/>
-      <c r="H22" s="47"/>
-      <c r="I22" s="47"/>
-      <c r="J22" s="47"/>
+      <c r="B23" s="45"/>
+      <c r="C23" s="45"/>
+      <c r="D23" s="45"/>
+      <c r="E23" s="46"/>
+      <c r="F23" s="47"/>
+      <c r="G23" s="47"/>
+      <c r="H23" s="47"/>
+      <c r="I23" s="47"/>
+      <c r="J23" s="47"/>
     </row>
   </sheetData>
   <dataValidations xWindow="363" yWindow="440" count="8">
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Time to do recent graphs from" prompt="Calendar year that output graphs for recent time start from." sqref="B13:B14">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Time to do recent graphs from" prompt="Calendar year that output graphs for recent time start from." sqref="B14:B15">
       <formula1>-10000</formula1>
       <formula2>3000</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Time to start model" prompt="Enter the calendar year that the model runs from." sqref="B12">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Time to start model" prompt="Enter the calendar year that the model runs from." sqref="B13">
       <formula1>-10000</formula1>
       <formula2>3000</formula2>
     </dataValidation>
@@ -2587,12 +2624,12 @@
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Strains" prompt="Number of strains (0: single strain model, 2: DS-TB and MDR-TB, 3: DS-TB, MDR-TB and XDR-TB)." sqref="B3:D3"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Comorbidities" prompt="Number of comorbidities (currently up to three, but will be revised as model develops)." sqref="B4:D4"/>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Function smoothness" prompt="From zero up, with zero being exact fit and higher values being greater smoothness." sqref="B16:B19">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Function smoothness" prompt="From zero up, with zero being exact fit and higher values being greater smoothness." sqref="B17:B20">
       <formula1>0</formula1>
       <formula2>1000</formula2>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Age breakpoints" prompt="Enter consecutively increasing age breakpoints to create age strata. (Can enter any number, don't enter zero and no upper limit is needed.)" sqref="B22:E22"/>
-    <dataValidation allowBlank="1" showErrorMessage="1" sqref="B8:C11"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Age breakpoints" prompt="Enter consecutively increasing age breakpoints to create age strata. (Can enter any number, don't enter zero and no upper limit is needed.)" sqref="B23:E23"/>
+    <dataValidation allowBlank="1" showErrorMessage="1" sqref="B9:C12"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2639,7 +2676,7 @@
           <x14:formula1>
             <xm:f>dropdown_lists!$C$2:$C$3</xm:f>
           </x14:formula1>
-          <xm:sqref>B20</xm:sqref>
+          <xm:sqref>B21</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2655,7 +2692,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2771,8 +2808,11 @@
   </sheetPr>
   <dimension ref="A1:AZ27"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AX13" sqref="AX13"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="Y2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="AZ5" sqref="AZ5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3014,7 +3054,7 @@
       <c r="AW2" s="28"/>
       <c r="AX2" s="28"/>
       <c r="AZ2" s="7">
-        <v>95</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:52" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -3078,6 +3118,9 @@
       <c r="AV4" s="29"/>
       <c r="AW4" s="29"/>
       <c r="AX4" s="29"/>
+      <c r="AZ4" s="9">
+        <v>80</v>
+      </c>
     </row>
     <row r="5" spans="1:52" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
@@ -3111,9 +3154,6 @@
       </c>
       <c r="AX6" s="11">
         <v>85</v>
-      </c>
-      <c r="AZ6" s="11">
-        <v>75</v>
       </c>
     </row>
     <row r="7" spans="1:52" s="11" customFormat="1" x14ac:dyDescent="0.25">
@@ -3604,11 +3644,11 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:BB2 C4:BB4 C6:BB6 C8:BB8 C18:BB18 C20:BB20 C22:BB22 C24:BB24 C10:BB10 C12:BB12 C14:BB14 C16:BB16 C26:BB26">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C26:BA26 C16:BA16 C14:BA14 C12:BA12 C10:BA10 C24:BA24 C22:BA22 C20:BA20 C18:BA18 C8:BA8 C6:BA6 C4:BA4 C2:BA2">
       <formula1>0</formula1>
       <formula2>100</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:BB3 C5:BB5 C7:BB7 C9:BB9 C11:BB11 C13:BB13 C15:BB15 C17:BB17 C19:BB19 C21:BB21 C23:BB23 C25:BB25 C27:BB27">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C27:BA27 C25:BA25 C23:BA23 C21:BA21 C19:BA19 C17:BA17 C15:BA15 C13:BA13 C11:BA11 C9:BA9 C7:BA7 C5:BA5 C3:BA3">
       <formula1>0</formula1>
       <formula2>100000000000000000000</formula2>
     </dataValidation>

</xml_diff>

<commit_message>
Model can run single scenario into future now
</commit_message>
<xml_diff>
--- a/autumn/xls/programs_fiji.xlsx
+++ b/autumn/xls/programs_fiji.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="315" windowWidth="20370" windowHeight="7530" tabRatio="807" activeTab="2"/>
+    <workbookView xWindow="120" yWindow="315" windowWidth="20370" windowHeight="7530" tabRatio="807"/>
   </bookViews>
   <sheets>
     <sheet name="model_attributes" sheetId="4" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="83">
   <si>
     <t>program_rate_restart_presenting</t>
   </si>
@@ -257,6 +257,15 @@
   </si>
   <si>
     <t>scenarios_to_run</t>
+  </si>
+  <si>
+    <t>scenario_2</t>
+  </si>
+  <si>
+    <t>scenario_start_time</t>
+  </si>
+  <si>
+    <t>scenario_full_time</t>
   </si>
 </sst>
 </file>
@@ -2383,10 +2392,10 @@
   <sheetPr>
     <tabColor theme="3" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:J23"/>
+  <dimension ref="A1:J25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2540,77 +2549,93 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="51" t="s">
+        <v>81</v>
+      </c>
+      <c r="B16" s="35">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="51" t="s">
+        <v>82</v>
+      </c>
+      <c r="B17" s="35">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="51" t="s">
         <v>77</v>
       </c>
-      <c r="B16" s="90">
+      <c r="B18" s="90">
         <v>2035</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="75" t="s">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="75" t="s">
         <v>70</v>
       </c>
-      <c r="B17" s="77">
+      <c r="B19" s="77">
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="84" t="s">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="84" t="s">
         <v>65</v>
       </c>
-      <c r="B18" s="85">
+      <c r="B20" s="85">
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="84" t="s">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="84" t="s">
         <v>71</v>
       </c>
-      <c r="B19" s="85">
+      <c r="B21" s="85">
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="76" t="s">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="76" t="s">
         <v>64</v>
       </c>
-      <c r="B20" s="78">
+      <c r="B22" s="78">
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="67" t="s">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="67" t="s">
         <v>57</v>
       </c>
-      <c r="B21" s="74" t="s">
+      <c r="B23" s="74" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="22" spans="1:10" s="48" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="68" t="s">
+    <row r="24" spans="1:10" s="48" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="68" t="s">
         <v>47</v>
       </c>
-      <c r="B22" s="48" t="s">
+      <c r="B24" s="48" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="56" t="s">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="56" t="s">
         <v>46</v>
       </c>
-      <c r="B23" s="45"/>
-      <c r="C23" s="45"/>
-      <c r="D23" s="45"/>
-      <c r="E23" s="46"/>
-      <c r="F23" s="47"/>
-      <c r="G23" s="47"/>
-      <c r="H23" s="47"/>
-      <c r="I23" s="47"/>
-      <c r="J23" s="47"/>
+      <c r="B25" s="45"/>
+      <c r="C25" s="45"/>
+      <c r="D25" s="45"/>
+      <c r="E25" s="46"/>
+      <c r="F25" s="47"/>
+      <c r="G25" s="47"/>
+      <c r="H25" s="47"/>
+      <c r="I25" s="47"/>
+      <c r="J25" s="47"/>
     </row>
   </sheetData>
   <dataValidations xWindow="363" yWindow="440" count="8">
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Time to do recent graphs from" prompt="Calendar year that output graphs for recent time start from." sqref="B14:B15">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Time to do recent graphs from" prompt="Calendar year that output graphs for recent time start from." sqref="B14:B17">
       <formula1>-10000</formula1>
       <formula2>3000</formula2>
     </dataValidation>
@@ -2624,11 +2649,11 @@
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Strains" prompt="Number of strains (0: single strain model, 2: DS-TB and MDR-TB, 3: DS-TB, MDR-TB and XDR-TB)." sqref="B3:D3"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Comorbidities" prompt="Number of comorbidities (currently up to three, but will be revised as model develops)." sqref="B4:D4"/>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Function smoothness" prompt="From zero up, with zero being exact fit and higher values being greater smoothness." sqref="B17:B20">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Function smoothness" prompt="From zero up, with zero being exact fit and higher values being greater smoothness." sqref="B19:B22">
       <formula1>0</formula1>
       <formula2>1000</formula2>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Age breakpoints" prompt="Enter consecutively increasing age breakpoints to create age strata. (Can enter any number, don't enter zero and no upper limit is needed.)" sqref="B23:E23"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Age breakpoints" prompt="Enter consecutively increasing age breakpoints to create age strata. (Can enter any number, don't enter zero and no upper limit is needed.)" sqref="B25:E25"/>
     <dataValidation allowBlank="1" showErrorMessage="1" sqref="B9:C12"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2676,7 +2701,7 @@
           <x14:formula1>
             <xm:f>dropdown_lists!$C$2:$C$3</xm:f>
           </x14:formula1>
-          <xm:sqref>B21</xm:sqref>
+          <xm:sqref>B23</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2806,13 +2831,13 @@
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:AZ27"/>
+  <dimension ref="A1:BA27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="Y2" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="AB2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AZ5" sqref="AZ5"/>
+      <selection pane="bottomRight" activeCell="AZ26" sqref="AZ26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2844,7 +2869,7 @@
     <col min="52" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:52" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>17</v>
       </c>
@@ -3001,8 +3026,11 @@
       <c r="AZ1" s="5" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="2" spans="1:52" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="BA1" s="5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:53" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>9</v>
       </c>
@@ -3054,10 +3082,13 @@
       <c r="AW2" s="28"/>
       <c r="AX2" s="28"/>
       <c r="AZ2" s="7">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="3" spans="1:52" s="7" customFormat="1" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+      <c r="BA2" s="7">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:53" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
         <v>18</v>
       </c>
@@ -3077,7 +3108,7 @@
         <v>39034561</v>
       </c>
     </row>
-    <row r="4" spans="1:52" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="19" t="s">
         <v>10</v>
       </c>
@@ -3118,11 +3149,8 @@
       <c r="AV4" s="29"/>
       <c r="AW4" s="29"/>
       <c r="AX4" s="29"/>
-      <c r="AZ4" s="9">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="5" spans="1:52" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
         <v>19</v>
       </c>
@@ -3133,7 +3161,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:52" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:53" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
         <v>11</v>
       </c>
@@ -3155,8 +3183,14 @@
       <c r="AX6" s="11">
         <v>85</v>
       </c>
-    </row>
-    <row r="7" spans="1:52" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AZ6" s="11">
+        <v>40</v>
+      </c>
+      <c r="BA6" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="1:53" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
         <v>20</v>
       </c>
@@ -3173,7 +3207,7 @@
         <v>4049504</v>
       </c>
     </row>
-    <row r="8" spans="1:52" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:53" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="21" t="s">
         <v>4</v>
       </c>
@@ -3190,7 +3224,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:52" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:53" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="21" t="s">
         <v>21</v>
       </c>
@@ -3198,7 +3232,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:52" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:53" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="22" t="s">
         <v>12</v>
       </c>
@@ -3215,7 +3249,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:52" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:53" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="22" t="s">
         <v>22</v>
       </c>
@@ -3223,7 +3257,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:52" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:53" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="23" t="s">
         <v>13</v>
       </c>
@@ -3243,7 +3277,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="13" spans="1:52" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:53" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="23" t="s">
         <v>23</v>
       </c>
@@ -3251,7 +3285,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:52" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:53" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="21" t="s">
         <v>25</v>
       </c>
@@ -3287,8 +3321,14 @@
       <c r="AU14" s="30"/>
       <c r="AV14" s="30"/>
       <c r="AW14" s="30"/>
-    </row>
-    <row r="15" spans="1:52" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AZ14" s="13">
+        <v>40</v>
+      </c>
+      <c r="BA14" s="13">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="15" spans="1:53" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="21" t="s">
         <v>26</v>
       </c>
@@ -3311,7 +3351,7 @@
         <v>52431253</v>
       </c>
     </row>
-    <row r="16" spans="1:52" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:53" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="21" t="s">
         <v>27</v>
       </c>
@@ -3347,8 +3387,11 @@
       <c r="AU16" s="30"/>
       <c r="AV16" s="30"/>
       <c r="AW16" s="30"/>
-    </row>
-    <row r="17" spans="1:50" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AZ16" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:53" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="21" t="s">
         <v>28</v>
       </c>
@@ -3359,7 +3402,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:50" s="27" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:53" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="25" t="s">
         <v>29</v>
       </c>
@@ -3399,7 +3442,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="1:50" s="27" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:53" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="25" t="s">
         <v>30</v>
       </c>
@@ -3422,7 +3465,7 @@
         <v>52431253</v>
       </c>
     </row>
-    <row r="20" spans="1:50" s="27" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:53" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="25" t="s">
         <v>31</v>
       </c>
@@ -3462,7 +3505,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:50" s="27" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:53" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="25" t="s">
         <v>32</v>
       </c>
@@ -3473,7 +3516,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:50" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="19" t="s">
         <v>33</v>
       </c>
@@ -3513,7 +3556,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="1:50" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="19" t="s">
         <v>34</v>
       </c>
@@ -3536,7 +3579,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:50" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="19" t="s">
         <v>35</v>
       </c>
@@ -3576,7 +3619,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="25" spans="1:50" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="19" t="s">
         <v>36</v>
       </c>
@@ -3587,7 +3630,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:50" s="88" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:53" s="88" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="86" t="s">
         <v>74</v>
       </c>
@@ -3621,8 +3664,11 @@
       <c r="AX26" s="88">
         <v>0.04</v>
       </c>
-    </row>
-    <row r="27" spans="1:50" s="88" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="BA26" s="88">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="27" spans="1:53" s="88" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="86" t="s">
         <v>75</v>
       </c>

</xml_diff>

<commit_message>
Forgot to divide proportions by 100 in last commit
</commit_message>
<xml_diff>
--- a/autumn/xls/programs_fiji.xlsx
+++ b/autumn/xls/programs_fiji.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="315" windowWidth="20370" windowHeight="7530" tabRatio="807"/>
+    <workbookView xWindow="120" yWindow="315" windowWidth="20370" windowHeight="7530" tabRatio="807" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="model_attributes" sheetId="4" r:id="rId1"/>
@@ -2394,8 +2394,8 @@
   </sheetPr>
   <dimension ref="A1:J25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2484,7 +2484,9 @@
       <c r="B8" s="92">
         <v>1</v>
       </c>
-      <c r="C8" s="92"/>
+      <c r="C8" s="92">
+        <v>2</v>
+      </c>
       <c r="D8" s="93"/>
     </row>
     <row r="9" spans="1:4" s="82" customFormat="1" x14ac:dyDescent="0.25">
@@ -2833,11 +2835,11 @@
   </sheetPr>
   <dimension ref="A1:BA27"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="AB2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AZ26" sqref="AZ26"/>
+      <selection pane="bottomRight" activeCell="AZ5" sqref="AZ5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3082,10 +3084,10 @@
       <c r="AW2" s="28"/>
       <c r="AX2" s="28"/>
       <c r="AZ2" s="7">
-        <v>20</v>
+        <v>99</v>
       </c>
       <c r="BA2" s="7">
-        <v>50</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" spans="1:53" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -3149,6 +3151,12 @@
       <c r="AV4" s="29"/>
       <c r="AW4" s="29"/>
       <c r="AX4" s="29"/>
+      <c r="AZ4" s="9">
+        <v>70</v>
+      </c>
+      <c r="BA4" s="9">
+        <v>60</v>
+      </c>
     </row>
     <row r="5" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
@@ -3184,10 +3192,10 @@
         <v>85</v>
       </c>
       <c r="AZ6" s="11">
-        <v>40</v>
+        <v>85</v>
       </c>
       <c r="BA6" s="11">
-        <v>70</v>
+        <v>85</v>
       </c>
     </row>
     <row r="7" spans="1:53" s="11" customFormat="1" x14ac:dyDescent="0.25">
@@ -3322,10 +3330,10 @@
       <c r="AV14" s="30"/>
       <c r="AW14" s="30"/>
       <c r="AZ14" s="13">
-        <v>40</v>
+        <v>90</v>
       </c>
       <c r="BA14" s="13">
-        <v>80</v>
+        <v>90</v>
       </c>
     </row>
     <row r="15" spans="1:53" s="13" customFormat="1" x14ac:dyDescent="0.25">
@@ -3388,10 +3396,10 @@
       <c r="AV16" s="30"/>
       <c r="AW16" s="30"/>
       <c r="AZ16" s="13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:53" s="13" customFormat="1" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:50" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="21" t="s">
         <v>28</v>
       </c>
@@ -3402,7 +3410,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:53" s="27" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:50" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="25" t="s">
         <v>29</v>
       </c>
@@ -3442,7 +3450,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="1:53" s="27" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:50" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="25" t="s">
         <v>30</v>
       </c>
@@ -3465,7 +3473,7 @@
         <v>52431253</v>
       </c>
     </row>
-    <row r="20" spans="1:53" s="27" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:50" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="25" t="s">
         <v>31</v>
       </c>
@@ -3505,7 +3513,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:53" s="27" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:50" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="25" t="s">
         <v>32</v>
       </c>
@@ -3516,7 +3524,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:50" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="19" t="s">
         <v>33</v>
       </c>
@@ -3556,7 +3564,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:50" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="19" t="s">
         <v>34</v>
       </c>
@@ -3579,7 +3587,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:50" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="19" t="s">
         <v>35</v>
       </c>
@@ -3619,7 +3627,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:50" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="19" t="s">
         <v>36</v>
       </c>
@@ -3630,7 +3638,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:53" s="88" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:50" s="88" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="86" t="s">
         <v>74</v>
       </c>
@@ -3664,11 +3672,8 @@
       <c r="AX26" s="88">
         <v>0.04</v>
       </c>
-      <c r="BA26" s="88">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="27" spans="1:53" s="88" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:50" s="88" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="86" t="s">
         <v>75</v>
       </c>

</xml_diff>

<commit_message>
More generalisation of curve fitting
</commit_message>
<xml_diff>
--- a/autumn/xls/programs_fiji.xlsx
+++ b/autumn/xls/programs_fiji.xlsx
@@ -2425,7 +2425,7 @@
   <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2874,10 +2874,10 @@
   <dimension ref="A1:BB27"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="AA2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E12" sqref="E12"/>
+      <selection pane="bottomRight" activeCell="BA16" sqref="BA16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added data for 1986 for every data cell to test cost functions
</commit_message>
<xml_diff>
--- a/autumn/xls/programs_fiji.xlsx
+++ b/autumn/xls/programs_fiji.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="315" windowWidth="20370" windowHeight="7530" tabRatio="807"/>
+    <workbookView xWindow="120" yWindow="315" windowWidth="20370" windowHeight="7530" tabRatio="807" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="model_attributes" sheetId="4" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="86">
   <si>
     <t>program_rate_restart_presenting</t>
   </si>
@@ -272,6 +272,9 @@
   </si>
   <si>
     <t>smoothness</t>
+  </si>
+  <si>
+    <t>cost function attributes</t>
   </si>
 </sst>
 </file>
@@ -1345,7 +1348,7 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="105">
+  <cellXfs count="106">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1455,6 +1458,7 @@
     <xf numFmtId="0" fontId="7" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="664">
     <cellStyle name="Comma 2" xfId="5"/>
@@ -2422,10 +2426,10 @@
   <sheetPr>
     <tabColor theme="3" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:J26"/>
+  <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2672,6 +2676,11 @@
       <c r="H26" s="47"/>
       <c r="I26" s="47"/>
       <c r="J26" s="47"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" s="105" t="s">
+        <v>85</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations xWindow="363" yWindow="440" count="8">
@@ -2873,11 +2882,11 @@
   </sheetPr>
   <dimension ref="A1:BB27"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="AA2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="BA16" sqref="BA16"/>
+      <selection pane="bottomRight" activeCell="W19" sqref="W19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3099,7 +3108,9 @@
       <c r="T2" s="28"/>
       <c r="U2" s="28"/>
       <c r="V2" s="28"/>
-      <c r="W2" s="28"/>
+      <c r="W2" s="28">
+        <v>0</v>
+      </c>
       <c r="X2" s="28"/>
       <c r="Y2" s="28"/>
       <c r="Z2" s="28"/>
@@ -3155,6 +3166,9 @@
       <c r="V3" s="7">
         <v>39034561</v>
       </c>
+      <c r="W3" s="7">
+        <v>0</v>
+      </c>
     </row>
     <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="19" t="s">
@@ -3174,6 +3188,9 @@
       </c>
       <c r="S4" s="9">
         <v>30</v>
+      </c>
+      <c r="W4" s="9">
+        <v>0</v>
       </c>
       <c r="AA4" s="29"/>
       <c r="AB4" s="29"/>
@@ -3218,6 +3235,9 @@
       <c r="E5" s="9">
         <v>0</v>
       </c>
+      <c r="W5" s="9">
+        <v>0</v>
+      </c>
     </row>
     <row r="6" spans="1:54" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
@@ -3235,6 +3255,9 @@
       <c r="I6" s="11">
         <v>80</v>
       </c>
+      <c r="W6" s="11">
+        <v>0</v>
+      </c>
       <c r="Y6" s="11">
         <v>82</v>
       </c>
@@ -3265,6 +3288,9 @@
       <c r="I7" s="11">
         <v>2040504</v>
       </c>
+      <c r="W7" s="11">
+        <v>0</v>
+      </c>
       <c r="Y7" s="11">
         <v>4049504</v>
       </c>
@@ -3285,6 +3311,9 @@
       <c r="J8" s="13">
         <v>40</v>
       </c>
+      <c r="W8" s="13">
+        <v>0</v>
+      </c>
       <c r="AA8" s="13">
         <v>40</v>
       </c>
@@ -3297,6 +3326,9 @@
         <v>24</v>
       </c>
       <c r="C9" s="99"/>
+      <c r="W9" s="13">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:54" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="22" t="s">
@@ -3311,6 +3343,9 @@
       <c r="Q10" s="15">
         <v>30</v>
       </c>
+      <c r="W10" s="15">
+        <v>0</v>
+      </c>
       <c r="AA10" s="15">
         <v>40</v>
       </c>
@@ -3326,6 +3361,9 @@
         <v>24</v>
       </c>
       <c r="C11" s="100"/>
+      <c r="W11" s="15">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:54" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="23" t="s">
@@ -3343,6 +3381,9 @@
       <c r="V12" s="17">
         <v>0</v>
       </c>
+      <c r="W12" s="17">
+        <v>0</v>
+      </c>
       <c r="AF12" s="17">
         <v>50</v>
       </c>
@@ -3358,6 +3399,9 @@
         <v>24</v>
       </c>
       <c r="C13" s="101"/>
+      <c r="W13" s="17">
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:54" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="21" t="s">
@@ -3483,6 +3527,9 @@
       <c r="H17" s="13">
         <v>0</v>
       </c>
+      <c r="W17" s="13">
+        <v>0</v>
+      </c>
     </row>
     <row r="18" spans="1:51" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="25" t="s">
@@ -3605,6 +3652,9 @@
       <c r="H21" s="27">
         <v>0</v>
       </c>
+      <c r="W21" s="27">
+        <v>0</v>
+      </c>
     </row>
     <row r="22" spans="1:51" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="19" t="s">
@@ -3727,6 +3777,9 @@
       <c r="H25" s="9">
         <v>0</v>
       </c>
+      <c r="W25" s="9">
+        <v>0</v>
+      </c>
     </row>
     <row r="26" spans="1:51" s="88" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="86" t="s">
@@ -3741,6 +3794,9 @@
       <c r="D26" s="88">
         <f>1/26</f>
         <v>3.8461538461538464E-2</v>
+      </c>
+      <c r="W26" s="88">
+        <v>0</v>
       </c>
       <c r="AE26" s="89"/>
       <c r="AF26" s="89"/>

</xml_diff>

<commit_message>
Add epi parameters to programs
Will change the name, but this code creates data for time-variant
parameters that aren't necessarily programs.
</commit_message>
<xml_diff>
--- a/autumn/xls/programs_fiji.xlsx
+++ b/autumn/xls/programs_fiji.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="315" windowWidth="20370" windowHeight="7530" tabRatio="807" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="315" windowWidth="20370" windowHeight="7530" tabRatio="807" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="model_attributes" sheetId="4" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="89">
   <si>
     <t>program_rate_restart_presenting</t>
   </si>
@@ -272,6 +272,18 @@
   </si>
   <si>
     <t>program_prop_death_reporting</t>
+  </si>
+  <si>
+    <t>epi_life_expectancy</t>
+  </si>
+  <si>
+    <t>epi_birth_rate</t>
+  </si>
+  <si>
+    <t>tb_prop_smearpos</t>
+  </si>
+  <si>
+    <t>tb_prop_smearneg</t>
   </si>
 </sst>
 </file>
@@ -2729,7 +2741,7 @@
   </sheetPr>
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
@@ -2855,13 +2867,13 @@
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:BB27"/>
+  <dimension ref="A1:BB31"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="AA2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="BA16" sqref="BA16"/>
+      <selection pane="bottomRight" activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3769,6 +3781,50 @@
       </c>
       <c r="AY27" s="86">
         <v>739284639</v>
+      </c>
+    </row>
+    <row r="28" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="A28" s="24" t="s">
+        <v>85</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C28" s="102">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="A29" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C29" s="102">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="A30" s="24" t="s">
+        <v>87</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C30" s="102">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="A31" s="24" t="s">
+        <v>88</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C31" s="102">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Rename 'programs' to 'time_variants'
because there are time-variant parameters that aren't programs now.
</commit_message>
<xml_diff>
--- a/autumn/xls/programs_fiji.xlsx
+++ b/autumn/xls/programs_fiji.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="315" windowWidth="20370" windowHeight="7530" tabRatio="807" activeTab="2"/>
+    <workbookView xWindow="120" yWindow="315" windowWidth="20370" windowHeight="7530" tabRatio="807"/>
   </bookViews>
   <sheets>
     <sheet name="model_attributes" sheetId="4" r:id="rId1"/>
     <sheet name="miscellaneous_constants" sheetId="1" r:id="rId2"/>
-    <sheet name="programs" sheetId="2" r:id="rId3"/>
+    <sheet name="time_variants" sheetId="2" r:id="rId3"/>
     <sheet name="dropdown_lists" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
@@ -2425,8 +2425,8 @@
   </sheetPr>
   <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2633,7 +2633,7 @@
         <v>55</v>
       </c>
       <c r="B22" s="74" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="23" spans="1:10" s="48" customFormat="1" x14ac:dyDescent="0.25">
@@ -2869,11 +2869,11 @@
   </sheetPr>
   <dimension ref="A1:BB31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I28" sqref="I28"/>
+      <selection pane="bottomRight" activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Time-variant choice for parameters
Choose through the spreadsheet whether you want the parameter to vary
over time or be fixed.
</commit_message>
<xml_diff>
--- a/autumn/xls/programs_fiji.xlsx
+++ b/autumn/xls/programs_fiji.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="90">
   <si>
     <t>program_rate_restart_presenting</t>
   </si>
@@ -284,6 +284,9 @@
   </si>
   <si>
     <t>tb_prop_smearneg</t>
+  </si>
+  <si>
+    <t>time_variant</t>
   </si>
 </sst>
 </file>
@@ -1348,7 +1351,7 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="104">
+  <cellXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1447,15 +1450,6 @@
     <xf numFmtId="0" fontId="0" fillId="13" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="664">
@@ -2868,229 +2862,234 @@
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:BB31"/>
+  <dimension ref="A1:BC31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J30" sqref="J30"/>
+      <selection pane="bottomRight" activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="47.42578125" style="24" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11" style="102" customWidth="1"/>
-    <col min="4" max="4" width="7.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7" style="1" customWidth="1"/>
-    <col min="7" max="8" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.42578125" style="1" customWidth="1"/>
-    <col min="10" max="11" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.7109375" style="1" customWidth="1"/>
-    <col min="13" max="16" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="7.28515625" style="1" customWidth="1"/>
-    <col min="18" max="21" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="23" width="7.42578125" style="1" customWidth="1"/>
-    <col min="24" max="24" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="7.140625" style="1" customWidth="1"/>
-    <col min="26" max="37" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="8" style="1" customWidth="1"/>
-    <col min="39" max="45" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="8" style="1" customWidth="1"/>
-    <col min="47" max="47" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="6.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="49" max="50" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="7.85546875" style="1" customWidth="1"/>
-    <col min="52" max="52" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="53" max="16384" width="9.140625" style="1"/>
+    <col min="3" max="4" width="11" style="2" customWidth="1"/>
+    <col min="5" max="5" width="7.42578125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7" style="1" customWidth="1"/>
+    <col min="8" max="9" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.42578125" style="1" customWidth="1"/>
+    <col min="11" max="12" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.7109375" style="1" customWidth="1"/>
+    <col min="14" max="17" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="7.28515625" style="1" customWidth="1"/>
+    <col min="19" max="22" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="24" width="7.42578125" style="1" customWidth="1"/>
+    <col min="25" max="25" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="7.140625" style="1" customWidth="1"/>
+    <col min="27" max="38" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="8" style="1" customWidth="1"/>
+    <col min="40" max="46" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="8" style="1" customWidth="1"/>
+    <col min="48" max="48" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="6.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="50" max="51" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="7.85546875" style="1" customWidth="1"/>
+    <col min="53" max="53" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="54" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:55" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="D1" s="5">
+      <c r="D1" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1" s="5">
         <v>1920</v>
       </c>
-      <c r="E1" s="5">
+      <c r="F1" s="5">
         <v>1930</v>
       </c>
-      <c r="F1" s="5">
+      <c r="G1" s="5">
         <v>1940</v>
       </c>
-      <c r="G1" s="5">
+      <c r="H1" s="5">
         <v>1950</v>
       </c>
-      <c r="H1" s="5">
+      <c r="I1" s="5">
         <v>1955</v>
       </c>
-      <c r="I1" s="5">
+      <c r="J1" s="5">
         <v>1960</v>
       </c>
-      <c r="J1" s="5">
+      <c r="K1" s="5">
         <v>1965</v>
       </c>
-      <c r="K1" s="5">
+      <c r="L1" s="5">
         <v>1970</v>
       </c>
-      <c r="L1" s="5">
+      <c r="M1" s="5">
         <v>1975</v>
       </c>
-      <c r="M1" s="5">
+      <c r="N1" s="5">
         <v>1976</v>
       </c>
-      <c r="N1" s="5">
+      <c r="O1" s="5">
         <v>1977</v>
       </c>
-      <c r="O1" s="5">
+      <c r="P1" s="5">
         <v>1978</v>
       </c>
-      <c r="P1" s="5">
+      <c r="Q1" s="5">
         <v>1979</v>
       </c>
-      <c r="Q1" s="5">
+      <c r="R1" s="5">
         <v>1980</v>
       </c>
-      <c r="R1" s="5">
+      <c r="S1" s="5">
         <v>1981</v>
       </c>
-      <c r="S1" s="5">
+      <c r="T1" s="5">
         <v>1982</v>
       </c>
-      <c r="T1" s="5">
+      <c r="U1" s="5">
         <v>1983</v>
       </c>
-      <c r="U1" s="5">
+      <c r="V1" s="5">
         <v>1984</v>
       </c>
-      <c r="V1" s="5">
+      <c r="W1" s="5">
         <v>1985</v>
       </c>
-      <c r="W1" s="5">
+      <c r="X1" s="5">
         <v>1986</v>
       </c>
-      <c r="X1" s="5">
+      <c r="Y1" s="5">
         <v>1987</v>
       </c>
-      <c r="Y1" s="5">
+      <c r="Z1" s="5">
         <v>1988</v>
       </c>
-      <c r="Z1" s="5">
+      <c r="AA1" s="5">
         <v>1989</v>
       </c>
-      <c r="AA1" s="5">
+      <c r="AB1" s="5">
         <v>1990</v>
       </c>
-      <c r="AB1" s="5">
+      <c r="AC1" s="5">
         <v>1991</v>
       </c>
-      <c r="AC1" s="5">
+      <c r="AD1" s="5">
         <v>1992</v>
       </c>
-      <c r="AD1" s="5">
+      <c r="AE1" s="5">
         <v>1993</v>
       </c>
-      <c r="AE1" s="5">
+      <c r="AF1" s="5">
         <v>1994</v>
       </c>
-      <c r="AF1" s="5">
+      <c r="AG1" s="5">
         <v>1995</v>
       </c>
-      <c r="AG1" s="5">
+      <c r="AH1" s="5">
         <v>1996</v>
       </c>
-      <c r="AH1" s="5">
+      <c r="AI1" s="5">
         <v>1997</v>
       </c>
-      <c r="AI1" s="5">
+      <c r="AJ1" s="5">
         <v>1998</v>
       </c>
-      <c r="AJ1" s="5">
+      <c r="AK1" s="5">
         <v>1999</v>
       </c>
-      <c r="AK1" s="5">
+      <c r="AL1" s="5">
         <v>2000</v>
       </c>
-      <c r="AL1" s="5">
+      <c r="AM1" s="5">
         <v>2001</v>
       </c>
-      <c r="AM1" s="5">
+      <c r="AN1" s="5">
         <v>2002</v>
       </c>
-      <c r="AN1" s="5">
+      <c r="AO1" s="5">
         <v>2003</v>
       </c>
-      <c r="AO1" s="5">
+      <c r="AP1" s="5">
         <v>2004</v>
       </c>
-      <c r="AP1" s="5">
+      <c r="AQ1" s="5">
         <v>2005</v>
       </c>
-      <c r="AQ1" s="5">
+      <c r="AR1" s="5">
         <v>2006</v>
       </c>
-      <c r="AR1" s="5">
+      <c r="AS1" s="5">
         <v>2007</v>
       </c>
-      <c r="AS1" s="5">
+      <c r="AT1" s="5">
         <v>2008</v>
       </c>
-      <c r="AT1" s="5">
+      <c r="AU1" s="5">
         <v>2009</v>
       </c>
-      <c r="AU1" s="5">
+      <c r="AV1" s="5">
         <v>2010</v>
       </c>
-      <c r="AV1" s="5">
+      <c r="AW1" s="5">
         <v>2011</v>
       </c>
-      <c r="AW1" s="5">
+      <c r="AX1" s="5">
         <v>2012</v>
       </c>
-      <c r="AX1" s="5">
+      <c r="AY1" s="5">
         <v>2013</v>
       </c>
-      <c r="AY1" s="5">
+      <c r="AZ1" s="5">
         <v>2014</v>
       </c>
-      <c r="AZ1" s="5">
+      <c r="BA1" s="5">
         <v>2015</v>
       </c>
-      <c r="BA1" s="5" t="s">
+      <c r="BB1" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="BB1" s="5" t="s">
+      <c r="BC1" s="5" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:54" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:55" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="94">
+      <c r="C2" s="6">
         <v>1</v>
       </c>
-      <c r="G2" s="7">
+      <c r="D2" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="7">
         <v>0</v>
       </c>
-      <c r="I2" s="7">
+      <c r="J2" s="7">
         <v>25</v>
       </c>
-      <c r="L2" s="7">
+      <c r="M2" s="7">
         <v>40</v>
       </c>
-      <c r="Q2" s="28"/>
       <c r="R2" s="28"/>
       <c r="S2" s="28"/>
       <c r="T2" s="28"/>
@@ -3125,54 +3124,60 @@
       <c r="AW2" s="28"/>
       <c r="AX2" s="28"/>
       <c r="AY2" s="28"/>
-      <c r="BA2" s="7">
-        <v>99</v>
-      </c>
+      <c r="AZ2" s="28"/>
       <c r="BB2" s="7">
         <v>99</v>
       </c>
-    </row>
-    <row r="3" spans="1:54" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="BC2" s="7">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:55" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
         <v>17</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="94"/>
-      <c r="G3" s="7">
+      <c r="C3" s="6"/>
+      <c r="D3" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" s="7">
         <v>0</v>
       </c>
-      <c r="I3" s="7">
+      <c r="J3" s="7">
         <v>10000000</v>
       </c>
-      <c r="L3" s="7">
+      <c r="M3" s="7">
         <v>15040500</v>
       </c>
-      <c r="V3" s="7">
+      <c r="W3" s="7">
         <v>39034561</v>
       </c>
     </row>
-    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:55" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="19" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="95">
+      <c r="C4" s="8">
         <v>5</v>
       </c>
-      <c r="E4" s="9">
+      <c r="D4" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="9">
         <v>0</v>
       </c>
-      <c r="J4" s="9">
+      <c r="K4" s="9">
         <v>10</v>
       </c>
-      <c r="S4" s="9">
+      <c r="T4" s="9">
         <v>30</v>
       </c>
-      <c r="AA4" s="29"/>
       <c r="AB4" s="29"/>
       <c r="AC4" s="29"/>
       <c r="AD4" s="29"/>
@@ -3197,185 +3202,215 @@
       <c r="AW4" s="29"/>
       <c r="AX4" s="29"/>
       <c r="AY4" s="29"/>
-      <c r="BA4" s="9">
+      <c r="AZ4" s="29"/>
+      <c r="BB4" s="9">
         <v>70</v>
       </c>
-      <c r="BB4" s="9">
+      <c r="BC4" s="9">
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:55" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
         <v>18</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="95"/>
-      <c r="E5" s="9">
+      <c r="C5" s="8"/>
+      <c r="D5" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" s="9">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:54" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:55" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="96">
+      <c r="C6" s="10">
         <v>1</v>
       </c>
-      <c r="F6" s="11">
+      <c r="D6" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="11">
         <v>70</v>
       </c>
-      <c r="I6" s="11">
+      <c r="J6" s="11">
         <v>80</v>
       </c>
-      <c r="Y6" s="11">
+      <c r="Z6" s="11">
         <v>82</v>
       </c>
-      <c r="AL6" s="11">
+      <c r="AM6" s="11">
         <v>84</v>
       </c>
-      <c r="AY6" s="11">
-        <v>85</v>
-      </c>
-      <c r="BA6" s="11">
+      <c r="AZ6" s="11">
         <v>85</v>
       </c>
       <c r="BB6" s="11">
         <v>85</v>
       </c>
-    </row>
-    <row r="7" spans="1:54" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="BC6" s="11">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="7" spans="1:55" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
         <v>19</v>
       </c>
       <c r="B7" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="96"/>
-      <c r="F7" s="11">
+      <c r="C7" s="10"/>
+      <c r="D7" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="G7" s="11">
         <v>1005000</v>
       </c>
-      <c r="I7" s="11">
+      <c r="J7" s="11">
         <v>2040504</v>
       </c>
-      <c r="Y7" s="11">
+      <c r="Z7" s="11">
         <v>4049504</v>
       </c>
     </row>
-    <row r="8" spans="1:54" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:55" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="21" t="s">
         <v>3</v>
       </c>
       <c r="B8" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="97">
+      <c r="C8" s="12">
         <v>1</v>
       </c>
-      <c r="G8" s="13">
+      <c r="D8" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="H8" s="13">
         <v>30</v>
       </c>
-      <c r="J8" s="13">
+      <c r="K8" s="13">
         <v>40</v>
       </c>
-      <c r="AA8" s="13">
+      <c r="AB8" s="13">
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:54" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:55" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="21" t="s">
         <v>20</v>
       </c>
       <c r="B9" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="97"/>
-    </row>
-    <row r="10" spans="1:54" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C9" s="12"/>
+      <c r="D9" s="12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:55" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="22" t="s">
         <v>11</v>
       </c>
       <c r="B10" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="98">
+      <c r="C10" s="14">
         <v>1</v>
       </c>
-      <c r="Q10" s="15">
+      <c r="D10" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="R10" s="15">
         <v>30</v>
       </c>
-      <c r="AA10" s="15">
+      <c r="AB10" s="15">
         <v>40</v>
       </c>
-      <c r="AK10" s="15">
+      <c r="AL10" s="15">
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:54" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:55" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="22" t="s">
         <v>21</v>
       </c>
       <c r="B11" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="98"/>
-    </row>
-    <row r="12" spans="1:54" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C11" s="14"/>
+      <c r="D11" s="14" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:55" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="23" t="s">
         <v>12</v>
       </c>
       <c r="B12" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="99">
+      <c r="C12" s="16">
         <v>1</v>
       </c>
-      <c r="H12" s="17">
+      <c r="D12" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="I12" s="17">
         <v>7</v>
       </c>
-      <c r="V12" s="17">
+      <c r="W12" s="17">
         <v>0</v>
       </c>
-      <c r="AF12" s="17">
+      <c r="AG12" s="17">
         <v>50</v>
       </c>
-      <c r="AK12" s="17">
+      <c r="AL12" s="17">
         <v>70</v>
       </c>
     </row>
-    <row r="13" spans="1:54" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:55" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="23" t="s">
         <v>22</v>
       </c>
       <c r="B13" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="99"/>
-    </row>
-    <row r="14" spans="1:54" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C13" s="16"/>
+      <c r="D13" s="16" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:55" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="21" t="s">
         <v>24</v>
       </c>
       <c r="B14" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="97">
+      <c r="C14" s="12">
         <v>1</v>
       </c>
-      <c r="H14" s="13">
+      <c r="D14" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="I14" s="13">
         <v>0</v>
       </c>
-      <c r="Q14" s="13">
+      <c r="R14" s="13">
         <v>30</v>
       </c>
-      <c r="W14" s="13">
+      <c r="X14" s="13">
         <v>50</v>
       </c>
-      <c r="AE14" s="30"/>
       <c r="AF14" s="30"/>
       <c r="AG14" s="30"/>
       <c r="AH14" s="30"/>
@@ -3395,57 +3430,63 @@
       <c r="AV14" s="30"/>
       <c r="AW14" s="30"/>
       <c r="AX14" s="30"/>
-      <c r="BA14" s="13">
-        <v>90</v>
-      </c>
+      <c r="AY14" s="30"/>
       <c r="BB14" s="13">
         <v>90</v>
       </c>
-    </row>
-    <row r="15" spans="1:54" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="BC14" s="13">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="15" spans="1:55" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="21" t="s">
         <v>25</v>
       </c>
       <c r="B15" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="C15" s="97"/>
-      <c r="H15" s="13">
+      <c r="C15" s="12"/>
+      <c r="D15" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="I15" s="13">
         <v>0</v>
       </c>
-      <c r="Q15" s="13">
+      <c r="R15" s="13">
         <v>1926492</v>
       </c>
-      <c r="W15" s="13">
+      <c r="X15" s="13">
         <v>4573928</v>
       </c>
-      <c r="AL15" s="13">
+      <c r="AM15" s="13">
         <v>9382947</v>
       </c>
-      <c r="AT15" s="13">
+      <c r="AU15" s="13">
         <v>52431253</v>
       </c>
     </row>
-    <row r="16" spans="1:54" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:55" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="21" t="s">
         <v>26</v>
       </c>
       <c r="B16" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="97">
+      <c r="C16" s="12">
         <v>1</v>
       </c>
-      <c r="H16" s="13">
+      <c r="D16" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="I16" s="13">
         <v>0</v>
       </c>
-      <c r="Q16" s="13">
+      <c r="R16" s="13">
         <v>15</v>
       </c>
-      <c r="W16" s="13">
+      <c r="X16" s="13">
         <v>12</v>
       </c>
-      <c r="AE16" s="30"/>
       <c r="AF16" s="30"/>
       <c r="AG16" s="30"/>
       <c r="AH16" s="30"/>
@@ -3465,42 +3506,48 @@
       <c r="AV16" s="30"/>
       <c r="AW16" s="30"/>
       <c r="AX16" s="30"/>
-      <c r="BA16" s="13">
+      <c r="AY16" s="30"/>
+      <c r="BB16" s="13">
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:51" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:52" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="21" t="s">
         <v>27</v>
       </c>
       <c r="B17" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="C17" s="97"/>
-      <c r="H17" s="13">
+      <c r="C17" s="12"/>
+      <c r="D17" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="I17" s="13">
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:51" s="27" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:52" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="25" t="s">
         <v>28</v>
       </c>
       <c r="B18" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="C18" s="100">
+      <c r="C18" s="26">
         <v>1</v>
       </c>
-      <c r="H18" s="27">
+      <c r="D18" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="I18" s="27">
         <v>0</v>
       </c>
-      <c r="Q18" s="27">
+      <c r="R18" s="27">
         <v>15</v>
       </c>
-      <c r="W18" s="27">
+      <c r="X18" s="27">
         <v>30</v>
       </c>
-      <c r="AE18" s="31"/>
       <c r="AF18" s="31"/>
       <c r="AG18" s="31"/>
       <c r="AH18" s="31"/>
@@ -3520,54 +3567,60 @@
       <c r="AV18" s="31"/>
       <c r="AW18" s="31"/>
       <c r="AX18" s="31"/>
-      <c r="AY18" s="27">
+      <c r="AY18" s="31"/>
+      <c r="AZ18" s="27">
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="1:51" s="27" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:52" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="25" t="s">
         <v>29</v>
       </c>
       <c r="B19" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="C19" s="100"/>
-      <c r="H19" s="27">
+      <c r="C19" s="26"/>
+      <c r="D19" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="I19" s="27">
         <v>0</v>
       </c>
-      <c r="Q19" s="27">
+      <c r="R19" s="27">
         <v>492549</v>
       </c>
-      <c r="W19" s="27">
+      <c r="X19" s="27">
         <v>256491</v>
       </c>
-      <c r="AL19" s="27">
+      <c r="AM19" s="27">
         <v>9382947</v>
       </c>
-      <c r="AT19" s="27">
+      <c r="AU19" s="27">
         <v>52431253</v>
       </c>
     </row>
-    <row r="20" spans="1:51" s="27" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:52" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="25" t="s">
         <v>30</v>
       </c>
       <c r="B20" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="C20" s="100">
+      <c r="C20" s="26">
         <v>1</v>
       </c>
-      <c r="H20" s="27">
+      <c r="D20" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="I20" s="27">
         <v>0</v>
       </c>
-      <c r="Q20" s="27">
+      <c r="R20" s="27">
         <v>55</v>
       </c>
-      <c r="W20" s="27">
+      <c r="X20" s="27">
         <v>50</v>
       </c>
-      <c r="AE20" s="31"/>
       <c r="AF20" s="31"/>
       <c r="AG20" s="31"/>
       <c r="AH20" s="31"/>
@@ -3587,42 +3640,48 @@
       <c r="AV20" s="31"/>
       <c r="AW20" s="31"/>
       <c r="AX20" s="31"/>
-      <c r="AY20" s="27">
+      <c r="AY20" s="31"/>
+      <c r="AZ20" s="27">
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:51" s="27" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:52" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="25" t="s">
         <v>31</v>
       </c>
       <c r="B21" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="C21" s="100"/>
-      <c r="H21" s="27">
+      <c r="C21" s="26"/>
+      <c r="D21" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="I21" s="27">
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:51" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:52" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="19" t="s">
         <v>32</v>
       </c>
       <c r="B22" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C22" s="95">
+      <c r="C22" s="8">
         <v>1</v>
       </c>
-      <c r="H22" s="9">
+      <c r="D22" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I22" s="9">
         <v>0</v>
       </c>
-      <c r="Q22" s="9">
+      <c r="R22" s="9">
         <v>5</v>
       </c>
-      <c r="W22" s="9">
+      <c r="X22" s="9">
         <v>15</v>
       </c>
-      <c r="AE22" s="29"/>
       <c r="AF22" s="29"/>
       <c r="AG22" s="29"/>
       <c r="AH22" s="29"/>
@@ -3642,54 +3701,60 @@
       <c r="AV22" s="29"/>
       <c r="AW22" s="29"/>
       <c r="AX22" s="29"/>
-      <c r="AY22" s="9">
+      <c r="AY22" s="29"/>
+      <c r="AZ22" s="9">
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="1:51" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:52" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="19" t="s">
         <v>33</v>
       </c>
       <c r="B23" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C23" s="95"/>
-      <c r="H23" s="9">
+      <c r="C23" s="8"/>
+      <c r="D23" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="I23" s="9">
         <v>0</v>
       </c>
-      <c r="Q23" s="9">
+      <c r="R23" s="9">
         <v>0</v>
       </c>
-      <c r="W23" s="9">
+      <c r="X23" s="9">
         <v>0</v>
       </c>
-      <c r="AL23" s="9">
+      <c r="AM23" s="9">
         <v>0</v>
       </c>
-      <c r="AT23" s="9">
+      <c r="AU23" s="9">
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:51" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:52" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="19" t="s">
         <v>34</v>
       </c>
       <c r="B24" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C24" s="95">
+      <c r="C24" s="8">
         <v>1</v>
       </c>
-      <c r="H24" s="9">
+      <c r="D24" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I24" s="9">
         <v>0</v>
       </c>
-      <c r="Q24" s="9">
+      <c r="R24" s="9">
         <v>65</v>
       </c>
-      <c r="W24" s="9">
+      <c r="X24" s="9">
         <v>62</v>
       </c>
-      <c r="AE24" s="29"/>
       <c r="AF24" s="29"/>
       <c r="AG24" s="29"/>
       <c r="AH24" s="29"/>
@@ -3709,37 +3774,43 @@
       <c r="AV24" s="29"/>
       <c r="AW24" s="29"/>
       <c r="AX24" s="29"/>
-      <c r="AY24" s="9">
+      <c r="AY24" s="29"/>
+      <c r="AZ24" s="9">
         <v>35</v>
       </c>
     </row>
-    <row r="25" spans="1:51" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:52" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="19" t="s">
         <v>35</v>
       </c>
       <c r="B25" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C25" s="95"/>
-      <c r="H25" s="9">
+      <c r="C25" s="8"/>
+      <c r="D25" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="I25" s="9">
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:51" s="86" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:52" s="86" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="84" t="s">
         <v>67</v>
       </c>
       <c r="B26" s="85" t="s">
         <v>13</v>
       </c>
-      <c r="C26" s="101">
+      <c r="C26" s="85">
         <v>1</v>
       </c>
-      <c r="D26" s="86">
+      <c r="D26" s="85" t="s">
+        <v>13</v>
+      </c>
+      <c r="E26" s="86">
         <f>1/26</f>
         <v>3.8461538461538464E-2</v>
       </c>
-      <c r="AE26" s="87"/>
       <c r="AF26" s="87"/>
       <c r="AG26" s="87"/>
       <c r="AH26" s="87"/>
@@ -3759,154 +3830,177 @@
       <c r="AV26" s="87"/>
       <c r="AW26" s="87"/>
       <c r="AX26" s="87"/>
-      <c r="AY26" s="86">
+      <c r="AY26" s="87"/>
+      <c r="AZ26" s="86">
         <v>0.04</v>
       </c>
     </row>
-    <row r="27" spans="1:51" s="86" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:52" s="86" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="84" t="s">
         <v>68</v>
       </c>
       <c r="B27" s="85" t="s">
         <v>23</v>
       </c>
-      <c r="C27" s="101"/>
-      <c r="H27" s="86">
+      <c r="C27" s="85"/>
+      <c r="D27" s="85" t="s">
+        <v>23</v>
+      </c>
+      <c r="I27" s="86">
         <v>0</v>
       </c>
-      <c r="Q27" s="86">
+      <c r="R27" s="86">
         <v>532947</v>
       </c>
-      <c r="W27" s="86">
+      <c r="X27" s="86">
         <v>9283747</v>
       </c>
-      <c r="AY27" s="86">
+      <c r="AZ27" s="86">
         <v>739284639</v>
       </c>
     </row>
-    <row r="28" spans="1:51" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:52" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="18" t="s">
         <v>85</v>
       </c>
       <c r="B28" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C28" s="94">
+      <c r="C28" s="6">
         <v>1</v>
       </c>
-      <c r="AA28" s="103"/>
-      <c r="AK28" s="103"/>
-      <c r="AQ28" s="103"/>
-      <c r="AR28" s="103"/>
-      <c r="AS28" s="103"/>
-      <c r="AT28" s="103"/>
-      <c r="AU28" s="103"/>
-      <c r="AV28" s="103"/>
-      <c r="AW28" s="103"/>
-      <c r="AX28" s="103"/>
-      <c r="AY28" s="103"/>
-    </row>
-    <row r="29" spans="1:51" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D28" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="AB28" s="94"/>
+      <c r="AL28" s="94"/>
+      <c r="AR28" s="94"/>
+      <c r="AS28" s="94"/>
+      <c r="AT28" s="94"/>
+      <c r="AU28" s="94"/>
+      <c r="AV28" s="94"/>
+      <c r="AW28" s="94"/>
+      <c r="AX28" s="94"/>
+      <c r="AY28" s="94"/>
+      <c r="AZ28" s="94"/>
+    </row>
+    <row r="29" spans="1:52" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="18" t="s">
         <v>86</v>
       </c>
       <c r="B29" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C29" s="94">
+      <c r="C29" s="6">
         <v>1</v>
       </c>
-      <c r="I29" s="103"/>
-      <c r="J29" s="103"/>
-      <c r="K29" s="103"/>
-      <c r="L29" s="103"/>
-      <c r="M29" s="103"/>
-      <c r="N29" s="103"/>
-      <c r="O29" s="103"/>
-      <c r="P29" s="103"/>
-      <c r="Q29" s="103"/>
-      <c r="R29" s="103"/>
-      <c r="S29" s="103"/>
-      <c r="T29" s="103"/>
-      <c r="U29" s="103"/>
-      <c r="V29" s="103"/>
-      <c r="W29" s="103"/>
-      <c r="X29" s="103"/>
-      <c r="Y29" s="103"/>
-      <c r="Z29" s="103"/>
-      <c r="AA29" s="103"/>
-      <c r="AB29" s="103"/>
-      <c r="AC29" s="103"/>
-      <c r="AD29" s="103"/>
-      <c r="AE29" s="103"/>
-      <c r="AF29" s="103"/>
-      <c r="AG29" s="103"/>
-      <c r="AH29" s="103"/>
-      <c r="AI29" s="103"/>
-      <c r="AJ29" s="103"/>
-      <c r="AK29" s="103"/>
-      <c r="AL29" s="103"/>
-      <c r="AM29" s="103"/>
-      <c r="AN29" s="103"/>
-      <c r="AO29" s="103"/>
-      <c r="AP29" s="103"/>
-      <c r="AQ29" s="103"/>
-      <c r="AR29" s="103"/>
-      <c r="AS29" s="103"/>
-      <c r="AT29" s="103"/>
-      <c r="AU29" s="103"/>
-      <c r="AV29" s="103"/>
-      <c r="AW29" s="103"/>
-      <c r="AX29" s="103"/>
-      <c r="AY29" s="103"/>
-    </row>
-    <row r="30" spans="1:51" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D29" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="J29" s="94"/>
+      <c r="K29" s="94"/>
+      <c r="L29" s="94"/>
+      <c r="M29" s="94"/>
+      <c r="N29" s="94"/>
+      <c r="O29" s="94"/>
+      <c r="P29" s="94"/>
+      <c r="Q29" s="94"/>
+      <c r="R29" s="94"/>
+      <c r="S29" s="94"/>
+      <c r="T29" s="94"/>
+      <c r="U29" s="94"/>
+      <c r="V29" s="94"/>
+      <c r="W29" s="94"/>
+      <c r="X29" s="94"/>
+      <c r="Y29" s="94"/>
+      <c r="Z29" s="94"/>
+      <c r="AA29" s="94"/>
+      <c r="AB29" s="94"/>
+      <c r="AC29" s="94"/>
+      <c r="AD29" s="94"/>
+      <c r="AE29" s="94"/>
+      <c r="AF29" s="94"/>
+      <c r="AG29" s="94"/>
+      <c r="AH29" s="94"/>
+      <c r="AI29" s="94"/>
+      <c r="AJ29" s="94"/>
+      <c r="AK29" s="94"/>
+      <c r="AL29" s="94"/>
+      <c r="AM29" s="94"/>
+      <c r="AN29" s="94"/>
+      <c r="AO29" s="94"/>
+      <c r="AP29" s="94"/>
+      <c r="AQ29" s="94"/>
+      <c r="AR29" s="94"/>
+      <c r="AS29" s="94"/>
+      <c r="AT29" s="94"/>
+      <c r="AU29" s="94"/>
+      <c r="AV29" s="94"/>
+      <c r="AW29" s="94"/>
+      <c r="AX29" s="94"/>
+      <c r="AY29" s="94"/>
+      <c r="AZ29" s="94"/>
+    </row>
+    <row r="30" spans="1:52" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="18" t="s">
         <v>87</v>
       </c>
       <c r="B30" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C30" s="94">
+      <c r="C30" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:51" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D30" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="31" spans="1:52" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="18" t="s">
         <v>88</v>
       </c>
       <c r="B31" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C31" s="94">
+      <c r="C31" s="6">
         <v>1</v>
       </c>
+      <c r="D31" s="6" t="s">
+        <v>13</v>
+      </c>
     </row>
   </sheetData>
-  <dataValidations xWindow="343" yWindow="238" count="3">
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D26:BB26 D16:BB16 D14:BB14 D12:BB12 D10:BB10 D24:BB24 D22:BB22 D20:BB20 D18:BB18 D8:BB8 D6:BB6 D4:BB4 D2:BB2">
+  <dataValidations xWindow="343" yWindow="238" count="4">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E26:BC26 E16:BC16 E14:BC14 E12:BC12 E10:BC10 E24:BC24 E22:BC22 E20:BC20 E18:BC18 E8:BC8 E6:BC6 E4:BC4 E2:BC2">
       <formula1>0</formula1>
       <formula2>100</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D27:BB27 D25:BB25 D23:BB23 D21:BB21 D19:BB19 D17:BB17 D15:BB15 D13:BB13 D11:BB11 D9:BB9 D7:BB7 D5:BB5 D3:BB3">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E27:BC27 E25:BC25 E23:BC23 E21:BC21 E19:BC19 E17:BC17 E15:BC15 E13:BC13 E11:BC11 E9:BC9 E7:BC7 E5:BC5 E3:BC3">
       <formula1>0</formula1>
       <formula2>100000000000000000000</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Smoothness for fitting function" prompt="Must be positive." sqref="C1:C1048576">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Smoothness for fitting function" prompt="Must be positive." sqref="C2:C1048576">
       <formula1>0</formula1>
       <formula2>100</formula2>
     </dataValidation>
+    <dataValidation allowBlank="1" showErrorMessage="1" sqref="C1 D1"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xWindow="343" yWindow="238" count="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xWindow="343" yWindow="238" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>dropdown_lists!$A$2:$A$4</xm:f>
           </x14:formula1>
           <xm:sqref>B2:B27</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Time-variant?" prompt="If no, the most recent value will be selected.">
+          <x14:formula1>
+            <xm:f>dropdown_lists!$A$2:$A$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>D2:D1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Updated the code to reflect James' changes in spreadsheet.py
</commit_message>
<xml_diff>
--- a/autumn/xls/programs_fiji.xlsx
+++ b/autumn/xls/programs_fiji.xlsx
@@ -2868,7 +2868,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D32" sqref="D32"/>
+      <selection pane="bottomRight" activeCell="Q43" sqref="Q43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3096,7 +3096,9 @@
       <c r="U2" s="28"/>
       <c r="V2" s="28"/>
       <c r="W2" s="28"/>
-      <c r="X2" s="28"/>
+      <c r="X2" s="28">
+        <v>1</v>
+      </c>
       <c r="Y2" s="28"/>
       <c r="Z2" s="28"/>
       <c r="AA2" s="28"/>
@@ -3155,6 +3157,9 @@
       <c r="W3" s="7">
         <v>39034561</v>
       </c>
+      <c r="X3" s="7">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="1:55" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="19" t="s">
@@ -3177,6 +3182,9 @@
       </c>
       <c r="T4" s="9">
         <v>30</v>
+      </c>
+      <c r="X4" s="9">
+        <v>1</v>
       </c>
       <c r="AB4" s="29"/>
       <c r="AC4" s="29"/>
@@ -3224,6 +3232,9 @@
       <c r="F5" s="9">
         <v>0</v>
       </c>
+      <c r="X5" s="9">
+        <v>1</v>
+      </c>
     </row>
     <row r="6" spans="1:55" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
@@ -3244,6 +3255,9 @@
       <c r="J6" s="11">
         <v>80</v>
       </c>
+      <c r="X6" s="11">
+        <v>1</v>
+      </c>
       <c r="Z6" s="11">
         <v>82</v>
       </c>
@@ -3277,6 +3291,9 @@
       <c r="J7" s="11">
         <v>2040504</v>
       </c>
+      <c r="X7" s="11">
+        <v>1</v>
+      </c>
       <c r="Z7" s="11">
         <v>4049504</v>
       </c>
@@ -3300,6 +3317,9 @@
       <c r="K8" s="13">
         <v>40</v>
       </c>
+      <c r="X8" s="13">
+        <v>1</v>
+      </c>
       <c r="AB8" s="13">
         <v>40</v>
       </c>
@@ -3315,6 +3335,9 @@
       <c r="D9" s="12" t="s">
         <v>23</v>
       </c>
+      <c r="X9" s="13">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" spans="1:55" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="22" t="s">
@@ -3332,6 +3355,9 @@
       <c r="R10" s="15">
         <v>30</v>
       </c>
+      <c r="X10" s="15">
+        <v>1</v>
+      </c>
       <c r="AB10" s="15">
         <v>40</v>
       </c>
@@ -3350,6 +3376,9 @@
       <c r="D11" s="14" t="s">
         <v>23</v>
       </c>
+      <c r="X11" s="15">
+        <v>1</v>
+      </c>
     </row>
     <row r="12" spans="1:55" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="23" t="s">
@@ -3370,6 +3399,9 @@
       <c r="W12" s="17">
         <v>0</v>
       </c>
+      <c r="X12" s="17">
+        <v>1</v>
+      </c>
       <c r="AG12" s="17">
         <v>50</v>
       </c>
@@ -3387,6 +3419,9 @@
       <c r="C13" s="16"/>
       <c r="D13" s="16" t="s">
         <v>23</v>
+      </c>
+      <c r="X13" s="17">
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:55" s="13" customFormat="1" x14ac:dyDescent="0.25">
@@ -3525,6 +3560,9 @@
       <c r="I17" s="13">
         <v>0</v>
       </c>
+      <c r="X17" s="13">
+        <v>1</v>
+      </c>
     </row>
     <row r="18" spans="1:52" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="25" t="s">
@@ -3659,6 +3697,9 @@
       <c r="I21" s="27">
         <v>0</v>
       </c>
+      <c r="X21" s="27">
+        <v>1</v>
+      </c>
     </row>
     <row r="22" spans="1:52" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="19" t="s">
@@ -3793,6 +3834,9 @@
       <c r="I25" s="9">
         <v>0</v>
       </c>
+      <c r="X25" s="9">
+        <v>1</v>
+      </c>
     </row>
     <row r="26" spans="1:52" s="86" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="84" t="s">
@@ -3810,6 +3854,9 @@
       <c r="E26" s="86">
         <f>1/26</f>
         <v>3.8461538461538464E-2</v>
+      </c>
+      <c r="X26" s="86">
+        <v>1</v>
       </c>
       <c r="AF26" s="87"/>
       <c r="AG26" s="87"/>

</xml_diff>

<commit_message>
Revert "Updated the code to reflect James' changes in spreadsheet.py"
This reverts commit cde7e9080e138fa657d7377fef0708c73fdadb3c.
</commit_message>
<xml_diff>
--- a/autumn/xls/programs_fiji.xlsx
+++ b/autumn/xls/programs_fiji.xlsx
@@ -2868,7 +2868,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Q43" sqref="Q43"/>
+      <selection pane="bottomRight" activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3096,9 +3096,7 @@
       <c r="U2" s="28"/>
       <c r="V2" s="28"/>
       <c r="W2" s="28"/>
-      <c r="X2" s="28">
-        <v>1</v>
-      </c>
+      <c r="X2" s="28"/>
       <c r="Y2" s="28"/>
       <c r="Z2" s="28"/>
       <c r="AA2" s="28"/>
@@ -3157,9 +3155,6 @@
       <c r="W3" s="7">
         <v>39034561</v>
       </c>
-      <c r="X3" s="7">
-        <v>1</v>
-      </c>
     </row>
     <row r="4" spans="1:55" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="19" t="s">
@@ -3182,9 +3177,6 @@
       </c>
       <c r="T4" s="9">
         <v>30</v>
-      </c>
-      <c r="X4" s="9">
-        <v>1</v>
       </c>
       <c r="AB4" s="29"/>
       <c r="AC4" s="29"/>
@@ -3232,9 +3224,6 @@
       <c r="F5" s="9">
         <v>0</v>
       </c>
-      <c r="X5" s="9">
-        <v>1</v>
-      </c>
     </row>
     <row r="6" spans="1:55" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
@@ -3255,9 +3244,6 @@
       <c r="J6" s="11">
         <v>80</v>
       </c>
-      <c r="X6" s="11">
-        <v>1</v>
-      </c>
       <c r="Z6" s="11">
         <v>82</v>
       </c>
@@ -3291,9 +3277,6 @@
       <c r="J7" s="11">
         <v>2040504</v>
       </c>
-      <c r="X7" s="11">
-        <v>1</v>
-      </c>
       <c r="Z7" s="11">
         <v>4049504</v>
       </c>
@@ -3317,9 +3300,6 @@
       <c r="K8" s="13">
         <v>40</v>
       </c>
-      <c r="X8" s="13">
-        <v>1</v>
-      </c>
       <c r="AB8" s="13">
         <v>40</v>
       </c>
@@ -3335,9 +3315,6 @@
       <c r="D9" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="X9" s="13">
-        <v>1</v>
-      </c>
     </row>
     <row r="10" spans="1:55" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="22" t="s">
@@ -3355,9 +3332,6 @@
       <c r="R10" s="15">
         <v>30</v>
       </c>
-      <c r="X10" s="15">
-        <v>1</v>
-      </c>
       <c r="AB10" s="15">
         <v>40</v>
       </c>
@@ -3376,9 +3350,6 @@
       <c r="D11" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="X11" s="15">
-        <v>1</v>
-      </c>
     </row>
     <row r="12" spans="1:55" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="23" t="s">
@@ -3399,9 +3370,6 @@
       <c r="W12" s="17">
         <v>0</v>
       </c>
-      <c r="X12" s="17">
-        <v>1</v>
-      </c>
       <c r="AG12" s="17">
         <v>50</v>
       </c>
@@ -3419,9 +3387,6 @@
       <c r="C13" s="16"/>
       <c r="D13" s="16" t="s">
         <v>23</v>
-      </c>
-      <c r="X13" s="17">
-        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:55" s="13" customFormat="1" x14ac:dyDescent="0.25">
@@ -3560,9 +3525,6 @@
       <c r="I17" s="13">
         <v>0</v>
       </c>
-      <c r="X17" s="13">
-        <v>1</v>
-      </c>
     </row>
     <row r="18" spans="1:52" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="25" t="s">
@@ -3697,9 +3659,6 @@
       <c r="I21" s="27">
         <v>0</v>
       </c>
-      <c r="X21" s="27">
-        <v>1</v>
-      </c>
     </row>
     <row r="22" spans="1:52" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="19" t="s">
@@ -3834,9 +3793,6 @@
       <c r="I25" s="9">
         <v>0</v>
       </c>
-      <c r="X25" s="9">
-        <v>1</v>
-      </c>
     </row>
     <row r="26" spans="1:52" s="86" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="84" t="s">
@@ -3854,9 +3810,6 @@
       <c r="E26" s="86">
         <f>1/26</f>
         <v>3.8461538461538464E-2</v>
-      </c>
-      <c r="X26" s="86">
-        <v>1</v>
       </c>
       <c r="AF26" s="87"/>
       <c r="AG26" s="87"/>

</xml_diff>

<commit_message>
Revert "Time-variant choice for parameters"
This reverts commit e3a7284a1e99d349314de6bedddbc40c48203c16.
</commit_message>
<xml_diff>
--- a/autumn/xls/programs_fiji.xlsx
+++ b/autumn/xls/programs_fiji.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="89">
   <si>
     <t>program_rate_restart_presenting</t>
   </si>
@@ -284,9 +284,6 @@
   </si>
   <si>
     <t>tb_prop_smearneg</t>
-  </si>
-  <si>
-    <t>time_variant</t>
   </si>
 </sst>
 </file>
@@ -1351,7 +1348,7 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="95">
+  <cellXfs count="104">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1450,6 +1447,15 @@
     <xf numFmtId="0" fontId="0" fillId="13" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="664">
@@ -2862,234 +2868,229 @@
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:BC31"/>
+  <dimension ref="A1:BB31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D32" sqref="D32"/>
+      <selection pane="bottomRight" activeCell="J30" sqref="J30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="47.42578125" style="24" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="11" style="2" customWidth="1"/>
-    <col min="5" max="5" width="7.42578125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7" style="1" customWidth="1"/>
-    <col min="8" max="9" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.42578125" style="1" customWidth="1"/>
-    <col min="11" max="12" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.7109375" style="1" customWidth="1"/>
-    <col min="14" max="17" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="7.28515625" style="1" customWidth="1"/>
-    <col min="19" max="22" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="24" width="7.42578125" style="1" customWidth="1"/>
-    <col min="25" max="25" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="7.140625" style="1" customWidth="1"/>
-    <col min="27" max="38" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="8" style="1" customWidth="1"/>
-    <col min="40" max="46" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="8" style="1" customWidth="1"/>
-    <col min="48" max="48" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="6.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="50" max="51" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="7.85546875" style="1" customWidth="1"/>
-    <col min="53" max="53" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="54" max="16384" width="9.140625" style="1"/>
+    <col min="3" max="3" width="11" style="102" customWidth="1"/>
+    <col min="4" max="4" width="7.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7" style="1" customWidth="1"/>
+    <col min="7" max="8" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.42578125" style="1" customWidth="1"/>
+    <col min="10" max="11" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.7109375" style="1" customWidth="1"/>
+    <col min="13" max="16" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="7.28515625" style="1" customWidth="1"/>
+    <col min="18" max="21" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="23" width="7.42578125" style="1" customWidth="1"/>
+    <col min="24" max="24" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="7.140625" style="1" customWidth="1"/>
+    <col min="26" max="37" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="8" style="1" customWidth="1"/>
+    <col min="39" max="45" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="8" style="1" customWidth="1"/>
+    <col min="47" max="47" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="6.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="49" max="50" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="7.85546875" style="1" customWidth="1"/>
+    <col min="52" max="52" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="53" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:55" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:54" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="D1" s="4" t="s">
-        <v>89</v>
+      <c r="D1" s="5">
+        <v>1920</v>
       </c>
       <c r="E1" s="5">
-        <v>1920</v>
+        <v>1930</v>
       </c>
       <c r="F1" s="5">
-        <v>1930</v>
+        <v>1940</v>
       </c>
       <c r="G1" s="5">
-        <v>1940</v>
+        <v>1950</v>
       </c>
       <c r="H1" s="5">
-        <v>1950</v>
+        <v>1955</v>
       </c>
       <c r="I1" s="5">
-        <v>1955</v>
+        <v>1960</v>
       </c>
       <c r="J1" s="5">
-        <v>1960</v>
+        <v>1965</v>
       </c>
       <c r="K1" s="5">
-        <v>1965</v>
+        <v>1970</v>
       </c>
       <c r="L1" s="5">
-        <v>1970</v>
+        <v>1975</v>
       </c>
       <c r="M1" s="5">
-        <v>1975</v>
+        <v>1976</v>
       </c>
       <c r="N1" s="5">
-        <v>1976</v>
+        <v>1977</v>
       </c>
       <c r="O1" s="5">
-        <v>1977</v>
+        <v>1978</v>
       </c>
       <c r="P1" s="5">
-        <v>1978</v>
+        <v>1979</v>
       </c>
       <c r="Q1" s="5">
-        <v>1979</v>
+        <v>1980</v>
       </c>
       <c r="R1" s="5">
-        <v>1980</v>
+        <v>1981</v>
       </c>
       <c r="S1" s="5">
-        <v>1981</v>
+        <v>1982</v>
       </c>
       <c r="T1" s="5">
-        <v>1982</v>
+        <v>1983</v>
       </c>
       <c r="U1" s="5">
-        <v>1983</v>
+        <v>1984</v>
       </c>
       <c r="V1" s="5">
-        <v>1984</v>
+        <v>1985</v>
       </c>
       <c r="W1" s="5">
-        <v>1985</v>
+        <v>1986</v>
       </c>
       <c r="X1" s="5">
-        <v>1986</v>
+        <v>1987</v>
       </c>
       <c r="Y1" s="5">
-        <v>1987</v>
+        <v>1988</v>
       </c>
       <c r="Z1" s="5">
-        <v>1988</v>
+        <v>1989</v>
       </c>
       <c r="AA1" s="5">
-        <v>1989</v>
+        <v>1990</v>
       </c>
       <c r="AB1" s="5">
-        <v>1990</v>
+        <v>1991</v>
       </c>
       <c r="AC1" s="5">
-        <v>1991</v>
+        <v>1992</v>
       </c>
       <c r="AD1" s="5">
-        <v>1992</v>
+        <v>1993</v>
       </c>
       <c r="AE1" s="5">
-        <v>1993</v>
+        <v>1994</v>
       </c>
       <c r="AF1" s="5">
-        <v>1994</v>
+        <v>1995</v>
       </c>
       <c r="AG1" s="5">
-        <v>1995</v>
+        <v>1996</v>
       </c>
       <c r="AH1" s="5">
-        <v>1996</v>
+        <v>1997</v>
       </c>
       <c r="AI1" s="5">
-        <v>1997</v>
+        <v>1998</v>
       </c>
       <c r="AJ1" s="5">
-        <v>1998</v>
+        <v>1999</v>
       </c>
       <c r="AK1" s="5">
-        <v>1999</v>
+        <v>2000</v>
       </c>
       <c r="AL1" s="5">
-        <v>2000</v>
+        <v>2001</v>
       </c>
       <c r="AM1" s="5">
-        <v>2001</v>
+        <v>2002</v>
       </c>
       <c r="AN1" s="5">
-        <v>2002</v>
+        <v>2003</v>
       </c>
       <c r="AO1" s="5">
-        <v>2003</v>
+        <v>2004</v>
       </c>
       <c r="AP1" s="5">
-        <v>2004</v>
+        <v>2005</v>
       </c>
       <c r="AQ1" s="5">
-        <v>2005</v>
+        <v>2006</v>
       </c>
       <c r="AR1" s="5">
-        <v>2006</v>
+        <v>2007</v>
       </c>
       <c r="AS1" s="5">
-        <v>2007</v>
+        <v>2008</v>
       </c>
       <c r="AT1" s="5">
-        <v>2008</v>
+        <v>2009</v>
       </c>
       <c r="AU1" s="5">
-        <v>2009</v>
+        <v>2010</v>
       </c>
       <c r="AV1" s="5">
-        <v>2010</v>
+        <v>2011</v>
       </c>
       <c r="AW1" s="5">
-        <v>2011</v>
+        <v>2012</v>
       </c>
       <c r="AX1" s="5">
-        <v>2012</v>
+        <v>2013</v>
       </c>
       <c r="AY1" s="5">
-        <v>2013</v>
+        <v>2014</v>
       </c>
       <c r="AZ1" s="5">
-        <v>2014</v>
-      </c>
-      <c r="BA1" s="5">
         <v>2015</v>
       </c>
+      <c r="BA1" s="5" t="s">
+        <v>69</v>
+      </c>
       <c r="BB1" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="BC1" s="5" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:55" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:54" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="6">
+      <c r="C2" s="94">
         <v>1</v>
       </c>
-      <c r="D2" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" s="7">
+      <c r="G2" s="7">
         <v>0</v>
       </c>
-      <c r="J2" s="7">
+      <c r="I2" s="7">
         <v>25</v>
       </c>
-      <c r="M2" s="7">
+      <c r="L2" s="7">
         <v>40</v>
       </c>
+      <c r="Q2" s="28"/>
       <c r="R2" s="28"/>
       <c r="S2" s="28"/>
       <c r="T2" s="28"/>
@@ -3124,60 +3125,54 @@
       <c r="AW2" s="28"/>
       <c r="AX2" s="28"/>
       <c r="AY2" s="28"/>
-      <c r="AZ2" s="28"/>
+      <c r="BA2" s="7">
+        <v>99</v>
+      </c>
       <c r="BB2" s="7">
         <v>99</v>
       </c>
-      <c r="BC2" s="7">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="3" spans="1:55" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:54" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
         <v>17</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="H3" s="7">
+      <c r="C3" s="94"/>
+      <c r="G3" s="7">
         <v>0</v>
       </c>
-      <c r="J3" s="7">
+      <c r="I3" s="7">
         <v>10000000</v>
       </c>
-      <c r="M3" s="7">
+      <c r="L3" s="7">
         <v>15040500</v>
       </c>
-      <c r="W3" s="7">
+      <c r="V3" s="7">
         <v>39034561</v>
       </c>
     </row>
-    <row r="4" spans="1:55" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="19" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="8">
+      <c r="C4" s="95">
         <v>5</v>
       </c>
-      <c r="D4" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="9">
+      <c r="E4" s="9">
         <v>0</v>
       </c>
-      <c r="K4" s="9">
+      <c r="J4" s="9">
         <v>10</v>
       </c>
-      <c r="T4" s="9">
+      <c r="S4" s="9">
         <v>30</v>
       </c>
+      <c r="AA4" s="29"/>
       <c r="AB4" s="29"/>
       <c r="AC4" s="29"/>
       <c r="AD4" s="29"/>
@@ -3202,215 +3197,185 @@
       <c r="AW4" s="29"/>
       <c r="AX4" s="29"/>
       <c r="AY4" s="29"/>
-      <c r="AZ4" s="29"/>
+      <c r="BA4" s="9">
+        <v>70</v>
+      </c>
       <c r="BB4" s="9">
-        <v>70</v>
-      </c>
-      <c r="BC4" s="9">
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:55" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
         <v>18</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="F5" s="9">
+      <c r="C5" s="95"/>
+      <c r="E5" s="9">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:55" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:54" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="10">
+      <c r="C6" s="96">
         <v>1</v>
       </c>
-      <c r="D6" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="G6" s="11">
+      <c r="F6" s="11">
         <v>70</v>
       </c>
-      <c r="J6" s="11">
+      <c r="I6" s="11">
         <v>80</v>
       </c>
-      <c r="Z6" s="11">
+      <c r="Y6" s="11">
         <v>82</v>
       </c>
-      <c r="AM6" s="11">
+      <c r="AL6" s="11">
         <v>84</v>
       </c>
-      <c r="AZ6" s="11">
+      <c r="AY6" s="11">
+        <v>85</v>
+      </c>
+      <c r="BA6" s="11">
         <v>85</v>
       </c>
       <c r="BB6" s="11">
         <v>85</v>
       </c>
-      <c r="BC6" s="11">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="7" spans="1:55" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:54" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
         <v>19</v>
       </c>
       <c r="B7" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="G7" s="11">
+      <c r="C7" s="96"/>
+      <c r="F7" s="11">
         <v>1005000</v>
       </c>
-      <c r="J7" s="11">
+      <c r="I7" s="11">
         <v>2040504</v>
       </c>
-      <c r="Z7" s="11">
+      <c r="Y7" s="11">
         <v>4049504</v>
       </c>
     </row>
-    <row r="8" spans="1:55" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:54" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="21" t="s">
         <v>3</v>
       </c>
       <c r="B8" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="12">
+      <c r="C8" s="97">
         <v>1</v>
       </c>
-      <c r="D8" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="H8" s="13">
+      <c r="G8" s="13">
         <v>30</v>
       </c>
-      <c r="K8" s="13">
+      <c r="J8" s="13">
         <v>40</v>
       </c>
-      <c r="AB8" s="13">
+      <c r="AA8" s="13">
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:55" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:54" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="21" t="s">
         <v>20</v>
       </c>
       <c r="B9" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:55" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C9" s="97"/>
+    </row>
+    <row r="10" spans="1:54" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="22" t="s">
         <v>11</v>
       </c>
       <c r="B10" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="14">
+      <c r="C10" s="98">
         <v>1</v>
       </c>
-      <c r="D10" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="R10" s="15">
+      <c r="Q10" s="15">
         <v>30</v>
       </c>
-      <c r="AB10" s="15">
+      <c r="AA10" s="15">
         <v>40</v>
       </c>
-      <c r="AL10" s="15">
+      <c r="AK10" s="15">
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:55" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:54" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="22" t="s">
         <v>21</v>
       </c>
       <c r="B11" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="14"/>
-      <c r="D11" s="14" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="12" spans="1:55" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C11" s="98"/>
+    </row>
+    <row r="12" spans="1:54" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="23" t="s">
         <v>12</v>
       </c>
       <c r="B12" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="16">
+      <c r="C12" s="99">
         <v>1</v>
       </c>
-      <c r="D12" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="I12" s="17">
+      <c r="H12" s="17">
         <v>7</v>
       </c>
-      <c r="W12" s="17">
+      <c r="V12" s="17">
         <v>0</v>
       </c>
-      <c r="AG12" s="17">
+      <c r="AF12" s="17">
         <v>50</v>
       </c>
-      <c r="AL12" s="17">
+      <c r="AK12" s="17">
         <v>70</v>
       </c>
     </row>
-    <row r="13" spans="1:55" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:54" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="23" t="s">
         <v>22</v>
       </c>
       <c r="B13" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="16"/>
-      <c r="D13" s="16" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="14" spans="1:55" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C13" s="99"/>
+    </row>
+    <row r="14" spans="1:54" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="21" t="s">
         <v>24</v>
       </c>
       <c r="B14" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="12">
+      <c r="C14" s="97">
         <v>1</v>
       </c>
-      <c r="D14" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="I14" s="13">
+      <c r="H14" s="13">
         <v>0</v>
       </c>
-      <c r="R14" s="13">
+      <c r="Q14" s="13">
         <v>30</v>
       </c>
-      <c r="X14" s="13">
+      <c r="W14" s="13">
         <v>50</v>
       </c>
+      <c r="AE14" s="30"/>
       <c r="AF14" s="30"/>
       <c r="AG14" s="30"/>
       <c r="AH14" s="30"/>
@@ -3430,63 +3395,57 @@
       <c r="AV14" s="30"/>
       <c r="AW14" s="30"/>
       <c r="AX14" s="30"/>
-      <c r="AY14" s="30"/>
+      <c r="BA14" s="13">
+        <v>90</v>
+      </c>
       <c r="BB14" s="13">
         <v>90</v>
       </c>
-      <c r="BC14" s="13">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="15" spans="1:55" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:54" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="21" t="s">
         <v>25</v>
       </c>
       <c r="B15" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="I15" s="13">
+      <c r="C15" s="97"/>
+      <c r="H15" s="13">
         <v>0</v>
       </c>
-      <c r="R15" s="13">
+      <c r="Q15" s="13">
         <v>1926492</v>
       </c>
-      <c r="X15" s="13">
+      <c r="W15" s="13">
         <v>4573928</v>
       </c>
-      <c r="AM15" s="13">
+      <c r="AL15" s="13">
         <v>9382947</v>
       </c>
-      <c r="AU15" s="13">
+      <c r="AT15" s="13">
         <v>52431253</v>
       </c>
     </row>
-    <row r="16" spans="1:55" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:54" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="21" t="s">
         <v>26</v>
       </c>
       <c r="B16" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="12">
+      <c r="C16" s="97">
         <v>1</v>
       </c>
-      <c r="D16" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="I16" s="13">
+      <c r="H16" s="13">
         <v>0</v>
       </c>
-      <c r="R16" s="13">
+      <c r="Q16" s="13">
         <v>15</v>
       </c>
-      <c r="X16" s="13">
+      <c r="W16" s="13">
         <v>12</v>
       </c>
+      <c r="AE16" s="30"/>
       <c r="AF16" s="30"/>
       <c r="AG16" s="30"/>
       <c r="AH16" s="30"/>
@@ -3506,48 +3465,42 @@
       <c r="AV16" s="30"/>
       <c r="AW16" s="30"/>
       <c r="AX16" s="30"/>
-      <c r="AY16" s="30"/>
-      <c r="BB16" s="13">
+      <c r="BA16" s="13">
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:52" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:51" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="21" t="s">
         <v>27</v>
       </c>
       <c r="B17" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="I17" s="13">
+      <c r="C17" s="97"/>
+      <c r="H17" s="13">
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:52" s="27" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:51" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="25" t="s">
         <v>28</v>
       </c>
       <c r="B18" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="C18" s="26">
+      <c r="C18" s="100">
         <v>1</v>
       </c>
-      <c r="D18" s="26" t="s">
-        <v>13</v>
-      </c>
-      <c r="I18" s="27">
+      <c r="H18" s="27">
         <v>0</v>
       </c>
-      <c r="R18" s="27">
+      <c r="Q18" s="27">
         <v>15</v>
       </c>
-      <c r="X18" s="27">
+      <c r="W18" s="27">
         <v>30</v>
       </c>
+      <c r="AE18" s="31"/>
       <c r="AF18" s="31"/>
       <c r="AG18" s="31"/>
       <c r="AH18" s="31"/>
@@ -3567,60 +3520,54 @@
       <c r="AV18" s="31"/>
       <c r="AW18" s="31"/>
       <c r="AX18" s="31"/>
-      <c r="AY18" s="31"/>
-      <c r="AZ18" s="27">
+      <c r="AY18" s="27">
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="1:52" s="27" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:51" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="25" t="s">
         <v>29</v>
       </c>
       <c r="B19" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="C19" s="26"/>
-      <c r="D19" s="26" t="s">
-        <v>23</v>
-      </c>
-      <c r="I19" s="27">
+      <c r="C19" s="100"/>
+      <c r="H19" s="27">
         <v>0</v>
       </c>
-      <c r="R19" s="27">
+      <c r="Q19" s="27">
         <v>492549</v>
       </c>
-      <c r="X19" s="27">
+      <c r="W19" s="27">
         <v>256491</v>
       </c>
-      <c r="AM19" s="27">
+      <c r="AL19" s="27">
         <v>9382947</v>
       </c>
-      <c r="AU19" s="27">
+      <c r="AT19" s="27">
         <v>52431253</v>
       </c>
     </row>
-    <row r="20" spans="1:52" s="27" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:51" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="25" t="s">
         <v>30</v>
       </c>
       <c r="B20" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="C20" s="26">
+      <c r="C20" s="100">
         <v>1</v>
       </c>
-      <c r="D20" s="26" t="s">
-        <v>13</v>
-      </c>
-      <c r="I20" s="27">
+      <c r="H20" s="27">
         <v>0</v>
       </c>
-      <c r="R20" s="27">
+      <c r="Q20" s="27">
         <v>55</v>
       </c>
-      <c r="X20" s="27">
+      <c r="W20" s="27">
         <v>50</v>
       </c>
+      <c r="AE20" s="31"/>
       <c r="AF20" s="31"/>
       <c r="AG20" s="31"/>
       <c r="AH20" s="31"/>
@@ -3640,48 +3587,42 @@
       <c r="AV20" s="31"/>
       <c r="AW20" s="31"/>
       <c r="AX20" s="31"/>
-      <c r="AY20" s="31"/>
-      <c r="AZ20" s="27">
+      <c r="AY20" s="27">
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:52" s="27" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:51" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="25" t="s">
         <v>31</v>
       </c>
       <c r="B21" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="C21" s="26"/>
-      <c r="D21" s="26" t="s">
-        <v>23</v>
-      </c>
-      <c r="I21" s="27">
+      <c r="C21" s="100"/>
+      <c r="H21" s="27">
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:52" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:51" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="19" t="s">
         <v>32</v>
       </c>
       <c r="B22" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C22" s="8">
+      <c r="C22" s="95">
         <v>1</v>
       </c>
-      <c r="D22" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="I22" s="9">
+      <c r="H22" s="9">
         <v>0</v>
       </c>
-      <c r="R22" s="9">
+      <c r="Q22" s="9">
         <v>5</v>
       </c>
-      <c r="X22" s="9">
+      <c r="W22" s="9">
         <v>15</v>
       </c>
+      <c r="AE22" s="29"/>
       <c r="AF22" s="29"/>
       <c r="AG22" s="29"/>
       <c r="AH22" s="29"/>
@@ -3701,60 +3642,54 @@
       <c r="AV22" s="29"/>
       <c r="AW22" s="29"/>
       <c r="AX22" s="29"/>
-      <c r="AY22" s="29"/>
-      <c r="AZ22" s="9">
+      <c r="AY22" s="9">
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="1:52" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:51" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="19" t="s">
         <v>33</v>
       </c>
       <c r="B23" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C23" s="8"/>
-      <c r="D23" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="I23" s="9">
+      <c r="C23" s="95"/>
+      <c r="H23" s="9">
         <v>0</v>
       </c>
-      <c r="R23" s="9">
+      <c r="Q23" s="9">
         <v>0</v>
       </c>
-      <c r="X23" s="9">
+      <c r="W23" s="9">
         <v>0</v>
       </c>
-      <c r="AM23" s="9">
+      <c r="AL23" s="9">
         <v>0</v>
       </c>
-      <c r="AU23" s="9">
+      <c r="AT23" s="9">
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:52" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:51" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="19" t="s">
         <v>34</v>
       </c>
       <c r="B24" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C24" s="8">
+      <c r="C24" s="95">
         <v>1</v>
       </c>
-      <c r="D24" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="I24" s="9">
+      <c r="H24" s="9">
         <v>0</v>
       </c>
-      <c r="R24" s="9">
+      <c r="Q24" s="9">
         <v>65</v>
       </c>
-      <c r="X24" s="9">
+      <c r="W24" s="9">
         <v>62</v>
       </c>
+      <c r="AE24" s="29"/>
       <c r="AF24" s="29"/>
       <c r="AG24" s="29"/>
       <c r="AH24" s="29"/>
@@ -3774,43 +3709,37 @@
       <c r="AV24" s="29"/>
       <c r="AW24" s="29"/>
       <c r="AX24" s="29"/>
-      <c r="AY24" s="29"/>
-      <c r="AZ24" s="9">
+      <c r="AY24" s="9">
         <v>35</v>
       </c>
     </row>
-    <row r="25" spans="1:52" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:51" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="19" t="s">
         <v>35</v>
       </c>
       <c r="B25" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C25" s="8"/>
-      <c r="D25" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="I25" s="9">
+      <c r="C25" s="95"/>
+      <c r="H25" s="9">
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:52" s="86" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:51" s="86" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="84" t="s">
         <v>67</v>
       </c>
       <c r="B26" s="85" t="s">
         <v>13</v>
       </c>
-      <c r="C26" s="85">
+      <c r="C26" s="101">
         <v>1</v>
       </c>
-      <c r="D26" s="85" t="s">
-        <v>13</v>
-      </c>
-      <c r="E26" s="86">
+      <c r="D26" s="86">
         <f>1/26</f>
         <v>3.8461538461538464E-2</v>
       </c>
+      <c r="AE26" s="87"/>
       <c r="AF26" s="87"/>
       <c r="AG26" s="87"/>
       <c r="AH26" s="87"/>
@@ -3830,177 +3759,154 @@
       <c r="AV26" s="87"/>
       <c r="AW26" s="87"/>
       <c r="AX26" s="87"/>
-      <c r="AY26" s="87"/>
-      <c r="AZ26" s="86">
+      <c r="AY26" s="86">
         <v>0.04</v>
       </c>
     </row>
-    <row r="27" spans="1:52" s="86" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:51" s="86" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="84" t="s">
         <v>68</v>
       </c>
       <c r="B27" s="85" t="s">
         <v>23</v>
       </c>
-      <c r="C27" s="85"/>
-      <c r="D27" s="85" t="s">
-        <v>23</v>
-      </c>
-      <c r="I27" s="86">
+      <c r="C27" s="101"/>
+      <c r="H27" s="86">
         <v>0</v>
       </c>
-      <c r="R27" s="86">
+      <c r="Q27" s="86">
         <v>532947</v>
       </c>
-      <c r="X27" s="86">
+      <c r="W27" s="86">
         <v>9283747</v>
       </c>
-      <c r="AZ27" s="86">
+      <c r="AY27" s="86">
         <v>739284639</v>
       </c>
     </row>
-    <row r="28" spans="1:52" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:51" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="18" t="s">
         <v>85</v>
       </c>
       <c r="B28" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C28" s="6">
+      <c r="C28" s="94">
         <v>1</v>
       </c>
-      <c r="D28" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="AB28" s="94"/>
-      <c r="AL28" s="94"/>
-      <c r="AR28" s="94"/>
-      <c r="AS28" s="94"/>
-      <c r="AT28" s="94"/>
-      <c r="AU28" s="94"/>
-      <c r="AV28" s="94"/>
-      <c r="AW28" s="94"/>
-      <c r="AX28" s="94"/>
-      <c r="AY28" s="94"/>
-      <c r="AZ28" s="94"/>
-    </row>
-    <row r="29" spans="1:52" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AA28" s="103"/>
+      <c r="AK28" s="103"/>
+      <c r="AQ28" s="103"/>
+      <c r="AR28" s="103"/>
+      <c r="AS28" s="103"/>
+      <c r="AT28" s="103"/>
+      <c r="AU28" s="103"/>
+      <c r="AV28" s="103"/>
+      <c r="AW28" s="103"/>
+      <c r="AX28" s="103"/>
+      <c r="AY28" s="103"/>
+    </row>
+    <row r="29" spans="1:51" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="18" t="s">
         <v>86</v>
       </c>
       <c r="B29" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C29" s="6">
+      <c r="C29" s="94">
         <v>1</v>
       </c>
-      <c r="D29" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="J29" s="94"/>
-      <c r="K29" s="94"/>
-      <c r="L29" s="94"/>
-      <c r="M29" s="94"/>
-      <c r="N29" s="94"/>
-      <c r="O29" s="94"/>
-      <c r="P29" s="94"/>
-      <c r="Q29" s="94"/>
-      <c r="R29" s="94"/>
-      <c r="S29" s="94"/>
-      <c r="T29" s="94"/>
-      <c r="U29" s="94"/>
-      <c r="V29" s="94"/>
-      <c r="W29" s="94"/>
-      <c r="X29" s="94"/>
-      <c r="Y29" s="94"/>
-      <c r="Z29" s="94"/>
-      <c r="AA29" s="94"/>
-      <c r="AB29" s="94"/>
-      <c r="AC29" s="94"/>
-      <c r="AD29" s="94"/>
-      <c r="AE29" s="94"/>
-      <c r="AF29" s="94"/>
-      <c r="AG29" s="94"/>
-      <c r="AH29" s="94"/>
-      <c r="AI29" s="94"/>
-      <c r="AJ29" s="94"/>
-      <c r="AK29" s="94"/>
-      <c r="AL29" s="94"/>
-      <c r="AM29" s="94"/>
-      <c r="AN29" s="94"/>
-      <c r="AO29" s="94"/>
-      <c r="AP29" s="94"/>
-      <c r="AQ29" s="94"/>
-      <c r="AR29" s="94"/>
-      <c r="AS29" s="94"/>
-      <c r="AT29" s="94"/>
-      <c r="AU29" s="94"/>
-      <c r="AV29" s="94"/>
-      <c r="AW29" s="94"/>
-      <c r="AX29" s="94"/>
-      <c r="AY29" s="94"/>
-      <c r="AZ29" s="94"/>
-    </row>
-    <row r="30" spans="1:52" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I29" s="103"/>
+      <c r="J29" s="103"/>
+      <c r="K29" s="103"/>
+      <c r="L29" s="103"/>
+      <c r="M29" s="103"/>
+      <c r="N29" s="103"/>
+      <c r="O29" s="103"/>
+      <c r="P29" s="103"/>
+      <c r="Q29" s="103"/>
+      <c r="R29" s="103"/>
+      <c r="S29" s="103"/>
+      <c r="T29" s="103"/>
+      <c r="U29" s="103"/>
+      <c r="V29" s="103"/>
+      <c r="W29" s="103"/>
+      <c r="X29" s="103"/>
+      <c r="Y29" s="103"/>
+      <c r="Z29" s="103"/>
+      <c r="AA29" s="103"/>
+      <c r="AB29" s="103"/>
+      <c r="AC29" s="103"/>
+      <c r="AD29" s="103"/>
+      <c r="AE29" s="103"/>
+      <c r="AF29" s="103"/>
+      <c r="AG29" s="103"/>
+      <c r="AH29" s="103"/>
+      <c r="AI29" s="103"/>
+      <c r="AJ29" s="103"/>
+      <c r="AK29" s="103"/>
+      <c r="AL29" s="103"/>
+      <c r="AM29" s="103"/>
+      <c r="AN29" s="103"/>
+      <c r="AO29" s="103"/>
+      <c r="AP29" s="103"/>
+      <c r="AQ29" s="103"/>
+      <c r="AR29" s="103"/>
+      <c r="AS29" s="103"/>
+      <c r="AT29" s="103"/>
+      <c r="AU29" s="103"/>
+      <c r="AV29" s="103"/>
+      <c r="AW29" s="103"/>
+      <c r="AX29" s="103"/>
+      <c r="AY29" s="103"/>
+    </row>
+    <row r="30" spans="1:51" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="18" t="s">
         <v>87</v>
       </c>
       <c r="B30" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C30" s="6">
+      <c r="C30" s="94">
         <v>1</v>
       </c>
-      <c r="D30" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="31" spans="1:52" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:51" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="18" t="s">
         <v>88</v>
       </c>
       <c r="B31" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C31" s="6">
+      <c r="C31" s="94">
         <v>1</v>
       </c>
-      <c r="D31" s="6" t="s">
-        <v>13</v>
-      </c>
     </row>
   </sheetData>
-  <dataValidations xWindow="343" yWindow="238" count="4">
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E26:BC26 E16:BC16 E14:BC14 E12:BC12 E10:BC10 E24:BC24 E22:BC22 E20:BC20 E18:BC18 E8:BC8 E6:BC6 E4:BC4 E2:BC2">
+  <dataValidations xWindow="343" yWindow="238" count="3">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D26:BB26 D16:BB16 D14:BB14 D12:BB12 D10:BB10 D24:BB24 D22:BB22 D20:BB20 D18:BB18 D8:BB8 D6:BB6 D4:BB4 D2:BB2">
       <formula1>0</formula1>
       <formula2>100</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E27:BC27 E25:BC25 E23:BC23 E21:BC21 E19:BC19 E17:BC17 E15:BC15 E13:BC13 E11:BC11 E9:BC9 E7:BC7 E5:BC5 E3:BC3">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D27:BB27 D25:BB25 D23:BB23 D21:BB21 D19:BB19 D17:BB17 D15:BB15 D13:BB13 D11:BB11 D9:BB9 D7:BB7 D5:BB5 D3:BB3">
       <formula1>0</formula1>
       <formula2>100000000000000000000</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Smoothness for fitting function" prompt="Must be positive." sqref="C2:C1048576">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Smoothness for fitting function" prompt="Must be positive." sqref="C1:C1048576">
       <formula1>0</formula1>
       <formula2>100</formula2>
     </dataValidation>
-    <dataValidation allowBlank="1" showErrorMessage="1" sqref="C1 D1"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xWindow="343" yWindow="238" count="2">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xWindow="343" yWindow="238" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>dropdown_lists!$A$2:$A$4</xm:f>
           </x14:formula1>
           <xm:sqref>B2:B27</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Time-variant?" prompt="If no, the most recent value will be selected.">
-          <x14:formula1>
-            <xm:f>dropdown_lists!$A$2:$A$4</xm:f>
-          </x14:formula1>
-          <xm:sqref>D2:D1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Revert "Revert "Time-variant choice for parameters""
This reverts commit 048b93f8c606af0acb698dde72f1c317a44ca075.
</commit_message>
<xml_diff>
--- a/autumn/xls/programs_fiji.xlsx
+++ b/autumn/xls/programs_fiji.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="90">
   <si>
     <t>program_rate_restart_presenting</t>
   </si>
@@ -284,6 +284,9 @@
   </si>
   <si>
     <t>tb_prop_smearneg</t>
+  </si>
+  <si>
+    <t>time_variant</t>
   </si>
 </sst>
 </file>
@@ -1348,7 +1351,7 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="104">
+  <cellXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1447,15 +1450,6 @@
     <xf numFmtId="0" fontId="0" fillId="13" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="664">
@@ -2868,229 +2862,234 @@
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:BB31"/>
+  <dimension ref="A1:BC31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J30" sqref="J30"/>
+      <selection pane="bottomRight" activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="47.42578125" style="24" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11" style="102" customWidth="1"/>
-    <col min="4" max="4" width="7.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7" style="1" customWidth="1"/>
-    <col min="7" max="8" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.42578125" style="1" customWidth="1"/>
-    <col min="10" max="11" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.7109375" style="1" customWidth="1"/>
-    <col min="13" max="16" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="7.28515625" style="1" customWidth="1"/>
-    <col min="18" max="21" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="23" width="7.42578125" style="1" customWidth="1"/>
-    <col min="24" max="24" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="7.140625" style="1" customWidth="1"/>
-    <col min="26" max="37" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="8" style="1" customWidth="1"/>
-    <col min="39" max="45" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="8" style="1" customWidth="1"/>
-    <col min="47" max="47" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="6.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="49" max="50" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="7.85546875" style="1" customWidth="1"/>
-    <col min="52" max="52" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="53" max="16384" width="9.140625" style="1"/>
+    <col min="3" max="4" width="11" style="2" customWidth="1"/>
+    <col min="5" max="5" width="7.42578125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7" style="1" customWidth="1"/>
+    <col min="8" max="9" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.42578125" style="1" customWidth="1"/>
+    <col min="11" max="12" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.7109375" style="1" customWidth="1"/>
+    <col min="14" max="17" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="7.28515625" style="1" customWidth="1"/>
+    <col min="19" max="22" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="24" width="7.42578125" style="1" customWidth="1"/>
+    <col min="25" max="25" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="7.140625" style="1" customWidth="1"/>
+    <col min="27" max="38" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="8" style="1" customWidth="1"/>
+    <col min="40" max="46" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="8" style="1" customWidth="1"/>
+    <col min="48" max="48" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="6.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="50" max="51" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="7.85546875" style="1" customWidth="1"/>
+    <col min="53" max="53" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="54" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:55" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="D1" s="5">
+      <c r="D1" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1" s="5">
         <v>1920</v>
       </c>
-      <c r="E1" s="5">
+      <c r="F1" s="5">
         <v>1930</v>
       </c>
-      <c r="F1" s="5">
+      <c r="G1" s="5">
         <v>1940</v>
       </c>
-      <c r="G1" s="5">
+      <c r="H1" s="5">
         <v>1950</v>
       </c>
-      <c r="H1" s="5">
+      <c r="I1" s="5">
         <v>1955</v>
       </c>
-      <c r="I1" s="5">
+      <c r="J1" s="5">
         <v>1960</v>
       </c>
-      <c r="J1" s="5">
+      <c r="K1" s="5">
         <v>1965</v>
       </c>
-      <c r="K1" s="5">
+      <c r="L1" s="5">
         <v>1970</v>
       </c>
-      <c r="L1" s="5">
+      <c r="M1" s="5">
         <v>1975</v>
       </c>
-      <c r="M1" s="5">
+      <c r="N1" s="5">
         <v>1976</v>
       </c>
-      <c r="N1" s="5">
+      <c r="O1" s="5">
         <v>1977</v>
       </c>
-      <c r="O1" s="5">
+      <c r="P1" s="5">
         <v>1978</v>
       </c>
-      <c r="P1" s="5">
+      <c r="Q1" s="5">
         <v>1979</v>
       </c>
-      <c r="Q1" s="5">
+      <c r="R1" s="5">
         <v>1980</v>
       </c>
-      <c r="R1" s="5">
+      <c r="S1" s="5">
         <v>1981</v>
       </c>
-      <c r="S1" s="5">
+      <c r="T1" s="5">
         <v>1982</v>
       </c>
-      <c r="T1" s="5">
+      <c r="U1" s="5">
         <v>1983</v>
       </c>
-      <c r="U1" s="5">
+      <c r="V1" s="5">
         <v>1984</v>
       </c>
-      <c r="V1" s="5">
+      <c r="W1" s="5">
         <v>1985</v>
       </c>
-      <c r="W1" s="5">
+      <c r="X1" s="5">
         <v>1986</v>
       </c>
-      <c r="X1" s="5">
+      <c r="Y1" s="5">
         <v>1987</v>
       </c>
-      <c r="Y1" s="5">
+      <c r="Z1" s="5">
         <v>1988</v>
       </c>
-      <c r="Z1" s="5">
+      <c r="AA1" s="5">
         <v>1989</v>
       </c>
-      <c r="AA1" s="5">
+      <c r="AB1" s="5">
         <v>1990</v>
       </c>
-      <c r="AB1" s="5">
+      <c r="AC1" s="5">
         <v>1991</v>
       </c>
-      <c r="AC1" s="5">
+      <c r="AD1" s="5">
         <v>1992</v>
       </c>
-      <c r="AD1" s="5">
+      <c r="AE1" s="5">
         <v>1993</v>
       </c>
-      <c r="AE1" s="5">
+      <c r="AF1" s="5">
         <v>1994</v>
       </c>
-      <c r="AF1" s="5">
+      <c r="AG1" s="5">
         <v>1995</v>
       </c>
-      <c r="AG1" s="5">
+      <c r="AH1" s="5">
         <v>1996</v>
       </c>
-      <c r="AH1" s="5">
+      <c r="AI1" s="5">
         <v>1997</v>
       </c>
-      <c r="AI1" s="5">
+      <c r="AJ1" s="5">
         <v>1998</v>
       </c>
-      <c r="AJ1" s="5">
+      <c r="AK1" s="5">
         <v>1999</v>
       </c>
-      <c r="AK1" s="5">
+      <c r="AL1" s="5">
         <v>2000</v>
       </c>
-      <c r="AL1" s="5">
+      <c r="AM1" s="5">
         <v>2001</v>
       </c>
-      <c r="AM1" s="5">
+      <c r="AN1" s="5">
         <v>2002</v>
       </c>
-      <c r="AN1" s="5">
+      <c r="AO1" s="5">
         <v>2003</v>
       </c>
-      <c r="AO1" s="5">
+      <c r="AP1" s="5">
         <v>2004</v>
       </c>
-      <c r="AP1" s="5">
+      <c r="AQ1" s="5">
         <v>2005</v>
       </c>
-      <c r="AQ1" s="5">
+      <c r="AR1" s="5">
         <v>2006</v>
       </c>
-      <c r="AR1" s="5">
+      <c r="AS1" s="5">
         <v>2007</v>
       </c>
-      <c r="AS1" s="5">
+      <c r="AT1" s="5">
         <v>2008</v>
       </c>
-      <c r="AT1" s="5">
+      <c r="AU1" s="5">
         <v>2009</v>
       </c>
-      <c r="AU1" s="5">
+      <c r="AV1" s="5">
         <v>2010</v>
       </c>
-      <c r="AV1" s="5">
+      <c r="AW1" s="5">
         <v>2011</v>
       </c>
-      <c r="AW1" s="5">
+      <c r="AX1" s="5">
         <v>2012</v>
       </c>
-      <c r="AX1" s="5">
+      <c r="AY1" s="5">
         <v>2013</v>
       </c>
-      <c r="AY1" s="5">
+      <c r="AZ1" s="5">
         <v>2014</v>
       </c>
-      <c r="AZ1" s="5">
+      <c r="BA1" s="5">
         <v>2015</v>
       </c>
-      <c r="BA1" s="5" t="s">
+      <c r="BB1" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="BB1" s="5" t="s">
+      <c r="BC1" s="5" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:54" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:55" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="94">
+      <c r="C2" s="6">
         <v>1</v>
       </c>
-      <c r="G2" s="7">
+      <c r="D2" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="7">
         <v>0</v>
       </c>
-      <c r="I2" s="7">
+      <c r="J2" s="7">
         <v>25</v>
       </c>
-      <c r="L2" s="7">
+      <c r="M2" s="7">
         <v>40</v>
       </c>
-      <c r="Q2" s="28"/>
       <c r="R2" s="28"/>
       <c r="S2" s="28"/>
       <c r="T2" s="28"/>
@@ -3125,54 +3124,60 @@
       <c r="AW2" s="28"/>
       <c r="AX2" s="28"/>
       <c r="AY2" s="28"/>
-      <c r="BA2" s="7">
-        <v>99</v>
-      </c>
+      <c r="AZ2" s="28"/>
       <c r="BB2" s="7">
         <v>99</v>
       </c>
-    </row>
-    <row r="3" spans="1:54" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="BC2" s="7">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:55" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
         <v>17</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="94"/>
-      <c r="G3" s="7">
+      <c r="C3" s="6"/>
+      <c r="D3" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" s="7">
         <v>0</v>
       </c>
-      <c r="I3" s="7">
+      <c r="J3" s="7">
         <v>10000000</v>
       </c>
-      <c r="L3" s="7">
+      <c r="M3" s="7">
         <v>15040500</v>
       </c>
-      <c r="V3" s="7">
+      <c r="W3" s="7">
         <v>39034561</v>
       </c>
     </row>
-    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:55" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="19" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="95">
+      <c r="C4" s="8">
         <v>5</v>
       </c>
-      <c r="E4" s="9">
+      <c r="D4" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="9">
         <v>0</v>
       </c>
-      <c r="J4" s="9">
+      <c r="K4" s="9">
         <v>10</v>
       </c>
-      <c r="S4" s="9">
+      <c r="T4" s="9">
         <v>30</v>
       </c>
-      <c r="AA4" s="29"/>
       <c r="AB4" s="29"/>
       <c r="AC4" s="29"/>
       <c r="AD4" s="29"/>
@@ -3197,185 +3202,215 @@
       <c r="AW4" s="29"/>
       <c r="AX4" s="29"/>
       <c r="AY4" s="29"/>
-      <c r="BA4" s="9">
+      <c r="AZ4" s="29"/>
+      <c r="BB4" s="9">
         <v>70</v>
       </c>
-      <c r="BB4" s="9">
+      <c r="BC4" s="9">
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:55" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
         <v>18</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="95"/>
-      <c r="E5" s="9">
+      <c r="C5" s="8"/>
+      <c r="D5" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" s="9">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:54" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:55" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="96">
+      <c r="C6" s="10">
         <v>1</v>
       </c>
-      <c r="F6" s="11">
+      <c r="D6" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="11">
         <v>70</v>
       </c>
-      <c r="I6" s="11">
+      <c r="J6" s="11">
         <v>80</v>
       </c>
-      <c r="Y6" s="11">
+      <c r="Z6" s="11">
         <v>82</v>
       </c>
-      <c r="AL6" s="11">
+      <c r="AM6" s="11">
         <v>84</v>
       </c>
-      <c r="AY6" s="11">
-        <v>85</v>
-      </c>
-      <c r="BA6" s="11">
+      <c r="AZ6" s="11">
         <v>85</v>
       </c>
       <c r="BB6" s="11">
         <v>85</v>
       </c>
-    </row>
-    <row r="7" spans="1:54" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="BC6" s="11">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="7" spans="1:55" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
         <v>19</v>
       </c>
       <c r="B7" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="96"/>
-      <c r="F7" s="11">
+      <c r="C7" s="10"/>
+      <c r="D7" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="G7" s="11">
         <v>1005000</v>
       </c>
-      <c r="I7" s="11">
+      <c r="J7" s="11">
         <v>2040504</v>
       </c>
-      <c r="Y7" s="11">
+      <c r="Z7" s="11">
         <v>4049504</v>
       </c>
     </row>
-    <row r="8" spans="1:54" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:55" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="21" t="s">
         <v>3</v>
       </c>
       <c r="B8" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="97">
+      <c r="C8" s="12">
         <v>1</v>
       </c>
-      <c r="G8" s="13">
+      <c r="D8" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="H8" s="13">
         <v>30</v>
       </c>
-      <c r="J8" s="13">
+      <c r="K8" s="13">
         <v>40</v>
       </c>
-      <c r="AA8" s="13">
+      <c r="AB8" s="13">
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:54" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:55" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="21" t="s">
         <v>20</v>
       </c>
       <c r="B9" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="97"/>
-    </row>
-    <row r="10" spans="1:54" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C9" s="12"/>
+      <c r="D9" s="12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:55" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="22" t="s">
         <v>11</v>
       </c>
       <c r="B10" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="98">
+      <c r="C10" s="14">
         <v>1</v>
       </c>
-      <c r="Q10" s="15">
+      <c r="D10" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="R10" s="15">
         <v>30</v>
       </c>
-      <c r="AA10" s="15">
+      <c r="AB10" s="15">
         <v>40</v>
       </c>
-      <c r="AK10" s="15">
+      <c r="AL10" s="15">
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:54" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:55" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="22" t="s">
         <v>21</v>
       </c>
       <c r="B11" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="98"/>
-    </row>
-    <row r="12" spans="1:54" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C11" s="14"/>
+      <c r="D11" s="14" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:55" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="23" t="s">
         <v>12</v>
       </c>
       <c r="B12" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="99">
+      <c r="C12" s="16">
         <v>1</v>
       </c>
-      <c r="H12" s="17">
+      <c r="D12" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="I12" s="17">
         <v>7</v>
       </c>
-      <c r="V12" s="17">
+      <c r="W12" s="17">
         <v>0</v>
       </c>
-      <c r="AF12" s="17">
+      <c r="AG12" s="17">
         <v>50</v>
       </c>
-      <c r="AK12" s="17">
+      <c r="AL12" s="17">
         <v>70</v>
       </c>
     </row>
-    <row r="13" spans="1:54" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:55" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="23" t="s">
         <v>22</v>
       </c>
       <c r="B13" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="99"/>
-    </row>
-    <row r="14" spans="1:54" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C13" s="16"/>
+      <c r="D13" s="16" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:55" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="21" t="s">
         <v>24</v>
       </c>
       <c r="B14" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="97">
+      <c r="C14" s="12">
         <v>1</v>
       </c>
-      <c r="H14" s="13">
+      <c r="D14" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="I14" s="13">
         <v>0</v>
       </c>
-      <c r="Q14" s="13">
+      <c r="R14" s="13">
         <v>30</v>
       </c>
-      <c r="W14" s="13">
+      <c r="X14" s="13">
         <v>50</v>
       </c>
-      <c r="AE14" s="30"/>
       <c r="AF14" s="30"/>
       <c r="AG14" s="30"/>
       <c r="AH14" s="30"/>
@@ -3395,57 +3430,63 @@
       <c r="AV14" s="30"/>
       <c r="AW14" s="30"/>
       <c r="AX14" s="30"/>
-      <c r="BA14" s="13">
-        <v>90</v>
-      </c>
+      <c r="AY14" s="30"/>
       <c r="BB14" s="13">
         <v>90</v>
       </c>
-    </row>
-    <row r="15" spans="1:54" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="BC14" s="13">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="15" spans="1:55" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="21" t="s">
         <v>25</v>
       </c>
       <c r="B15" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="C15" s="97"/>
-      <c r="H15" s="13">
+      <c r="C15" s="12"/>
+      <c r="D15" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="I15" s="13">
         <v>0</v>
       </c>
-      <c r="Q15" s="13">
+      <c r="R15" s="13">
         <v>1926492</v>
       </c>
-      <c r="W15" s="13">
+      <c r="X15" s="13">
         <v>4573928</v>
       </c>
-      <c r="AL15" s="13">
+      <c r="AM15" s="13">
         <v>9382947</v>
       </c>
-      <c r="AT15" s="13">
+      <c r="AU15" s="13">
         <v>52431253</v>
       </c>
     </row>
-    <row r="16" spans="1:54" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:55" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="21" t="s">
         <v>26</v>
       </c>
       <c r="B16" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="97">
+      <c r="C16" s="12">
         <v>1</v>
       </c>
-      <c r="H16" s="13">
+      <c r="D16" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="I16" s="13">
         <v>0</v>
       </c>
-      <c r="Q16" s="13">
+      <c r="R16" s="13">
         <v>15</v>
       </c>
-      <c r="W16" s="13">
+      <c r="X16" s="13">
         <v>12</v>
       </c>
-      <c r="AE16" s="30"/>
       <c r="AF16" s="30"/>
       <c r="AG16" s="30"/>
       <c r="AH16" s="30"/>
@@ -3465,42 +3506,48 @@
       <c r="AV16" s="30"/>
       <c r="AW16" s="30"/>
       <c r="AX16" s="30"/>
-      <c r="BA16" s="13">
+      <c r="AY16" s="30"/>
+      <c r="BB16" s="13">
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:51" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:52" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="21" t="s">
         <v>27</v>
       </c>
       <c r="B17" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="C17" s="97"/>
-      <c r="H17" s="13">
+      <c r="C17" s="12"/>
+      <c r="D17" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="I17" s="13">
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:51" s="27" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:52" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="25" t="s">
         <v>28</v>
       </c>
       <c r="B18" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="C18" s="100">
+      <c r="C18" s="26">
         <v>1</v>
       </c>
-      <c r="H18" s="27">
+      <c r="D18" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="I18" s="27">
         <v>0</v>
       </c>
-      <c r="Q18" s="27">
+      <c r="R18" s="27">
         <v>15</v>
       </c>
-      <c r="W18" s="27">
+      <c r="X18" s="27">
         <v>30</v>
       </c>
-      <c r="AE18" s="31"/>
       <c r="AF18" s="31"/>
       <c r="AG18" s="31"/>
       <c r="AH18" s="31"/>
@@ -3520,54 +3567,60 @@
       <c r="AV18" s="31"/>
       <c r="AW18" s="31"/>
       <c r="AX18" s="31"/>
-      <c r="AY18" s="27">
+      <c r="AY18" s="31"/>
+      <c r="AZ18" s="27">
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="1:51" s="27" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:52" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="25" t="s">
         <v>29</v>
       </c>
       <c r="B19" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="C19" s="100"/>
-      <c r="H19" s="27">
+      <c r="C19" s="26"/>
+      <c r="D19" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="I19" s="27">
         <v>0</v>
       </c>
-      <c r="Q19" s="27">
+      <c r="R19" s="27">
         <v>492549</v>
       </c>
-      <c r="W19" s="27">
+      <c r="X19" s="27">
         <v>256491</v>
       </c>
-      <c r="AL19" s="27">
+      <c r="AM19" s="27">
         <v>9382947</v>
       </c>
-      <c r="AT19" s="27">
+      <c r="AU19" s="27">
         <v>52431253</v>
       </c>
     </row>
-    <row r="20" spans="1:51" s="27" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:52" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="25" t="s">
         <v>30</v>
       </c>
       <c r="B20" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="C20" s="100">
+      <c r="C20" s="26">
         <v>1</v>
       </c>
-      <c r="H20" s="27">
+      <c r="D20" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="I20" s="27">
         <v>0</v>
       </c>
-      <c r="Q20" s="27">
+      <c r="R20" s="27">
         <v>55</v>
       </c>
-      <c r="W20" s="27">
+      <c r="X20" s="27">
         <v>50</v>
       </c>
-      <c r="AE20" s="31"/>
       <c r="AF20" s="31"/>
       <c r="AG20" s="31"/>
       <c r="AH20" s="31"/>
@@ -3587,42 +3640,48 @@
       <c r="AV20" s="31"/>
       <c r="AW20" s="31"/>
       <c r="AX20" s="31"/>
-      <c r="AY20" s="27">
+      <c r="AY20" s="31"/>
+      <c r="AZ20" s="27">
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:51" s="27" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:52" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="25" t="s">
         <v>31</v>
       </c>
       <c r="B21" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="C21" s="100"/>
-      <c r="H21" s="27">
+      <c r="C21" s="26"/>
+      <c r="D21" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="I21" s="27">
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:51" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:52" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="19" t="s">
         <v>32</v>
       </c>
       <c r="B22" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C22" s="95">
+      <c r="C22" s="8">
         <v>1</v>
       </c>
-      <c r="H22" s="9">
+      <c r="D22" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I22" s="9">
         <v>0</v>
       </c>
-      <c r="Q22" s="9">
+      <c r="R22" s="9">
         <v>5</v>
       </c>
-      <c r="W22" s="9">
+      <c r="X22" s="9">
         <v>15</v>
       </c>
-      <c r="AE22" s="29"/>
       <c r="AF22" s="29"/>
       <c r="AG22" s="29"/>
       <c r="AH22" s="29"/>
@@ -3642,54 +3701,60 @@
       <c r="AV22" s="29"/>
       <c r="AW22" s="29"/>
       <c r="AX22" s="29"/>
-      <c r="AY22" s="9">
+      <c r="AY22" s="29"/>
+      <c r="AZ22" s="9">
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="1:51" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:52" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="19" t="s">
         <v>33</v>
       </c>
       <c r="B23" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C23" s="95"/>
-      <c r="H23" s="9">
+      <c r="C23" s="8"/>
+      <c r="D23" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="I23" s="9">
         <v>0</v>
       </c>
-      <c r="Q23" s="9">
+      <c r="R23" s="9">
         <v>0</v>
       </c>
-      <c r="W23" s="9">
+      <c r="X23" s="9">
         <v>0</v>
       </c>
-      <c r="AL23" s="9">
+      <c r="AM23" s="9">
         <v>0</v>
       </c>
-      <c r="AT23" s="9">
+      <c r="AU23" s="9">
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:51" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:52" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="19" t="s">
         <v>34</v>
       </c>
       <c r="B24" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C24" s="95">
+      <c r="C24" s="8">
         <v>1</v>
       </c>
-      <c r="H24" s="9">
+      <c r="D24" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I24" s="9">
         <v>0</v>
       </c>
-      <c r="Q24" s="9">
+      <c r="R24" s="9">
         <v>65</v>
       </c>
-      <c r="W24" s="9">
+      <c r="X24" s="9">
         <v>62</v>
       </c>
-      <c r="AE24" s="29"/>
       <c r="AF24" s="29"/>
       <c r="AG24" s="29"/>
       <c r="AH24" s="29"/>
@@ -3709,37 +3774,43 @@
       <c r="AV24" s="29"/>
       <c r="AW24" s="29"/>
       <c r="AX24" s="29"/>
-      <c r="AY24" s="9">
+      <c r="AY24" s="29"/>
+      <c r="AZ24" s="9">
         <v>35</v>
       </c>
     </row>
-    <row r="25" spans="1:51" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:52" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="19" t="s">
         <v>35</v>
       </c>
       <c r="B25" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C25" s="95"/>
-      <c r="H25" s="9">
+      <c r="C25" s="8"/>
+      <c r="D25" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="I25" s="9">
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:51" s="86" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:52" s="86" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="84" t="s">
         <v>67</v>
       </c>
       <c r="B26" s="85" t="s">
         <v>13</v>
       </c>
-      <c r="C26" s="101">
+      <c r="C26" s="85">
         <v>1</v>
       </c>
-      <c r="D26" s="86">
+      <c r="D26" s="85" t="s">
+        <v>13</v>
+      </c>
+      <c r="E26" s="86">
         <f>1/26</f>
         <v>3.8461538461538464E-2</v>
       </c>
-      <c r="AE26" s="87"/>
       <c r="AF26" s="87"/>
       <c r="AG26" s="87"/>
       <c r="AH26" s="87"/>
@@ -3759,154 +3830,177 @@
       <c r="AV26" s="87"/>
       <c r="AW26" s="87"/>
       <c r="AX26" s="87"/>
-      <c r="AY26" s="86">
+      <c r="AY26" s="87"/>
+      <c r="AZ26" s="86">
         <v>0.04</v>
       </c>
     </row>
-    <row r="27" spans="1:51" s="86" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:52" s="86" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="84" t="s">
         <v>68</v>
       </c>
       <c r="B27" s="85" t="s">
         <v>23</v>
       </c>
-      <c r="C27" s="101"/>
-      <c r="H27" s="86">
+      <c r="C27" s="85"/>
+      <c r="D27" s="85" t="s">
+        <v>23</v>
+      </c>
+      <c r="I27" s="86">
         <v>0</v>
       </c>
-      <c r="Q27" s="86">
+      <c r="R27" s="86">
         <v>532947</v>
       </c>
-      <c r="W27" s="86">
+      <c r="X27" s="86">
         <v>9283747</v>
       </c>
-      <c r="AY27" s="86">
+      <c r="AZ27" s="86">
         <v>739284639</v>
       </c>
     </row>
-    <row r="28" spans="1:51" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:52" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="18" t="s">
         <v>85</v>
       </c>
       <c r="B28" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C28" s="94">
+      <c r="C28" s="6">
         <v>1</v>
       </c>
-      <c r="AA28" s="103"/>
-      <c r="AK28" s="103"/>
-      <c r="AQ28" s="103"/>
-      <c r="AR28" s="103"/>
-      <c r="AS28" s="103"/>
-      <c r="AT28" s="103"/>
-      <c r="AU28" s="103"/>
-      <c r="AV28" s="103"/>
-      <c r="AW28" s="103"/>
-      <c r="AX28" s="103"/>
-      <c r="AY28" s="103"/>
-    </row>
-    <row r="29" spans="1:51" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D28" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="AB28" s="94"/>
+      <c r="AL28" s="94"/>
+      <c r="AR28" s="94"/>
+      <c r="AS28" s="94"/>
+      <c r="AT28" s="94"/>
+      <c r="AU28" s="94"/>
+      <c r="AV28" s="94"/>
+      <c r="AW28" s="94"/>
+      <c r="AX28" s="94"/>
+      <c r="AY28" s="94"/>
+      <c r="AZ28" s="94"/>
+    </row>
+    <row r="29" spans="1:52" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="18" t="s">
         <v>86</v>
       </c>
       <c r="B29" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C29" s="94">
+      <c r="C29" s="6">
         <v>1</v>
       </c>
-      <c r="I29" s="103"/>
-      <c r="J29" s="103"/>
-      <c r="K29" s="103"/>
-      <c r="L29" s="103"/>
-      <c r="M29" s="103"/>
-      <c r="N29" s="103"/>
-      <c r="O29" s="103"/>
-      <c r="P29" s="103"/>
-      <c r="Q29" s="103"/>
-      <c r="R29" s="103"/>
-      <c r="S29" s="103"/>
-      <c r="T29" s="103"/>
-      <c r="U29" s="103"/>
-      <c r="V29" s="103"/>
-      <c r="W29" s="103"/>
-      <c r="X29" s="103"/>
-      <c r="Y29" s="103"/>
-      <c r="Z29" s="103"/>
-      <c r="AA29" s="103"/>
-      <c r="AB29" s="103"/>
-      <c r="AC29" s="103"/>
-      <c r="AD29" s="103"/>
-      <c r="AE29" s="103"/>
-      <c r="AF29" s="103"/>
-      <c r="AG29" s="103"/>
-      <c r="AH29" s="103"/>
-      <c r="AI29" s="103"/>
-      <c r="AJ29" s="103"/>
-      <c r="AK29" s="103"/>
-      <c r="AL29" s="103"/>
-      <c r="AM29" s="103"/>
-      <c r="AN29" s="103"/>
-      <c r="AO29" s="103"/>
-      <c r="AP29" s="103"/>
-      <c r="AQ29" s="103"/>
-      <c r="AR29" s="103"/>
-      <c r="AS29" s="103"/>
-      <c r="AT29" s="103"/>
-      <c r="AU29" s="103"/>
-      <c r="AV29" s="103"/>
-      <c r="AW29" s="103"/>
-      <c r="AX29" s="103"/>
-      <c r="AY29" s="103"/>
-    </row>
-    <row r="30" spans="1:51" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D29" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="J29" s="94"/>
+      <c r="K29" s="94"/>
+      <c r="L29" s="94"/>
+      <c r="M29" s="94"/>
+      <c r="N29" s="94"/>
+      <c r="O29" s="94"/>
+      <c r="P29" s="94"/>
+      <c r="Q29" s="94"/>
+      <c r="R29" s="94"/>
+      <c r="S29" s="94"/>
+      <c r="T29" s="94"/>
+      <c r="U29" s="94"/>
+      <c r="V29" s="94"/>
+      <c r="W29" s="94"/>
+      <c r="X29" s="94"/>
+      <c r="Y29" s="94"/>
+      <c r="Z29" s="94"/>
+      <c r="AA29" s="94"/>
+      <c r="AB29" s="94"/>
+      <c r="AC29" s="94"/>
+      <c r="AD29" s="94"/>
+      <c r="AE29" s="94"/>
+      <c r="AF29" s="94"/>
+      <c r="AG29" s="94"/>
+      <c r="AH29" s="94"/>
+      <c r="AI29" s="94"/>
+      <c r="AJ29" s="94"/>
+      <c r="AK29" s="94"/>
+      <c r="AL29" s="94"/>
+      <c r="AM29" s="94"/>
+      <c r="AN29" s="94"/>
+      <c r="AO29" s="94"/>
+      <c r="AP29" s="94"/>
+      <c r="AQ29" s="94"/>
+      <c r="AR29" s="94"/>
+      <c r="AS29" s="94"/>
+      <c r="AT29" s="94"/>
+      <c r="AU29" s="94"/>
+      <c r="AV29" s="94"/>
+      <c r="AW29" s="94"/>
+      <c r="AX29" s="94"/>
+      <c r="AY29" s="94"/>
+      <c r="AZ29" s="94"/>
+    </row>
+    <row r="30" spans="1:52" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="18" t="s">
         <v>87</v>
       </c>
       <c r="B30" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C30" s="94">
+      <c r="C30" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:51" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D30" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="31" spans="1:52" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="18" t="s">
         <v>88</v>
       </c>
       <c r="B31" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C31" s="94">
+      <c r="C31" s="6">
         <v>1</v>
       </c>
+      <c r="D31" s="6" t="s">
+        <v>13</v>
+      </c>
     </row>
   </sheetData>
-  <dataValidations xWindow="343" yWindow="238" count="3">
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D26:BB26 D16:BB16 D14:BB14 D12:BB12 D10:BB10 D24:BB24 D22:BB22 D20:BB20 D18:BB18 D8:BB8 D6:BB6 D4:BB4 D2:BB2">
+  <dataValidations xWindow="343" yWindow="238" count="4">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E26:BC26 E16:BC16 E14:BC14 E12:BC12 E10:BC10 E24:BC24 E22:BC22 E20:BC20 E18:BC18 E8:BC8 E6:BC6 E4:BC4 E2:BC2">
       <formula1>0</formula1>
       <formula2>100</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D27:BB27 D25:BB25 D23:BB23 D21:BB21 D19:BB19 D17:BB17 D15:BB15 D13:BB13 D11:BB11 D9:BB9 D7:BB7 D5:BB5 D3:BB3">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E27:BC27 E25:BC25 E23:BC23 E21:BC21 E19:BC19 E17:BC17 E15:BC15 E13:BC13 E11:BC11 E9:BC9 E7:BC7 E5:BC5 E3:BC3">
       <formula1>0</formula1>
       <formula2>100000000000000000000</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Smoothness for fitting function" prompt="Must be positive." sqref="C1:C1048576">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Smoothness for fitting function" prompt="Must be positive." sqref="C2:C1048576">
       <formula1>0</formula1>
       <formula2>100</formula2>
     </dataValidation>
+    <dataValidation allowBlank="1" showErrorMessage="1" sqref="C1 D1"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xWindow="343" yWindow="238" count="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xWindow="343" yWindow="238" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>dropdown_lists!$A$2:$A$4</xm:f>
           </x14:formula1>
           <xm:sqref>B2:B27</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Time-variant?" prompt="If no, the most recent value will be selected.">
+          <x14:formula1>
+            <xm:f>dropdown_lists!$A$2:$A$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>D2:D1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Revert "Revert "Updated the code to reflect James' changes in spreadsheet.py""
This reverts commit d04d1f5477089e4a38600657b887104345c9d869.
</commit_message>
<xml_diff>
--- a/autumn/xls/programs_fiji.xlsx
+++ b/autumn/xls/programs_fiji.xlsx
@@ -2868,7 +2868,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D32" sqref="D32"/>
+      <selection pane="bottomRight" activeCell="Q43" sqref="Q43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3096,7 +3096,9 @@
       <c r="U2" s="28"/>
       <c r="V2" s="28"/>
       <c r="W2" s="28"/>
-      <c r="X2" s="28"/>
+      <c r="X2" s="28">
+        <v>1</v>
+      </c>
       <c r="Y2" s="28"/>
       <c r="Z2" s="28"/>
       <c r="AA2" s="28"/>
@@ -3155,6 +3157,9 @@
       <c r="W3" s="7">
         <v>39034561</v>
       </c>
+      <c r="X3" s="7">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="1:55" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="19" t="s">
@@ -3177,6 +3182,9 @@
       </c>
       <c r="T4" s="9">
         <v>30</v>
+      </c>
+      <c r="X4" s="9">
+        <v>1</v>
       </c>
       <c r="AB4" s="29"/>
       <c r="AC4" s="29"/>
@@ -3224,6 +3232,9 @@
       <c r="F5" s="9">
         <v>0</v>
       </c>
+      <c r="X5" s="9">
+        <v>1</v>
+      </c>
     </row>
     <row r="6" spans="1:55" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
@@ -3244,6 +3255,9 @@
       <c r="J6" s="11">
         <v>80</v>
       </c>
+      <c r="X6" s="11">
+        <v>1</v>
+      </c>
       <c r="Z6" s="11">
         <v>82</v>
       </c>
@@ -3277,6 +3291,9 @@
       <c r="J7" s="11">
         <v>2040504</v>
       </c>
+      <c r="X7" s="11">
+        <v>1</v>
+      </c>
       <c r="Z7" s="11">
         <v>4049504</v>
       </c>
@@ -3300,6 +3317,9 @@
       <c r="K8" s="13">
         <v>40</v>
       </c>
+      <c r="X8" s="13">
+        <v>1</v>
+      </c>
       <c r="AB8" s="13">
         <v>40</v>
       </c>
@@ -3315,6 +3335,9 @@
       <c r="D9" s="12" t="s">
         <v>23</v>
       </c>
+      <c r="X9" s="13">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" spans="1:55" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="22" t="s">
@@ -3332,6 +3355,9 @@
       <c r="R10" s="15">
         <v>30</v>
       </c>
+      <c r="X10" s="15">
+        <v>1</v>
+      </c>
       <c r="AB10" s="15">
         <v>40</v>
       </c>
@@ -3350,6 +3376,9 @@
       <c r="D11" s="14" t="s">
         <v>23</v>
       </c>
+      <c r="X11" s="15">
+        <v>1</v>
+      </c>
     </row>
     <row r="12" spans="1:55" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="23" t="s">
@@ -3370,6 +3399,9 @@
       <c r="W12" s="17">
         <v>0</v>
       </c>
+      <c r="X12" s="17">
+        <v>1</v>
+      </c>
       <c r="AG12" s="17">
         <v>50</v>
       </c>
@@ -3387,6 +3419,9 @@
       <c r="C13" s="16"/>
       <c r="D13" s="16" t="s">
         <v>23</v>
+      </c>
+      <c r="X13" s="17">
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:55" s="13" customFormat="1" x14ac:dyDescent="0.25">
@@ -3525,6 +3560,9 @@
       <c r="I17" s="13">
         <v>0</v>
       </c>
+      <c r="X17" s="13">
+        <v>1</v>
+      </c>
     </row>
     <row r="18" spans="1:52" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="25" t="s">
@@ -3659,6 +3697,9 @@
       <c r="I21" s="27">
         <v>0</v>
       </c>
+      <c r="X21" s="27">
+        <v>1</v>
+      </c>
     </row>
     <row r="22" spans="1:52" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="19" t="s">
@@ -3793,6 +3834,9 @@
       <c r="I25" s="9">
         <v>0</v>
       </c>
+      <c r="X25" s="9">
+        <v>1</v>
+      </c>
     </row>
     <row r="26" spans="1:52" s="86" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="84" t="s">
@@ -3810,6 +3854,9 @@
       <c r="E26" s="86">
         <f>1/26</f>
         <v>3.8461538461538464E-2</v>
+      </c>
+      <c r="X26" s="86">
+        <v>1</v>
       </c>
       <c r="AF26" s="87"/>
       <c r="AG26" s="87"/>

</xml_diff>

<commit_message>
More changes to naming
birth_rate to rate_birth - again for consistency
</commit_message>
<xml_diff>
--- a/autumn/xls/programs_fiji.xlsx
+++ b/autumn/xls/programs_fiji.xlsx
@@ -286,7 +286,7 @@
     <t>demo_life_expectancy</t>
   </si>
   <si>
-    <t>demo_birth_rate</t>
+    <t>demo_rate_birth</t>
   </si>
 </sst>
 </file>
@@ -2868,7 +2868,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A29" sqref="A29"/>
+      <selection pane="bottomRight" activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Allow constant or time-variant births
Now that all potentially time-variant parameter are dealt with the same
way, this is relatively easy.
</commit_message>
<xml_diff>
--- a/autumn/xls/programs_fiji.xlsx
+++ b/autumn/xls/programs_fiji.xlsx
@@ -2737,7 +2737,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2768,7 +2768,7 @@
         <v>7</v>
       </c>
       <c r="B2" s="62">
-        <v>6.5</v>
+        <v>6.7</v>
       </c>
       <c r="C2" s="58" t="s">
         <v>50</v>
@@ -2868,7 +2868,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A30" sqref="A30"/>
+      <selection pane="bottomRight" activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Finished code for demographic scaling
Birth rates can now be time-variant, although death rates can't (which
is something for later - if it's important).
</commit_message>
<xml_diff>
--- a/autumn/xls/programs_fiji.xlsx
+++ b/autumn/xls/programs_fiji.xlsx
@@ -2868,7 +2868,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H26" sqref="H26"/>
+      <selection pane="bottomRight" activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4036,7 +4036,7 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xWindow="343" yWindow="238" count="2">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xWindow="343" yWindow="238" count="3">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>dropdown_lists!$A$2:$A$4</xm:f>
@@ -4047,7 +4047,13 @@
           <x14:formula1>
             <xm:f>dropdown_lists!$A$2:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>D2:D1048576</xm:sqref>
+          <xm:sqref>D2:D27 D29:D1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Cannot be time-variant" prompt="Will work on this later, but currently this must be fixed.">
+          <x14:formula1>
+            <xm:f>dropdown_lists!$A$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>D28</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Allow variable or fixed organ status parameter
</commit_message>
<xml_diff>
--- a/autumn/xls/programs_fiji.xlsx
+++ b/autumn/xls/programs_fiji.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="90">
   <si>
     <t>program_rate_restart_presenting</t>
   </si>
@@ -389,7 +389,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="17">
+  <fills count="18">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -482,6 +482,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1351,7 +1357,7 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="95">
+  <cellXfs count="96">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1451,6 +1457,7 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="664">
     <cellStyle name="Comma 2" xfId="5"/>
@@ -2868,7 +2875,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G20" sqref="G20"/>
+      <selection pane="bottomRight" activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3096,9 +3103,7 @@
       <c r="U2" s="28"/>
       <c r="V2" s="28"/>
       <c r="W2" s="28"/>
-      <c r="X2" s="28">
-        <v>1</v>
-      </c>
+      <c r="X2" s="28"/>
       <c r="Y2" s="28"/>
       <c r="Z2" s="28"/>
       <c r="AA2" s="28"/>
@@ -3142,7 +3147,7 @@
         <v>23</v>
       </c>
       <c r="C3" s="6"/>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="95" t="s">
         <v>23</v>
       </c>
       <c r="H3" s="7">
@@ -3182,9 +3187,6 @@
       </c>
       <c r="T4" s="9">
         <v>30</v>
-      </c>
-      <c r="X4" s="9">
-        <v>1</v>
       </c>
       <c r="AB4" s="29"/>
       <c r="AC4" s="29"/>
@@ -3226,7 +3228,7 @@
         <v>23</v>
       </c>
       <c r="C5" s="8"/>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="95" t="s">
         <v>23</v>
       </c>
       <c r="F5" s="9">
@@ -3255,9 +3257,6 @@
       <c r="J6" s="11">
         <v>80</v>
       </c>
-      <c r="X6" s="11">
-        <v>1</v>
-      </c>
       <c r="Z6" s="11">
         <v>82</v>
       </c>
@@ -3282,7 +3281,7 @@
         <v>23</v>
       </c>
       <c r="C7" s="10"/>
-      <c r="D7" s="10" t="s">
+      <c r="D7" s="95" t="s">
         <v>23</v>
       </c>
       <c r="G7" s="11">
@@ -3317,9 +3316,6 @@
       <c r="K8" s="13">
         <v>40</v>
       </c>
-      <c r="X8" s="13">
-        <v>1</v>
-      </c>
       <c r="AB8" s="13">
         <v>40</v>
       </c>
@@ -3332,7 +3328,7 @@
         <v>23</v>
       </c>
       <c r="C9" s="12"/>
-      <c r="D9" s="12" t="s">
+      <c r="D9" s="95" t="s">
         <v>23</v>
       </c>
       <c r="X9" s="13">
@@ -3355,9 +3351,6 @@
       <c r="R10" s="15">
         <v>30</v>
       </c>
-      <c r="X10" s="15">
-        <v>1</v>
-      </c>
       <c r="AB10" s="15">
         <v>40</v>
       </c>
@@ -3373,7 +3366,7 @@
         <v>23</v>
       </c>
       <c r="C11" s="14"/>
-      <c r="D11" s="14" t="s">
+      <c r="D11" s="95" t="s">
         <v>23</v>
       </c>
       <c r="X11" s="15">
@@ -3399,9 +3392,6 @@
       <c r="W12" s="17">
         <v>0</v>
       </c>
-      <c r="X12" s="17">
-        <v>1</v>
-      </c>
       <c r="AG12" s="17">
         <v>50</v>
       </c>
@@ -3417,7 +3407,7 @@
         <v>23</v>
       </c>
       <c r="C13" s="16"/>
-      <c r="D13" s="16" t="s">
+      <c r="D13" s="95" t="s">
         <v>23</v>
       </c>
       <c r="X13" s="17">
@@ -3481,7 +3471,7 @@
         <v>23</v>
       </c>
       <c r="C15" s="12"/>
-      <c r="D15" s="12" t="s">
+      <c r="D15" s="95" t="s">
         <v>23</v>
       </c>
       <c r="I15" s="13">
@@ -3554,7 +3544,7 @@
         <v>23</v>
       </c>
       <c r="C17" s="12"/>
-      <c r="D17" s="12" t="s">
+      <c r="D17" s="95" t="s">
         <v>23</v>
       </c>
       <c r="I17" s="13">
@@ -3618,7 +3608,7 @@
         <v>23</v>
       </c>
       <c r="C19" s="26"/>
-      <c r="D19" s="26" t="s">
+      <c r="D19" s="95" t="s">
         <v>23</v>
       </c>
       <c r="I19" s="27">
@@ -3691,7 +3681,7 @@
         <v>23</v>
       </c>
       <c r="C21" s="26"/>
-      <c r="D21" s="26" t="s">
+      <c r="D21" s="95" t="s">
         <v>23</v>
       </c>
       <c r="I21" s="27">
@@ -3755,7 +3745,7 @@
         <v>23</v>
       </c>
       <c r="C23" s="8"/>
-      <c r="D23" s="8" t="s">
+      <c r="D23" s="95" t="s">
         <v>23</v>
       </c>
       <c r="I23" s="9">
@@ -3828,7 +3818,7 @@
         <v>23</v>
       </c>
       <c r="C25" s="8"/>
-      <c r="D25" s="8" t="s">
+      <c r="D25" s="95" t="s">
         <v>23</v>
       </c>
       <c r="I25" s="9">
@@ -3854,9 +3844,6 @@
       <c r="E26" s="86">
         <f>1/26</f>
         <v>3.8461538461538464E-2</v>
-      </c>
-      <c r="X26" s="86">
-        <v>1</v>
       </c>
       <c r="AF26" s="87"/>
       <c r="AG26" s="87"/>
@@ -3890,7 +3877,7 @@
         <v>23</v>
       </c>
       <c r="C27" s="85"/>
-      <c r="D27" s="85" t="s">
+      <c r="D27" s="95" t="s">
         <v>23</v>
       </c>
       <c r="I27" s="86">
@@ -3999,7 +3986,7 @@
         <v>1</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="31" spans="1:52" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -4012,8 +3999,9 @@
       <c r="C31" s="6">
         <v>1</v>
       </c>
-      <c r="D31" s="6" t="s">
-        <v>13</v>
+      <c r="D31" s="6" t="str">
+        <f>D30</f>
+        <v>no</v>
       </c>
     </row>
   </sheetData>
@@ -4030,13 +4018,13 @@
       <formula1>0</formula1>
       <formula2>100</formula2>
     </dataValidation>
-    <dataValidation allowBlank="1" showErrorMessage="1" sqref="C1 D1"/>
+    <dataValidation allowBlank="1" showErrorMessage="1" sqref="C1:D1"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xWindow="343" yWindow="238" count="3">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xWindow="343" yWindow="238" count="4">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>dropdown_lists!$A$2:$A$4</xm:f>
@@ -4047,13 +4035,19 @@
           <x14:formula1>
             <xm:f>dropdown_lists!$A$2:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>D2:D27 D29:D1048576</xm:sqref>
+          <xm:sqref>D2:D27 D29:D30 D32:D1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Cannot be time-variant" prompt="Will work on this later, but currently this must be fixed.">
           <x14:formula1>
             <xm:f>dropdown_lists!$A$3</xm:f>
           </x14:formula1>
           <xm:sqref>D28</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Don't enter data here">
+          <x14:formula1>
+            <xm:f>dropdown_lists!$A$2:$A$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>D31</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Adjust infectiousness for organ-unstratified models
Reduce the infectiousness of patients with active disease in models
unstratified by organ status (so that they run a bit more like the ones
that are).
</commit_message>
<xml_diff>
--- a/autumn/xls/programs_fiji.xlsx
+++ b/autumn/xls/programs_fiji.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="315" windowWidth="20370" windowHeight="7530" tabRatio="807" activeTab="2"/>
+    <workbookView xWindow="120" yWindow="315" windowWidth="20370" windowHeight="7530" tabRatio="807"/>
   </bookViews>
   <sheets>
     <sheet name="model_attributes" sheetId="4" r:id="rId1"/>
@@ -2427,8 +2427,8 @@
   </sheetPr>
   <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2871,11 +2871,11 @@
   </sheetPr>
   <dimension ref="A1:BC31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F30" sqref="F30"/>
+      <selection pane="bottomRight" activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3903,7 +3903,7 @@
       <c r="C28" s="6">
         <v>1</v>
       </c>
-      <c r="D28" s="6" t="s">
+      <c r="D28" s="95" t="s">
         <v>14</v>
       </c>
       <c r="AB28" s="94"/>
@@ -3999,7 +3999,7 @@
       <c r="C31" s="6">
         <v>1</v>
       </c>
-      <c r="D31" s="6" t="str">
+      <c r="D31" s="95" t="str">
         <f>D30</f>
         <v>no</v>
       </c>

</xml_diff>

<commit_message>
Allow additional_diagnostics to be turned off
Creates quite a lot of model attributes that aren't necessarily used and
probably adds slightly to running time (although not noticeable).
</commit_message>
<xml_diff>
--- a/autumn/xls/programs_fiji.xlsx
+++ b/autumn/xls/programs_fiji.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="91">
   <si>
     <t>program_rate_restart_presenting</t>
   </si>
@@ -287,6 +287,9 @@
   </si>
   <si>
     <t>epi_prop_smearneg</t>
+  </si>
+  <si>
+    <t>is_additional_diagnostics</t>
   </si>
 </sst>
 </file>
@@ -492,7 +495,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -690,6 +693,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="664">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1399,9 +1411,7 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1411,8 +1421,6 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1450,14 +1458,18 @@
     <xf numFmtId="0" fontId="7" fillId="15" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="17" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="664">
     <cellStyle name="Comma 2" xfId="5"/>
@@ -2425,15 +2437,15 @@
   <sheetPr>
     <tabColor theme="3" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:J24"/>
+  <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.7109375" style="55" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.7109375" style="51" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25" bestFit="1" customWidth="1"/>
@@ -2454,7 +2466,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="49" t="s">
+      <c r="A2" s="47" t="s">
         <v>40</v>
       </c>
       <c r="B2" s="36">
@@ -2464,7 +2476,7 @@
       <c r="D2" s="34"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="49" t="s">
+      <c r="A3" s="47" t="s">
         <v>41</v>
       </c>
       <c r="B3" s="36">
@@ -2474,7 +2486,7 @@
       <c r="D3" s="34"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="50" t="s">
+      <c r="A4" s="48" t="s">
         <v>37</v>
       </c>
       <c r="B4" s="37">
@@ -2484,7 +2496,7 @@
       <c r="D4" s="38"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="52" t="s">
+      <c r="A5" s="50" t="s">
         <v>42</v>
       </c>
       <c r="B5" s="39" t="b">
@@ -2493,180 +2505,189 @@
       <c r="C5" s="40"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="53" t="s">
+      <c r="A6" s="92" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="41" t="b">
+      <c r="B6" s="95" t="b">
         <v>0</v>
       </c>
-      <c r="C6" s="42"/>
+      <c r="C6" s="41"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="54" t="s">
+      <c r="A7" s="92" t="s">
         <v>44</v>
       </c>
-      <c r="B7" s="43" t="b">
+      <c r="B7" s="95" t="b">
         <v>0</v>
       </c>
-      <c r="C7" s="44"/>
+      <c r="C7" s="41"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="88" t="s">
+      <c r="A8" s="93" t="s">
+        <v>90</v>
+      </c>
+      <c r="B8" s="94" t="b">
+        <v>0</v>
+      </c>
+      <c r="C8" s="42"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="90" t="s">
         <v>72</v>
       </c>
-      <c r="B8" s="89">
+      <c r="B9" s="91">
         <v>1</v>
       </c>
-      <c r="C8" s="89">
+      <c r="C9" s="91">
         <v>2</v>
       </c>
-      <c r="D8" s="90"/>
-    </row>
-    <row r="9" spans="1:4" s="82" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="72" t="s">
+      <c r="D9" s="84"/>
+    </row>
+    <row r="10" spans="1:4" s="78" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="68" t="s">
         <v>65</v>
       </c>
-      <c r="B9" s="73" t="s">
+      <c r="B10" s="69" t="s">
         <v>62</v>
       </c>
-      <c r="C9" s="73"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="79" t="s">
+      <c r="C10" s="69"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="75" t="s">
         <v>63</v>
       </c>
-      <c r="B10" s="83">
+      <c r="B11" s="79">
         <v>457200</v>
       </c>
-      <c r="C10" s="47"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="80" t="s">
+      <c r="C11" s="45"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="76" t="s">
         <v>64</v>
       </c>
-      <c r="B11" s="81">
+      <c r="B12" s="77">
         <v>3</v>
       </c>
-      <c r="C11" s="47"/>
-    </row>
-    <row r="12" spans="1:4" s="69" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="72" t="s">
+      <c r="C12" s="45"/>
+    </row>
+    <row r="13" spans="1:4" s="65" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="68" t="s">
         <v>36</v>
       </c>
-      <c r="B12" s="73" t="s">
+      <c r="B13" s="69" t="s">
         <v>58</v>
       </c>
-      <c r="C12" s="47"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="70" t="s">
+      <c r="C13" s="45"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="66" t="s">
         <v>38</v>
       </c>
-      <c r="B13" s="71">
+      <c r="B14" s="67">
         <v>1900</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="51" t="s">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="49" t="s">
         <v>39</v>
       </c>
-      <c r="B14" s="35">
+      <c r="B15" s="35">
         <v>1990</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="51" t="s">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="49" t="s">
         <v>71</v>
       </c>
-      <c r="B15" s="35">
+      <c r="B16" s="35">
         <v>2015</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="51" t="s">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="49" t="s">
         <v>74</v>
       </c>
-      <c r="B16" s="35">
+      <c r="B17" s="35">
         <v>2016</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="51" t="s">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="49" t="s">
         <v>75</v>
       </c>
-      <c r="B17" s="35">
+      <c r="B18" s="35">
         <v>2019</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="51" t="s">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="49" t="s">
         <v>70</v>
       </c>
-      <c r="B18" s="91">
+      <c r="B19" s="85">
         <v>2035</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="92" t="s">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="86" t="s">
         <v>76</v>
       </c>
-      <c r="B19" s="93">
+      <c r="B20" s="87">
         <v>0.1</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="75" t="s">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="71" t="s">
         <v>66</v>
       </c>
-      <c r="B20" s="77">
+      <c r="B21" s="73">
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="76" t="s">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="72" t="s">
         <v>79</v>
       </c>
-      <c r="B21" s="78">
+      <c r="B22" s="74">
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="67" t="s">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="63" t="s">
         <v>55</v>
       </c>
-      <c r="B22" s="74" t="s">
+      <c r="B23" s="70" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="23" spans="1:10" s="48" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="68" t="s">
+    <row r="24" spans="1:10" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="64" t="s">
         <v>46</v>
       </c>
-      <c r="B23" s="48" t="s">
+      <c r="B24" s="46" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="56" t="s">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="52" t="s">
         <v>45</v>
       </c>
-      <c r="B24" s="45"/>
-      <c r="C24" s="45"/>
-      <c r="D24" s="45"/>
-      <c r="E24" s="46"/>
-      <c r="F24" s="47"/>
-      <c r="G24" s="47"/>
-      <c r="H24" s="47"/>
-      <c r="I24" s="47"/>
-      <c r="J24" s="47"/>
+      <c r="B25" s="43"/>
+      <c r="C25" s="43"/>
+      <c r="D25" s="43"/>
+      <c r="E25" s="44"/>
+      <c r="F25" s="45"/>
+      <c r="G25" s="45"/>
+      <c r="H25" s="45"/>
+      <c r="I25" s="45"/>
+      <c r="J25" s="45"/>
     </row>
   </sheetData>
   <dataValidations xWindow="363" yWindow="440" count="8">
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Time to do recent graphs from" prompt="Calendar year that output graphs for recent time start from." sqref="B14:B17">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Time to do recent graphs from" prompt="Calendar year that output graphs for recent time start from." sqref="B15:B18">
       <formula1>-10000</formula1>
       <formula2>3000</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Time to start model" prompt="Enter the calendar year that the model runs from." sqref="B13">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Time to start model" prompt="Enter the calendar year that the model runs from." sqref="B14">
       <formula1>-10000</formula1>
       <formula2>3000</formula2>
     </dataValidation>
@@ -2676,12 +2697,12 @@
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Strains" prompt="Number of strains (0: single strain model, 2: DS-TB and MDR-TB, 3: DS-TB, MDR-TB and XDR-TB)." sqref="B3:D3"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Comorbidities" prompt="Number of comorbidities (currently up to three, but will be revised as model develops)." sqref="B4:D4"/>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Function smoothness" prompt="From zero up, with zero being exact fit and higher values being greater smoothness." sqref="B20:B21">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Function smoothness" prompt="From zero up, with zero being exact fit and higher values being greater smoothness." sqref="B21:B22">
       <formula1>0</formula1>
       <formula2>1000</formula2>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Age breakpoints" prompt="Enter consecutively increasing age breakpoints to create age strata. (Can enter any number, don't enter zero and no upper limit is needed.)" sqref="B24:E24"/>
-    <dataValidation allowBlank="1" showErrorMessage="1" sqref="B9:C12"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Age breakpoints" prompt="Enter consecutively increasing age breakpoints to create age strata. (Can enter any number, don't enter zero and no upper limit is needed.)" sqref="B25:E25"/>
+    <dataValidation allowBlank="1" showErrorMessage="1" sqref="B10:C13"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2716,19 +2737,19 @@
           <x14:formula1>
             <xm:f>dropdown_lists!$B$2:$B$3</xm:f>
           </x14:formula1>
-          <xm:sqref>B7</xm:sqref>
+          <xm:sqref>B7:B8</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Misassignment" prompt="Whether patients can be incorrectly detected with the wrong strain.">
           <x14:formula1>
             <xm:f>dropdown_lists!$B$2:$B$4</xm:f>
           </x14:formula1>
-          <xm:sqref>C7</xm:sqref>
+          <xm:sqref>C7:C8</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Integration" prompt="Which integration package. Explicitly coded or Scipy's integration package.">
           <x14:formula1>
             <xm:f>dropdown_lists!$C$2:$C$3</xm:f>
           </x14:formula1>
-          <xm:sqref>B22</xm:sqref>
+          <xm:sqref>B23</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2749,112 +2770,112 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="48.28515625" style="61" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.85546875" style="64" customWidth="1"/>
-    <col min="3" max="3" width="84.28515625" style="59" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.7109375" style="59" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="59"/>
+    <col min="1" max="1" width="48.28515625" style="57" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" style="60" customWidth="1"/>
+    <col min="3" max="3" width="84.28515625" style="55" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" style="55" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="55"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="65" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="65" t="s">
+    <row r="1" spans="1:4" s="61" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="61" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="66" t="s">
+      <c r="B1" s="62" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="65" t="s">
+      <c r="C1" s="61" t="s">
         <v>48</v>
       </c>
-      <c r="D1" s="65" t="s">
+      <c r="D1" s="61" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="58" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="57" t="s">
+    <row r="2" spans="1:4" s="54" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="53" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="62">
+      <c r="B2" s="58">
         <v>6.7</v>
       </c>
-      <c r="C2" s="58" t="s">
+      <c r="C2" s="54" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="57" t="s">
+      <c r="A3" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="62">
+      <c r="B3" s="58">
         <v>26</v>
       </c>
-      <c r="C3" s="59" t="s">
+      <c r="C3" s="55" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="57" t="s">
+      <c r="A4" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="62">
+      <c r="B4" s="58">
         <v>4</v>
       </c>
-      <c r="C4" s="59" t="s">
+      <c r="C4" s="55" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="57" t="s">
+      <c r="A5" s="53" t="s">
         <v>80</v>
       </c>
-      <c r="B5" s="62">
+      <c r="B5" s="58">
         <v>1945</v>
       </c>
-      <c r="C5" s="59" t="s">
+      <c r="C5" s="55" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="57" t="s">
+      <c r="A6" s="53" t="s">
         <v>81</v>
       </c>
-      <c r="B6" s="62">
+      <c r="B6" s="58">
         <v>1955</v>
       </c>
-      <c r="C6" s="59" t="s">
+      <c r="C6" s="55" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="57" t="s">
+      <c r="A7" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="62">
+      <c r="B7" s="58">
         <v>2050</v>
       </c>
-      <c r="C7" s="59" t="s">
+      <c r="C7" s="55" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="57" t="s">
+      <c r="A8" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="62">
+      <c r="B8" s="58">
         <v>2</v>
       </c>
-      <c r="C8" s="59" t="s">
+      <c r="C8" s="55" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="60" t="s">
+      <c r="A9" s="56" t="s">
         <v>84</v>
       </c>
-      <c r="B9" s="63">
+      <c r="B9" s="59">
         <v>0.32</v>
       </c>
-      <c r="C9" s="59" t="s">
+      <c r="C9" s="55" t="s">
         <v>77</v>
       </c>
     </row>
@@ -3147,7 +3168,7 @@
         <v>23</v>
       </c>
       <c r="C3" s="6"/>
-      <c r="D3" s="95" t="s">
+      <c r="D3" s="89" t="s">
         <v>23</v>
       </c>
       <c r="H3" s="7">
@@ -3228,7 +3249,7 @@
         <v>23</v>
       </c>
       <c r="C5" s="8"/>
-      <c r="D5" s="95" t="s">
+      <c r="D5" s="89" t="s">
         <v>23</v>
       </c>
       <c r="F5" s="9">
@@ -3281,7 +3302,7 @@
         <v>23</v>
       </c>
       <c r="C7" s="10"/>
-      <c r="D7" s="95" t="s">
+      <c r="D7" s="89" t="s">
         <v>23</v>
       </c>
       <c r="G7" s="11">
@@ -3328,7 +3349,7 @@
         <v>23</v>
       </c>
       <c r="C9" s="12"/>
-      <c r="D9" s="95" t="s">
+      <c r="D9" s="89" t="s">
         <v>23</v>
       </c>
       <c r="X9" s="13">
@@ -3366,7 +3387,7 @@
         <v>23</v>
       </c>
       <c r="C11" s="14"/>
-      <c r="D11" s="95" t="s">
+      <c r="D11" s="89" t="s">
         <v>23</v>
       </c>
       <c r="X11" s="15">
@@ -3407,7 +3428,7 @@
         <v>23</v>
       </c>
       <c r="C13" s="16"/>
-      <c r="D13" s="95" t="s">
+      <c r="D13" s="89" t="s">
         <v>23</v>
       </c>
       <c r="X13" s="17">
@@ -3471,7 +3492,7 @@
         <v>23</v>
       </c>
       <c r="C15" s="12"/>
-      <c r="D15" s="95" t="s">
+      <c r="D15" s="89" t="s">
         <v>23</v>
       </c>
       <c r="I15" s="13">
@@ -3544,7 +3565,7 @@
         <v>23</v>
       </c>
       <c r="C17" s="12"/>
-      <c r="D17" s="95" t="s">
+      <c r="D17" s="89" t="s">
         <v>23</v>
       </c>
       <c r="I17" s="13">
@@ -3608,7 +3629,7 @@
         <v>23</v>
       </c>
       <c r="C19" s="26"/>
-      <c r="D19" s="95" t="s">
+      <c r="D19" s="89" t="s">
         <v>23</v>
       </c>
       <c r="I19" s="27">
@@ -3681,7 +3702,7 @@
         <v>23</v>
       </c>
       <c r="C21" s="26"/>
-      <c r="D21" s="95" t="s">
+      <c r="D21" s="89" t="s">
         <v>23</v>
       </c>
       <c r="I21" s="27">
@@ -3745,7 +3766,7 @@
         <v>23</v>
       </c>
       <c r="C23" s="8"/>
-      <c r="D23" s="95" t="s">
+      <c r="D23" s="89" t="s">
         <v>23</v>
       </c>
       <c r="I23" s="9">
@@ -3818,7 +3839,7 @@
         <v>23</v>
       </c>
       <c r="C25" s="8"/>
-      <c r="D25" s="95" t="s">
+      <c r="D25" s="89" t="s">
         <v>23</v>
       </c>
       <c r="I25" s="9">
@@ -3828,68 +3849,68 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:52" s="86" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="84" t="s">
+    <row r="26" spans="1:52" s="82" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="80" t="s">
         <v>67</v>
       </c>
-      <c r="B26" s="85" t="s">
+      <c r="B26" s="81" t="s">
         <v>13</v>
       </c>
-      <c r="C26" s="85">
+      <c r="C26" s="81">
         <v>1</v>
       </c>
-      <c r="D26" s="85" t="s">
+      <c r="D26" s="81" t="s">
         <v>13</v>
       </c>
-      <c r="E26" s="86">
+      <c r="E26" s="82">
         <f>1/26</f>
         <v>3.8461538461538464E-2</v>
       </c>
-      <c r="AF26" s="87"/>
-      <c r="AG26" s="87"/>
-      <c r="AH26" s="87"/>
-      <c r="AI26" s="87"/>
-      <c r="AJ26" s="87"/>
-      <c r="AK26" s="87"/>
-      <c r="AL26" s="87"/>
-      <c r="AM26" s="87"/>
-      <c r="AN26" s="87"/>
-      <c r="AO26" s="87"/>
-      <c r="AP26" s="87"/>
-      <c r="AQ26" s="87"/>
-      <c r="AR26" s="87"/>
-      <c r="AS26" s="87"/>
-      <c r="AT26" s="87"/>
-      <c r="AU26" s="87"/>
-      <c r="AV26" s="87"/>
-      <c r="AW26" s="87"/>
-      <c r="AX26" s="87"/>
-      <c r="AY26" s="87"/>
-      <c r="AZ26" s="86">
+      <c r="AF26" s="83"/>
+      <c r="AG26" s="83"/>
+      <c r="AH26" s="83"/>
+      <c r="AI26" s="83"/>
+      <c r="AJ26" s="83"/>
+      <c r="AK26" s="83"/>
+      <c r="AL26" s="83"/>
+      <c r="AM26" s="83"/>
+      <c r="AN26" s="83"/>
+      <c r="AO26" s="83"/>
+      <c r="AP26" s="83"/>
+      <c r="AQ26" s="83"/>
+      <c r="AR26" s="83"/>
+      <c r="AS26" s="83"/>
+      <c r="AT26" s="83"/>
+      <c r="AU26" s="83"/>
+      <c r="AV26" s="83"/>
+      <c r="AW26" s="83"/>
+      <c r="AX26" s="83"/>
+      <c r="AY26" s="83"/>
+      <c r="AZ26" s="82">
         <v>0.04</v>
       </c>
     </row>
-    <row r="27" spans="1:52" s="86" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="84" t="s">
+    <row r="27" spans="1:52" s="82" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="80" t="s">
         <v>68</v>
       </c>
-      <c r="B27" s="85" t="s">
+      <c r="B27" s="81" t="s">
         <v>23</v>
       </c>
-      <c r="C27" s="85"/>
-      <c r="D27" s="95" t="s">
+      <c r="C27" s="81"/>
+      <c r="D27" s="89" t="s">
         <v>23</v>
       </c>
-      <c r="I27" s="86">
+      <c r="I27" s="82">
         <v>0</v>
       </c>
-      <c r="R27" s="86">
+      <c r="R27" s="82">
         <v>532947</v>
       </c>
-      <c r="X27" s="86">
+      <c r="X27" s="82">
         <v>9283747</v>
       </c>
-      <c r="AZ27" s="86">
+      <c r="AZ27" s="82">
         <v>739284639</v>
       </c>
     </row>
@@ -3903,20 +3924,20 @@
       <c r="C28" s="6">
         <v>1</v>
       </c>
-      <c r="D28" s="95" t="s">
+      <c r="D28" s="89" t="s">
         <v>14</v>
       </c>
-      <c r="AB28" s="94"/>
-      <c r="AL28" s="94"/>
-      <c r="AR28" s="94"/>
-      <c r="AS28" s="94"/>
-      <c r="AT28" s="94"/>
-      <c r="AU28" s="94"/>
-      <c r="AV28" s="94"/>
-      <c r="AW28" s="94"/>
-      <c r="AX28" s="94"/>
-      <c r="AY28" s="94"/>
-      <c r="AZ28" s="94"/>
+      <c r="AB28" s="88"/>
+      <c r="AL28" s="88"/>
+      <c r="AR28" s="88"/>
+      <c r="AS28" s="88"/>
+      <c r="AT28" s="88"/>
+      <c r="AU28" s="88"/>
+      <c r="AV28" s="88"/>
+      <c r="AW28" s="88"/>
+      <c r="AX28" s="88"/>
+      <c r="AY28" s="88"/>
+      <c r="AZ28" s="88"/>
     </row>
     <row r="29" spans="1:52" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="18" t="s">
@@ -3931,49 +3952,49 @@
       <c r="D29" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="J29" s="94"/>
-      <c r="K29" s="94"/>
-      <c r="L29" s="94"/>
-      <c r="M29" s="94"/>
-      <c r="N29" s="94"/>
-      <c r="O29" s="94"/>
-      <c r="P29" s="94"/>
-      <c r="Q29" s="94"/>
-      <c r="R29" s="94"/>
-      <c r="S29" s="94"/>
-      <c r="T29" s="94"/>
-      <c r="U29" s="94"/>
-      <c r="V29" s="94"/>
-      <c r="W29" s="94"/>
-      <c r="X29" s="94"/>
-      <c r="Y29" s="94"/>
-      <c r="Z29" s="94"/>
-      <c r="AA29" s="94"/>
-      <c r="AB29" s="94"/>
-      <c r="AC29" s="94"/>
-      <c r="AD29" s="94"/>
-      <c r="AE29" s="94"/>
-      <c r="AF29" s="94"/>
-      <c r="AG29" s="94"/>
-      <c r="AH29" s="94"/>
-      <c r="AI29" s="94"/>
-      <c r="AJ29" s="94"/>
-      <c r="AK29" s="94"/>
-      <c r="AL29" s="94"/>
-      <c r="AM29" s="94"/>
-      <c r="AN29" s="94"/>
-      <c r="AO29" s="94"/>
-      <c r="AP29" s="94"/>
-      <c r="AQ29" s="94"/>
-      <c r="AR29" s="94"/>
-      <c r="AS29" s="94"/>
-      <c r="AT29" s="94"/>
-      <c r="AU29" s="94"/>
-      <c r="AV29" s="94"/>
-      <c r="AW29" s="94"/>
-      <c r="AX29" s="94"/>
-      <c r="AY29" s="94"/>
-      <c r="AZ29" s="94"/>
+      <c r="J29" s="88"/>
+      <c r="K29" s="88"/>
+      <c r="L29" s="88"/>
+      <c r="M29" s="88"/>
+      <c r="N29" s="88"/>
+      <c r="O29" s="88"/>
+      <c r="P29" s="88"/>
+      <c r="Q29" s="88"/>
+      <c r="R29" s="88"/>
+      <c r="S29" s="88"/>
+      <c r="T29" s="88"/>
+      <c r="U29" s="88"/>
+      <c r="V29" s="88"/>
+      <c r="W29" s="88"/>
+      <c r="X29" s="88"/>
+      <c r="Y29" s="88"/>
+      <c r="Z29" s="88"/>
+      <c r="AA29" s="88"/>
+      <c r="AB29" s="88"/>
+      <c r="AC29" s="88"/>
+      <c r="AD29" s="88"/>
+      <c r="AE29" s="88"/>
+      <c r="AF29" s="88"/>
+      <c r="AG29" s="88"/>
+      <c r="AH29" s="88"/>
+      <c r="AI29" s="88"/>
+      <c r="AJ29" s="88"/>
+      <c r="AK29" s="88"/>
+      <c r="AL29" s="88"/>
+      <c r="AM29" s="88"/>
+      <c r="AN29" s="88"/>
+      <c r="AO29" s="88"/>
+      <c r="AP29" s="88"/>
+      <c r="AQ29" s="88"/>
+      <c r="AR29" s="88"/>
+      <c r="AS29" s="88"/>
+      <c r="AT29" s="88"/>
+      <c r="AU29" s="88"/>
+      <c r="AV29" s="88"/>
+      <c r="AW29" s="88"/>
+      <c r="AX29" s="88"/>
+      <c r="AY29" s="88"/>
+      <c r="AZ29" s="88"/>
     </row>
     <row r="30" spans="1:52" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="18" t="s">
@@ -3999,7 +4020,7 @@
       <c r="C31" s="6">
         <v>1</v>
       </c>
-      <c r="D31" s="95" t="str">
+      <c r="D31" s="89" t="str">
         <f>D30</f>
         <v>no</v>
       </c>

</xml_diff>

<commit_message>
Classify and plot scaling parameters
</commit_message>
<xml_diff>
--- a/autumn/xls/programs_fiji.xlsx
+++ b/autumn/xls/programs_fiji.xlsx
@@ -2440,7 +2440,7 @@
   <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2896,7 +2896,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H14" sqref="H14"/>
+      <selection pane="bottomRight" activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4007,7 +4007,7 @@
         <v>1</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="31" spans="1:52" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -4022,7 +4022,7 @@
       </c>
       <c r="D31" s="89" t="str">
         <f>D30</f>
-        <v>no</v>
+        <v>yes</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Scaling parameters on single axis finished
Last change was to make sure the bottom of the y-axis goes down to zero.
Now for the multiple panel plots next.
</commit_message>
<xml_diff>
--- a/autumn/xls/programs_fiji.xlsx
+++ b/autumn/xls/programs_fiji.xlsx
@@ -2440,7 +2440,7 @@
   <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2470,7 +2470,7 @@
         <v>40</v>
       </c>
       <c r="B2" s="36">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C2" s="36"/>
       <c r="D2" s="34"/>
@@ -2682,7 +2682,7 @@
       <c r="J25" s="45"/>
     </row>
   </sheetData>
-  <dataValidations xWindow="363" yWindow="440" count="8">
+  <dataValidations xWindow="363" yWindow="440" count="9">
     <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Time to do recent graphs from" prompt="Calendar year that output graphs for recent time start from." sqref="B15:B18">
       <formula1>-10000</formula1>
       <formula2>3000</formula2>
@@ -2691,7 +2691,7 @@
       <formula1>-10000</formula1>
       <formula2>3000</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Organ stratification" prompt="Number of organs allowed (0: no stratification, 2: smear-positive and smear-negative, 3: smear-positive, smear-negative and extra-pulmonary)." sqref="B2:D2">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Organ stratification" prompt="Number of organs allowed (0: no stratification, 2: smear-positive and smear-negative, 3: smear-positive, smear-negative and extra-pulmonary)." sqref="C2:D2">
       <formula1>0</formula1>
       <formula2>3</formula2>
     </dataValidation>
@@ -2703,6 +2703,10 @@
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Age breakpoints" prompt="Enter consecutively increasing age breakpoints to create age strata. (Can enter any number, don't enter zero and no upper limit is needed.)" sqref="B25:E25"/>
     <dataValidation allowBlank="1" showErrorMessage="1" sqref="B10:C13"/>
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Organ stratification" prompt="Number of organs allowed (0: no stratification, 2: smear-positive and smear-negative, 3: smear-positive, smear-negative and extra-pulmonary). WARNING: No organ stratification should be selected if this is zero (or one)." sqref="B2">
+      <formula1>0</formula1>
+      <formula2>3</formula2>
+    </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2896,7 +2900,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F28" sqref="F28"/>
+      <selection pane="bottomRight" activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4007,7 +4011,7 @@
         <v>1</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="31" spans="1:52" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -4022,7 +4026,7 @@
       </c>
       <c r="D31" s="89" t="str">
         <f>D30</f>
-        <v>yes</v>
+        <v>no</v>
       </c>
     </row>
   </sheetData>
@@ -4045,7 +4049,7 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xWindow="343" yWindow="238" count="4">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xWindow="343" yWindow="238" count="5">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>dropdown_lists!$A$2:$A$4</xm:f>
@@ -4056,7 +4060,7 @@
           <x14:formula1>
             <xm:f>dropdown_lists!$A$2:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>D2:D27 D29:D30 D32:D1048576</xm:sqref>
+          <xm:sqref>D2:D27 D32:D1048576 D29</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Cannot be time-variant" prompt="Will work on this later, but currently this must be fixed.">
           <x14:formula1>
@@ -4069,6 +4073,12 @@
             <xm:f>dropdown_lists!$A$2:$A$4</xm:f>
           </x14:formula1>
           <xm:sqref>D31</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Time-variant?" prompt="If no, the most recent value will be selected. WARNING: No should be selected if no organ stratification selected.">
+          <x14:formula1>
+            <xm:f>dropdown_lists!$A$2:$A$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>D30</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Finish plotting of scale-up functions
Handle plots against data by panel in the same way as plots of all
functions together - plus a few little finishing touches.
</commit_message>
<xml_diff>
--- a/autumn/xls/programs_fiji.xlsx
+++ b/autumn/xls/programs_fiji.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="315" windowWidth="20370" windowHeight="7530" tabRatio="807"/>
+    <workbookView xWindow="120" yWindow="315" windowWidth="20370" windowHeight="7530" tabRatio="807" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="model_attributes" sheetId="4" r:id="rId1"/>
@@ -2439,8 +2439,8 @@
   </sheetPr>
   <dimension ref="A1:J25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2470,7 +2470,7 @@
         <v>40</v>
       </c>
       <c r="B2" s="36">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C2" s="36"/>
       <c r="D2" s="34"/>
@@ -2896,11 +2896,11 @@
   </sheetPr>
   <dimension ref="A1:BC31"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D30" sqref="D30"/>
+      <selection pane="bottomRight" activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Reinstate some important code
Not sure why I commented out part of calculate_force_infection_vars
previously, but I shouldn't have. It was critically important. Back in
now.
</commit_message>
<xml_diff>
--- a/autumn/xls/programs_fiji.xlsx
+++ b/autumn/xls/programs_fiji.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="315" windowWidth="20370" windowHeight="7530" tabRatio="807" activeTab="2"/>
+    <workbookView xWindow="120" yWindow="315" windowWidth="20370" windowHeight="7530" tabRatio="807"/>
   </bookViews>
   <sheets>
     <sheet name="model_attributes" sheetId="4" r:id="rId1"/>
@@ -2439,8 +2439,8 @@
   </sheetPr>
   <dimension ref="A1:J25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2896,11 +2896,11 @@
   </sheetPr>
   <dimension ref="A1:BC31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A32" sqref="A32"/>
+      <selection pane="bottomRight" activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3237,7 +3237,9 @@
       <c r="AW4" s="29"/>
       <c r="AX4" s="29"/>
       <c r="AY4" s="29"/>
-      <c r="AZ4" s="29"/>
+      <c r="AZ4" s="29">
+        <v>50</v>
+      </c>
       <c r="BB4" s="9">
         <v>70</v>
       </c>
@@ -4011,7 +4013,7 @@
         <v>1</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="31" spans="1:52" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -4026,7 +4028,7 @@
       </c>
       <c r="D31" s="89" t="str">
         <f>D30</f>
-        <v>yes</v>
+        <v>no</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Code to plot scenarios nicely
Plotting module now needs a fair bit of tidying.
</commit_message>
<xml_diff>
--- a/autumn/xls/programs_fiji.xlsx
+++ b/autumn/xls/programs_fiji.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="93">
   <si>
     <t>program_rate_restart_presenting</t>
   </si>
@@ -290,6 +290,12 @@
   </si>
   <si>
     <t>is_additional_diagnostics</t>
+  </si>
+  <si>
+    <t>scenario_3</t>
+  </si>
+  <si>
+    <t>scenario_4</t>
   </si>
 </sst>
 </file>
@@ -1369,7 +1375,7 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="96">
+  <cellXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1470,6 +1476,7 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="664">
     <cellStyle name="Comma 2" xfId="5"/>
@@ -2440,7 +2447,7 @@
   <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2451,7 +2458,7 @@
     <col min="4" max="4" width="25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="33" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="32" t="s">
         <v>36</v>
       </c>
@@ -2465,7 +2472,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="47" t="s">
         <v>40</v>
       </c>
@@ -2475,7 +2482,7 @@
       <c r="C2" s="36"/>
       <c r="D2" s="34"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="47" t="s">
         <v>41</v>
       </c>
@@ -2485,7 +2492,7 @@
       <c r="C3" s="36"/>
       <c r="D3" s="34"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="48" t="s">
         <v>37</v>
       </c>
@@ -2495,7 +2502,7 @@
       <c r="C4" s="37"/>
       <c r="D4" s="38"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="50" t="s">
         <v>42</v>
       </c>
@@ -2504,7 +2511,7 @@
       </c>
       <c r="C5" s="40"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="92" t="s">
         <v>43</v>
       </c>
@@ -2513,7 +2520,7 @@
       </c>
       <c r="C6" s="41"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="92" t="s">
         <v>44</v>
       </c>
@@ -2522,7 +2529,7 @@
       </c>
       <c r="C7" s="41"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="93" t="s">
         <v>90</v>
       </c>
@@ -2531,7 +2538,7 @@
       </c>
       <c r="C8" s="42"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="90" t="s">
         <v>72</v>
       </c>
@@ -2541,9 +2548,14 @@
       <c r="C9" s="91">
         <v>2</v>
       </c>
-      <c r="D9" s="84"/>
-    </row>
-    <row r="10" spans="1:4" s="78" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D9" s="84">
+        <v>3</v>
+      </c>
+      <c r="E9" s="96">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" s="78" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="68" t="s">
         <v>65</v>
       </c>
@@ -2552,7 +2564,7 @@
       </c>
       <c r="C10" s="69"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="75" t="s">
         <v>63</v>
       </c>
@@ -2561,7 +2573,7 @@
       </c>
       <c r="C11" s="45"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="76" t="s">
         <v>64</v>
       </c>
@@ -2570,7 +2582,7 @@
       </c>
       <c r="C12" s="45"/>
     </row>
-    <row r="13" spans="1:4" s="65" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" s="65" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="68" t="s">
         <v>36</v>
       </c>
@@ -2579,7 +2591,7 @@
       </c>
       <c r="C13" s="45"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="66" t="s">
         <v>38</v>
       </c>
@@ -2587,7 +2599,7 @@
         <v>1910</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="49" t="s">
         <v>39</v>
       </c>
@@ -2595,7 +2607,7 @@
         <v>1990</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="49" t="s">
         <v>71</v>
       </c>
@@ -2769,7 +2781,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2877,7 +2889,7 @@
         <v>84</v>
       </c>
       <c r="B9" s="59">
-        <v>0.32</v>
+        <v>0.25</v>
       </c>
       <c r="C9" s="55" t="s">
         <v>77</v>
@@ -2894,13 +2906,13 @@
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:BC31"/>
+  <dimension ref="A1:BE31"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="AF2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A6" sqref="A6"/>
+      <selection pane="bottomRight" activeCell="BD5" sqref="BD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2933,7 +2945,7 @@
     <col min="54" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:55" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:57" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>16</v>
       </c>
@@ -3099,8 +3111,14 @@
       <c r="BC1" s="5" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="2" spans="1:55" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="BD1" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="BE1" s="5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="1:57" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -3164,7 +3182,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="3" spans="1:55" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:57" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
         <v>17</v>
       </c>
@@ -3191,7 +3209,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:55" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:57" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="19" t="s">
         <v>9</v>
       </c>
@@ -3246,8 +3264,11 @@
       <c r="BC4" s="9">
         <v>60</v>
       </c>
-    </row>
-    <row r="5" spans="1:55" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="BD4" s="9">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="5" spans="1:57" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
         <v>18</v>
       </c>
@@ -3265,7 +3286,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:55" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:57" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
         <v>10</v>
       </c>
@@ -3299,8 +3320,11 @@
       <c r="BC6" s="11">
         <v>85</v>
       </c>
-    </row>
-    <row r="7" spans="1:55" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="BE6" s="11">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="7" spans="1:57" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
         <v>19</v>
       </c>
@@ -3324,7 +3348,7 @@
         <v>4049504</v>
       </c>
     </row>
-    <row r="8" spans="1:55" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:57" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="21" t="s">
         <v>3</v>
       </c>
@@ -3347,7 +3371,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:55" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:57" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="21" t="s">
         <v>20</v>
       </c>
@@ -3362,7 +3386,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:55" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:57" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="22" t="s">
         <v>11</v>
       </c>
@@ -3385,7 +3409,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:55" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:57" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="22" t="s">
         <v>21</v>
       </c>
@@ -3400,7 +3424,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:55" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:57" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="23" t="s">
         <v>12</v>
       </c>
@@ -3426,7 +3450,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="13" spans="1:55" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:57" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="23" t="s">
         <v>22</v>
       </c>
@@ -3441,7 +3465,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:55" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:57" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="21" t="s">
         <v>24</v>
       </c>
@@ -3489,8 +3513,11 @@
       <c r="BC14" s="13">
         <v>90</v>
       </c>
-    </row>
-    <row r="15" spans="1:55" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="BD14" s="13">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="15" spans="1:57" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="21" t="s">
         <v>25</v>
       </c>
@@ -3517,7 +3544,7 @@
         <v>52431253</v>
       </c>
     </row>
-    <row r="16" spans="1:55" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:57" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="21" t="s">
         <v>26</v>
       </c>

</xml_diff>

<commit_message>
Put some dummy values in workbook time_variants, column 1986 to test cost modules
</commit_message>
<xml_diff>
--- a/autumn/xls/programs_fiji.xlsx
+++ b/autumn/xls/programs_fiji.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="315" windowWidth="20370" windowHeight="7530" tabRatio="807"/>
+    <workbookView xWindow="120" yWindow="315" windowWidth="20370" windowHeight="7530" tabRatio="807" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="model_attributes" sheetId="4" r:id="rId1"/>
@@ -2439,8 +2439,8 @@
   </sheetPr>
   <dimension ref="A1:J25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2896,11 +2896,11 @@
   </sheetPr>
   <dimension ref="A1:BC31"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G21" sqref="G21"/>
+      <selection pane="bottomRight" activeCell="X29" sqref="X29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3128,7 +3128,9 @@
       <c r="U2" s="28"/>
       <c r="V2" s="28"/>
       <c r="W2" s="28"/>
-      <c r="X2" s="28"/>
+      <c r="X2" s="28">
+        <v>1</v>
+      </c>
       <c r="Y2" s="28"/>
       <c r="Z2" s="28"/>
       <c r="AA2" s="28"/>
@@ -3213,6 +3215,9 @@
       <c r="T4" s="9">
         <v>30</v>
       </c>
+      <c r="X4" s="9">
+        <v>1</v>
+      </c>
       <c r="AB4" s="29"/>
       <c r="AC4" s="29"/>
       <c r="AD4" s="29"/>
@@ -3284,6 +3289,9 @@
       <c r="J6" s="11">
         <v>80</v>
       </c>
+      <c r="X6" s="11">
+        <v>1</v>
+      </c>
       <c r="Z6" s="11">
         <v>82</v>
       </c>
@@ -3343,6 +3351,9 @@
       <c r="K8" s="13">
         <v>40</v>
       </c>
+      <c r="X8" s="13">
+        <v>1</v>
+      </c>
       <c r="AB8" s="13">
         <v>40</v>
       </c>
@@ -3378,6 +3389,9 @@
       <c r="R10" s="15">
         <v>30</v>
       </c>
+      <c r="X10" s="15">
+        <v>1</v>
+      </c>
       <c r="AB10" s="15">
         <v>40</v>
       </c>
@@ -3418,6 +3432,9 @@
       </c>
       <c r="W12" s="17">
         <v>0</v>
+      </c>
+      <c r="X12" s="17">
+        <v>1</v>
       </c>
       <c r="AG12" s="17">
         <v>50</v>
@@ -3871,6 +3888,9 @@
       <c r="E26" s="82">
         <f>1/26</f>
         <v>3.8461538461538464E-2</v>
+      </c>
+      <c r="X26" s="82">
+        <v>1</v>
       </c>
       <c r="AF26" s="83"/>
       <c r="AG26" s="83"/>

</xml_diff>

<commit_message>
Tidying to plotting module
A fair bit of work on making the plot_all_outputs_against_gtb function
plot all scenarios simultaneously.
</commit_message>
<xml_diff>
--- a/autumn/xls/programs_fiji.xlsx
+++ b/autumn/xls/programs_fiji.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="315" windowWidth="20370" windowHeight="7530" tabRatio="807" activeTab="2"/>
+    <workbookView xWindow="120" yWindow="315" windowWidth="20370" windowHeight="7530" tabRatio="807"/>
   </bookViews>
   <sheets>
     <sheet name="model_attributes" sheetId="4" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="93">
   <si>
     <t>program_rate_restart_presenting</t>
   </si>
@@ -290,6 +290,12 @@
   </si>
   <si>
     <t>is_additional_diagnostics</t>
+  </si>
+  <si>
+    <t>scenario_3</t>
+  </si>
+  <si>
+    <t>scenario_4</t>
   </si>
 </sst>
 </file>
@@ -1369,7 +1375,7 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="96">
+  <cellXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1412,7 +1418,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1464,12 +1469,12 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="17" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="664">
     <cellStyle name="Comma 2" xfId="5"/>
@@ -2439,19 +2444,19 @@
   </sheetPr>
   <dimension ref="A1:J25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.7109375" style="51" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.7109375" style="50" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="33" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="32" t="s">
         <v>36</v>
       </c>
@@ -2465,8 +2470,8 @@
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="47" t="s">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="46" t="s">
         <v>40</v>
       </c>
       <c r="B2" s="36">
@@ -2475,8 +2480,8 @@
       <c r="C2" s="36"/>
       <c r="D2" s="34"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="47" t="s">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="46" t="s">
         <v>41</v>
       </c>
       <c r="B3" s="36">
@@ -2485,8 +2490,8 @@
       <c r="C3" s="36"/>
       <c r="D3" s="34"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="48" t="s">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="47" t="s">
         <v>37</v>
       </c>
       <c r="B4" s="37">
@@ -2495,8 +2500,8 @@
       <c r="C4" s="37"/>
       <c r="D4" s="38"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="50" t="s">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="49" t="s">
         <v>42</v>
       </c>
       <c r="B5" s="39" t="b">
@@ -2504,99 +2509,109 @@
       </c>
       <c r="C5" s="40"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="92" t="s">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="89" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="95" t="b">
+      <c r="B6" s="91" t="b">
         <v>0</v>
       </c>
       <c r="C6" s="41"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="92" t="s">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="89" t="s">
         <v>44</v>
       </c>
-      <c r="B7" s="95" t="b">
+      <c r="B7" s="91" t="b">
         <v>0</v>
       </c>
       <c r="C7" s="41"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="93" t="s">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="90" t="s">
         <v>90</v>
       </c>
-      <c r="B8" s="94" t="b">
+      <c r="B8" s="91" t="b">
         <v>0</v>
       </c>
-      <c r="C8" s="42"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="90" t="s">
+      <c r="C8" s="41"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="92" t="s">
         <v>72</v>
       </c>
-      <c r="B9" s="91">
+      <c r="B9" s="93">
         <v>1</v>
       </c>
-      <c r="C9" s="91">
+      <c r="C9" s="94">
         <v>2</v>
       </c>
-      <c r="D9" s="84"/>
-    </row>
-    <row r="10" spans="1:4" s="78" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="68" t="s">
+      <c r="D9" s="94">
+        <v>3</v>
+      </c>
+      <c r="E9" s="94">
+        <v>4</v>
+      </c>
+      <c r="F9" s="94"/>
+      <c r="G9" s="94"/>
+      <c r="H9" s="94"/>
+      <c r="I9" s="94"/>
+      <c r="J9" s="83"/>
+    </row>
+    <row r="10" spans="1:10" s="77" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="67" t="s">
         <v>65</v>
       </c>
-      <c r="B10" s="69" t="s">
+      <c r="B10" s="68" t="s">
         <v>62</v>
       </c>
-      <c r="C10" s="69"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="75" t="s">
+      <c r="C10" s="68"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="74" t="s">
         <v>63</v>
       </c>
-      <c r="B11" s="79">
-        <v>457200</v>
-      </c>
-      <c r="C11" s="45"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="76" t="s">
+      <c r="B11" s="78">
+        <v>300000</v>
+      </c>
+      <c r="C11" s="44"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="75" t="s">
         <v>64</v>
       </c>
-      <c r="B12" s="77">
+      <c r="B12" s="76">
         <v>3</v>
       </c>
-      <c r="C12" s="45"/>
-    </row>
-    <row r="13" spans="1:4" s="65" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="68" t="s">
+      <c r="C12" s="44"/>
+    </row>
+    <row r="13" spans="1:10" s="64" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="67" t="s">
         <v>36</v>
       </c>
-      <c r="B13" s="69" t="s">
+      <c r="B13" s="68" t="s">
         <v>58</v>
       </c>
-      <c r="C13" s="45"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="66" t="s">
+      <c r="C13" s="44"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="65" t="s">
         <v>38</v>
       </c>
-      <c r="B14" s="67">
-        <v>1900</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="49" t="s">
+      <c r="B14" s="66">
+        <v>1903</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="48" t="s">
         <v>39</v>
       </c>
       <c r="B15" s="35">
         <v>1990</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="49" t="s">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="48" t="s">
         <v>71</v>
       </c>
       <c r="B16" s="35">
@@ -2604,7 +2619,7 @@
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="49" t="s">
+      <c r="A17" s="48" t="s">
         <v>74</v>
       </c>
       <c r="B17" s="35">
@@ -2612,7 +2627,7 @@
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="49" t="s">
+      <c r="A18" s="48" t="s">
         <v>75</v>
       </c>
       <c r="B18" s="35">
@@ -2620,66 +2635,66 @@
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="49" t="s">
+      <c r="A19" s="48" t="s">
         <v>70</v>
       </c>
-      <c r="B19" s="85">
+      <c r="B19" s="84">
         <v>2035</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="86" t="s">
+      <c r="A20" s="85" t="s">
         <v>76</v>
       </c>
-      <c r="B20" s="87">
+      <c r="B20" s="86">
         <v>0.1</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="71" t="s">
+      <c r="A21" s="70" t="s">
         <v>66</v>
       </c>
-      <c r="B21" s="73">
+      <c r="B21" s="72">
         <v>5</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="72" t="s">
+      <c r="A22" s="71" t="s">
         <v>79</v>
       </c>
-      <c r="B22" s="74">
+      <c r="B22" s="73">
         <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="63" t="s">
+      <c r="A23" s="62" t="s">
         <v>55</v>
       </c>
-      <c r="B23" s="70" t="s">
+      <c r="B23" s="69" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="24" spans="1:10" s="46" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="64" t="s">
+    <row r="24" spans="1:10" s="45" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="63" t="s">
         <v>46</v>
       </c>
-      <c r="B24" s="46" t="s">
+      <c r="B24" s="45" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="52" t="s">
+      <c r="A25" s="51" t="s">
         <v>45</v>
       </c>
-      <c r="B25" s="43"/>
-      <c r="C25" s="43"/>
-      <c r="D25" s="43"/>
-      <c r="E25" s="44"/>
-      <c r="F25" s="45"/>
-      <c r="G25" s="45"/>
-      <c r="H25" s="45"/>
-      <c r="I25" s="45"/>
-      <c r="J25" s="45"/>
+      <c r="B25" s="42"/>
+      <c r="C25" s="42"/>
+      <c r="D25" s="42"/>
+      <c r="E25" s="43"/>
+      <c r="F25" s="44"/>
+      <c r="G25" s="44"/>
+      <c r="H25" s="44"/>
+      <c r="I25" s="44"/>
+      <c r="J25" s="44"/>
     </row>
   </sheetData>
   <dataValidations xWindow="363" yWindow="440" count="9">
@@ -2769,117 +2784,117 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="48.28515625" style="57" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.85546875" style="60" customWidth="1"/>
-    <col min="3" max="3" width="84.28515625" style="55" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.7109375" style="55" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="55"/>
+    <col min="1" max="1" width="48.28515625" style="56" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" style="59" customWidth="1"/>
+    <col min="3" max="3" width="84.28515625" style="54" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" style="54" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="54"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="61" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="61" t="s">
+    <row r="1" spans="1:4" s="60" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="60" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="62" t="s">
+      <c r="B1" s="61" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="61" t="s">
+      <c r="C1" s="60" t="s">
         <v>48</v>
       </c>
-      <c r="D1" s="61" t="s">
+      <c r="D1" s="60" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="54" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="53" t="s">
+    <row r="2" spans="1:4" s="53" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="58">
+      <c r="B2" s="57">
         <v>6.7</v>
       </c>
-      <c r="C2" s="54" t="s">
+      <c r="C2" s="53" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="53" t="s">
+      <c r="A3" s="52" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="58">
+      <c r="B3" s="57">
         <v>26</v>
       </c>
-      <c r="C3" s="55" t="s">
+      <c r="C3" s="54" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="53" t="s">
+      <c r="A4" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="58">
+      <c r="B4" s="57">
         <v>4</v>
       </c>
-      <c r="C4" s="55" t="s">
+      <c r="C4" s="54" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="53" t="s">
+      <c r="A5" s="52" t="s">
         <v>80</v>
       </c>
-      <c r="B5" s="58">
+      <c r="B5" s="57">
         <v>1945</v>
       </c>
-      <c r="C5" s="55" t="s">
+      <c r="C5" s="54" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="53" t="s">
+      <c r="A6" s="52" t="s">
         <v>81</v>
       </c>
-      <c r="B6" s="58">
+      <c r="B6" s="57">
         <v>1955</v>
       </c>
-      <c r="C6" s="55" t="s">
+      <c r="C6" s="54" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="53" t="s">
+      <c r="A7" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="58">
+      <c r="B7" s="57">
         <v>2050</v>
       </c>
-      <c r="C7" s="55" t="s">
+      <c r="C7" s="54" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="53" t="s">
+      <c r="A8" s="52" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="58">
+      <c r="B8" s="57">
         <v>2</v>
       </c>
-      <c r="C8" s="55" t="s">
+      <c r="C8" s="54" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="56" t="s">
+      <c r="A9" s="55" t="s">
         <v>84</v>
       </c>
-      <c r="B9" s="59">
+      <c r="B9" s="58">
         <v>0.32</v>
       </c>
-      <c r="C9" s="55" t="s">
+      <c r="C9" s="54" t="s">
         <v>77</v>
       </c>
     </row>
@@ -2894,13 +2909,13 @@
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:BC31"/>
+  <dimension ref="A1:BF31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="AH2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="X29" sqref="X29"/>
+      <selection pane="bottomRight" activeCell="BF14" sqref="BF14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2933,7 +2948,7 @@
     <col min="54" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:55" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:58" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>16</v>
       </c>
@@ -3099,8 +3114,14 @@
       <c r="BC1" s="5" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="2" spans="1:55" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="BE1" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="BF1" s="5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="1:58" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -3166,7 +3187,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="3" spans="1:55" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:58" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
         <v>17</v>
       </c>
@@ -3174,7 +3195,7 @@
         <v>23</v>
       </c>
       <c r="C3" s="6"/>
-      <c r="D3" s="89" t="s">
+      <c r="D3" s="88" t="s">
         <v>23</v>
       </c>
       <c r="H3" s="7">
@@ -3193,7 +3214,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:55" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:58" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="19" t="s">
         <v>9</v>
       </c>
@@ -3252,7 +3273,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:55" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:58" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
         <v>18</v>
       </c>
@@ -3260,7 +3281,7 @@
         <v>23</v>
       </c>
       <c r="C5" s="8"/>
-      <c r="D5" s="89" t="s">
+      <c r="D5" s="88" t="s">
         <v>23</v>
       </c>
       <c r="F5" s="9">
@@ -3270,7 +3291,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:55" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:58" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
         <v>10</v>
       </c>
@@ -3307,8 +3328,11 @@
       <c r="BC6" s="11">
         <v>85</v>
       </c>
-    </row>
-    <row r="7" spans="1:55" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="BE6" s="11">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="7" spans="1:58" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
         <v>19</v>
       </c>
@@ -3316,7 +3340,7 @@
         <v>23</v>
       </c>
       <c r="C7" s="10"/>
-      <c r="D7" s="89" t="s">
+      <c r="D7" s="88" t="s">
         <v>23</v>
       </c>
       <c r="G7" s="11">
@@ -3332,7 +3356,7 @@
         <v>4049504</v>
       </c>
     </row>
-    <row r="8" spans="1:55" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:58" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="21" t="s">
         <v>3</v>
       </c>
@@ -3358,7 +3382,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:55" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:58" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="21" t="s">
         <v>20</v>
       </c>
@@ -3366,14 +3390,14 @@
         <v>23</v>
       </c>
       <c r="C9" s="12"/>
-      <c r="D9" s="89" t="s">
+      <c r="D9" s="88" t="s">
         <v>23</v>
       </c>
       <c r="X9" s="13">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:55" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:58" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="22" t="s">
         <v>11</v>
       </c>
@@ -3399,7 +3423,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:55" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:58" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="22" t="s">
         <v>21</v>
       </c>
@@ -3407,14 +3431,14 @@
         <v>23</v>
       </c>
       <c r="C11" s="14"/>
-      <c r="D11" s="89" t="s">
+      <c r="D11" s="88" t="s">
         <v>23</v>
       </c>
       <c r="X11" s="15">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:55" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:58" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="23" t="s">
         <v>12</v>
       </c>
@@ -3443,7 +3467,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="13" spans="1:55" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:58" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="23" t="s">
         <v>22</v>
       </c>
@@ -3451,14 +3475,14 @@
         <v>23</v>
       </c>
       <c r="C13" s="16"/>
-      <c r="D13" s="89" t="s">
+      <c r="D13" s="88" t="s">
         <v>23</v>
       </c>
       <c r="X13" s="17">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:55" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:58" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="21" t="s">
         <v>24</v>
       </c>
@@ -3506,8 +3530,11 @@
       <c r="BC14" s="13">
         <v>90</v>
       </c>
-    </row>
-    <row r="15" spans="1:55" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="BF14" s="13">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="15" spans="1:58" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="21" t="s">
         <v>25</v>
       </c>
@@ -3515,7 +3542,7 @@
         <v>23</v>
       </c>
       <c r="C15" s="12"/>
-      <c r="D15" s="89" t="s">
+      <c r="D15" s="88" t="s">
         <v>23</v>
       </c>
       <c r="I15" s="13">
@@ -3534,7 +3561,7 @@
         <v>52431253</v>
       </c>
     </row>
-    <row r="16" spans="1:55" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:58" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="21" t="s">
         <v>26</v>
       </c>
@@ -3588,7 +3615,7 @@
         <v>23</v>
       </c>
       <c r="C17" s="12"/>
-      <c r="D17" s="89" t="s">
+      <c r="D17" s="88" t="s">
         <v>23</v>
       </c>
       <c r="I17" s="13">
@@ -3652,7 +3679,7 @@
         <v>23</v>
       </c>
       <c r="C19" s="26"/>
-      <c r="D19" s="89" t="s">
+      <c r="D19" s="88" t="s">
         <v>23</v>
       </c>
       <c r="I19" s="27">
@@ -3725,7 +3752,7 @@
         <v>23</v>
       </c>
       <c r="C21" s="26"/>
-      <c r="D21" s="89" t="s">
+      <c r="D21" s="88" t="s">
         <v>23</v>
       </c>
       <c r="I21" s="27">
@@ -3789,7 +3816,7 @@
         <v>23</v>
       </c>
       <c r="C23" s="8"/>
-      <c r="D23" s="89" t="s">
+      <c r="D23" s="88" t="s">
         <v>23</v>
       </c>
       <c r="I23" s="9">
@@ -3862,7 +3889,7 @@
         <v>23</v>
       </c>
       <c r="C25" s="8"/>
-      <c r="D25" s="89" t="s">
+      <c r="D25" s="88" t="s">
         <v>23</v>
       </c>
       <c r="I25" s="9">
@@ -3872,71 +3899,71 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:52" s="82" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="80" t="s">
+    <row r="26" spans="1:52" s="81" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="79" t="s">
         <v>67</v>
       </c>
-      <c r="B26" s="81" t="s">
+      <c r="B26" s="80" t="s">
         <v>13</v>
       </c>
-      <c r="C26" s="81">
+      <c r="C26" s="80">
         <v>1</v>
       </c>
-      <c r="D26" s="81" t="s">
+      <c r="D26" s="80" t="s">
         <v>13</v>
       </c>
-      <c r="E26" s="82">
+      <c r="E26" s="81">
         <f>1/26</f>
         <v>3.8461538461538464E-2</v>
       </c>
-      <c r="X26" s="82">
+      <c r="X26" s="81">
         <v>1</v>
       </c>
-      <c r="AF26" s="83"/>
-      <c r="AG26" s="83"/>
-      <c r="AH26" s="83"/>
-      <c r="AI26" s="83"/>
-      <c r="AJ26" s="83"/>
-      <c r="AK26" s="83"/>
-      <c r="AL26" s="83"/>
-      <c r="AM26" s="83"/>
-      <c r="AN26" s="83"/>
-      <c r="AO26" s="83"/>
-      <c r="AP26" s="83"/>
-      <c r="AQ26" s="83"/>
-      <c r="AR26" s="83"/>
-      <c r="AS26" s="83"/>
-      <c r="AT26" s="83"/>
-      <c r="AU26" s="83"/>
-      <c r="AV26" s="83"/>
-      <c r="AW26" s="83"/>
-      <c r="AX26" s="83"/>
-      <c r="AY26" s="83"/>
-      <c r="AZ26" s="82">
+      <c r="AF26" s="82"/>
+      <c r="AG26" s="82"/>
+      <c r="AH26" s="82"/>
+      <c r="AI26" s="82"/>
+      <c r="AJ26" s="82"/>
+      <c r="AK26" s="82"/>
+      <c r="AL26" s="82"/>
+      <c r="AM26" s="82"/>
+      <c r="AN26" s="82"/>
+      <c r="AO26" s="82"/>
+      <c r="AP26" s="82"/>
+      <c r="AQ26" s="82"/>
+      <c r="AR26" s="82"/>
+      <c r="AS26" s="82"/>
+      <c r="AT26" s="82"/>
+      <c r="AU26" s="82"/>
+      <c r="AV26" s="82"/>
+      <c r="AW26" s="82"/>
+      <c r="AX26" s="82"/>
+      <c r="AY26" s="82"/>
+      <c r="AZ26" s="81">
         <v>0.04</v>
       </c>
     </row>
-    <row r="27" spans="1:52" s="82" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="80" t="s">
+    <row r="27" spans="1:52" s="81" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="79" t="s">
         <v>68</v>
       </c>
-      <c r="B27" s="81" t="s">
+      <c r="B27" s="80" t="s">
         <v>23</v>
       </c>
-      <c r="C27" s="81"/>
-      <c r="D27" s="89" t="s">
+      <c r="C27" s="80"/>
+      <c r="D27" s="88" t="s">
         <v>23</v>
       </c>
-      <c r="I27" s="82">
+      <c r="I27" s="81">
         <v>0</v>
       </c>
-      <c r="R27" s="82">
+      <c r="R27" s="81">
         <v>532947</v>
       </c>
-      <c r="X27" s="82">
+      <c r="X27" s="81">
         <v>9283747</v>
       </c>
-      <c r="AZ27" s="82">
+      <c r="AZ27" s="81">
         <v>739284639</v>
       </c>
     </row>
@@ -3950,20 +3977,20 @@
       <c r="C28" s="6">
         <v>1</v>
       </c>
-      <c r="D28" s="89" t="s">
+      <c r="D28" s="88" t="s">
         <v>14</v>
       </c>
-      <c r="AB28" s="88"/>
-      <c r="AL28" s="88"/>
-      <c r="AR28" s="88"/>
-      <c r="AS28" s="88"/>
-      <c r="AT28" s="88"/>
-      <c r="AU28" s="88"/>
-      <c r="AV28" s="88"/>
-      <c r="AW28" s="88"/>
-      <c r="AX28" s="88"/>
-      <c r="AY28" s="88"/>
-      <c r="AZ28" s="88"/>
+      <c r="AB28" s="87"/>
+      <c r="AL28" s="87"/>
+      <c r="AR28" s="87"/>
+      <c r="AS28" s="87"/>
+      <c r="AT28" s="87"/>
+      <c r="AU28" s="87"/>
+      <c r="AV28" s="87"/>
+      <c r="AW28" s="87"/>
+      <c r="AX28" s="87"/>
+      <c r="AY28" s="87"/>
+      <c r="AZ28" s="87"/>
     </row>
     <row r="29" spans="1:52" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="18" t="s">
@@ -3978,49 +4005,49 @@
       <c r="D29" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="J29" s="88"/>
-      <c r="K29" s="88"/>
-      <c r="L29" s="88"/>
-      <c r="M29" s="88"/>
-      <c r="N29" s="88"/>
-      <c r="O29" s="88"/>
-      <c r="P29" s="88"/>
-      <c r="Q29" s="88"/>
-      <c r="R29" s="88"/>
-      <c r="S29" s="88"/>
-      <c r="T29" s="88"/>
-      <c r="U29" s="88"/>
-      <c r="V29" s="88"/>
-      <c r="W29" s="88"/>
-      <c r="X29" s="88"/>
-      <c r="Y29" s="88"/>
-      <c r="Z29" s="88"/>
-      <c r="AA29" s="88"/>
-      <c r="AB29" s="88"/>
-      <c r="AC29" s="88"/>
-      <c r="AD29" s="88"/>
-      <c r="AE29" s="88"/>
-      <c r="AF29" s="88"/>
-      <c r="AG29" s="88"/>
-      <c r="AH29" s="88"/>
-      <c r="AI29" s="88"/>
-      <c r="AJ29" s="88"/>
-      <c r="AK29" s="88"/>
-      <c r="AL29" s="88"/>
-      <c r="AM29" s="88"/>
-      <c r="AN29" s="88"/>
-      <c r="AO29" s="88"/>
-      <c r="AP29" s="88"/>
-      <c r="AQ29" s="88"/>
-      <c r="AR29" s="88"/>
-      <c r="AS29" s="88"/>
-      <c r="AT29" s="88"/>
-      <c r="AU29" s="88"/>
-      <c r="AV29" s="88"/>
-      <c r="AW29" s="88"/>
-      <c r="AX29" s="88"/>
-      <c r="AY29" s="88"/>
-      <c r="AZ29" s="88"/>
+      <c r="J29" s="87"/>
+      <c r="K29" s="87"/>
+      <c r="L29" s="87"/>
+      <c r="M29" s="87"/>
+      <c r="N29" s="87"/>
+      <c r="O29" s="87"/>
+      <c r="P29" s="87"/>
+      <c r="Q29" s="87"/>
+      <c r="R29" s="87"/>
+      <c r="S29" s="87"/>
+      <c r="T29" s="87"/>
+      <c r="U29" s="87"/>
+      <c r="V29" s="87"/>
+      <c r="W29" s="87"/>
+      <c r="X29" s="87"/>
+      <c r="Y29" s="87"/>
+      <c r="Z29" s="87"/>
+      <c r="AA29" s="87"/>
+      <c r="AB29" s="87"/>
+      <c r="AC29" s="87"/>
+      <c r="AD29" s="87"/>
+      <c r="AE29" s="87"/>
+      <c r="AF29" s="87"/>
+      <c r="AG29" s="87"/>
+      <c r="AH29" s="87"/>
+      <c r="AI29" s="87"/>
+      <c r="AJ29" s="87"/>
+      <c r="AK29" s="87"/>
+      <c r="AL29" s="87"/>
+      <c r="AM29" s="87"/>
+      <c r="AN29" s="87"/>
+      <c r="AO29" s="87"/>
+      <c r="AP29" s="87"/>
+      <c r="AQ29" s="87"/>
+      <c r="AR29" s="87"/>
+      <c r="AS29" s="87"/>
+      <c r="AT29" s="87"/>
+      <c r="AU29" s="87"/>
+      <c r="AV29" s="87"/>
+      <c r="AW29" s="87"/>
+      <c r="AX29" s="87"/>
+      <c r="AY29" s="87"/>
+      <c r="AZ29" s="87"/>
     </row>
     <row r="30" spans="1:52" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="18" t="s">
@@ -4046,7 +4073,7 @@
       <c r="C31" s="6">
         <v>1</v>
       </c>
-      <c r="D31" s="89" t="str">
+      <c r="D31" s="88" t="str">
         <f>D30</f>
         <v>no</v>
       </c>

</xml_diff>

<commit_message>
Plotting of scaling parameters by scenario
Sort of done, although a fair amount of inelegant code that could be
improved.
</commit_message>
<xml_diff>
--- a/autumn/xls/programs_fiji.xlsx
+++ b/autumn/xls/programs_fiji.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="315" windowWidth="20370" windowHeight="7530" tabRatio="807" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="315" windowWidth="20370" windowHeight="7530" tabRatio="807"/>
   </bookViews>
   <sheets>
     <sheet name="model_attributes" sheetId="4" r:id="rId1"/>
@@ -2444,8 +2444,8 @@
   </sheetPr>
   <dimension ref="A1:J25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2546,8 +2546,12 @@
       <c r="C9" s="94">
         <v>2</v>
       </c>
-      <c r="D9" s="94"/>
-      <c r="E9" s="94"/>
+      <c r="D9" s="94">
+        <v>3</v>
+      </c>
+      <c r="E9" s="94">
+        <v>4</v>
+      </c>
       <c r="F9" s="94"/>
       <c r="G9" s="94"/>
       <c r="H9" s="94"/>
@@ -2627,7 +2631,7 @@
         <v>75</v>
       </c>
       <c r="B18" s="35">
-        <v>2019</v>
+        <v>2020</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
@@ -2779,7 +2783,7 @@
   </sheetPr>
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
@@ -2908,7 +2912,7 @@
   <dimension ref="A1:BF31"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="N2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="AF2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="Y13" sqref="Y13"/>

</xml_diff>

<commit_message>
Allow for Runge-Kutta integration
Add Runge-Kutta to drop-down list. Also renamed methods to be strictly
snake case.
</commit_message>
<xml_diff>
--- a/autumn/xls/programs_fiji.xlsx
+++ b/autumn/xls/programs_fiji.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="94">
   <si>
     <t>program_rate_restart_presenting</t>
   </si>
@@ -296,6 +296,9 @@
   </si>
   <si>
     <t>scenario_4</t>
+  </si>
+  <si>
+    <t>runge_kutta</t>
   </si>
 </sst>
 </file>
@@ -2445,7 +2448,7 @@
   <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2766,7 +2769,7 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Integration" prompt="Which integration package. Explicitly coded or Scipy's integration package.">
           <x14:formula1>
-            <xm:f>dropdown_lists!$C$2:$C$3</xm:f>
+            <xm:f>dropdown_lists!$C$2:$C$4</xm:f>
           </x14:formula1>
           <xm:sqref>B23</xm:sqref>
         </x14:dataValidation>
@@ -4123,7 +4126,7 @@
   <dimension ref="A2:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4154,6 +4157,9 @@
       <c r="A4" t="s">
         <v>23</v>
       </c>
+      <c r="C4" t="s">
+        <v>93</v>
+      </c>
     </row>
   </sheetData>
   <sheetProtection password="D0CB" sheet="1" objects="1" scenarios="1"/>

</xml_diff>

<commit_message>
Pare off a control panel spreadsheet
Move what was previously model_attributes to a different spreadsheet,
which can now be used as the control panel.
</commit_message>
<xml_diff>
--- a/autumn/xls/programs_fiji.xlsx
+++ b/autumn/xls/programs_fiji.xlsx
@@ -7,17 +7,16 @@
     <workbookView xWindow="120" yWindow="315" windowWidth="20370" windowHeight="7530" tabRatio="807"/>
   </bookViews>
   <sheets>
-    <sheet name="model_attributes" sheetId="4" r:id="rId1"/>
-    <sheet name="miscellaneous_constants" sheetId="1" r:id="rId2"/>
-    <sheet name="time_variants" sheetId="2" r:id="rId3"/>
-    <sheet name="dropdown_lists" sheetId="3" r:id="rId4"/>
+    <sheet name="miscellaneous_constants" sheetId="1" r:id="rId1"/>
+    <sheet name="time_variants" sheetId="2" r:id="rId2"/>
+    <sheet name="dropdown_lists" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="64">
   <si>
     <t>program_rate_restart_presenting</t>
   </si>
@@ -127,42 +126,6 @@
     <t>program_cost_treatment_death_xdr</t>
   </si>
   <si>
-    <t>attribute</t>
-  </si>
-  <si>
-    <t>n_comorbidities</t>
-  </si>
-  <si>
-    <t>start_time</t>
-  </si>
-  <si>
-    <t>recent_time</t>
-  </si>
-  <si>
-    <t>n_organs</t>
-  </si>
-  <si>
-    <t>n_strains</t>
-  </si>
-  <si>
-    <t>is_lowquality</t>
-  </si>
-  <si>
-    <t>is_amplification</t>
-  </si>
-  <si>
-    <t>is_misassignment</t>
-  </si>
-  <si>
-    <t>age_breakpoints</t>
-  </si>
-  <si>
-    <t>age_stratification</t>
-  </si>
-  <si>
-    <t>consecutive age breakpoints</t>
-  </si>
-  <si>
     <t>description</t>
   </si>
   <si>
@@ -184,42 +147,12 @@
     <t>Rate at which patients change from the low quality to the high quality health system</t>
   </si>
   <si>
-    <t>integration</t>
-  </si>
-  <si>
     <t>explicit</t>
   </si>
   <si>
     <t>scipy</t>
   </si>
   <si>
-    <t>single value needed</t>
-  </si>
-  <si>
-    <t>first value</t>
-  </si>
-  <si>
-    <t>value at iteration</t>
-  </si>
-  <si>
-    <t>value at second iteration</t>
-  </si>
-  <si>
-    <t>population</t>
-  </si>
-  <si>
-    <t>susceptible_fully</t>
-  </si>
-  <si>
-    <t>active</t>
-  </si>
-  <si>
-    <t>start_compartments</t>
-  </si>
-  <si>
-    <t>fitting_method</t>
-  </si>
-  <si>
     <t>program_timeperiod_await_treatment</t>
   </si>
   <si>
@@ -229,36 +162,15 @@
     <t>scenario_1</t>
   </si>
   <si>
-    <t>scenario_end_time</t>
-  </si>
-  <si>
-    <t>current_time</t>
-  </si>
-  <si>
-    <t>scenarios_to_run</t>
-  </si>
-  <si>
     <t>scenario_2</t>
   </si>
   <si>
-    <t>scenario_start_time</t>
-  </si>
-  <si>
-    <t>scenario_full_time</t>
-  </si>
-  <si>
-    <t>time_step</t>
-  </si>
-  <si>
     <t>Proportion of TB-related deaths not already under treatment that are correctly reported as such</t>
   </si>
   <si>
     <t>smoothness</t>
   </si>
   <si>
-    <t>default_smoothness</t>
-  </si>
-  <si>
     <t>start_mdr_introduce_period</t>
   </si>
   <si>
@@ -287,9 +199,6 @@
   </si>
   <si>
     <t>epi_prop_smearneg</t>
-  </si>
-  <si>
-    <t>is_additional_diagnostics</t>
   </si>
   <si>
     <t>scenario_3</t>
@@ -308,7 +217,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -386,14 +295,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="5" tint="-0.499984740745262"/>
       <name val="Calibri"/>
@@ -401,7 +302,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="18">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -493,18 +394,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -595,122 +490,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="664">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1378,7 +1157,7 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="95">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1411,33 +1190,13 @@
     <xf numFmtId="0" fontId="10" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="6" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
@@ -1445,39 +1204,12 @@
     <xf numFmtId="2" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="8" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="11" fontId="0" fillId="8" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="15" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="15" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="664">
     <cellStyle name="Comma 2" xfId="5"/>
@@ -2443,462 +2175,123 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
-    <tabColor theme="3" tint="0.39997558519241921"/>
+    <tabColor theme="9" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:J25"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.7109375" style="50" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="48.28515625" style="36" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" style="39" customWidth="1"/>
+    <col min="3" max="3" width="84.28515625" style="34" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" style="34" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="34"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="32" t="s">
+    <row r="1" spans="1:4" s="40" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="40" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="41" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="40" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="33" t="s">
-        <v>59</v>
-      </c>
-      <c r="C1" s="33" t="s">
-        <v>60</v>
-      </c>
-      <c r="D1" s="32" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="46" t="s">
+      <c r="D1" s="40" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="37">
+        <v>6.7</v>
+      </c>
+      <c r="C2" s="33" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="32" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="37">
+        <v>26</v>
+      </c>
+      <c r="C3" s="34" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="37">
+        <v>4</v>
+      </c>
+      <c r="C4" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="B2" s="36">
-        <v>3</v>
-      </c>
-      <c r="C2" s="36"/>
-      <c r="D2" s="34"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="46" t="s">
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="32" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5" s="37">
+        <v>1945</v>
+      </c>
+      <c r="C5" s="34" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="32" t="s">
+        <v>52</v>
+      </c>
+      <c r="B6" s="37">
+        <v>1955</v>
+      </c>
+      <c r="C6" s="34" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="37">
+        <v>2050</v>
+      </c>
+      <c r="C7" s="34" t="s">
         <v>41</v>
       </c>
-      <c r="B3" s="36">
-        <v>0</v>
-      </c>
-      <c r="C3" s="36"/>
-      <c r="D3" s="34"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="47" t="s">
-        <v>37</v>
-      </c>
-      <c r="B4" s="37">
-        <v>0</v>
-      </c>
-      <c r="C4" s="37"/>
-      <c r="D4" s="38"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="49" t="s">
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="37">
+        <v>2</v>
+      </c>
+      <c r="C8" s="34" t="s">
         <v>42</v>
       </c>
-      <c r="B5" s="39" t="b">
-        <v>0</v>
-      </c>
-      <c r="C5" s="40"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="89" t="s">
-        <v>43</v>
-      </c>
-      <c r="B6" s="91" t="b">
-        <v>0</v>
-      </c>
-      <c r="C6" s="41"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="89" t="s">
-        <v>44</v>
-      </c>
-      <c r="B7" s="91" t="b">
-        <v>0</v>
-      </c>
-      <c r="C7" s="41"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="90" t="s">
-        <v>90</v>
-      </c>
-      <c r="B8" s="91" t="b">
-        <v>0</v>
-      </c>
-      <c r="C8" s="41"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="92" t="s">
-        <v>72</v>
-      </c>
-      <c r="B9" s="93">
-        <v>1</v>
-      </c>
-      <c r="C9" s="94">
-        <v>2</v>
-      </c>
-      <c r="D9" s="94">
-        <v>3</v>
-      </c>
-      <c r="E9" s="94">
-        <v>4</v>
-      </c>
-      <c r="F9" s="94"/>
-      <c r="G9" s="94"/>
-      <c r="H9" s="94"/>
-      <c r="I9" s="94"/>
-      <c r="J9" s="83"/>
-    </row>
-    <row r="10" spans="1:10" s="77" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="67" t="s">
-        <v>65</v>
-      </c>
-      <c r="B10" s="68" t="s">
-        <v>62</v>
-      </c>
-      <c r="C10" s="68"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="74" t="s">
-        <v>63</v>
-      </c>
-      <c r="B11" s="78">
-        <v>200000</v>
-      </c>
-      <c r="C11" s="44"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="75" t="s">
-        <v>64</v>
-      </c>
-      <c r="B12" s="76">
-        <v>3</v>
-      </c>
-      <c r="C12" s="44"/>
-    </row>
-    <row r="13" spans="1:10" s="64" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="67" t="s">
-        <v>36</v>
-      </c>
-      <c r="B13" s="68" t="s">
-        <v>58</v>
-      </c>
-      <c r="C13" s="44"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="65" t="s">
-        <v>38</v>
-      </c>
-      <c r="B14" s="66">
-        <v>1909</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="B15" s="35">
-        <v>1990</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="48" t="s">
-        <v>71</v>
-      </c>
-      <c r="B16" s="35">
-        <v>2015</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="48" t="s">
-        <v>74</v>
-      </c>
-      <c r="B17" s="35">
-        <v>2016</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="48" t="s">
-        <v>75</v>
-      </c>
-      <c r="B18" s="35">
-        <v>2020</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="48" t="s">
-        <v>70</v>
-      </c>
-      <c r="B19" s="84">
-        <v>2035</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="85" t="s">
-        <v>76</v>
-      </c>
-      <c r="B20" s="86">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="70" t="s">
-        <v>66</v>
-      </c>
-      <c r="B21" s="72">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="71" t="s">
-        <v>79</v>
-      </c>
-      <c r="B22" s="73">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="62" t="s">
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="35" t="s">
         <v>55</v>
       </c>
-      <c r="B23" s="69" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" s="45" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="63" t="s">
-        <v>46</v>
-      </c>
-      <c r="B24" s="45" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="51" t="s">
-        <v>45</v>
-      </c>
-      <c r="B25" s="42"/>
-      <c r="C25" s="42"/>
-      <c r="D25" s="42"/>
-      <c r="E25" s="43"/>
-      <c r="F25" s="44"/>
-      <c r="G25" s="44"/>
-      <c r="H25" s="44"/>
-      <c r="I25" s="44"/>
-      <c r="J25" s="44"/>
-    </row>
-  </sheetData>
-  <dataValidations xWindow="363" yWindow="440" count="9">
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Time to do recent graphs from" prompt="Calendar year that output graphs for recent time start from." sqref="B15:B18">
-      <formula1>-10000</formula1>
-      <formula2>3000</formula2>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Time to start model" prompt="Enter the calendar year that the model runs from." sqref="B14">
-      <formula1>-10000</formula1>
-      <formula2>3000</formula2>
-    </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Organ stratification" prompt="Number of organs allowed (0: no stratification, 2: smear-positive and smear-negative, 3: smear-positive, smear-negative and extra-pulmonary)." sqref="C2:D2">
-      <formula1>0</formula1>
-      <formula2>3</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Strains" prompt="Number of strains (0: single strain model, 2: DS-TB and MDR-TB, 3: DS-TB, MDR-TB and XDR-TB)." sqref="B3:D3"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Comorbidities" prompt="Number of comorbidities (currently up to three, but will be revised as model develops)." sqref="B4:D4"/>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Function smoothness" prompt="From zero up, with zero being exact fit and higher values being greater smoothness." sqref="B21:B22">
-      <formula1>0</formula1>
-      <formula2>1000</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Age breakpoints" prompt="Enter consecutively increasing age breakpoints to create age strata. (Can enter any number, don't enter zero and no upper limit is needed.)" sqref="B25:E25"/>
-    <dataValidation allowBlank="1" showErrorMessage="1" sqref="B10:C13"/>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Organ stratification" prompt="Number of organs allowed (0: no stratification, 2: smear-positive and smear-negative, 3: smear-positive, smear-negative and extra-pulmonary). WARNING: No organ stratification should be selected if this is zero (or one)." sqref="B2">
-      <formula1>0</formula1>
-      <formula2>3</formula2>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xWindow="363" yWindow="440" count="7">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Low quality care access" prompt="Whether to incorporate low quality care access into the model.">
-          <x14:formula1>
-            <xm:f>dropdown_lists!$B$2:$B$3</xm:f>
-          </x14:formula1>
-          <xm:sqref>B5</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Low quality care access" prompt="Whether to incorporate low quality care access into the model.">
-          <x14:formula1>
-            <xm:f>dropdown_lists!$B$2:$B$4</xm:f>
-          </x14:formula1>
-          <xm:sqref>C5</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Amplification" prompt="Whether amplification to progressively more resistant strains permitted.">
-          <x14:formula1>
-            <xm:f>dropdown_lists!$B$2:$B$4</xm:f>
-          </x14:formula1>
-          <xm:sqref>C6</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Amplification" prompt="Whether amplification to progressively more resistant strains permitted.">
-          <x14:formula1>
-            <xm:f>dropdown_lists!$B$2:$B$3</xm:f>
-          </x14:formula1>
-          <xm:sqref>B6</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Misassignment" prompt="Whether patients can be incorrectly detected with the wrong strain.">
-          <x14:formula1>
-            <xm:f>dropdown_lists!$B$2:$B$3</xm:f>
-          </x14:formula1>
-          <xm:sqref>B7:B8</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Misassignment" prompt="Whether patients can be incorrectly detected with the wrong strain.">
-          <x14:formula1>
-            <xm:f>dropdown_lists!$B$2:$B$4</xm:f>
-          </x14:formula1>
-          <xm:sqref>C7:C8</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Integration" prompt="Which integration package. Explicitly coded or Scipy's integration package.">
-          <x14:formula1>
-            <xm:f>dropdown_lists!$C$2:$C$4</xm:f>
-          </x14:formula1>
-          <xm:sqref>B23</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <tabColor theme="9" tint="-0.249977111117893"/>
-  </sheetPr>
-  <dimension ref="A1:D9"/>
-  <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="48.28515625" style="56" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.85546875" style="59" customWidth="1"/>
-    <col min="3" max="3" width="84.28515625" style="54" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.7109375" style="54" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="54"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" s="60" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="60" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" s="61" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" s="60" t="s">
-        <v>48</v>
-      </c>
-      <c r="D1" s="60" t="s">
+      <c r="B9" s="38">
+        <v>0.2</v>
+      </c>
+      <c r="C9" s="34" t="s">
         <v>49</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="52" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="57">
-        <v>6.7</v>
-      </c>
-      <c r="C2" s="53" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="52" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="57">
-        <v>26</v>
-      </c>
-      <c r="C3" s="54" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="52" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="57">
-        <v>4</v>
-      </c>
-      <c r="C4" s="54" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="52" t="s">
-        <v>80</v>
-      </c>
-      <c r="B5" s="57">
-        <v>1945</v>
-      </c>
-      <c r="C5" s="54" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="52" t="s">
-        <v>81</v>
-      </c>
-      <c r="B6" s="57">
-        <v>1955</v>
-      </c>
-      <c r="C6" s="54" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="52" t="s">
-        <v>1</v>
-      </c>
-      <c r="B7" s="57">
-        <v>2050</v>
-      </c>
-      <c r="C7" s="54" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="52" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" s="57">
-        <v>2</v>
-      </c>
-      <c r="C8" s="54" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="55" t="s">
-        <v>84</v>
-      </c>
-      <c r="B9" s="58">
-        <v>0.2</v>
-      </c>
-      <c r="C9" s="54" t="s">
-        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -2907,7 +2300,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
@@ -2959,10 +2352,10 @@
         <v>15</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>78</v>
+        <v>50</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>85</v>
+        <v>56</v>
       </c>
       <c r="E1" s="5">
         <v>1920</v>
@@ -3112,16 +2505,16 @@
         <v>2015</v>
       </c>
       <c r="BB1" s="5" t="s">
-        <v>69</v>
+        <v>47</v>
       </c>
       <c r="BC1" s="5" t="s">
-        <v>73</v>
+        <v>48</v>
       </c>
       <c r="BE1" s="5" t="s">
-        <v>91</v>
+        <v>61</v>
       </c>
       <c r="BF1" s="5" t="s">
-        <v>92</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:58" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -3196,7 +2589,7 @@
         <v>23</v>
       </c>
       <c r="C3" s="6"/>
-      <c r="D3" s="88" t="s">
+      <c r="D3" s="47" t="s">
         <v>23</v>
       </c>
       <c r="H3" s="7">
@@ -3279,7 +2672,7 @@
         <v>23</v>
       </c>
       <c r="C5" s="8"/>
-      <c r="D5" s="88" t="s">
+      <c r="D5" s="47" t="s">
         <v>23</v>
       </c>
       <c r="F5" s="9">
@@ -3335,7 +2728,7 @@
         <v>23</v>
       </c>
       <c r="C7" s="10"/>
-      <c r="D7" s="88" t="s">
+      <c r="D7" s="47" t="s">
         <v>23</v>
       </c>
       <c r="G7" s="11">
@@ -3382,7 +2775,7 @@
         <v>23</v>
       </c>
       <c r="C9" s="12"/>
-      <c r="D9" s="88" t="s">
+      <c r="D9" s="47" t="s">
         <v>23</v>
       </c>
       <c r="X9" s="13">
@@ -3420,7 +2813,7 @@
         <v>23</v>
       </c>
       <c r="C11" s="14"/>
-      <c r="D11" s="88" t="s">
+      <c r="D11" s="47" t="s">
         <v>23</v>
       </c>
       <c r="X11" s="15">
@@ -3461,7 +2854,7 @@
         <v>23</v>
       </c>
       <c r="C13" s="16"/>
-      <c r="D13" s="88" t="s">
+      <c r="D13" s="47" t="s">
         <v>23</v>
       </c>
       <c r="X13" s="17">
@@ -3528,7 +2921,7 @@
         <v>23</v>
       </c>
       <c r="C15" s="12"/>
-      <c r="D15" s="88" t="s">
+      <c r="D15" s="47" t="s">
         <v>23</v>
       </c>
       <c r="I15" s="13">
@@ -3601,7 +2994,7 @@
         <v>23</v>
       </c>
       <c r="C17" s="12"/>
-      <c r="D17" s="88" t="s">
+      <c r="D17" s="47" t="s">
         <v>23</v>
       </c>
       <c r="I17" s="13">
@@ -3665,7 +3058,7 @@
         <v>23</v>
       </c>
       <c r="C19" s="26"/>
-      <c r="D19" s="88" t="s">
+      <c r="D19" s="47" t="s">
         <v>23</v>
       </c>
       <c r="I19" s="27">
@@ -3738,7 +3131,7 @@
         <v>23</v>
       </c>
       <c r="C21" s="26"/>
-      <c r="D21" s="88" t="s">
+      <c r="D21" s="47" t="s">
         <v>23</v>
       </c>
       <c r="I21" s="27">
@@ -3802,7 +3195,7 @@
         <v>23</v>
       </c>
       <c r="C23" s="8"/>
-      <c r="D23" s="88" t="s">
+      <c r="D23" s="47" t="s">
         <v>23</v>
       </c>
       <c r="I23" s="9">
@@ -3875,7 +3268,7 @@
         <v>23</v>
       </c>
       <c r="C25" s="8"/>
-      <c r="D25" s="88" t="s">
+      <c r="D25" s="47" t="s">
         <v>23</v>
       </c>
       <c r="I25" s="9">
@@ -3885,74 +3278,74 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:52" s="81" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="79" t="s">
-        <v>67</v>
-      </c>
-      <c r="B26" s="80" t="s">
+    <row r="26" spans="1:52" s="44" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="42" t="s">
+        <v>45</v>
+      </c>
+      <c r="B26" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="C26" s="80">
+      <c r="C26" s="43">
         <v>1</v>
       </c>
-      <c r="D26" s="80" t="s">
+      <c r="D26" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="E26" s="81">
+      <c r="E26" s="44">
         <f>1/26</f>
         <v>3.8461538461538464E-2</v>
       </c>
-      <c r="AF26" s="82"/>
-      <c r="AG26" s="82"/>
-      <c r="AH26" s="82"/>
-      <c r="AI26" s="82"/>
-      <c r="AJ26" s="82"/>
-      <c r="AK26" s="82"/>
-      <c r="AL26" s="82"/>
-      <c r="AM26" s="82"/>
-      <c r="AN26" s="82"/>
-      <c r="AO26" s="82"/>
-      <c r="AP26" s="82"/>
-      <c r="AQ26" s="82"/>
-      <c r="AR26" s="82"/>
-      <c r="AS26" s="82"/>
-      <c r="AT26" s="82"/>
-      <c r="AU26" s="82"/>
-      <c r="AV26" s="82"/>
-      <c r="AW26" s="82"/>
-      <c r="AX26" s="82"/>
-      <c r="AY26" s="82"/>
-      <c r="AZ26" s="81">
+      <c r="AF26" s="45"/>
+      <c r="AG26" s="45"/>
+      <c r="AH26" s="45"/>
+      <c r="AI26" s="45"/>
+      <c r="AJ26" s="45"/>
+      <c r="AK26" s="45"/>
+      <c r="AL26" s="45"/>
+      <c r="AM26" s="45"/>
+      <c r="AN26" s="45"/>
+      <c r="AO26" s="45"/>
+      <c r="AP26" s="45"/>
+      <c r="AQ26" s="45"/>
+      <c r="AR26" s="45"/>
+      <c r="AS26" s="45"/>
+      <c r="AT26" s="45"/>
+      <c r="AU26" s="45"/>
+      <c r="AV26" s="45"/>
+      <c r="AW26" s="45"/>
+      <c r="AX26" s="45"/>
+      <c r="AY26" s="45"/>
+      <c r="AZ26" s="44">
         <v>0.04</v>
       </c>
     </row>
-    <row r="27" spans="1:52" s="81" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="79" t="s">
-        <v>68</v>
-      </c>
-      <c r="B27" s="80" t="s">
+    <row r="27" spans="1:52" s="44" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="42" t="s">
+        <v>46</v>
+      </c>
+      <c r="B27" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="C27" s="80"/>
-      <c r="D27" s="88" t="s">
+      <c r="C27" s="43"/>
+      <c r="D27" s="47" t="s">
         <v>23</v>
       </c>
-      <c r="I27" s="81">
+      <c r="I27" s="44">
         <v>0</v>
       </c>
-      <c r="R27" s="81">
+      <c r="R27" s="44">
         <v>532947</v>
       </c>
-      <c r="X27" s="81">
+      <c r="X27" s="44">
         <v>9283747</v>
       </c>
-      <c r="AZ27" s="81">
+      <c r="AZ27" s="44">
         <v>739284639</v>
       </c>
     </row>
     <row r="28" spans="1:52" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="18" t="s">
-        <v>86</v>
+        <v>57</v>
       </c>
       <c r="B28" s="6" t="s">
         <v>13</v>
@@ -3960,24 +3353,24 @@
       <c r="C28" s="6">
         <v>1</v>
       </c>
-      <c r="D28" s="88" t="s">
+      <c r="D28" s="47" t="s">
         <v>14</v>
       </c>
-      <c r="AB28" s="87"/>
-      <c r="AL28" s="87"/>
-      <c r="AR28" s="87"/>
-      <c r="AS28" s="87"/>
-      <c r="AT28" s="87"/>
-      <c r="AU28" s="87"/>
-      <c r="AV28" s="87"/>
-      <c r="AW28" s="87"/>
-      <c r="AX28" s="87"/>
-      <c r="AY28" s="87"/>
-      <c r="AZ28" s="87"/>
+      <c r="AB28" s="46"/>
+      <c r="AL28" s="46"/>
+      <c r="AR28" s="46"/>
+      <c r="AS28" s="46"/>
+      <c r="AT28" s="46"/>
+      <c r="AU28" s="46"/>
+      <c r="AV28" s="46"/>
+      <c r="AW28" s="46"/>
+      <c r="AX28" s="46"/>
+      <c r="AY28" s="46"/>
+      <c r="AZ28" s="46"/>
     </row>
     <row r="29" spans="1:52" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="18" t="s">
-        <v>87</v>
+        <v>58</v>
       </c>
       <c r="B29" s="6" t="s">
         <v>13</v>
@@ -3988,53 +3381,53 @@
       <c r="D29" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="J29" s="87"/>
-      <c r="K29" s="87"/>
-      <c r="L29" s="87"/>
-      <c r="M29" s="87"/>
-      <c r="N29" s="87"/>
-      <c r="O29" s="87"/>
-      <c r="P29" s="87"/>
-      <c r="Q29" s="87"/>
-      <c r="R29" s="87"/>
-      <c r="S29" s="87"/>
-      <c r="T29" s="87"/>
-      <c r="U29" s="87"/>
-      <c r="V29" s="87"/>
-      <c r="W29" s="87"/>
-      <c r="X29" s="87"/>
-      <c r="Y29" s="87"/>
-      <c r="Z29" s="87"/>
-      <c r="AA29" s="87"/>
-      <c r="AB29" s="87"/>
-      <c r="AC29" s="87"/>
-      <c r="AD29" s="87"/>
-      <c r="AE29" s="87"/>
-      <c r="AF29" s="87"/>
-      <c r="AG29" s="87"/>
-      <c r="AH29" s="87"/>
-      <c r="AI29" s="87"/>
-      <c r="AJ29" s="87"/>
-      <c r="AK29" s="87"/>
-      <c r="AL29" s="87"/>
-      <c r="AM29" s="87"/>
-      <c r="AN29" s="87"/>
-      <c r="AO29" s="87"/>
-      <c r="AP29" s="87"/>
-      <c r="AQ29" s="87"/>
-      <c r="AR29" s="87"/>
-      <c r="AS29" s="87"/>
-      <c r="AT29" s="87"/>
-      <c r="AU29" s="87"/>
-      <c r="AV29" s="87"/>
-      <c r="AW29" s="87"/>
-      <c r="AX29" s="87"/>
-      <c r="AY29" s="87"/>
-      <c r="AZ29" s="87"/>
+      <c r="J29" s="46"/>
+      <c r="K29" s="46"/>
+      <c r="L29" s="46"/>
+      <c r="M29" s="46"/>
+      <c r="N29" s="46"/>
+      <c r="O29" s="46"/>
+      <c r="P29" s="46"/>
+      <c r="Q29" s="46"/>
+      <c r="R29" s="46"/>
+      <c r="S29" s="46"/>
+      <c r="T29" s="46"/>
+      <c r="U29" s="46"/>
+      <c r="V29" s="46"/>
+      <c r="W29" s="46"/>
+      <c r="X29" s="46"/>
+      <c r="Y29" s="46"/>
+      <c r="Z29" s="46"/>
+      <c r="AA29" s="46"/>
+      <c r="AB29" s="46"/>
+      <c r="AC29" s="46"/>
+      <c r="AD29" s="46"/>
+      <c r="AE29" s="46"/>
+      <c r="AF29" s="46"/>
+      <c r="AG29" s="46"/>
+      <c r="AH29" s="46"/>
+      <c r="AI29" s="46"/>
+      <c r="AJ29" s="46"/>
+      <c r="AK29" s="46"/>
+      <c r="AL29" s="46"/>
+      <c r="AM29" s="46"/>
+      <c r="AN29" s="46"/>
+      <c r="AO29" s="46"/>
+      <c r="AP29" s="46"/>
+      <c r="AQ29" s="46"/>
+      <c r="AR29" s="46"/>
+      <c r="AS29" s="46"/>
+      <c r="AT29" s="46"/>
+      <c r="AU29" s="46"/>
+      <c r="AV29" s="46"/>
+      <c r="AW29" s="46"/>
+      <c r="AX29" s="46"/>
+      <c r="AY29" s="46"/>
+      <c r="AZ29" s="46"/>
     </row>
     <row r="30" spans="1:52" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="18" t="s">
-        <v>88</v>
+        <v>59</v>
       </c>
       <c r="B30" s="6" t="s">
         <v>13</v>
@@ -4048,7 +3441,7 @@
     </row>
     <row r="31" spans="1:52" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="18" t="s">
-        <v>89</v>
+        <v>60</v>
       </c>
       <c r="B31" s="6" t="s">
         <v>13</v>
@@ -4056,7 +3449,7 @@
       <c r="C31" s="6">
         <v>1</v>
       </c>
-      <c r="D31" s="88" t="str">
+      <c r="D31" s="47" t="str">
         <f>D30</f>
         <v>no</v>
       </c>
@@ -4118,7 +3511,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="0" tint="-4.9989318521683403E-2"/>
@@ -4139,7 +3532,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -4150,7 +3543,7 @@
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -4158,7 +3551,7 @@
         <v>23</v>
       </c>
       <c r="C4" t="s">
-        <v>93</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Some scenarios for Philippines analysis
</commit_message>
<xml_diff>
--- a/autumn/xls/programs_fiji.xlsx
+++ b/autumn/xls/programs_fiji.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="315" windowWidth="20370" windowHeight="7530" tabRatio="807"/>
+    <workbookView xWindow="120" yWindow="315" windowWidth="20370" windowHeight="7530" tabRatio="807" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="country_constants" sheetId="1" r:id="rId1"/>
@@ -2218,7 +2218,7 @@
   </sheetPr>
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -2401,11 +2401,11 @@
   </sheetPr>
   <dimension ref="A1:BE31"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="AK2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="BC8" sqref="BC8"/>
+      <selection pane="bottomRight" activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3532,7 +3532,7 @@
         <v>1</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="31" spans="1:52" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -3547,7 +3547,7 @@
       </c>
       <c r="D31" s="47" t="str">
         <f>D30</f>
-        <v>no</v>
+        <v>yes</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update treatment success rates
As per Tan's advice in the Slack forum.
</commit_message>
<xml_diff>
--- a/autumn/xls/programs_fiji.xlsx
+++ b/autumn/xls/programs_fiji.xlsx
@@ -2393,10 +2393,10 @@
   <dimension ref="A1:BC33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="AK2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A28" sqref="A28"/>
+      <selection pane="bottomRight" activeCell="AZ15" sqref="AZ15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2964,9 +2964,8 @@
       <c r="AX14" s="27">
         <v>93</v>
       </c>
-      <c r="AY14" s="27"/>
-      <c r="AZ14" s="13">
-        <v>90</v>
+      <c r="AY14" s="27">
+        <v>85</v>
       </c>
       <c r="BB14" s="13">
         <v>91.1</v>

</xml_diff>

<commit_message>
Simplify time to start treatment code
Shorten code with loop. Note that default behaviour for single strain is
now to use the smear-positive waiting time.
</commit_message>
<xml_diff>
--- a/autumn/xls/programs_fiji.xlsx
+++ b/autumn/xls/programs_fiji.xlsx
@@ -147,9 +147,6 @@
     <t>Rate at which patients change from the low quality to the high quality health system</t>
   </si>
   <si>
-    <t>program_timeperiod_await_treatment</t>
-  </si>
-  <si>
     <t>program_cost_await_treatment</t>
   </si>
   <si>
@@ -232,6 +229,9 @@
   </si>
   <si>
     <t>scenario_3</t>
+  </si>
+  <si>
+    <t>program_timeperiod_await_treatment_smearpos</t>
   </si>
 </sst>
 </file>
@@ -2274,24 +2274,24 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="29" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B5" s="34">
         <v>1945</v>
       </c>
       <c r="C5" s="31" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="29" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B6" s="34">
         <v>1955</v>
       </c>
       <c r="C6" s="31" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -2318,68 +2318,68 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="32" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B9" s="35">
         <v>0.22</v>
       </c>
       <c r="C9" s="31" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:4" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="47" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B10" s="48">
         <v>1895</v>
       </c>
       <c r="C10" s="47" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="11" spans="1:4" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="47" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B11" s="48">
         <v>2016</v>
       </c>
       <c r="C11" s="47" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:4" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="47" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B12" s="48">
         <v>2020</v>
       </c>
       <c r="C12" s="47" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="13" spans="1:4" s="45" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="45" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B13" s="46">
         <v>190000</v>
       </c>
       <c r="C13" s="45" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="14" spans="1:4" s="45" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="45" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B14" s="46">
         <v>3</v>
       </c>
       <c r="C14" s="45" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -2399,7 +2399,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A28" sqref="A28"/>
+      <selection pane="bottomRight" activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2442,10 +2442,10 @@
         <v>15</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E1" s="5">
         <v>1920</v>
@@ -2595,13 +2595,13 @@
         <v>2015</v>
       </c>
       <c r="BB1" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="BC1" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="BC1" s="5" t="s">
-        <v>46</v>
-      </c>
       <c r="BD1" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:56" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -3353,7 +3353,7 @@
     </row>
     <row r="26" spans="1:56" s="41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="39" t="s">
-        <v>43</v>
+        <v>71</v>
       </c>
       <c r="B26" s="40" t="s">
         <v>13</v>
@@ -3395,7 +3395,7 @@
     </row>
     <row r="27" spans="1:56" s="41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="39" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B27" s="40" t="s">
         <v>13</v>
@@ -3441,7 +3441,7 @@
     </row>
     <row r="28" spans="1:56" s="41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="39" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B28" s="40" t="s">
         <v>13</v>
@@ -3483,7 +3483,7 @@
     </row>
     <row r="29" spans="1:56" s="41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="39" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B29" s="40" t="s">
         <v>23</v>
@@ -3507,7 +3507,7 @@
     </row>
     <row r="30" spans="1:56" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="16" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B30" s="6" t="s">
         <v>13</v>
@@ -3532,7 +3532,7 @@
     </row>
     <row r="31" spans="1:56" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="16" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B31" s="6" t="s">
         <v>13</v>
@@ -3589,7 +3589,7 @@
     </row>
     <row r="32" spans="1:56" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B32" s="6" t="s">
         <v>13</v>
@@ -3603,7 +3603,7 @@
     </row>
     <row r="33" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B33" s="6" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
Added a row of inflation data to time_variant sheet
</commit_message>
<xml_diff>
--- a/autumn/xls/programs_fiji.xlsx
+++ b/autumn/xls/programs_fiji.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="81">
   <si>
     <t>program_rate_restart_presenting</t>
   </si>
@@ -256,6 +256,9 @@
   </si>
   <si>
     <t>program_cost_ipt</t>
+  </si>
+  <si>
+    <t>inflation</t>
   </si>
 </sst>
 </file>
@@ -2417,13 +2420,13 @@
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:BI36"/>
+  <dimension ref="A1:BI37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A6" sqref="A6"/>
+      <selection pane="bottomRight" activeCell="J37" sqref="J37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3639,7 +3642,7 @@
         <v>739284639</v>
       </c>
     </row>
-    <row r="33" spans="1:52" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:53" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="16" t="s">
         <v>54</v>
       </c>
@@ -3664,7 +3667,7 @@
       <c r="AY33" s="43"/>
       <c r="AZ33" s="43"/>
     </row>
-    <row r="34" spans="1:52" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:53" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="16" t="s">
         <v>55</v>
       </c>
@@ -3721,7 +3724,7 @@
       <c r="AY34" s="43"/>
       <c r="AZ34" s="43"/>
     </row>
-    <row r="35" spans="1:52" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:53" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="16" t="s">
         <v>56</v>
       </c>
@@ -3735,7 +3738,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="36" spans="1:52" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:53" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="16" t="s">
         <v>57</v>
       </c>
@@ -3750,9 +3753,149 @@
         <v>yes</v>
       </c>
     </row>
+    <row r="37" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="A37" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C37" s="2">
+        <v>1</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="L37" s="1">
+        <v>4.1000000000000002E-2</v>
+      </c>
+      <c r="M37" s="1">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="N37">
+        <v>0.114</v>
+      </c>
+      <c r="O37">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="P37">
+        <v>6.0999999999999999E-2</v>
+      </c>
+      <c r="Q37">
+        <v>7.8E-2</v>
+      </c>
+      <c r="R37">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="S37">
+        <v>0.11199999999999999</v>
+      </c>
+      <c r="T37">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="U37">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="V37">
+        <v>5.2999999999999999E-2</v>
+      </c>
+      <c r="W37">
+        <v>4.4000000000000004E-2</v>
+      </c>
+      <c r="X37">
+        <v>1.8000000000000002E-2</v>
+      </c>
+      <c r="Y37">
+        <v>5.7000000000000002E-2</v>
+      </c>
+      <c r="Z37">
+        <v>0.11800000000000001</v>
+      </c>
+      <c r="AA37">
+        <v>6.2E-2</v>
+      </c>
+      <c r="AB37">
+        <v>8.199999999999999E-2</v>
+      </c>
+      <c r="AC37">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="AD37">
+        <v>4.9000000000000002E-2</v>
+      </c>
+      <c r="AE37">
+        <v>5.2000000000000005E-2</v>
+      </c>
+      <c r="AF37">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="AG37">
+        <v>2.2000000000000002E-2</v>
+      </c>
+      <c r="AH37">
+        <v>3.1E-2</v>
+      </c>
+      <c r="AI37">
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="AJ37">
+        <v>5.7000000000000002E-2</v>
+      </c>
+      <c r="AK37">
+        <v>0.02</v>
+      </c>
+      <c r="AL37">
+        <v>1.1000000000000001E-2</v>
+      </c>
+      <c r="AM37">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="AN37">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="AO37">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="AP37">
+        <v>2.7999999999999997E-2</v>
+      </c>
+      <c r="AQ37">
+        <v>2.4E-2</v>
+      </c>
+      <c r="AR37">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="AS37">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="AT37">
+        <v>7.6999999999999999E-2</v>
+      </c>
+      <c r="AU37">
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="AV37">
+        <v>3.7000000000000005E-2</v>
+      </c>
+      <c r="AW37">
+        <v>7.2999999999999995E-2</v>
+      </c>
+      <c r="AX37">
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="AY37">
+        <v>2.8999999999999998E-2</v>
+      </c>
+      <c r="AZ37">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="BA37" s="7">
+        <v>1.4E-2</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations xWindow="343" yWindow="238" count="4">
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E28:BA31 E2:BC2 E4:BC4 E10:BC10 E20:BC20 E22:BC22 E24:BC24 E26:BC26 E12:BC12 E14:BC14 E16:BC16 E18:BC18 E8:BC8 BB28:BC30">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E28:BA31 E2:BC2 E4:BC4 E10:BC10 E20:BC20 E22:BC22 E24:BC24 E26:BC26 E12:BC12 E14:BC14 E16:BC16 E18:BC18 E8:BC8 BB28:BC30 N37:AW37">
       <formula1>0</formula1>
       <formula2>100</formula2>
     </dataValidation>

</xml_diff>

<commit_message>
Restrict IPT to DS-TB patients only
Doesn't make a big difference for Fiji or the Philippines, which don't
have MDR-TB yet, but important for later.
</commit_message>
<xml_diff>
--- a/autumn/xls/programs_fiji.xlsx
+++ b/autumn/xls/programs_fiji.xlsx
@@ -2423,10 +2423,10 @@
   <dimension ref="A1:BI37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="AQ2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J37" sqref="J37"/>
+      <selection pane="bottomRight" activeCell="BB16" sqref="BB16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added CPI data to programs_fiji.xlxls
</commit_message>
<xml_diff>
--- a/autumn/xls/programs_fiji.xlsx
+++ b/autumn/xls/programs_fiji.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="83">
   <si>
     <t>program_rate_restart_presenting</t>
   </si>
@@ -262,6 +262,9 @@
   </si>
   <si>
     <t>scenario_9</t>
+  </si>
+  <si>
+    <t>cpi</t>
   </si>
 </sst>
 </file>
@@ -271,7 +274,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -365,6 +368,13 @@
     <font>
       <sz val="11"/>
       <color theme="6" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1219,7 +1229,7 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1273,6 +1283,7 @@
     <xf numFmtId="2" fontId="12" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="13" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="664">
     <cellStyle name="Comma 2" xfId="5"/>
@@ -2423,13 +2434,13 @@
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:BJ37"/>
+  <dimension ref="A1:BJ38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="AY2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C22" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="BJ7" sqref="BJ7"/>
+      <selection pane="bottomRight" activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3903,6 +3914,158 @@
       </c>
       <c r="BA37" s="7">
         <v>1.4E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="A38" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="E38" s="49">
+        <v>116.4</v>
+      </c>
+      <c r="F38" s="49">
+        <v>116.4</v>
+      </c>
+      <c r="G38" s="49">
+        <v>116.4</v>
+      </c>
+      <c r="H38" s="49">
+        <v>116.4</v>
+      </c>
+      <c r="I38" s="49">
+        <v>116.4</v>
+      </c>
+      <c r="J38" s="49">
+        <v>116.4</v>
+      </c>
+      <c r="K38" s="49">
+        <v>116.4</v>
+      </c>
+      <c r="L38" s="49">
+        <v>116.4</v>
+      </c>
+      <c r="M38" s="49">
+        <v>116.4</v>
+      </c>
+      <c r="N38" s="49">
+        <v>116.4</v>
+      </c>
+      <c r="O38" s="49">
+        <v>116.4</v>
+      </c>
+      <c r="P38" s="49">
+        <v>116.4</v>
+      </c>
+      <c r="Q38" s="49">
+        <v>116.4</v>
+      </c>
+      <c r="R38" s="49">
+        <v>116.4</v>
+      </c>
+      <c r="S38" s="1">
+        <v>28.8</v>
+      </c>
+      <c r="T38" s="1">
+        <v>30.8</v>
+      </c>
+      <c r="U38" s="1">
+        <v>32.9</v>
+      </c>
+      <c r="V38" s="1">
+        <v>34.6</v>
+      </c>
+      <c r="W38" s="1">
+        <v>36.1</v>
+      </c>
+      <c r="X38" s="1">
+        <v>36.799999999999997</v>
+      </c>
+      <c r="Y38" s="1">
+        <v>38.9</v>
+      </c>
+      <c r="Z38" s="1">
+        <v>43.4</v>
+      </c>
+      <c r="AA38" s="1">
+        <v>46.1</v>
+      </c>
+      <c r="AB38" s="1">
+        <v>49.9</v>
+      </c>
+      <c r="AC38" s="1">
+        <v>53.1</v>
+      </c>
+      <c r="AD38" s="1">
+        <v>55.7</v>
+      </c>
+      <c r="AE38" s="1">
+        <v>58.6</v>
+      </c>
+      <c r="AF38" s="1">
+        <v>59.1</v>
+      </c>
+      <c r="AG38" s="1">
+        <v>60.4</v>
+      </c>
+      <c r="AH38" s="1">
+        <v>62.2</v>
+      </c>
+      <c r="AI38" s="1">
+        <v>64.3</v>
+      </c>
+      <c r="AJ38" s="1">
+        <v>68</v>
+      </c>
+      <c r="AK38" s="1">
+        <v>69.3</v>
+      </c>
+      <c r="AL38" s="1">
+        <v>70.099999999999994</v>
+      </c>
+      <c r="AM38" s="1">
+        <v>73.099999999999994</v>
+      </c>
+      <c r="AN38" s="1">
+        <v>73.599999999999994</v>
+      </c>
+      <c r="AO38" s="1">
+        <v>76.7</v>
+      </c>
+      <c r="AP38" s="1">
+        <v>78.900000000000006</v>
+      </c>
+      <c r="AQ38" s="1">
+        <v>80.8</v>
+      </c>
+      <c r="AR38" s="1">
+        <v>82.8</v>
+      </c>
+      <c r="AS38" s="1">
+        <v>86.7</v>
+      </c>
+      <c r="AT38" s="1">
+        <v>93.4</v>
+      </c>
+      <c r="AU38" s="1">
+        <v>96.5</v>
+      </c>
+      <c r="AV38" s="1">
+        <v>100</v>
+      </c>
+      <c r="AW38" s="1">
+        <v>107.3</v>
+      </c>
+      <c r="AX38" s="1">
+        <v>110.9</v>
+      </c>
+      <c r="AY38" s="1">
+        <v>114.2</v>
+      </c>
+      <c r="AZ38" s="1">
+        <v>114.8</v>
+      </c>
+      <c r="BA38" s="1">
+        <v>116.4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
For years 1920 - 1970 for which we don't have inflation data, I assume inflation is the average of the next 5 years that we have data for
</commit_message>
<xml_diff>
--- a/autumn/xls/programs_fiji.xlsx
+++ b/autumn/xls/programs_fiji.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="83">
   <si>
     <t>program_rate_restart_presenting</t>
   </si>
@@ -274,7 +274,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -375,6 +375,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1229,7 +1236,7 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1284,6 +1291,7 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="13" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="664">
     <cellStyle name="Comma 2" xfId="5"/>
@@ -2437,10 +2445,10 @@
   <dimension ref="A1:BJ38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C22" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A38" sqref="A38"/>
+      <selection pane="bottomRight" activeCell="M37" sqref="M37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3789,6 +3797,27 @@
       <c r="D37" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="E37" s="49">
+        <v>0</v>
+      </c>
+      <c r="F37" s="49">
+        <v>0</v>
+      </c>
+      <c r="G37" s="49">
+        <v>0</v>
+      </c>
+      <c r="H37" s="49">
+        <v>0</v>
+      </c>
+      <c r="I37" s="49">
+        <v>0</v>
+      </c>
+      <c r="J37" s="49">
+        <v>0</v>
+      </c>
+      <c r="K37" s="49">
+        <v>0</v>
+      </c>
       <c r="L37" s="1">
         <v>4.1000000000000002E-2</v>
       </c>
@@ -3920,6 +3949,15 @@
       <c r="A38" s="21" t="s">
         <v>82</v>
       </c>
+      <c r="B38" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C38" s="2">
+        <v>1</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>13</v>
+      </c>
       <c r="E38" s="49">
         <v>116.4</v>
       </c>
@@ -3938,29 +3976,29 @@
       <c r="J38" s="49">
         <v>116.4</v>
       </c>
-      <c r="K38" s="49">
-        <v>116.4</v>
-      </c>
-      <c r="L38" s="49">
-        <v>116.4</v>
-      </c>
-      <c r="M38" s="49">
-        <v>116.4</v>
-      </c>
-      <c r="N38" s="49">
-        <v>116.4</v>
-      </c>
-      <c r="O38" s="49">
-        <v>116.4</v>
-      </c>
-      <c r="P38" s="49">
-        <v>116.4</v>
-      </c>
-      <c r="Q38" s="49">
-        <v>116.4</v>
-      </c>
-      <c r="R38" s="49">
-        <v>116.4</v>
+      <c r="K38" s="50">
+        <v>14.02</v>
+      </c>
+      <c r="L38" s="50">
+        <v>14.59</v>
+      </c>
+      <c r="M38" s="50">
+        <v>16.5</v>
+      </c>
+      <c r="N38" s="50">
+        <v>18.38</v>
+      </c>
+      <c r="O38" s="50">
+        <v>19.670000000000002</v>
+      </c>
+      <c r="P38" s="50">
+        <v>20.87</v>
+      </c>
+      <c r="Q38" s="50">
+        <v>22.5</v>
+      </c>
+      <c r="R38" s="50">
+        <v>25.9</v>
       </c>
       <c r="S38" s="1">
         <v>28.8</v>
@@ -4069,7 +4107,7 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations xWindow="343" yWindow="238" count="4">
+  <dataValidations xWindow="382" yWindow="552" count="4">
     <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E28:BA31 E2:BC2 E4:BC4 E10:BC10 E20:BC20 E22:BC22 E24:BC24 E26:BC26 E12:BC12 E14:BC14 E16:BC16 E18:BC18 E8:BC8 BB28:BC30 N37:AW37">
       <formula1>0</formula1>
       <formula2>100</formula2>
@@ -4088,7 +4126,7 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xWindow="343" yWindow="238" count="5">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xWindow="382" yWindow="552" count="5">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Time-variant?" prompt="If no, the most recent value will be selected.">
           <x14:formula1>
             <xm:f>dropdown_lists!$A$2:$A$4</xm:f>

</xml_diff>

<commit_message>
Estimated CPI from years from 1920 - 1970 for which CPI data are not available
Inflation rate is assumed to be average of the next 5 years; and CPI is
calculated based on inflation rate using standard inflation fomular.
</commit_message>
<xml_diff>
--- a/autumn/xls/programs_fiji.xlsx
+++ b/autumn/xls/programs_fiji.xlsx
@@ -1236,7 +1236,7 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1292,6 +1292,9 @@
     <xf numFmtId="2" fontId="13" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="664">
     <cellStyle name="Comma 2" xfId="5"/>
@@ -2442,13 +2445,13 @@
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:BJ38"/>
+  <dimension ref="A1:BN38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M37" sqref="M37"/>
+      <selection pane="bottomRight" activeCell="H45" sqref="H45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2462,28 +2465,29 @@
     <col min="8" max="9" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="7.42578125" style="1" customWidth="1"/>
     <col min="11" max="12" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.7109375" style="1" customWidth="1"/>
-    <col min="14" max="17" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="7.28515625" style="1" customWidth="1"/>
-    <col min="19" max="22" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="24" width="7.42578125" style="1" customWidth="1"/>
-    <col min="25" max="25" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="7.140625" style="1" customWidth="1"/>
-    <col min="27" max="38" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="8" style="1" customWidth="1"/>
-    <col min="40" max="46" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="8" style="1" customWidth="1"/>
-    <col min="48" max="48" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="6.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="50" max="51" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="7.85546875" style="1" customWidth="1"/>
-    <col min="53" max="53" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="14" style="1" bestFit="1" customWidth="1"/>
-    <col min="55" max="62" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="63" max="16384" width="9.140625" style="1"/>
+    <col min="13" max="16" width="7.42578125" style="1" customWidth="1"/>
+    <col min="17" max="17" width="7.7109375" style="1" customWidth="1"/>
+    <col min="18" max="21" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="7.28515625" style="1" customWidth="1"/>
+    <col min="23" max="26" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="28" width="7.42578125" style="1" customWidth="1"/>
+    <col min="29" max="29" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="7.140625" style="1" customWidth="1"/>
+    <col min="31" max="42" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="8" style="1" customWidth="1"/>
+    <col min="44" max="50" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="8" style="1" customWidth="1"/>
+    <col min="52" max="52" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="6.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="54" max="55" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="7.85546875" style="1" customWidth="1"/>
+    <col min="57" max="57" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="14" style="1" bestFit="1" customWidth="1"/>
+    <col min="59" max="66" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="67" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:62" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:66" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>16</v>
       </c>
@@ -2521,157 +2525,169 @@
         <v>1970</v>
       </c>
       <c r="M1" s="5">
+        <v>1971</v>
+      </c>
+      <c r="N1" s="5">
+        <v>1972</v>
+      </c>
+      <c r="O1" s="5">
+        <v>1973</v>
+      </c>
+      <c r="P1" s="5">
+        <v>1974</v>
+      </c>
+      <c r="Q1" s="5">
         <v>1975</v>
       </c>
-      <c r="N1" s="5">
+      <c r="R1" s="5">
         <v>1976</v>
       </c>
-      <c r="O1" s="5">
+      <c r="S1" s="5">
         <v>1977</v>
       </c>
-      <c r="P1" s="5">
+      <c r="T1" s="5">
         <v>1978</v>
       </c>
-      <c r="Q1" s="5">
+      <c r="U1" s="5">
         <v>1979</v>
       </c>
-      <c r="R1" s="5">
+      <c r="V1" s="5">
         <v>1980</v>
       </c>
-      <c r="S1" s="5">
+      <c r="W1" s="5">
         <v>1981</v>
       </c>
-      <c r="T1" s="5">
+      <c r="X1" s="5">
         <v>1982</v>
       </c>
-      <c r="U1" s="5">
+      <c r="Y1" s="5">
         <v>1983</v>
       </c>
-      <c r="V1" s="5">
+      <c r="Z1" s="5">
         <v>1984</v>
       </c>
-      <c r="W1" s="5">
+      <c r="AA1" s="5">
         <v>1985</v>
       </c>
-      <c r="X1" s="5">
+      <c r="AB1" s="5">
         <v>1986</v>
       </c>
-      <c r="Y1" s="5">
+      <c r="AC1" s="5">
         <v>1987</v>
       </c>
-      <c r="Z1" s="5">
+      <c r="AD1" s="5">
         <v>1988</v>
       </c>
-      <c r="AA1" s="5">
+      <c r="AE1" s="5">
         <v>1989</v>
       </c>
-      <c r="AB1" s="5">
+      <c r="AF1" s="5">
         <v>1990</v>
       </c>
-      <c r="AC1" s="5">
+      <c r="AG1" s="5">
         <v>1991</v>
       </c>
-      <c r="AD1" s="5">
+      <c r="AH1" s="5">
         <v>1992</v>
       </c>
-      <c r="AE1" s="5">
+      <c r="AI1" s="5">
         <v>1993</v>
       </c>
-      <c r="AF1" s="5">
+      <c r="AJ1" s="5">
         <v>1994</v>
       </c>
-      <c r="AG1" s="5">
+      <c r="AK1" s="5">
         <v>1995</v>
       </c>
-      <c r="AH1" s="5">
+      <c r="AL1" s="5">
         <v>1996</v>
       </c>
-      <c r="AI1" s="5">
+      <c r="AM1" s="5">
         <v>1997</v>
       </c>
-      <c r="AJ1" s="5">
+      <c r="AN1" s="5">
         <v>1998</v>
       </c>
-      <c r="AK1" s="5">
+      <c r="AO1" s="5">
         <v>1999</v>
       </c>
-      <c r="AL1" s="5">
+      <c r="AP1" s="5">
         <v>2000</v>
       </c>
-      <c r="AM1" s="5">
+      <c r="AQ1" s="5">
         <v>2001</v>
       </c>
-      <c r="AN1" s="5">
+      <c r="AR1" s="5">
         <v>2002</v>
       </c>
-      <c r="AO1" s="5">
+      <c r="AS1" s="5">
         <v>2003</v>
       </c>
-      <c r="AP1" s="5">
+      <c r="AT1" s="5">
         <v>2004</v>
       </c>
-      <c r="AQ1" s="5">
+      <c r="AU1" s="5">
         <v>2005</v>
       </c>
-      <c r="AR1" s="5">
+      <c r="AV1" s="5">
         <v>2006</v>
       </c>
-      <c r="AS1" s="5">
+      <c r="AW1" s="5">
         <v>2007</v>
       </c>
-      <c r="AT1" s="5">
+      <c r="AX1" s="5">
         <v>2008</v>
       </c>
-      <c r="AU1" s="5">
+      <c r="AY1" s="5">
         <v>2009</v>
       </c>
-      <c r="AV1" s="5">
+      <c r="AZ1" s="5">
         <v>2010</v>
       </c>
-      <c r="AW1" s="5">
+      <c r="BA1" s="5">
         <v>2011</v>
       </c>
-      <c r="AX1" s="5">
+      <c r="BB1" s="5">
         <v>2012</v>
       </c>
-      <c r="AY1" s="5">
+      <c r="BC1" s="5">
         <v>2013</v>
       </c>
-      <c r="AZ1" s="5">
+      <c r="BD1" s="5">
         <v>2014</v>
       </c>
-      <c r="BA1" s="5">
+      <c r="BE1" s="5">
         <v>2015</v>
       </c>
-      <c r="BB1" s="5" t="s">
+      <c r="BF1" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="BC1" s="5" t="s">
+      <c r="BG1" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="BD1" s="5" t="s">
+      <c r="BH1" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="BE1" s="5" t="s">
+      <c r="BI1" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="BF1" s="5" t="s">
+      <c r="BJ1" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="BG1" s="5" t="s">
+      <c r="BK1" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="BH1" s="5" t="s">
+      <c r="BL1" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="BI1" s="5" t="s">
+      <c r="BM1" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="BJ1" s="5" t="s">
+      <c r="BN1" s="5" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:62" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:66" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
         <v>8</v>
       </c>
@@ -2690,13 +2706,9 @@
       <c r="J2" s="7">
         <v>25</v>
       </c>
-      <c r="M2" s="7">
+      <c r="Q2" s="7">
         <v>55</v>
       </c>
-      <c r="R2" s="25"/>
-      <c r="S2" s="25"/>
-      <c r="T2" s="25"/>
-      <c r="U2" s="25"/>
       <c r="V2" s="25"/>
       <c r="W2" s="25"/>
       <c r="X2" s="25"/>
@@ -2728,14 +2740,18 @@
       <c r="AX2" s="25"/>
       <c r="AY2" s="25"/>
       <c r="AZ2" s="25"/>
-      <c r="BG2" s="7">
+      <c r="BA2" s="25"/>
+      <c r="BB2" s="25"/>
+      <c r="BC2" s="25"/>
+      <c r="BD2" s="25"/>
+      <c r="BK2" s="7">
         <v>100</v>
       </c>
-      <c r="BJ2" s="7">
+      <c r="BN2" s="7">
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:62" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:66" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
         <v>17</v>
       </c>
@@ -2752,17 +2768,17 @@
       <c r="J3" s="7">
         <v>10000000</v>
       </c>
-      <c r="M3" s="7">
+      <c r="Q3" s="7">
         <v>15040500</v>
       </c>
-      <c r="W3" s="7">
+      <c r="AA3" s="7">
         <v>39034561</v>
       </c>
-      <c r="X3" s="7">
+      <c r="AB3" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:62" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:66" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
         <v>9</v>
       </c>
@@ -2781,13 +2797,9 @@
       <c r="K4" s="9">
         <v>10</v>
       </c>
-      <c r="T4" s="9">
+      <c r="X4" s="9">
         <v>30</v>
       </c>
-      <c r="AB4" s="26"/>
-      <c r="AC4" s="26"/>
-      <c r="AD4" s="26"/>
-      <c r="AE4" s="26"/>
       <c r="AF4" s="26"/>
       <c r="AG4" s="26"/>
       <c r="AH4" s="26"/>
@@ -2808,20 +2820,24 @@
       <c r="AW4" s="26"/>
       <c r="AX4" s="26"/>
       <c r="AY4" s="26"/>
-      <c r="AZ4" s="26">
+      <c r="AZ4" s="26"/>
+      <c r="BA4" s="26"/>
+      <c r="BB4" s="26"/>
+      <c r="BC4" s="26"/>
+      <c r="BD4" s="26">
         <v>50</v>
       </c>
-      <c r="BD4" s="9">
+      <c r="BH4" s="9">
         <v>85</v>
       </c>
-      <c r="BE4" s="9">
+      <c r="BI4" s="9">
         <v>90</v>
       </c>
-      <c r="BJ4" s="9">
+      <c r="BN4" s="9">
         <v>90</v>
       </c>
     </row>
-    <row r="5" spans="1:62" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:66" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
         <v>18</v>
       </c>
@@ -2835,11 +2851,11 @@
       <c r="F5" s="9">
         <v>0</v>
       </c>
-      <c r="X5" s="9">
+      <c r="AB5" s="9">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:62" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:66" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
         <v>78</v>
       </c>
@@ -2852,17 +2868,17 @@
       <c r="D6" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="AX6" s="9">
+      <c r="BB6" s="9">
         <v>0</v>
       </c>
-      <c r="BI6" s="9">
+      <c r="BM6" s="9">
         <v>50</v>
       </c>
-      <c r="BJ6" s="9">
+      <c r="BN6" s="9">
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:62" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:66" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
         <v>79</v>
       </c>
@@ -2874,7 +2890,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:62" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:66" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
         <v>10</v>
       </c>
@@ -2893,23 +2909,23 @@
       <c r="J8" s="11">
         <v>80</v>
       </c>
-      <c r="Z8" s="11">
+      <c r="AD8" s="11">
         <v>82</v>
       </c>
-      <c r="AM8" s="11">
+      <c r="AQ8" s="11">
         <v>84</v>
       </c>
-      <c r="AY8" s="11">
+      <c r="BC8" s="11">
         <v>85</v>
-      </c>
-      <c r="BF8" s="11">
-        <v>90</v>
       </c>
       <c r="BJ8" s="11">
         <v>90</v>
       </c>
-    </row>
-    <row r="9" spans="1:62" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="BN8" s="11">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="9" spans="1:66" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
         <v>19</v>
       </c>
@@ -2926,14 +2942,14 @@
       <c r="J9" s="11">
         <v>2040504</v>
       </c>
-      <c r="X9" s="11">
+      <c r="AB9" s="11">
         <v>1</v>
       </c>
-      <c r="Z9" s="11">
+      <c r="AD9" s="11">
         <v>4049504</v>
       </c>
     </row>
-    <row r="10" spans="1:62" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:66" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="19" t="s">
         <v>3</v>
       </c>
@@ -2952,14 +2968,14 @@
       <c r="K10" s="13">
         <v>40</v>
       </c>
-      <c r="AB10" s="13">
+      <c r="AF10" s="13">
         <v>40</v>
       </c>
-      <c r="BJ10" s="13">
+      <c r="BN10" s="13">
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:62" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:66" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="19" t="s">
         <v>20</v>
       </c>
@@ -2970,11 +2986,11 @@
       <c r="D11" s="44" t="s">
         <v>23</v>
       </c>
-      <c r="X11" s="13">
+      <c r="AB11" s="13">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:62" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:66" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="20" t="s">
         <v>11</v>
       </c>
@@ -2987,17 +3003,17 @@
       <c r="D12" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="R12" s="15">
+      <c r="V12" s="15">
         <v>30</v>
       </c>
-      <c r="AB12" s="15">
+      <c r="AF12" s="15">
         <v>40</v>
       </c>
-      <c r="AL12" s="15">
+      <c r="AP12" s="15">
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:62" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:66" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="20" t="s">
         <v>21</v>
       </c>
@@ -3008,11 +3024,11 @@
       <c r="D13" s="44" t="s">
         <v>23</v>
       </c>
-      <c r="X13" s="15">
+      <c r="AB13" s="15">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:62" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:66" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="20" t="s">
         <v>12</v>
       </c>
@@ -3028,17 +3044,17 @@
       <c r="I14" s="15">
         <v>7</v>
       </c>
-      <c r="W14" s="15">
+      <c r="AA14" s="15">
         <v>0</v>
       </c>
-      <c r="AG14" s="15">
+      <c r="AK14" s="15">
         <v>50</v>
       </c>
-      <c r="AL14" s="15">
+      <c r="AP14" s="15">
         <v>70</v>
       </c>
     </row>
-    <row r="15" spans="1:62" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:66" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="20" t="s">
         <v>22</v>
       </c>
@@ -3049,11 +3065,11 @@
       <c r="D15" s="44" t="s">
         <v>23</v>
       </c>
-      <c r="X15" s="15">
+      <c r="AB15" s="15">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:62" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:66" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="19" t="s">
         <v>24</v>
       </c>
@@ -3069,16 +3085,12 @@
       <c r="I16" s="13">
         <v>0</v>
       </c>
-      <c r="R16" s="13">
+      <c r="V16" s="13">
         <v>40</v>
       </c>
-      <c r="X16" s="13">
+      <c r="AB16" s="13">
         <v>65</v>
       </c>
-      <c r="AF16" s="27"/>
-      <c r="AG16" s="27"/>
-      <c r="AH16" s="27"/>
-      <c r="AI16" s="27"/>
       <c r="AJ16" s="27"/>
       <c r="AK16" s="27"/>
       <c r="AL16" s="27"/>
@@ -3093,23 +3105,27 @@
       <c r="AU16" s="27"/>
       <c r="AV16" s="27"/>
       <c r="AW16" s="27"/>
-      <c r="AX16" s="27">
+      <c r="AX16" s="27"/>
+      <c r="AY16" s="27"/>
+      <c r="AZ16" s="27"/>
+      <c r="BA16" s="27"/>
+      <c r="BB16" s="27">
         <v>93</v>
       </c>
-      <c r="AY16" s="27">
+      <c r="BC16" s="27">
         <v>85</v>
       </c>
-      <c r="BB16" s="13">
+      <c r="BF16" s="13">
         <v>91.1</v>
       </c>
-      <c r="BC16" s="13">
+      <c r="BG16" s="13">
         <v>96</v>
       </c>
-      <c r="BJ16" s="13">
+      <c r="BN16" s="13">
         <v>96</v>
       </c>
     </row>
-    <row r="17" spans="1:62" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:66" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="19" t="s">
         <v>25</v>
       </c>
@@ -3123,20 +3139,20 @@
       <c r="I17" s="13">
         <v>0</v>
       </c>
-      <c r="R17" s="13">
+      <c r="V17" s="13">
         <v>1926492</v>
       </c>
-      <c r="X17" s="13">
+      <c r="AB17" s="13">
         <v>4573928</v>
       </c>
-      <c r="AM17" s="13">
+      <c r="AQ17" s="13">
         <v>9382947</v>
       </c>
-      <c r="AU17" s="13">
+      <c r="AY17" s="13">
         <v>52431253</v>
       </c>
     </row>
-    <row r="18" spans="1:62" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:66" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="19" t="s">
         <v>26</v>
       </c>
@@ -3152,16 +3168,12 @@
       <c r="I18" s="13">
         <v>0</v>
       </c>
-      <c r="R18" s="13">
+      <c r="V18" s="13">
         <v>10</v>
       </c>
-      <c r="X18" s="13">
+      <c r="AB18" s="13">
         <v>8</v>
       </c>
-      <c r="AF18" s="27"/>
-      <c r="AG18" s="27"/>
-      <c r="AH18" s="27"/>
-      <c r="AI18" s="27"/>
       <c r="AJ18" s="27"/>
       <c r="AK18" s="27"/>
       <c r="AL18" s="27"/>
@@ -3178,20 +3190,24 @@
       <c r="AW18" s="27"/>
       <c r="AX18" s="27"/>
       <c r="AY18" s="27"/>
-      <c r="AZ18" s="13">
+      <c r="AZ18" s="27"/>
+      <c r="BA18" s="27"/>
+      <c r="BB18" s="27"/>
+      <c r="BC18" s="27"/>
+      <c r="BD18" s="13">
         <v>5</v>
       </c>
-      <c r="BB18" s="13">
+      <c r="BF18" s="13">
         <v>1.6</v>
       </c>
-      <c r="BC18" s="13">
+      <c r="BG18" s="13">
         <v>1.25</v>
       </c>
-      <c r="BJ18" s="13">
+      <c r="BN18" s="13">
         <v>1.25</v>
       </c>
     </row>
-    <row r="19" spans="1:62" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:66" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="19" t="s">
         <v>27</v>
       </c>
@@ -3205,11 +3221,11 @@
       <c r="I19" s="13">
         <v>0</v>
       </c>
-      <c r="X19" s="13">
+      <c r="AB19" s="13">
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:62" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:66" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="22" t="s">
         <v>28</v>
       </c>
@@ -3225,16 +3241,12 @@
       <c r="I20" s="24">
         <v>0</v>
       </c>
-      <c r="R20" s="24">
+      <c r="V20" s="24">
         <v>15</v>
       </c>
-      <c r="X20" s="24">
+      <c r="AB20" s="24">
         <v>30</v>
       </c>
-      <c r="AF20" s="28"/>
-      <c r="AG20" s="28"/>
-      <c r="AH20" s="28"/>
-      <c r="AI20" s="28"/>
       <c r="AJ20" s="28"/>
       <c r="AK20" s="28"/>
       <c r="AL20" s="28"/>
@@ -3251,11 +3263,15 @@
       <c r="AW20" s="28"/>
       <c r="AX20" s="28"/>
       <c r="AY20" s="28"/>
-      <c r="AZ20" s="24">
+      <c r="AZ20" s="28"/>
+      <c r="BA20" s="28"/>
+      <c r="BB20" s="28"/>
+      <c r="BC20" s="28"/>
+      <c r="BD20" s="24">
         <v>50</v>
       </c>
     </row>
-    <row r="21" spans="1:62" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:66" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="22" t="s">
         <v>29</v>
       </c>
@@ -3269,20 +3285,20 @@
       <c r="I21" s="24">
         <v>0</v>
       </c>
-      <c r="R21" s="24">
+      <c r="V21" s="24">
         <v>492549</v>
       </c>
-      <c r="X21" s="24">
+      <c r="AB21" s="24">
         <v>256491</v>
       </c>
-      <c r="AM21" s="24">
+      <c r="AQ21" s="24">
         <v>9382947</v>
       </c>
-      <c r="AU21" s="24">
+      <c r="AY21" s="24">
         <v>52431253</v>
       </c>
     </row>
-    <row r="22" spans="1:62" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:66" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="22" t="s">
         <v>30</v>
       </c>
@@ -3298,16 +3314,12 @@
       <c r="I22" s="24">
         <v>0</v>
       </c>
-      <c r="R22" s="24">
+      <c r="V22" s="24">
         <v>55</v>
       </c>
-      <c r="X22" s="24">
+      <c r="AB22" s="24">
         <v>50</v>
       </c>
-      <c r="AF22" s="28"/>
-      <c r="AG22" s="28"/>
-      <c r="AH22" s="28"/>
-      <c r="AI22" s="28"/>
       <c r="AJ22" s="28"/>
       <c r="AK22" s="28"/>
       <c r="AL22" s="28"/>
@@ -3324,11 +3336,15 @@
       <c r="AW22" s="28"/>
       <c r="AX22" s="28"/>
       <c r="AY22" s="28"/>
-      <c r="AZ22" s="24">
+      <c r="AZ22" s="28"/>
+      <c r="BA22" s="28"/>
+      <c r="BB22" s="28"/>
+      <c r="BC22" s="28"/>
+      <c r="BD22" s="24">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:62" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:66" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="22" t="s">
         <v>31</v>
       </c>
@@ -3342,11 +3358,11 @@
       <c r="I23" s="24">
         <v>0</v>
       </c>
-      <c r="X23" s="24">
+      <c r="AB23" s="24">
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:62" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:66" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="17" t="s">
         <v>32</v>
       </c>
@@ -3362,16 +3378,12 @@
       <c r="I24" s="9">
         <v>0</v>
       </c>
-      <c r="R24" s="9">
+      <c r="V24" s="9">
         <v>5</v>
       </c>
-      <c r="X24" s="9">
+      <c r="AB24" s="9">
         <v>15</v>
       </c>
-      <c r="AF24" s="26"/>
-      <c r="AG24" s="26"/>
-      <c r="AH24" s="26"/>
-      <c r="AI24" s="26"/>
       <c r="AJ24" s="26"/>
       <c r="AK24" s="26"/>
       <c r="AL24" s="26"/>
@@ -3388,11 +3400,15 @@
       <c r="AW24" s="26"/>
       <c r="AX24" s="26"/>
       <c r="AY24" s="26"/>
-      <c r="AZ24" s="9">
+      <c r="AZ24" s="26"/>
+      <c r="BA24" s="26"/>
+      <c r="BB24" s="26"/>
+      <c r="BC24" s="26"/>
+      <c r="BD24" s="9">
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:62" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:66" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="17" t="s">
         <v>33</v>
       </c>
@@ -3406,20 +3422,20 @@
       <c r="I25" s="9">
         <v>0</v>
       </c>
-      <c r="R25" s="9">
+      <c r="V25" s="9">
         <v>0</v>
       </c>
-      <c r="X25" s="9">
+      <c r="AB25" s="9">
         <v>0</v>
       </c>
-      <c r="AM25" s="9">
+      <c r="AQ25" s="9">
         <v>0</v>
       </c>
-      <c r="AU25" s="9">
+      <c r="AY25" s="9">
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:62" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:66" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="17" t="s">
         <v>34</v>
       </c>
@@ -3435,16 +3451,12 @@
       <c r="I26" s="9">
         <v>0</v>
       </c>
-      <c r="R26" s="9">
+      <c r="V26" s="9">
         <v>65</v>
       </c>
-      <c r="X26" s="9">
+      <c r="AB26" s="9">
         <v>62</v>
       </c>
-      <c r="AF26" s="26"/>
-      <c r="AG26" s="26"/>
-      <c r="AH26" s="26"/>
-      <c r="AI26" s="26"/>
       <c r="AJ26" s="26"/>
       <c r="AK26" s="26"/>
       <c r="AL26" s="26"/>
@@ -3461,11 +3473,15 @@
       <c r="AW26" s="26"/>
       <c r="AX26" s="26"/>
       <c r="AY26" s="26"/>
-      <c r="AZ26" s="9">
+      <c r="AZ26" s="26"/>
+      <c r="BA26" s="26"/>
+      <c r="BB26" s="26"/>
+      <c r="BC26" s="26"/>
+      <c r="BD26" s="9">
         <v>35</v>
       </c>
     </row>
-    <row r="27" spans="1:62" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:66" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="17" t="s">
         <v>35</v>
       </c>
@@ -3479,11 +3495,11 @@
       <c r="I27" s="9">
         <v>0</v>
       </c>
-      <c r="X27" s="9">
+      <c r="AB27" s="9">
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:62" s="41" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:66" s="41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="39" t="s">
         <v>71</v>
       </c>
@@ -3500,10 +3516,6 @@
         <f>2/365</f>
         <v>5.4794520547945206E-3</v>
       </c>
-      <c r="AF28" s="42"/>
-      <c r="AG28" s="42"/>
-      <c r="AH28" s="42"/>
-      <c r="AI28" s="42"/>
       <c r="AJ28" s="42"/>
       <c r="AK28" s="42"/>
       <c r="AL28" s="42"/>
@@ -3520,12 +3532,16 @@
       <c r="AW28" s="42"/>
       <c r="AX28" s="42"/>
       <c r="AY28" s="42"/>
-      <c r="AZ28" s="41">
+      <c r="AZ28" s="42"/>
+      <c r="BA28" s="42"/>
+      <c r="BB28" s="42"/>
+      <c r="BC28" s="42"/>
+      <c r="BD28" s="41">
         <f>2/365</f>
         <v>5.4794520547945206E-3</v>
       </c>
     </row>
-    <row r="29" spans="1:62" s="41" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:66" s="41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="39" t="s">
         <v>68</v>
       </c>
@@ -3542,10 +3558,6 @@
         <f>30/365</f>
         <v>8.2191780821917804E-2</v>
       </c>
-      <c r="AF29" s="42"/>
-      <c r="AG29" s="42"/>
-      <c r="AH29" s="42"/>
-      <c r="AI29" s="42"/>
       <c r="AJ29" s="42"/>
       <c r="AK29" s="42"/>
       <c r="AL29" s="42"/>
@@ -3562,12 +3574,16 @@
       <c r="AW29" s="42"/>
       <c r="AX29" s="42"/>
       <c r="AY29" s="42"/>
-      <c r="AZ29" s="41">
+      <c r="AZ29" s="42"/>
+      <c r="BA29" s="42"/>
+      <c r="BB29" s="42"/>
+      <c r="BC29" s="42"/>
+      <c r="BD29" s="41">
         <f>30/365</f>
         <v>8.2191780821917804E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:62" s="41" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:66" s="41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="39" t="s">
         <v>69</v>
       </c>
@@ -3584,10 +3600,6 @@
         <f>7/365</f>
         <v>1.9178082191780823E-2</v>
       </c>
-      <c r="AF30" s="42"/>
-      <c r="AG30" s="42"/>
-      <c r="AH30" s="42"/>
-      <c r="AI30" s="42"/>
       <c r="AJ30" s="42"/>
       <c r="AK30" s="42"/>
       <c r="AL30" s="42"/>
@@ -3604,12 +3616,16 @@
       <c r="AW30" s="42"/>
       <c r="AX30" s="42"/>
       <c r="AY30" s="42"/>
-      <c r="AZ30" s="41">
+      <c r="AZ30" s="42"/>
+      <c r="BA30" s="42"/>
+      <c r="BB30" s="42"/>
+      <c r="BC30" s="42"/>
+      <c r="BD30" s="41">
         <f>7/365</f>
         <v>1.9178082191780823E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:62" s="41" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:66" s="41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="39" t="s">
         <v>72</v>
       </c>
@@ -3622,10 +3638,6 @@
       <c r="D31" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="AF31" s="42"/>
-      <c r="AG31" s="42"/>
-      <c r="AH31" s="42"/>
-      <c r="AI31" s="42"/>
       <c r="AJ31" s="42"/>
       <c r="AK31" s="42"/>
       <c r="AL31" s="42"/>
@@ -3642,14 +3654,18 @@
       <c r="AW31" s="42"/>
       <c r="AX31" s="42"/>
       <c r="AY31" s="42"/>
-      <c r="AZ31" s="41">
+      <c r="AZ31" s="42"/>
+      <c r="BA31" s="42"/>
+      <c r="BB31" s="42"/>
+      <c r="BC31" s="42"/>
+      <c r="BD31" s="41">
         <v>0</v>
       </c>
-      <c r="BH31" s="41">
+      <c r="BL31" s="41">
         <v>100</v>
       </c>
     </row>
-    <row r="32" spans="1:62" s="41" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:66" s="41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="39" t="s">
         <v>43</v>
       </c>
@@ -3663,17 +3679,17 @@
       <c r="I32" s="41">
         <v>0</v>
       </c>
-      <c r="R32" s="41">
+      <c r="V32" s="41">
         <v>532947</v>
       </c>
-      <c r="X32" s="41">
+      <c r="AB32" s="41">
         <v>9283747</v>
       </c>
-      <c r="AZ32" s="41">
+      <c r="BD32" s="41">
         <v>739284639</v>
       </c>
     </row>
-    <row r="33" spans="1:53" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:57" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="16" t="s">
         <v>54</v>
       </c>
@@ -3686,19 +3702,19 @@
       <c r="D33" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="AB33" s="43"/>
-      <c r="AL33" s="43"/>
-      <c r="AR33" s="43"/>
-      <c r="AS33" s="43"/>
-      <c r="AT33" s="43"/>
-      <c r="AU33" s="43"/>
+      <c r="AF33" s="43"/>
+      <c r="AP33" s="43"/>
       <c r="AV33" s="43"/>
       <c r="AW33" s="43"/>
       <c r="AX33" s="43"/>
       <c r="AY33" s="43"/>
       <c r="AZ33" s="43"/>
-    </row>
-    <row r="34" spans="1:53" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="BA33" s="43"/>
+      <c r="BB33" s="43"/>
+      <c r="BC33" s="43"/>
+      <c r="BD33" s="43"/>
+    </row>
+    <row r="34" spans="1:57" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="16" t="s">
         <v>55</v>
       </c>
@@ -3754,8 +3770,12 @@
       <c r="AX34" s="43"/>
       <c r="AY34" s="43"/>
       <c r="AZ34" s="43"/>
-    </row>
-    <row r="35" spans="1:53" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="BA34" s="43"/>
+      <c r="BB34" s="43"/>
+      <c r="BC34" s="43"/>
+      <c r="BD34" s="43"/>
+    </row>
+    <row r="35" spans="1:57" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="16" t="s">
         <v>56</v>
       </c>
@@ -3769,7 +3789,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="36" spans="1:53" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:57" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="16" t="s">
         <v>57</v>
       </c>
@@ -3784,7 +3804,7 @@
         <v>yes</v>
       </c>
     </row>
-    <row r="37" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A37" s="21" t="s">
         <v>80</v>
       </c>
@@ -3798,154 +3818,166 @@
         <v>13</v>
       </c>
       <c r="E37" s="49">
-        <v>0</v>
+        <v>0.123</v>
       </c>
       <c r="F37" s="49">
-        <v>0</v>
+        <v>0.123</v>
       </c>
       <c r="G37" s="49">
-        <v>0</v>
+        <v>0.123</v>
       </c>
       <c r="H37" s="49">
-        <v>0</v>
+        <v>0.123</v>
       </c>
       <c r="I37" s="49">
-        <v>0</v>
+        <v>0.123</v>
       </c>
       <c r="J37" s="49">
-        <v>0</v>
+        <v>0.123</v>
       </c>
       <c r="K37" s="49">
-        <v>0</v>
+        <v>0.123</v>
       </c>
       <c r="L37" s="1">
         <v>4.1000000000000002E-2</v>
       </c>
-      <c r="M37" s="1">
+      <c r="M37" s="51">
+        <v>9.0999999999999998E-2</v>
+      </c>
+      <c r="N37" s="51">
+        <v>0.22</v>
+      </c>
+      <c r="O37" s="51">
+        <v>0.111</v>
+      </c>
+      <c r="P37" s="51">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="Q37" s="1">
         <v>0.13100000000000001</v>
       </c>
-      <c r="N37">
+      <c r="R37">
         <v>0.114</v>
       </c>
-      <c r="O37">
+      <c r="S37">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="P37">
+      <c r="T37">
         <v>6.0999999999999999E-2</v>
       </c>
-      <c r="Q37">
+      <c r="U37">
         <v>7.8E-2</v>
       </c>
-      <c r="R37">
+      <c r="V37">
         <v>0.14499999999999999</v>
       </c>
-      <c r="S37">
+      <c r="W37">
         <v>0.11199999999999999</v>
       </c>
-      <c r="T37">
+      <c r="X37">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="U37">
+      <c r="Y37">
         <v>6.7000000000000004E-2</v>
       </c>
-      <c r="V37">
+      <c r="Z37">
         <v>5.2999999999999999E-2</v>
       </c>
-      <c r="W37">
+      <c r="AA37">
         <v>4.4000000000000004E-2</v>
       </c>
-      <c r="X37">
+      <c r="AB37">
         <v>1.8000000000000002E-2</v>
       </c>
-      <c r="Y37">
+      <c r="AC37">
         <v>5.7000000000000002E-2</v>
       </c>
-      <c r="Z37">
+      <c r="AD37">
         <v>0.11800000000000001</v>
       </c>
-      <c r="AA37">
+      <c r="AE37">
         <v>6.2E-2</v>
       </c>
-      <c r="AB37">
+      <c r="AF37">
         <v>8.199999999999999E-2</v>
       </c>
-      <c r="AC37">
+      <c r="AG37">
         <v>6.5000000000000002E-2</v>
       </c>
-      <c r="AD37">
+      <c r="AH37">
         <v>4.9000000000000002E-2</v>
       </c>
-      <c r="AE37">
+      <c r="AI37">
         <v>5.2000000000000005E-2</v>
       </c>
-      <c r="AF37">
+      <c r="AJ37">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="AG37">
+      <c r="AK37">
         <v>2.2000000000000002E-2</v>
       </c>
-      <c r="AH37">
+      <c r="AL37">
         <v>3.1E-2</v>
       </c>
-      <c r="AI37">
+      <c r="AM37">
         <v>3.4000000000000002E-2</v>
       </c>
-      <c r="AJ37">
+      <c r="AN37">
         <v>5.7000000000000002E-2</v>
       </c>
-      <c r="AK37">
+      <c r="AO37">
         <v>0.02</v>
       </c>
-      <c r="AL37">
+      <c r="AP37">
         <v>1.1000000000000001E-2</v>
       </c>
-      <c r="AM37">
+      <c r="AQ37">
         <v>4.2999999999999997E-2</v>
       </c>
-      <c r="AN37">
+      <c r="AR37">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="AO37">
+      <c r="AS37">
         <v>4.2000000000000003E-2</v>
       </c>
-      <c r="AP37">
+      <c r="AT37">
         <v>2.7999999999999997E-2</v>
       </c>
-      <c r="AQ37">
+      <c r="AU37">
         <v>2.4E-2</v>
       </c>
-      <c r="AR37">
+      <c r="AV37">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="AS37">
+      <c r="AW37">
         <v>4.8000000000000001E-2</v>
       </c>
-      <c r="AT37">
+      <c r="AX37">
         <v>7.6999999999999999E-2</v>
       </c>
-      <c r="AU37">
+      <c r="AY37">
         <v>3.2000000000000001E-2</v>
       </c>
-      <c r="AV37">
+      <c r="AZ37">
         <v>3.7000000000000005E-2</v>
       </c>
-      <c r="AW37">
+      <c r="BA37">
         <v>7.2999999999999995E-2</v>
       </c>
-      <c r="AX37">
+      <c r="BB37">
         <v>3.4000000000000002E-2</v>
       </c>
-      <c r="AY37">
+      <c r="BC37">
         <v>2.8999999999999998E-2</v>
       </c>
-      <c r="AZ37">
+      <c r="BD37">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="BA37" s="7">
+      <c r="BE37" s="7">
         <v>1.4E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A38" s="21" t="s">
         <v>82</v>
       </c>
@@ -3959,160 +3991,172 @@
         <v>13</v>
       </c>
       <c r="E38" s="49">
-        <v>116.4</v>
+        <v>4.3099999999999996</v>
       </c>
       <c r="F38" s="49">
-        <v>116.4</v>
+        <v>4.84</v>
       </c>
       <c r="G38" s="49">
-        <v>116.4</v>
+        <v>5.44</v>
       </c>
       <c r="H38" s="49">
-        <v>116.4</v>
+        <v>6.11</v>
       </c>
       <c r="I38" s="49">
-        <v>116.4</v>
+        <v>6.86</v>
       </c>
       <c r="J38" s="49">
-        <v>116.4</v>
+        <v>7.7</v>
       </c>
       <c r="K38" s="50">
-        <v>14.02</v>
+        <v>8.68</v>
       </c>
       <c r="L38" s="50">
-        <v>14.59</v>
+        <v>9.0399999999999991</v>
       </c>
       <c r="M38" s="50">
+        <v>9.41</v>
+      </c>
+      <c r="N38" s="50">
+        <v>11.48</v>
+      </c>
+      <c r="O38" s="50">
+        <v>12.75</v>
+      </c>
+      <c r="P38" s="50">
+        <v>14.6</v>
+      </c>
+      <c r="Q38" s="50">
         <v>16.5</v>
       </c>
-      <c r="N38" s="50">
+      <c r="R38" s="50">
         <v>18.38</v>
       </c>
-      <c r="O38" s="50">
+      <c r="S38" s="50">
         <v>19.670000000000002</v>
       </c>
-      <c r="P38" s="50">
+      <c r="T38" s="50">
         <v>20.87</v>
       </c>
-      <c r="Q38" s="50">
+      <c r="U38" s="50">
         <v>22.5</v>
       </c>
-      <c r="R38" s="50">
+      <c r="V38" s="50">
         <v>25.9</v>
       </c>
-      <c r="S38" s="1">
+      <c r="W38" s="1">
         <v>28.8</v>
       </c>
-      <c r="T38" s="1">
+      <c r="X38" s="1">
         <v>30.8</v>
       </c>
-      <c r="U38" s="1">
+      <c r="Y38" s="1">
         <v>32.9</v>
       </c>
-      <c r="V38" s="1">
+      <c r="Z38" s="1">
         <v>34.6</v>
       </c>
-      <c r="W38" s="1">
+      <c r="AA38" s="1">
         <v>36.1</v>
       </c>
-      <c r="X38" s="1">
+      <c r="AB38" s="1">
         <v>36.799999999999997</v>
       </c>
-      <c r="Y38" s="1">
+      <c r="AC38" s="1">
         <v>38.9</v>
       </c>
-      <c r="Z38" s="1">
+      <c r="AD38" s="1">
         <v>43.4</v>
       </c>
-      <c r="AA38" s="1">
+      <c r="AE38" s="1">
         <v>46.1</v>
       </c>
-      <c r="AB38" s="1">
+      <c r="AF38" s="1">
         <v>49.9</v>
       </c>
-      <c r="AC38" s="1">
+      <c r="AG38" s="1">
         <v>53.1</v>
       </c>
-      <c r="AD38" s="1">
+      <c r="AH38" s="1">
         <v>55.7</v>
       </c>
-      <c r="AE38" s="1">
+      <c r="AI38" s="1">
         <v>58.6</v>
       </c>
-      <c r="AF38" s="1">
+      <c r="AJ38" s="1">
         <v>59.1</v>
       </c>
-      <c r="AG38" s="1">
+      <c r="AK38" s="1">
         <v>60.4</v>
       </c>
-      <c r="AH38" s="1">
+      <c r="AL38" s="1">
         <v>62.2</v>
       </c>
-      <c r="AI38" s="1">
+      <c r="AM38" s="1">
         <v>64.3</v>
       </c>
-      <c r="AJ38" s="1">
+      <c r="AN38" s="1">
         <v>68</v>
       </c>
-      <c r="AK38" s="1">
+      <c r="AO38" s="1">
         <v>69.3</v>
       </c>
-      <c r="AL38" s="1">
+      <c r="AP38" s="1">
         <v>70.099999999999994</v>
       </c>
-      <c r="AM38" s="1">
+      <c r="AQ38" s="1">
         <v>73.099999999999994</v>
       </c>
-      <c r="AN38" s="1">
+      <c r="AR38" s="1">
         <v>73.599999999999994</v>
       </c>
-      <c r="AO38" s="1">
+      <c r="AS38" s="1">
         <v>76.7</v>
       </c>
-      <c r="AP38" s="1">
+      <c r="AT38" s="1">
         <v>78.900000000000006</v>
       </c>
-      <c r="AQ38" s="1">
+      <c r="AU38" s="1">
         <v>80.8</v>
       </c>
-      <c r="AR38" s="1">
+      <c r="AV38" s="1">
         <v>82.8</v>
       </c>
-      <c r="AS38" s="1">
+      <c r="AW38" s="1">
         <v>86.7</v>
       </c>
-      <c r="AT38" s="1">
+      <c r="AX38" s="1">
         <v>93.4</v>
       </c>
-      <c r="AU38" s="1">
+      <c r="AY38" s="1">
         <v>96.5</v>
       </c>
-      <c r="AV38" s="1">
+      <c r="AZ38" s="1">
         <v>100</v>
       </c>
-      <c r="AW38" s="1">
+      <c r="BA38" s="1">
         <v>107.3</v>
       </c>
-      <c r="AX38" s="1">
+      <c r="BB38" s="1">
         <v>110.9</v>
       </c>
-      <c r="AY38" s="1">
+      <c r="BC38" s="1">
         <v>114.2</v>
       </c>
-      <c r="AZ38" s="1">
+      <c r="BD38" s="1">
         <v>114.8</v>
       </c>
-      <c r="BA38" s="1">
+      <c r="BE38" s="1">
         <v>116.4</v>
       </c>
     </row>
   </sheetData>
   <dataValidations xWindow="382" yWindow="552" count="4">
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E28:BA31 E2:BC2 E4:BC4 E10:BC10 E20:BC20 E22:BC22 E24:BC24 E26:BC26 E12:BC12 E14:BC14 E16:BC16 E18:BC18 E8:BC8 BB28:BC30 N37:AW37">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E28:BE31 E2:BG2 E4:BG4 E10:BG10 E20:BG20 E22:BG22 E24:BG24 E26:BG26 E12:BG12 E14:BG14 E16:BG16 E18:BG18 E8:BG8 BF28:BG30 R37:BA37">
       <formula1>0</formula1>
       <formula2>100</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E9:BC9 BB31:BC31 E3:BC3 E11:BC11 E13:BC13 E15:BC15 E17:BC17 E19:BC19 E21:BC21 E23:BC23 E25:BC25 E27:BC27 E32:BC32 E5:BC7">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E9:BG9 BF31:BG31 E3:BG3 E11:BG11 E13:BG13 E15:BG15 E17:BG17 E19:BG19 E21:BG21 E23:BG23 E25:BG25 E27:BG27 E32:BG32 E5:BG7">
       <formula1>0</formula1>
       <formula2>100000000000000000000</formula2>
     </dataValidation>

</xml_diff>

<commit_message>
Allow time-variant functions for economics
</commit_message>
<xml_diff>
--- a/autumn/xls/programs_fiji.xlsx
+++ b/autumn/xls/programs_fiji.xlsx
@@ -2448,10 +2448,10 @@
   <dimension ref="A1:BN38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="U2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H45" sqref="H45"/>
+      <selection pane="bottomRight" activeCell="U3" sqref="U3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2760,7 +2760,7 @@
       </c>
       <c r="C3" s="6"/>
       <c r="D3" s="44" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="H3" s="7">
         <v>0</v>

</xml_diff>

<commit_message>
Added dummy values for cost of vaccination
</commit_message>
<xml_diff>
--- a/autumn/xls/programs_fiji.xlsx
+++ b/autumn/xls/programs_fiji.xlsx
@@ -2448,10 +2448,10 @@
   <dimension ref="A1:BN38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="U2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="AA2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="U3" sqref="U3"/>
+      <selection pane="bottomRight" activeCell="BD3" sqref="BD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2473,11 +2473,18 @@
     <col min="27" max="28" width="7.42578125" style="1" customWidth="1"/>
     <col min="29" max="29" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="7.140625" style="1" customWidth="1"/>
-    <col min="31" max="42" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="33" max="34" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="36" max="41" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="10" style="1" bestFit="1" customWidth="1"/>
     <col min="43" max="43" width="8" style="1" customWidth="1"/>
-    <col min="44" max="50" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="44" max="48" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="51" max="51" width="8" style="1" customWidth="1"/>
-    <col min="52" max="52" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="10" style="1" bestFit="1" customWidth="1"/>
     <col min="53" max="53" width="6.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="54" max="55" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="56" max="56" width="7.85546875" style="1" customWidth="1"/>
@@ -2756,26 +2763,49 @@
         <v>17</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3" s="6"/>
+        <v>13</v>
+      </c>
+      <c r="C3" s="6">
+        <v>1</v>
+      </c>
       <c r="D3" s="44" t="s">
         <v>13</v>
       </c>
+      <c r="E3" s="7">
+        <v>0</v>
+      </c>
+      <c r="F3" s="7">
+        <v>0</v>
+      </c>
+      <c r="G3" s="7">
+        <v>0</v>
+      </c>
       <c r="H3" s="7">
         <v>0</v>
       </c>
+      <c r="I3" s="7">
+        <v>0</v>
+      </c>
       <c r="J3" s="7">
-        <v>10000000</v>
+        <v>300000</v>
       </c>
       <c r="Q3" s="7">
-        <v>15040500</v>
+        <v>400000</v>
       </c>
       <c r="AA3" s="7">
-        <v>39034561</v>
-      </c>
-      <c r="AB3" s="7">
-        <v>1</v>
+        <v>500000</v>
+      </c>
+      <c r="AI3" s="7">
+        <v>1000000</v>
+      </c>
+      <c r="AP3" s="7">
+        <v>2000000</v>
+      </c>
+      <c r="AZ3" s="7">
+        <v>3000000</v>
+      </c>
+      <c r="BD3" s="7">
+        <v>3500000</v>
       </c>
     </row>
     <row r="4" spans="1:66" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -4156,7 +4186,7 @@
       <formula1>0</formula1>
       <formula2>100</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E9:BG9 BF31:BG31 E3:BG3 E11:BG11 E13:BG13 E15:BG15 E17:BG17 E19:BG19 E21:BG21 E23:BG23 E25:BG25 E27:BG27 E32:BG32 E5:BG7">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E9:BG9 BF31:BG31 E5:BG7 E11:BG11 E13:BG13 E15:BG15 E17:BG17 E19:BG19 E21:BG21 E23:BG23 E25:BG25 E27:BG27 E32:BG32 E3:BG3">
       <formula1>0</formula1>
       <formula2>100000000000000000000</formula2>
     </dataValidation>

</xml_diff>

<commit_message>
Added some dummy cost data
</commit_message>
<xml_diff>
--- a/autumn/xls/programs_fiji.xlsx
+++ b/autumn/xls/programs_fiji.xlsx
@@ -2451,7 +2451,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="AA2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="BD3" sqref="BD3"/>
+      <selection pane="bottomRight" activeCell="AZ5" sqref="AZ5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2480,7 +2480,9 @@
     <col min="36" max="41" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="42" max="42" width="10" style="1" bestFit="1" customWidth="1"/>
     <col min="43" max="43" width="8" style="1" customWidth="1"/>
-    <col min="44" max="48" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="44" max="45" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="46" max="47" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="49" max="49" width="10" style="1" bestFit="1" customWidth="1"/>
     <col min="50" max="50" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="51" max="51" width="8" style="1" customWidth="1"/>
@@ -2801,11 +2803,38 @@
       <c r="AP3" s="7">
         <v>2000000</v>
       </c>
+      <c r="AT3" s="7">
+        <v>2500000</v>
+      </c>
+      <c r="AU3" s="7">
+        <v>2500000</v>
+      </c>
+      <c r="AV3" s="7">
+        <v>2500000</v>
+      </c>
+      <c r="AW3" s="7">
+        <v>2500000</v>
+      </c>
+      <c r="AX3" s="7">
+        <v>2500000</v>
+      </c>
+      <c r="AY3" s="7">
+        <v>2500000</v>
+      </c>
       <c r="AZ3" s="7">
-        <v>3000000</v>
+        <v>2500000</v>
+      </c>
+      <c r="BA3" s="7">
+        <v>2500000</v>
+      </c>
+      <c r="BB3" s="7">
+        <v>2500000</v>
+      </c>
+      <c r="BC3" s="7">
+        <v>2500000</v>
       </c>
       <c r="BD3" s="7">
-        <v>3500000</v>
+        <v>2500000</v>
       </c>
     </row>
     <row r="4" spans="1:66" s="9" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Adjust case detection scenarios
</commit_message>
<xml_diff>
--- a/autumn/xls/programs_fiji.xlsx
+++ b/autumn/xls/programs_fiji.xlsx
@@ -2265,7 +2265,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2448,10 +2448,10 @@
   <dimension ref="A1:BN38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="AA2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="AN2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AZ5" sqref="AZ5"/>
+      <selection pane="bottomRight" activeCell="BC9" sqref="BC9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2887,13 +2887,13 @@
         <v>50</v>
       </c>
       <c r="BH4" s="9">
-        <v>85</v>
+        <v>60</v>
       </c>
       <c r="BI4" s="9">
-        <v>90</v>
+        <v>75</v>
       </c>
       <c r="BN4" s="9">
-        <v>90</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:66" s="9" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Refactor inflation to econ_inflation
Making sure all economic parameters are distinguished.
</commit_message>
<xml_diff>
--- a/autumn/xls/programs_fiji.xlsx
+++ b/autumn/xls/programs_fiji.xlsx
@@ -258,13 +258,13 @@
     <t>program_cost_ipt</t>
   </si>
   <si>
-    <t>inflation</t>
-  </si>
-  <si>
     <t>scenario_9</t>
   </si>
   <si>
     <t>econ_cpi</t>
+  </si>
+  <si>
+    <t>econ_inflation</t>
   </si>
 </sst>
 </file>
@@ -2451,7 +2451,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A39" sqref="A39"/>
+      <selection pane="bottomRight" activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2693,7 +2693,7 @@
         <v>77</v>
       </c>
       <c r="BN1" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:66" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -3865,7 +3865,7 @@
     </row>
     <row r="37" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A37" s="21" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>13</v>
@@ -4038,7 +4038,7 @@
     </row>
     <row r="38" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A38" s="21" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
Model now runs for any country
Even if spreadsheets absent, the model will still run.
</commit_message>
<xml_diff>
--- a/autumn/xls/programs_fiji.xlsx
+++ b/autumn/xls/programs_fiji.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="435" windowWidth="20370" windowHeight="7410" tabRatio="807" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="435" windowWidth="20370" windowHeight="7410" tabRatio="807"/>
   </bookViews>
   <sheets>
     <sheet name="country_constants" sheetId="1" r:id="rId1"/>
@@ -2242,8 +2242,8 @@
   </sheetPr>
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2425,7 +2425,7 @@
   </sheetPr>
   <dimension ref="A1:BN33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>

</xml_diff>